<commit_message>
Inclusão de melhorias @202405151026
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C76FB8D-5738-49D2-ABCF-C87DC37DB3C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A01DD2C-4C5F-4426-BE51-AA13217F20B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="3280" windowWidth="19420" windowHeight="10300" tabRatio="699" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -53951,8 +53951,8 @@
   <dimension ref="A1:C354"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A154" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B164" sqref="B164"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56186,10 +56186,10 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>3716</v>
-      </c>
-      <c r="B203" t="s">
-        <v>3717</v>
+        <v>40</v>
+      </c>
+      <c r="B203" s="3" t="s">
+        <v>3836</v>
       </c>
       <c r="C203" t="s">
         <v>3576</v>
@@ -56197,10 +56197,10 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>33</v>
-      </c>
-      <c r="B204" s="3" t="s">
-        <v>134</v>
+        <v>3716</v>
+      </c>
+      <c r="B204" t="s">
+        <v>3717</v>
       </c>
       <c r="C204" t="s">
         <v>3576</v>
@@ -56208,10 +56208,10 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C205" t="s">
         <v>3576</v>
@@ -56219,10 +56219,10 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B206" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C206" t="s">
         <v>3576</v>
@@ -56230,10 +56230,10 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B207" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C207" t="s">
         <v>3576</v>
@@ -56241,10 +56241,10 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B208" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C208" t="s">
         <v>3576</v>
@@ -56252,10 +56252,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
       <c r="B209" s="3" t="s">
-        <v>3836</v>
+        <v>133</v>
       </c>
       <c r="C209" t="s">
         <v>3576</v>
@@ -57857,7 +57857,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C354" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
+  <autoFilter ref="A1:C354" xr:uid="{00000000-0009-0000-0000-000007000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C354">
+      <sortCondition ref="C1:C354"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C276">
     <sortCondition ref="C2:C276"/>
     <sortCondition ref="B2:B276"/>

</xml_diff>

<commit_message>
Inclusão de melhorias @202405161042
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4BDB912-9FBC-44EB-9DFD-88EBEE2F5C10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6614D81C-744F-46AB-9C76-23FA739135CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" tabRatio="699" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="3280" windowWidth="19420" windowHeight="10300" tabRatio="699" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="market" sheetId="8" r:id="rId1"/>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11342" uniqueCount="3922">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11378" uniqueCount="3946">
   <si>
     <t>bbgTicker</t>
   </si>
@@ -11835,6 +11835,78 @@
   </si>
   <si>
     <t>br_ipca_38y</t>
+  </si>
+  <si>
+    <t>br_igp10_index</t>
+  </si>
+  <si>
+    <t>br_igp10_yoy</t>
+  </si>
+  <si>
+    <t>br_igp10_mom</t>
+  </si>
+  <si>
+    <t>IBREIGP1 Index</t>
+  </si>
+  <si>
+    <t>IBREIGPM Index</t>
+  </si>
+  <si>
+    <t>IBREGP1M Index</t>
+  </si>
+  <si>
+    <t>IBREGP1Y Index</t>
+  </si>
+  <si>
+    <t>IBREGPMM Index</t>
+  </si>
+  <si>
+    <t>IBREGPMY Index</t>
+  </si>
+  <si>
+    <t>br_igpm_index</t>
+  </si>
+  <si>
+    <t>br_igpm_mom</t>
+  </si>
+  <si>
+    <t>br_igpm_yoy</t>
+  </si>
+  <si>
+    <t>IBREIPA1 Index</t>
+  </si>
+  <si>
+    <t>IBREPA1M Index</t>
+  </si>
+  <si>
+    <t>IBREPA1Y Index</t>
+  </si>
+  <si>
+    <t>br_ipa10_index</t>
+  </si>
+  <si>
+    <t>br_ipa10_mom</t>
+  </si>
+  <si>
+    <t>br_ipa10_yoy</t>
+  </si>
+  <si>
+    <t>IBREINC1 Index</t>
+  </si>
+  <si>
+    <t>IBRENC1M Index</t>
+  </si>
+  <si>
+    <t>IBRENC1Y Index</t>
+  </si>
+  <si>
+    <t>br_incc10_index</t>
+  </si>
+  <si>
+    <t>br_incc10_mom</t>
+  </si>
+  <si>
+    <t>br_incc10_yoy</t>
   </si>
 </sst>
 </file>
@@ -54211,11 +54283,11 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Planilha9"/>
-  <dimension ref="A1:C389"/>
+  <dimension ref="A1:C401"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A228" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G245" sqref="G245"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56306,10 +56378,10 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>3717</v>
+        <v>3925</v>
       </c>
       <c r="B190" t="s">
-        <v>3720</v>
+        <v>3922</v>
       </c>
       <c r="C190" t="s">
         <v>3575</v>
@@ -56317,10 +56389,10 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>3718</v>
+        <v>3927</v>
       </c>
       <c r="B191" t="s">
-        <v>3721</v>
+        <v>3924</v>
       </c>
       <c r="C191" t="s">
         <v>3575</v>
@@ -56328,10 +56400,10 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>3719</v>
+        <v>3928</v>
       </c>
       <c r="B192" t="s">
-        <v>3722</v>
+        <v>3923</v>
       </c>
       <c r="C192" t="s">
         <v>3575</v>
@@ -56339,10 +56411,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>3529</v>
+        <v>3717</v>
       </c>
       <c r="B193" t="s">
-        <v>3530</v>
+        <v>3720</v>
       </c>
       <c r="C193" t="s">
         <v>3575</v>
@@ -56350,10 +56422,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>3532</v>
+        <v>3718</v>
       </c>
       <c r="B194" t="s">
-        <v>3531</v>
+        <v>3721</v>
       </c>
       <c r="C194" t="s">
         <v>3575</v>
@@ -56361,10 +56433,10 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>27</v>
-      </c>
-      <c r="B195" s="3" t="s">
-        <v>128</v>
+        <v>3719</v>
+      </c>
+      <c r="B195" t="s">
+        <v>3722</v>
       </c>
       <c r="C195" t="s">
         <v>3575</v>
@@ -56372,10 +56444,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>3867</v>
+        <v>3926</v>
       </c>
       <c r="B196" t="s">
-        <v>3895</v>
+        <v>3931</v>
       </c>
       <c r="C196" t="s">
         <v>3575</v>
@@ -56383,10 +56455,10 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>3865</v>
+        <v>3930</v>
       </c>
       <c r="B197" t="s">
-        <v>3896</v>
+        <v>3932</v>
       </c>
       <c r="C197" t="s">
         <v>3575</v>
@@ -56394,10 +56466,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>3868</v>
+        <v>3929</v>
       </c>
       <c r="B198" t="s">
-        <v>3897</v>
+        <v>3933</v>
       </c>
       <c r="C198" t="s">
         <v>3575</v>
@@ -56405,10 +56477,10 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>3869</v>
+        <v>3529</v>
       </c>
       <c r="B199" t="s">
-        <v>3898</v>
+        <v>3530</v>
       </c>
       <c r="C199" t="s">
         <v>3575</v>
@@ -56416,10 +56488,10 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>3857</v>
+        <v>3532</v>
       </c>
       <c r="B200" t="s">
-        <v>3899</v>
+        <v>3531</v>
       </c>
       <c r="C200" t="s">
         <v>3575</v>
@@ -56427,10 +56499,10 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>3870</v>
+        <v>3940</v>
       </c>
       <c r="B201" t="s">
-        <v>3900</v>
+        <v>3943</v>
       </c>
       <c r="C201" t="s">
         <v>3575</v>
@@ -56438,10 +56510,10 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>3871</v>
+        <v>3941</v>
       </c>
       <c r="B202" t="s">
-        <v>3901</v>
+        <v>3944</v>
       </c>
       <c r="C202" t="s">
         <v>3575</v>
@@ -56449,10 +56521,10 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>3872</v>
+        <v>3942</v>
       </c>
       <c r="B203" t="s">
-        <v>3902</v>
+        <v>3945</v>
       </c>
       <c r="C203" t="s">
         <v>3575</v>
@@ -56460,21 +56532,21 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>3873</v>
+        <v>3934</v>
       </c>
       <c r="B204" t="s">
-        <v>3903</v>
+        <v>3937</v>
       </c>
       <c r="C204" t="s">
         <v>3575</v>
       </c>
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A205" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B205" s="3" t="s">
-        <v>124</v>
+      <c r="A205" t="s">
+        <v>3935</v>
+      </c>
+      <c r="B205" t="s">
+        <v>3938</v>
       </c>
       <c r="C205" t="s">
         <v>3575</v>
@@ -56482,10 +56554,10 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>3861</v>
+        <v>3936</v>
       </c>
       <c r="B206" t="s">
-        <v>3904</v>
+        <v>3939</v>
       </c>
       <c r="C206" t="s">
         <v>3575</v>
@@ -56493,10 +56565,10 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>3874</v>
-      </c>
-      <c r="B207" t="s">
-        <v>3905</v>
+        <v>27</v>
+      </c>
+      <c r="B207" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="C207" t="s">
         <v>3575</v>
@@ -56504,10 +56576,10 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>3875</v>
+        <v>3867</v>
       </c>
       <c r="B208" t="s">
-        <v>3906</v>
+        <v>3895</v>
       </c>
       <c r="C208" t="s">
         <v>3575</v>
@@ -56515,10 +56587,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>3876</v>
+        <v>3865</v>
       </c>
       <c r="B209" t="s">
-        <v>3907</v>
+        <v>3896</v>
       </c>
       <c r="C209" t="s">
         <v>3575</v>
@@ -56526,10 +56598,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>3877</v>
+        <v>3868</v>
       </c>
       <c r="B210" t="s">
-        <v>3908</v>
+        <v>3897</v>
       </c>
       <c r="C210" t="s">
         <v>3575</v>
@@ -56537,10 +56609,10 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>3866</v>
+        <v>3869</v>
       </c>
       <c r="B211" t="s">
-        <v>3909</v>
+        <v>3898</v>
       </c>
       <c r="C211" t="s">
         <v>3575</v>
@@ -56548,10 +56620,10 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>3859</v>
+        <v>3857</v>
       </c>
       <c r="B212" t="s">
-        <v>3910</v>
+        <v>3899</v>
       </c>
       <c r="C212" t="s">
         <v>3575</v>
@@ -56559,10 +56631,10 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>3878</v>
+        <v>3870</v>
       </c>
       <c r="B213" t="s">
-        <v>3911</v>
+        <v>3900</v>
       </c>
       <c r="C213" t="s">
         <v>3575</v>
@@ -56570,10 +56642,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>3879</v>
+        <v>3871</v>
       </c>
       <c r="B214" t="s">
-        <v>3912</v>
+        <v>3901</v>
       </c>
       <c r="C214" t="s">
         <v>3575</v>
@@ -56581,32 +56653,32 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>3863</v>
+        <v>3872</v>
       </c>
       <c r="B215" t="s">
-        <v>3913</v>
+        <v>3902</v>
       </c>
       <c r="C215" t="s">
         <v>3575</v>
       </c>
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A216" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B216" s="3" t="s">
-        <v>125</v>
+      <c r="A216" t="s">
+        <v>3873</v>
+      </c>
+      <c r="B216" t="s">
+        <v>3903</v>
       </c>
       <c r="C216" t="s">
         <v>3575</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>3856</v>
-      </c>
-      <c r="B217" t="s">
-        <v>3914</v>
+      <c r="A217" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B217" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="C217" t="s">
         <v>3575</v>
@@ -56614,10 +56686,10 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>3880</v>
+        <v>3861</v>
       </c>
       <c r="B218" t="s">
-        <v>3915</v>
+        <v>3904</v>
       </c>
       <c r="C218" t="s">
         <v>3575</v>
@@ -56625,10 +56697,10 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>3881</v>
+        <v>3874</v>
       </c>
       <c r="B219" t="s">
-        <v>3916</v>
+        <v>3905</v>
       </c>
       <c r="C219" t="s">
         <v>3575</v>
@@ -56636,10 +56708,10 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>3882</v>
+        <v>3875</v>
       </c>
       <c r="B220" t="s">
-        <v>3917</v>
+        <v>3906</v>
       </c>
       <c r="C220" t="s">
         <v>3575</v>
@@ -56647,10 +56719,10 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>3883</v>
+        <v>3876</v>
       </c>
       <c r="B221" t="s">
-        <v>3918</v>
+        <v>3907</v>
       </c>
       <c r="C221" t="s">
         <v>3575</v>
@@ -56658,10 +56730,10 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>28</v>
-      </c>
-      <c r="B222" s="3" t="s">
-        <v>129</v>
+        <v>3877</v>
+      </c>
+      <c r="B222" t="s">
+        <v>3908</v>
       </c>
       <c r="C222" t="s">
         <v>3575</v>
@@ -56669,10 +56741,10 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>3884</v>
+        <v>3866</v>
       </c>
       <c r="B223" t="s">
-        <v>3919</v>
+        <v>3909</v>
       </c>
       <c r="C223" t="s">
         <v>3575</v>
@@ -56680,10 +56752,10 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>3885</v>
+        <v>3859</v>
       </c>
       <c r="B224" t="s">
-        <v>3920</v>
+        <v>3910</v>
       </c>
       <c r="C224" t="s">
         <v>3575</v>
@@ -56691,10 +56763,10 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>3886</v>
+        <v>3878</v>
       </c>
       <c r="B225" t="s">
-        <v>3921</v>
+        <v>3911</v>
       </c>
       <c r="C225" t="s">
         <v>3575</v>
@@ -56702,10 +56774,10 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>25</v>
-      </c>
-      <c r="B226" s="3" t="s">
-        <v>126</v>
+        <v>3879</v>
+      </c>
+      <c r="B226" t="s">
+        <v>3912</v>
       </c>
       <c r="C226" t="s">
         <v>3575</v>
@@ -56713,21 +56785,21 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>3862</v>
+        <v>3863</v>
       </c>
       <c r="B227" t="s">
-        <v>3890</v>
+        <v>3913</v>
       </c>
       <c r="C227" t="s">
         <v>3575</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228" t="s">
-        <v>26</v>
+      <c r="A228" s="3" t="s">
+        <v>24</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C228" t="s">
         <v>3575</v>
@@ -56735,10 +56807,10 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>3860</v>
+        <v>3856</v>
       </c>
       <c r="B229" t="s">
-        <v>3891</v>
+        <v>3914</v>
       </c>
       <c r="C229" t="s">
         <v>3575</v>
@@ -56746,10 +56818,10 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>3858</v>
+        <v>3880</v>
       </c>
       <c r="B230" t="s">
-        <v>3892</v>
+        <v>3915</v>
       </c>
       <c r="C230" t="s">
         <v>3575</v>
@@ -56757,10 +56829,10 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>3887</v>
+        <v>3881</v>
       </c>
       <c r="B231" t="s">
-        <v>3893</v>
+        <v>3916</v>
       </c>
       <c r="C231" t="s">
         <v>3575</v>
@@ -56768,10 +56840,10 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>3888</v>
+        <v>3882</v>
       </c>
       <c r="B232" t="s">
-        <v>3894</v>
+        <v>3917</v>
       </c>
       <c r="C232" t="s">
         <v>3575</v>
@@ -56779,10 +56851,10 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>3472</v>
+        <v>3883</v>
       </c>
       <c r="B233" t="s">
-        <v>3470</v>
+        <v>3918</v>
       </c>
       <c r="C233" t="s">
         <v>3575</v>
@@ -56790,10 +56862,10 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>3467</v>
-      </c>
-      <c r="B234" t="s">
-        <v>3471</v>
+        <v>28</v>
+      </c>
+      <c r="B234" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="C234" t="s">
         <v>3575</v>
@@ -56801,10 +56873,10 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>3469</v>
+        <v>3884</v>
       </c>
       <c r="B235" t="s">
-        <v>3468</v>
+        <v>3919</v>
       </c>
       <c r="C235" t="s">
         <v>3575</v>
@@ -56812,10 +56884,10 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>3528</v>
+        <v>3885</v>
       </c>
       <c r="B236" t="s">
-        <v>3569</v>
+        <v>3920</v>
       </c>
       <c r="C236" t="s">
         <v>3575</v>
@@ -56823,10 +56895,10 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>40</v>
-      </c>
-      <c r="B237" s="3" t="s">
-        <v>3834</v>
+        <v>3886</v>
+      </c>
+      <c r="B237" t="s">
+        <v>3921</v>
       </c>
       <c r="C237" t="s">
         <v>3575</v>
@@ -56834,10 +56906,10 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>3715</v>
-      </c>
-      <c r="B238" t="s">
-        <v>3716</v>
+        <v>25</v>
+      </c>
+      <c r="B238" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C238" t="s">
         <v>3575</v>
@@ -56845,10 +56917,10 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>33</v>
-      </c>
-      <c r="B239" s="3" t="s">
-        <v>134</v>
+        <v>3862</v>
+      </c>
+      <c r="B239" t="s">
+        <v>3890</v>
       </c>
       <c r="C239" t="s">
         <v>3575</v>
@@ -56856,10 +56928,10 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B240" s="3" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C240" t="s">
         <v>3575</v>
@@ -56867,10 +56939,10 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>30</v>
-      </c>
-      <c r="B241" s="3" t="s">
-        <v>131</v>
+        <v>3860</v>
+      </c>
+      <c r="B241" t="s">
+        <v>3891</v>
       </c>
       <c r="C241" t="s">
         <v>3575</v>
@@ -56878,10 +56950,10 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>31</v>
-      </c>
-      <c r="B242" s="3" t="s">
-        <v>132</v>
+        <v>3858</v>
+      </c>
+      <c r="B242" t="s">
+        <v>3892</v>
       </c>
       <c r="C242" t="s">
         <v>3575</v>
@@ -56889,10 +56961,10 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>3864</v>
-      </c>
-      <c r="B243" s="3" t="s">
-        <v>3889</v>
+        <v>3887</v>
+      </c>
+      <c r="B243" t="s">
+        <v>3893</v>
       </c>
       <c r="C243" t="s">
         <v>3575</v>
@@ -56900,10 +56972,10 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>32</v>
-      </c>
-      <c r="B244" s="3" t="s">
-        <v>133</v>
+        <v>3888</v>
+      </c>
+      <c r="B244" t="s">
+        <v>3894</v>
       </c>
       <c r="C244" t="s">
         <v>3575</v>
@@ -56911,10 +56983,10 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>3698</v>
+        <v>3472</v>
       </c>
       <c r="B245" t="s">
-        <v>3699</v>
+        <v>3470</v>
       </c>
       <c r="C245" t="s">
         <v>3575</v>
@@ -56922,10 +56994,10 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>3697</v>
+        <v>3467</v>
       </c>
       <c r="B246" t="s">
-        <v>3700</v>
+        <v>3471</v>
       </c>
       <c r="C246" t="s">
         <v>3575</v>
@@ -56933,10 +57005,10 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>42</v>
+        <v>3469</v>
       </c>
       <c r="B247" t="s">
-        <v>3701</v>
+        <v>3468</v>
       </c>
       <c r="C247" t="s">
         <v>3575</v>
@@ -56944,10 +57016,10 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>375</v>
+        <v>3528</v>
       </c>
       <c r="B248" t="s">
-        <v>376</v>
+        <v>3569</v>
       </c>
       <c r="C248" t="s">
         <v>3575</v>
@@ -56955,10 +57027,10 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>285</v>
-      </c>
-      <c r="B249" t="s">
-        <v>283</v>
+        <v>40</v>
+      </c>
+      <c r="B249" s="3" t="s">
+        <v>3834</v>
       </c>
       <c r="C249" t="s">
         <v>3575</v>
@@ -56966,10 +57038,10 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>286</v>
+        <v>3715</v>
       </c>
       <c r="B250" t="s">
-        <v>284</v>
+        <v>3716</v>
       </c>
       <c r="C250" t="s">
         <v>3575</v>
@@ -56977,10 +57049,10 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>395</v>
-      </c>
-      <c r="B251" t="s">
-        <v>396</v>
+        <v>33</v>
+      </c>
+      <c r="B251" s="3" t="s">
+        <v>134</v>
       </c>
       <c r="C251" t="s">
         <v>3575</v>
@@ -56988,10 +57060,10 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>325</v>
-      </c>
-      <c r="B252" t="s">
-        <v>323</v>
+        <v>29</v>
+      </c>
+      <c r="B252" s="3" t="s">
+        <v>130</v>
       </c>
       <c r="C252" t="s">
         <v>3575</v>
@@ -56999,10 +57071,10 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>326</v>
-      </c>
-      <c r="B253" t="s">
-        <v>324</v>
+        <v>30</v>
+      </c>
+      <c r="B253" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="C253" t="s">
         <v>3575</v>
@@ -57010,10 +57082,10 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>387</v>
-      </c>
-      <c r="B254" t="s">
-        <v>388</v>
+        <v>31</v>
+      </c>
+      <c r="B254" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="C254" t="s">
         <v>3575</v>
@@ -57021,10 +57093,10 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>309</v>
-      </c>
-      <c r="B255" t="s">
-        <v>307</v>
+        <v>3864</v>
+      </c>
+      <c r="B255" s="3" t="s">
+        <v>3889</v>
       </c>
       <c r="C255" t="s">
         <v>3575</v>
@@ -57032,10 +57104,10 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>310</v>
-      </c>
-      <c r="B256" t="s">
-        <v>308</v>
+        <v>32</v>
+      </c>
+      <c r="B256" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="C256" t="s">
         <v>3575</v>
@@ -57043,10 +57115,10 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>403</v>
+        <v>3698</v>
       </c>
       <c r="B257" t="s">
-        <v>404</v>
+        <v>3699</v>
       </c>
       <c r="C257" t="s">
         <v>3575</v>
@@ -57054,10 +57126,10 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>343</v>
+        <v>3697</v>
       </c>
       <c r="B258" t="s">
-        <v>339</v>
+        <v>3700</v>
       </c>
       <c r="C258" t="s">
         <v>3575</v>
@@ -57065,10 +57137,10 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>344</v>
+        <v>42</v>
       </c>
       <c r="B259" t="s">
-        <v>340</v>
+        <v>3701</v>
       </c>
       <c r="C259" t="s">
         <v>3575</v>
@@ -57076,10 +57148,10 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="B260" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="C260" t="s">
         <v>3575</v>
@@ -57087,10 +57159,10 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>269</v>
+        <v>285</v>
       </c>
       <c r="B261" t="s">
-        <v>271</v>
+        <v>283</v>
       </c>
       <c r="C261" t="s">
         <v>3575</v>
@@ -57098,10 +57170,10 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>270</v>
+        <v>286</v>
       </c>
       <c r="B262" t="s">
-        <v>272</v>
+        <v>284</v>
       </c>
       <c r="C262" t="s">
         <v>3575</v>
@@ -57109,10 +57181,10 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>364</v>
+        <v>395</v>
       </c>
       <c r="B263" t="s">
-        <v>365</v>
+        <v>396</v>
       </c>
       <c r="C263" t="s">
         <v>3575</v>
@@ -57120,10 +57192,10 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>267</v>
+        <v>325</v>
       </c>
       <c r="B264" t="s">
-        <v>261</v>
+        <v>323</v>
       </c>
       <c r="C264" t="s">
         <v>3575</v>
@@ -57131,10 +57203,10 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>268</v>
+        <v>326</v>
       </c>
       <c r="B265" t="s">
-        <v>262</v>
+        <v>324</v>
       </c>
       <c r="C265" t="s">
         <v>3575</v>
@@ -57142,10 +57214,10 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>405</v>
+        <v>387</v>
       </c>
       <c r="B266" t="s">
-        <v>406</v>
+        <v>388</v>
       </c>
       <c r="C266" t="s">
         <v>3575</v>
@@ -57153,10 +57225,10 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>345</v>
+        <v>309</v>
       </c>
       <c r="B267" t="s">
-        <v>341</v>
+        <v>307</v>
       </c>
       <c r="C267" t="s">
         <v>3575</v>
@@ -57164,10 +57236,10 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>346</v>
+        <v>310</v>
       </c>
       <c r="B268" t="s">
-        <v>342</v>
+        <v>308</v>
       </c>
       <c r="C268" t="s">
         <v>3575</v>
@@ -57175,10 +57247,10 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="B269" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="C269" t="s">
         <v>3575</v>
@@ -57186,10 +57258,10 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>335</v>
+        <v>343</v>
       </c>
       <c r="B270" t="s">
-        <v>331</v>
+        <v>339</v>
       </c>
       <c r="C270" t="s">
         <v>3575</v>
@@ -57197,10 +57269,10 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="B271" t="s">
-        <v>332</v>
+        <v>340</v>
       </c>
       <c r="C271" t="s">
         <v>3575</v>
@@ -57208,10 +57280,10 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>401</v>
+        <v>368</v>
       </c>
       <c r="B272" t="s">
-        <v>402</v>
+        <v>369</v>
       </c>
       <c r="C272" t="s">
         <v>3575</v>
@@ -57219,10 +57291,10 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>337</v>
+        <v>269</v>
       </c>
       <c r="B273" t="s">
-        <v>333</v>
+        <v>271</v>
       </c>
       <c r="C273" t="s">
         <v>3575</v>
@@ -57230,10 +57302,10 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>338</v>
+        <v>270</v>
       </c>
       <c r="B274" t="s">
-        <v>334</v>
+        <v>272</v>
       </c>
       <c r="C274" t="s">
         <v>3575</v>
@@ -57241,10 +57313,10 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="B275" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="C275" t="s">
         <v>3575</v>
@@ -57252,10 +57324,10 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>275</v>
+        <v>267</v>
       </c>
       <c r="B276" t="s">
-        <v>273</v>
+        <v>261</v>
       </c>
       <c r="C276" t="s">
         <v>3575</v>
@@ -57263,10 +57335,10 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>276</v>
+        <v>268</v>
       </c>
       <c r="B277" t="s">
-        <v>274</v>
+        <v>262</v>
       </c>
       <c r="C277" t="s">
         <v>3575</v>
@@ -57274,10 +57346,10 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>379</v>
+        <v>405</v>
       </c>
       <c r="B278" t="s">
-        <v>380</v>
+        <v>406</v>
       </c>
       <c r="C278" t="s">
         <v>3575</v>
@@ -57285,10 +57357,10 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>293</v>
+        <v>345</v>
       </c>
       <c r="B279" t="s">
-        <v>291</v>
+        <v>341</v>
       </c>
       <c r="C279" t="s">
         <v>3575</v>
@@ -57296,10 +57368,10 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>294</v>
+        <v>346</v>
       </c>
       <c r="B280" t="s">
-        <v>292</v>
+        <v>342</v>
       </c>
       <c r="C280" t="s">
         <v>3575</v>
@@ -57307,10 +57379,10 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="B281" t="s">
-        <v>398</v>
+        <v>400</v>
       </c>
       <c r="C281" t="s">
         <v>3575</v>
@@ -57318,10 +57390,10 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>329</v>
+        <v>335</v>
       </c>
       <c r="B282" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="C282" t="s">
         <v>3575</v>
@@ -57329,10 +57401,10 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>330</v>
+        <v>336</v>
       </c>
       <c r="B283" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="C283" t="s">
         <v>3575</v>
@@ -57340,10 +57412,10 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>372</v>
+        <v>401</v>
       </c>
       <c r="B284" t="s">
-        <v>3448</v>
+        <v>402</v>
       </c>
       <c r="C284" t="s">
         <v>3575</v>
@@ -57351,10 +57423,10 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>277</v>
+        <v>337</v>
       </c>
       <c r="B285" t="s">
-        <v>3449</v>
+        <v>333</v>
       </c>
       <c r="C285" t="s">
         <v>3575</v>
@@ -57362,10 +57434,10 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>278</v>
+        <v>338</v>
       </c>
       <c r="B286" t="s">
-        <v>3450</v>
+        <v>334</v>
       </c>
       <c r="C286" t="s">
         <v>3575</v>
@@ -57373,10 +57445,10 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="B287" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="C287" t="s">
         <v>3575</v>
@@ -57384,10 +57456,10 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>289</v>
+        <v>275</v>
       </c>
       <c r="B288" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="C288" t="s">
         <v>3575</v>
@@ -57395,10 +57467,10 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>290</v>
+        <v>276</v>
       </c>
       <c r="B289" t="s">
-        <v>288</v>
+        <v>274</v>
       </c>
       <c r="C289" t="s">
         <v>3575</v>
@@ -57406,10 +57478,10 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>409</v>
+        <v>379</v>
       </c>
       <c r="B290" t="s">
-        <v>410</v>
+        <v>380</v>
       </c>
       <c r="C290" t="s">
         <v>3575</v>
@@ -57417,10 +57489,10 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>353</v>
+        <v>293</v>
       </c>
       <c r="B291" t="s">
-        <v>349</v>
+        <v>291</v>
       </c>
       <c r="C291" t="s">
         <v>3575</v>
@@ -57428,10 +57500,10 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>354</v>
+        <v>294</v>
       </c>
       <c r="B292" t="s">
-        <v>350</v>
+        <v>292</v>
       </c>
       <c r="C292" t="s">
         <v>3575</v>
@@ -57439,10 +57511,10 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>407</v>
+        <v>397</v>
       </c>
       <c r="B293" t="s">
-        <v>408</v>
+        <v>398</v>
       </c>
       <c r="C293" t="s">
         <v>3575</v>
@@ -57450,10 +57522,10 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>351</v>
+        <v>329</v>
       </c>
       <c r="B294" t="s">
-        <v>347</v>
+        <v>327</v>
       </c>
       <c r="C294" t="s">
         <v>3575</v>
@@ -57461,10 +57533,10 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>352</v>
+        <v>330</v>
       </c>
       <c r="B295" t="s">
-        <v>348</v>
+        <v>328</v>
       </c>
       <c r="C295" t="s">
         <v>3575</v>
@@ -57472,10 +57544,10 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>391</v>
+        <v>372</v>
       </c>
       <c r="B296" t="s">
-        <v>392</v>
+        <v>3448</v>
       </c>
       <c r="C296" t="s">
         <v>3575</v>
@@ -57483,10 +57555,10 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>321</v>
+        <v>277</v>
       </c>
       <c r="B297" t="s">
-        <v>315</v>
+        <v>3449</v>
       </c>
       <c r="C297" t="s">
         <v>3575</v>
@@ -57494,10 +57566,10 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>322</v>
+        <v>278</v>
       </c>
       <c r="B298" t="s">
-        <v>316</v>
+        <v>3450</v>
       </c>
       <c r="C298" t="s">
         <v>3575</v>
@@ -57505,10 +57577,10 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>389</v>
+        <v>377</v>
       </c>
       <c r="B299" t="s">
-        <v>390</v>
+        <v>378</v>
       </c>
       <c r="C299" t="s">
         <v>3575</v>
@@ -57516,10 +57588,10 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>311</v>
+        <v>289</v>
       </c>
       <c r="B300" t="s">
-        <v>313</v>
+        <v>287</v>
       </c>
       <c r="C300" t="s">
         <v>3575</v>
@@ -57527,10 +57599,10 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>312</v>
+        <v>290</v>
       </c>
       <c r="B301" t="s">
-        <v>314</v>
+        <v>288</v>
       </c>
       <c r="C301" t="s">
         <v>3575</v>
@@ -57538,10 +57610,10 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>366</v>
+        <v>409</v>
       </c>
       <c r="B302" t="s">
-        <v>367</v>
+        <v>410</v>
       </c>
       <c r="C302" t="s">
         <v>3575</v>
@@ -57549,10 +57621,10 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>263</v>
+        <v>353</v>
       </c>
       <c r="B303" t="s">
-        <v>264</v>
+        <v>349</v>
       </c>
       <c r="C303" t="s">
         <v>3575</v>
@@ -57560,10 +57632,10 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>266</v>
+        <v>354</v>
       </c>
       <c r="B304" t="s">
-        <v>265</v>
+        <v>350</v>
       </c>
       <c r="C304" t="s">
         <v>3575</v>
@@ -57571,10 +57643,10 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>385</v>
+        <v>407</v>
       </c>
       <c r="B305" t="s">
-        <v>386</v>
+        <v>408</v>
       </c>
       <c r="C305" t="s">
         <v>3575</v>
@@ -57582,10 +57654,10 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>305</v>
+        <v>351</v>
       </c>
       <c r="B306" t="s">
-        <v>303</v>
+        <v>347</v>
       </c>
       <c r="C306" t="s">
         <v>3575</v>
@@ -57593,10 +57665,10 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>306</v>
+        <v>352</v>
       </c>
       <c r="B307" t="s">
-        <v>304</v>
+        <v>348</v>
       </c>
       <c r="C307" t="s">
         <v>3575</v>
@@ -57604,10 +57676,10 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>381</v>
+        <v>391</v>
       </c>
       <c r="B308" t="s">
-        <v>382</v>
+        <v>392</v>
       </c>
       <c r="C308" t="s">
         <v>3575</v>
@@ -57615,10 +57687,10 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>297</v>
+        <v>321</v>
       </c>
       <c r="B309" t="s">
-        <v>295</v>
+        <v>315</v>
       </c>
       <c r="C309" t="s">
         <v>3575</v>
@@ -57626,10 +57698,10 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>298</v>
+        <v>322</v>
       </c>
       <c r="B310" t="s">
-        <v>296</v>
+        <v>316</v>
       </c>
       <c r="C310" t="s">
         <v>3575</v>
@@ -57637,10 +57709,10 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="B311" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="C311" t="s">
         <v>3575</v>
@@ -57648,10 +57720,10 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>319</v>
+        <v>311</v>
       </c>
       <c r="B312" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C312" t="s">
         <v>3575</v>
@@ -57659,10 +57731,10 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>320</v>
+        <v>312</v>
       </c>
       <c r="B313" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C313" t="s">
         <v>3575</v>
@@ -57670,10 +57742,10 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>383</v>
+        <v>366</v>
       </c>
       <c r="B314" t="s">
-        <v>384</v>
+        <v>367</v>
       </c>
       <c r="C314" t="s">
         <v>3575</v>
@@ -57681,10 +57753,10 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>301</v>
+        <v>263</v>
       </c>
       <c r="B315" t="s">
-        <v>299</v>
+        <v>264</v>
       </c>
       <c r="C315" t="s">
         <v>3575</v>
@@ -57692,10 +57764,10 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>302</v>
+        <v>266</v>
       </c>
       <c r="B316" t="s">
-        <v>300</v>
+        <v>265</v>
       </c>
       <c r="C316" t="s">
         <v>3575</v>
@@ -57703,10 +57775,10 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>19</v>
-      </c>
-      <c r="B317" s="3" t="s">
-        <v>164</v>
+        <v>385</v>
+      </c>
+      <c r="B317" t="s">
+        <v>386</v>
       </c>
       <c r="C317" t="s">
         <v>3575</v>
@@ -57714,10 +57786,10 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>20</v>
-      </c>
-      <c r="B318" s="3" t="s">
-        <v>165</v>
+        <v>305</v>
+      </c>
+      <c r="B318" t="s">
+        <v>303</v>
       </c>
       <c r="C318" t="s">
         <v>3575</v>
@@ -57725,10 +57797,10 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>21</v>
-      </c>
-      <c r="B319" s="3" t="s">
-        <v>166</v>
+        <v>306</v>
+      </c>
+      <c r="B319" t="s">
+        <v>304</v>
       </c>
       <c r="C319" t="s">
         <v>3575</v>
@@ -57736,10 +57808,10 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>12</v>
-      </c>
-      <c r="B320" s="3" t="s">
-        <v>161</v>
+        <v>381</v>
+      </c>
+      <c r="B320" t="s">
+        <v>382</v>
       </c>
       <c r="C320" t="s">
         <v>3575</v>
@@ -57747,10 +57819,10 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>6</v>
-      </c>
-      <c r="B321" s="3" t="s">
-        <v>155</v>
+        <v>297</v>
+      </c>
+      <c r="B321" t="s">
+        <v>295</v>
       </c>
       <c r="C321" t="s">
         <v>3575</v>
@@ -57758,10 +57830,10 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>13</v>
-      </c>
-      <c r="B322" s="3" t="s">
-        <v>162</v>
+        <v>298</v>
+      </c>
+      <c r="B322" t="s">
+        <v>296</v>
       </c>
       <c r="C322" t="s">
         <v>3575</v>
@@ -57769,10 +57841,10 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>7</v>
-      </c>
-      <c r="B323" s="3" t="s">
-        <v>156</v>
+        <v>393</v>
+      </c>
+      <c r="B323" t="s">
+        <v>394</v>
       </c>
       <c r="C323" t="s">
         <v>3575</v>
@@ -57780,10 +57852,10 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>8</v>
-      </c>
-      <c r="B324" s="3" t="s">
-        <v>157</v>
+        <v>319</v>
+      </c>
+      <c r="B324" t="s">
+        <v>317</v>
       </c>
       <c r="C324" t="s">
         <v>3575</v>
@@ -57791,10 +57863,10 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>9</v>
-      </c>
-      <c r="B325" s="3" t="s">
-        <v>158</v>
+        <v>320</v>
+      </c>
+      <c r="B325" t="s">
+        <v>318</v>
       </c>
       <c r="C325" t="s">
         <v>3575</v>
@@ -57802,10 +57874,10 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>10</v>
-      </c>
-      <c r="B326" s="3" t="s">
-        <v>159</v>
+        <v>383</v>
+      </c>
+      <c r="B326" t="s">
+        <v>384</v>
       </c>
       <c r="C326" t="s">
         <v>3575</v>
@@ -57813,10 +57885,10 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>11</v>
-      </c>
-      <c r="B327" s="3" t="s">
-        <v>160</v>
+        <v>301</v>
+      </c>
+      <c r="B327" t="s">
+        <v>299</v>
       </c>
       <c r="C327" t="s">
         <v>3575</v>
@@ -57824,10 +57896,10 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>3466</v>
+        <v>302</v>
       </c>
       <c r="B328" t="s">
-        <v>3465</v>
+        <v>300</v>
       </c>
       <c r="C328" t="s">
         <v>3575</v>
@@ -57835,10 +57907,10 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>3459</v>
-      </c>
-      <c r="B329" t="s">
-        <v>3462</v>
+        <v>19</v>
+      </c>
+      <c r="B329" s="3" t="s">
+        <v>164</v>
       </c>
       <c r="C329" t="s">
         <v>3575</v>
@@ -57846,10 +57918,10 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>3463</v>
-      </c>
-      <c r="B330" t="s">
-        <v>3464</v>
+        <v>20</v>
+      </c>
+      <c r="B330" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="C330" t="s">
         <v>3575</v>
@@ -57857,10 +57929,10 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>415</v>
-      </c>
-      <c r="B331" t="s">
-        <v>227</v>
+        <v>21</v>
+      </c>
+      <c r="B331" s="3" t="s">
+        <v>166</v>
       </c>
       <c r="C331" t="s">
         <v>3575</v>
@@ -57868,10 +57940,10 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>118</v>
-      </c>
-      <c r="B332" t="s">
-        <v>3445</v>
+        <v>12</v>
+      </c>
+      <c r="B332" s="3" t="s">
+        <v>161</v>
       </c>
       <c r="C332" t="s">
         <v>3575</v>
@@ -57879,10 +57951,10 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>416</v>
-      </c>
-      <c r="B333" t="s">
-        <v>226</v>
+        <v>6</v>
+      </c>
+      <c r="B333" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="C333" t="s">
         <v>3575</v>
@@ -57890,21 +57962,21 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>117</v>
-      </c>
-      <c r="B334" t="s">
-        <v>3444</v>
+        <v>13</v>
+      </c>
+      <c r="B334" s="3" t="s">
+        <v>162</v>
       </c>
       <c r="C334" t="s">
         <v>3575</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A335" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="B335" t="s">
-        <v>225</v>
+      <c r="A335" t="s">
+        <v>7</v>
+      </c>
+      <c r="B335" s="3" t="s">
+        <v>156</v>
       </c>
       <c r="C335" t="s">
         <v>3575</v>
@@ -57912,10 +57984,10 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>116</v>
-      </c>
-      <c r="B336" t="s">
-        <v>3447</v>
+        <v>8</v>
+      </c>
+      <c r="B336" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="C336" t="s">
         <v>3575</v>
@@ -57923,10 +57995,10 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>418</v>
-      </c>
-      <c r="B337" t="s">
-        <v>224</v>
+        <v>9</v>
+      </c>
+      <c r="B337" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="C337" t="s">
         <v>3575</v>
@@ -57934,10 +58006,10 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>115</v>
-      </c>
-      <c r="B338" t="s">
-        <v>3446</v>
+        <v>10</v>
+      </c>
+      <c r="B338" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="C338" t="s">
         <v>3575</v>
@@ -57945,10 +58017,10 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>3547</v>
-      </c>
-      <c r="B339" t="s">
-        <v>3549</v>
+        <v>11</v>
+      </c>
+      <c r="B339" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="C339" t="s">
         <v>3575</v>
@@ -57956,10 +58028,10 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>3455</v>
+        <v>3466</v>
       </c>
       <c r="B340" t="s">
-        <v>3456</v>
+        <v>3465</v>
       </c>
       <c r="C340" t="s">
         <v>3575</v>
@@ -57967,10 +58039,10 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>3454</v>
+        <v>3459</v>
       </c>
       <c r="B341" t="s">
-        <v>3453</v>
+        <v>3462</v>
       </c>
       <c r="C341" t="s">
         <v>3575</v>
@@ -57978,10 +58050,10 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>3451</v>
+        <v>3463</v>
       </c>
       <c r="B342" t="s">
-        <v>3452</v>
+        <v>3464</v>
       </c>
       <c r="C342" t="s">
         <v>3575</v>
@@ -57989,10 +58061,10 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>3660</v>
-      </c>
-      <c r="B343" s="3" t="s">
-        <v>3661</v>
+        <v>415</v>
+      </c>
+      <c r="B343" t="s">
+        <v>227</v>
       </c>
       <c r="C343" t="s">
         <v>3575</v>
@@ -58000,10 +58072,10 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>22</v>
-      </c>
-      <c r="B344" s="3" t="s">
-        <v>412</v>
+        <v>118</v>
+      </c>
+      <c r="B344" t="s">
+        <v>3445</v>
       </c>
       <c r="C344" t="s">
         <v>3575</v>
@@ -58011,10 +58083,10 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>3833</v>
+        <v>416</v>
       </c>
       <c r="B345" t="s">
-        <v>3662</v>
+        <v>226</v>
       </c>
       <c r="C345" t="s">
         <v>3575</v>
@@ -58022,21 +58094,21 @@
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>3460</v>
+        <v>117</v>
       </c>
       <c r="B346" t="s">
-        <v>3475</v>
+        <v>3444</v>
       </c>
       <c r="C346" t="s">
         <v>3575</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A347" t="s">
-        <v>3477</v>
+      <c r="A347" s="2" t="s">
+        <v>417</v>
       </c>
       <c r="B347" t="s">
-        <v>3473</v>
+        <v>225</v>
       </c>
       <c r="C347" t="s">
         <v>3575</v>
@@ -58044,10 +58116,10 @@
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>17</v>
-      </c>
-      <c r="B348" s="3" t="s">
-        <v>359</v>
+        <v>116</v>
+      </c>
+      <c r="B348" t="s">
+        <v>3447</v>
       </c>
       <c r="C348" t="s">
         <v>3575</v>
@@ -58055,10 +58127,10 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>414</v>
-      </c>
-      <c r="B349" s="3" t="s">
-        <v>363</v>
+        <v>418</v>
+      </c>
+      <c r="B349" t="s">
+        <v>224</v>
       </c>
       <c r="C349" t="s">
         <v>3575</v>
@@ -58066,10 +58138,10 @@
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>15</v>
-      </c>
-      <c r="B350" s="3" t="s">
-        <v>360</v>
+        <v>115</v>
+      </c>
+      <c r="B350" t="s">
+        <v>3446</v>
       </c>
       <c r="C350" t="s">
         <v>3575</v>
@@ -58077,10 +58149,10 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>18</v>
-      </c>
-      <c r="B351" s="3" t="s">
-        <v>361</v>
+        <v>3547</v>
+      </c>
+      <c r="B351" t="s">
+        <v>3549</v>
       </c>
       <c r="C351" t="s">
         <v>3575</v>
@@ -58088,10 +58160,10 @@
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>16</v>
-      </c>
-      <c r="B352" s="3" t="s">
-        <v>362</v>
+        <v>3455</v>
+      </c>
+      <c r="B352" t="s">
+        <v>3456</v>
       </c>
       <c r="C352" t="s">
         <v>3575</v>
@@ -58099,10 +58171,10 @@
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>3</v>
-      </c>
-      <c r="B353" s="3" t="s">
-        <v>419</v>
+        <v>3454</v>
+      </c>
+      <c r="B353" t="s">
+        <v>3453</v>
       </c>
       <c r="C353" t="s">
         <v>3575</v>
@@ -58110,10 +58182,10 @@
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>4</v>
-      </c>
-      <c r="B354" s="3" t="s">
-        <v>420</v>
+        <v>3451</v>
+      </c>
+      <c r="B354" t="s">
+        <v>3452</v>
       </c>
       <c r="C354" t="s">
         <v>3575</v>
@@ -58121,10 +58193,10 @@
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>5</v>
+        <v>3660</v>
       </c>
       <c r="B355" s="3" t="s">
-        <v>421</v>
+        <v>3661</v>
       </c>
       <c r="C355" t="s">
         <v>3575</v>
@@ -58132,10 +58204,10 @@
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>422</v>
+        <v>412</v>
       </c>
       <c r="C356" t="s">
         <v>3575</v>
@@ -58143,10 +58215,10 @@
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>3639</v>
+        <v>3833</v>
       </c>
       <c r="B357" t="s">
-        <v>3640</v>
+        <v>3662</v>
       </c>
       <c r="C357" t="s">
         <v>3575</v>
@@ -58154,10 +58226,10 @@
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>3643</v>
+        <v>3460</v>
       </c>
       <c r="B358" t="s">
-        <v>3644</v>
+        <v>3475</v>
       </c>
       <c r="C358" t="s">
         <v>3575</v>
@@ -58165,10 +58237,10 @@
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>3641</v>
+        <v>3477</v>
       </c>
       <c r="B359" t="s">
-        <v>3642</v>
+        <v>3473</v>
       </c>
       <c r="C359" t="s">
         <v>3575</v>
@@ -58176,10 +58248,10 @@
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>3457</v>
-      </c>
-      <c r="B360" t="s">
-        <v>3458</v>
+        <v>17</v>
+      </c>
+      <c r="B360" s="3" t="s">
+        <v>359</v>
       </c>
       <c r="C360" t="s">
         <v>3575</v>
@@ -58187,10 +58259,10 @@
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>3649</v>
+        <v>414</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>3650</v>
+        <v>363</v>
       </c>
       <c r="C361" t="s">
         <v>3575</v>
@@ -58198,10 +58270,10 @@
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>3648</v>
+        <v>15</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>3646</v>
+        <v>360</v>
       </c>
       <c r="C362" t="s">
         <v>3575</v>
@@ -58209,10 +58281,10 @@
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>3647</v>
+        <v>18</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>3645</v>
+        <v>361</v>
       </c>
       <c r="C363" t="s">
         <v>3575</v>
@@ -58220,10 +58292,10 @@
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>3546</v>
-      </c>
-      <c r="B364" t="s">
-        <v>3548</v>
+        <v>16</v>
+      </c>
+      <c r="B364" s="3" t="s">
+        <v>362</v>
       </c>
       <c r="C364" t="s">
         <v>3575</v>
@@ -58231,10 +58303,10 @@
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>163</v>
+        <v>419</v>
       </c>
       <c r="C365" t="s">
         <v>3575</v>
@@ -58242,142 +58314,142 @@
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>112</v>
-      </c>
-      <c r="B366" t="s">
-        <v>194</v>
+        <v>4</v>
+      </c>
+      <c r="B366" s="3" t="s">
+        <v>420</v>
       </c>
       <c r="C366" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>108</v>
-      </c>
-      <c r="B367" t="s">
-        <v>198</v>
+        <v>5</v>
+      </c>
+      <c r="B367" s="3" t="s">
+        <v>421</v>
       </c>
       <c r="C367" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>106</v>
-      </c>
-      <c r="B368" t="s">
-        <v>196</v>
+        <v>2</v>
+      </c>
+      <c r="B368" s="3" t="s">
+        <v>422</v>
       </c>
       <c r="C368" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>107</v>
+        <v>3639</v>
       </c>
       <c r="B369" t="s">
-        <v>197</v>
+        <v>3640</v>
       </c>
       <c r="C369" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>109</v>
+        <v>3643</v>
       </c>
       <c r="B370" t="s">
-        <v>199</v>
+        <v>3644</v>
       </c>
       <c r="C370" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>95</v>
+        <v>3641</v>
       </c>
       <c r="B371" t="s">
-        <v>179</v>
+        <v>3642</v>
       </c>
       <c r="C371" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>103</v>
+        <v>3457</v>
       </c>
       <c r="B372" t="s">
-        <v>186</v>
+        <v>3458</v>
       </c>
       <c r="C372" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>96</v>
-      </c>
-      <c r="B373" t="s">
-        <v>180</v>
+        <v>3649</v>
+      </c>
+      <c r="B373" s="3" t="s">
+        <v>3650</v>
       </c>
       <c r="C373" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>97</v>
-      </c>
-      <c r="B374" t="s">
-        <v>181</v>
+        <v>3648</v>
+      </c>
+      <c r="B374" s="3" t="s">
+        <v>3646</v>
       </c>
       <c r="C374" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>93</v>
-      </c>
-      <c r="B375" t="s">
-        <v>177</v>
+        <v>3647</v>
+      </c>
+      <c r="B375" s="3" t="s">
+        <v>3645</v>
       </c>
       <c r="C375" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>94</v>
+        <v>3546</v>
       </c>
       <c r="B376" t="s">
-        <v>178</v>
+        <v>3548</v>
       </c>
       <c r="C376" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>98</v>
-      </c>
-      <c r="B377" t="s">
-        <v>182</v>
+        <v>14</v>
+      </c>
+      <c r="B377" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="C377" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="B378" t="s">
-        <v>183</v>
+        <v>194</v>
       </c>
       <c r="C378" t="s">
         <v>3576</v>
@@ -58385,10 +58457,10 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>121</v>
+        <v>108</v>
       </c>
       <c r="B379" t="s">
-        <v>191</v>
+        <v>198</v>
       </c>
       <c r="C379" t="s">
         <v>3576</v>
@@ -58396,10 +58468,10 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="B380" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C380" t="s">
         <v>3576</v>
@@ -58407,10 +58479,10 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>101</v>
+        <v>107</v>
       </c>
       <c r="B381" t="s">
-        <v>185</v>
+        <v>197</v>
       </c>
       <c r="C381" t="s">
         <v>3576</v>
@@ -58418,10 +58490,10 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>102</v>
+        <v>109</v>
       </c>
       <c r="B382" t="s">
-        <v>187</v>
+        <v>199</v>
       </c>
       <c r="C382" t="s">
         <v>3576</v>
@@ -58429,10 +58501,10 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>122</v>
+        <v>95</v>
       </c>
       <c r="B383" t="s">
-        <v>3723</v>
+        <v>179</v>
       </c>
       <c r="C383" t="s">
         <v>3576</v>
@@ -58440,10 +58512,10 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B384" t="s">
-        <v>193</v>
+        <v>186</v>
       </c>
       <c r="C384" t="s">
         <v>3576</v>
@@ -58451,10 +58523,10 @@
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B385" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="C385" t="s">
         <v>3576</v>
@@ -58462,10 +58534,10 @@
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>119</v>
+        <v>97</v>
       </c>
       <c r="B386" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C386" t="s">
         <v>3576</v>
@@ -58473,10 +58545,10 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>104</v>
+        <v>93</v>
       </c>
       <c r="B387" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="C387" t="s">
         <v>3576</v>
@@ -58484,10 +58556,10 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
       <c r="B388" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="C388" t="s">
         <v>3576</v>
@@ -58495,17 +58567,153 @@
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="B389" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="C389" t="s">
         <v>3576</v>
       </c>
     </row>
+    <row r="390" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A390" t="s">
+        <v>99</v>
+      </c>
+      <c r="B390" t="s">
+        <v>183</v>
+      </c>
+      <c r="C390" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="391" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A391" t="s">
+        <v>121</v>
+      </c>
+      <c r="B391" t="s">
+        <v>191</v>
+      </c>
+      <c r="C391" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="392" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A392" t="s">
+        <v>111</v>
+      </c>
+      <c r="B392" t="s">
+        <v>192</v>
+      </c>
+      <c r="C392" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="393" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A393" t="s">
+        <v>101</v>
+      </c>
+      <c r="B393" t="s">
+        <v>185</v>
+      </c>
+      <c r="C393" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="394" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A394" t="s">
+        <v>102</v>
+      </c>
+      <c r="B394" t="s">
+        <v>187</v>
+      </c>
+      <c r="C394" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="395" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A395" t="s">
+        <v>122</v>
+      </c>
+      <c r="B395" t="s">
+        <v>3723</v>
+      </c>
+      <c r="C395" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="396" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A396" t="s">
+        <v>110</v>
+      </c>
+      <c r="B396" t="s">
+        <v>193</v>
+      </c>
+      <c r="C396" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="397" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A397" t="s">
+        <v>100</v>
+      </c>
+      <c r="B397" t="s">
+        <v>184</v>
+      </c>
+      <c r="C397" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="398" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A398" t="s">
+        <v>119</v>
+      </c>
+      <c r="B398" t="s">
+        <v>190</v>
+      </c>
+      <c r="C398" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="399" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A399" t="s">
+        <v>104</v>
+      </c>
+      <c r="B399" t="s">
+        <v>188</v>
+      </c>
+      <c r="C399" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="400" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A400" t="s">
+        <v>105</v>
+      </c>
+      <c r="B400" t="s">
+        <v>189</v>
+      </c>
+      <c r="C400" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="401" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A401" t="s">
+        <v>120</v>
+      </c>
+      <c r="B401" t="s">
+        <v>195</v>
+      </c>
+      <c r="C401" t="s">
+        <v>3576</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C389" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
+  <autoFilter ref="A1:C389" xr:uid="{00000000-0009-0000-0000-000007000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C401">
+      <sortCondition ref="C1:C389"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A358:B444">
     <sortCondition ref="A358:A444"/>
   </sortState>

</xml_diff>

<commit_message>
Inclusão de melhorias @202405171158
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6614D81C-744F-46AB-9C76-23FA739135CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EE2F09-BF02-475B-922B-D51F182CDEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="3280" windowWidth="19420" windowHeight="10300" tabRatio="699" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -41,7 +41,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">income_cashflow!$A$1:$B$169</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">index_fundamentals!$A$1:$B$195</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">leverage!$A$1:$B$180</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">macro!$A$1:$C$357</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">macro!$A$1:$C$358</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">market!$A$1:$B$195</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">options!$A$1:$B$195</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">ratios!$A$1:$B$177</definedName>
@@ -69,7 +69,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11378" uniqueCount="3946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11381" uniqueCount="3948">
   <si>
     <t>bbgTicker</t>
   </si>
@@ -11907,6 +11907,12 @@
   </si>
   <si>
     <t>br_incc10_yoy</t>
+  </si>
+  <si>
+    <t>XLU US Equity</t>
+  </si>
+  <si>
+    <t>us_utilities_xlu</t>
   </si>
 </sst>
 </file>
@@ -54283,11 +54289,11 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Planilha9"/>
-  <dimension ref="A1:C401"/>
+  <dimension ref="A1:C402"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D5" sqref="D5"/>
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I134" sqref="I134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55751,10 +55757,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>3820</v>
+        <v>3946</v>
       </c>
       <c r="B133" t="s">
-        <v>3823</v>
+        <v>3947</v>
       </c>
       <c r="C133" t="s">
         <v>3574</v>
@@ -55762,10 +55768,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>3346</v>
+        <v>3820</v>
       </c>
       <c r="B134" t="s">
-        <v>3539</v>
+        <v>3823</v>
       </c>
       <c r="C134" t="s">
         <v>3574</v>
@@ -55773,10 +55779,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>3541</v>
+        <v>3346</v>
       </c>
       <c r="B135" t="s">
-        <v>3540</v>
+        <v>3539</v>
       </c>
       <c r="C135" t="s">
         <v>3574</v>
@@ -55784,10 +55790,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>3824</v>
+        <v>3541</v>
       </c>
       <c r="B136" t="s">
-        <v>3825</v>
+        <v>3540</v>
       </c>
       <c r="C136" t="s">
         <v>3574</v>
@@ -55795,10 +55801,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>3356</v>
+        <v>3824</v>
       </c>
       <c r="B137" t="s">
-        <v>3509</v>
+        <v>3825</v>
       </c>
       <c r="C137" t="s">
         <v>3574</v>
@@ -55806,10 +55812,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>3819</v>
+        <v>3356</v>
       </c>
       <c r="B138" t="s">
-        <v>3818</v>
+        <v>3509</v>
       </c>
       <c r="C138" t="s">
         <v>3574</v>
@@ -55817,10 +55823,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>38</v>
+        <v>3819</v>
       </c>
       <c r="B139" t="s">
-        <v>3511</v>
+        <v>3818</v>
       </c>
       <c r="C139" t="s">
         <v>3574</v>
@@ -55828,10 +55834,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>3352</v>
+        <v>38</v>
       </c>
       <c r="B140" t="s">
-        <v>3514</v>
+        <v>3511</v>
       </c>
       <c r="C140" t="s">
         <v>3574</v>
@@ -55839,10 +55845,10 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>3831</v>
+        <v>3352</v>
       </c>
       <c r="B141" t="s">
-        <v>3830</v>
+        <v>3514</v>
       </c>
       <c r="C141" t="s">
         <v>3574</v>
@@ -55850,21 +55856,21 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>3564</v>
+        <v>3831</v>
       </c>
       <c r="B142" t="s">
-        <v>3567</v>
+        <v>3830</v>
       </c>
       <c r="C142" t="s">
-        <v>3568</v>
+        <v>3574</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>3562</v>
+        <v>3564</v>
       </c>
       <c r="B143" t="s">
-        <v>3565</v>
+        <v>3567</v>
       </c>
       <c r="C143" t="s">
         <v>3568</v>
@@ -55872,10 +55878,10 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>3563</v>
+        <v>3562</v>
       </c>
       <c r="B144" t="s">
-        <v>3566</v>
+        <v>3565</v>
       </c>
       <c r="C144" t="s">
         <v>3568</v>
@@ -55883,21 +55889,21 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>373</v>
+        <v>3563</v>
       </c>
       <c r="B145" t="s">
-        <v>374</v>
+        <v>3566</v>
       </c>
       <c r="C145" t="s">
-        <v>3575</v>
+        <v>3568</v>
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>281</v>
+        <v>373</v>
       </c>
       <c r="B146" t="s">
-        <v>279</v>
+        <v>374</v>
       </c>
       <c r="C146" t="s">
         <v>3575</v>
@@ -55905,10 +55911,10 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B147" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="C147" t="s">
         <v>3575</v>
@@ -55916,10 +55922,10 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>3694</v>
+        <v>282</v>
       </c>
       <c r="B148" t="s">
-        <v>3696</v>
+        <v>280</v>
       </c>
       <c r="C148" t="s">
         <v>3575</v>
@@ -55927,10 +55933,10 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>3693</v>
+        <v>3694</v>
       </c>
       <c r="B149" t="s">
-        <v>3695</v>
+        <v>3696</v>
       </c>
       <c r="C149" t="s">
         <v>3575</v>
@@ -55938,10 +55944,10 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>3703</v>
+        <v>3693</v>
       </c>
       <c r="B150" t="s">
-        <v>3706</v>
+        <v>3695</v>
       </c>
       <c r="C150" t="s">
         <v>3575</v>
@@ -55949,10 +55955,10 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>3686</v>
+        <v>3703</v>
       </c>
       <c r="B151" t="s">
-        <v>3690</v>
+        <v>3706</v>
       </c>
       <c r="C151" t="s">
         <v>3575</v>
@@ -55960,10 +55966,10 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>3687</v>
+        <v>3686</v>
       </c>
       <c r="B152" t="s">
-        <v>3692</v>
+        <v>3690</v>
       </c>
       <c r="C152" t="s">
         <v>3575</v>
@@ -55971,10 +55977,10 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>3685</v>
+        <v>3687</v>
       </c>
       <c r="B153" t="s">
-        <v>3691</v>
+        <v>3692</v>
       </c>
       <c r="C153" t="s">
         <v>3575</v>
@@ -55982,10 +55988,10 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>3683</v>
+        <v>3685</v>
       </c>
       <c r="B154" t="s">
-        <v>3688</v>
+        <v>3691</v>
       </c>
       <c r="C154" t="s">
         <v>3575</v>
@@ -55993,10 +55999,10 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>3684</v>
+        <v>3683</v>
       </c>
       <c r="B155" t="s">
-        <v>3689</v>
+        <v>3688</v>
       </c>
       <c r="C155" t="s">
         <v>3575</v>
@@ -56004,10 +56010,10 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>3664</v>
+        <v>3684</v>
       </c>
       <c r="B156" t="s">
-        <v>3663</v>
+        <v>3689</v>
       </c>
       <c r="C156" t="s">
         <v>3575</v>
@@ -56015,10 +56021,10 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>113</v>
+        <v>3664</v>
       </c>
       <c r="B157" t="s">
-        <v>260</v>
+        <v>3663</v>
       </c>
       <c r="C157" t="s">
         <v>3575</v>
@@ -56026,10 +56032,10 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>228</v>
+        <v>113</v>
       </c>
       <c r="B158" t="s">
-        <v>229</v>
+        <v>260</v>
       </c>
       <c r="C158" t="s">
         <v>3575</v>
@@ -56037,10 +56043,10 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>35</v>
-      </c>
-      <c r="B159" s="3" t="s">
-        <v>176</v>
+        <v>228</v>
+      </c>
+      <c r="B159" t="s">
+        <v>229</v>
       </c>
       <c r="C159" t="s">
         <v>3575</v>
@@ -56048,10 +56054,10 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="B160" s="3" t="s">
-        <v>413</v>
+        <v>176</v>
       </c>
       <c r="C160" t="s">
         <v>3575</v>
@@ -56059,10 +56065,10 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>3705</v>
-      </c>
-      <c r="B161" t="s">
-        <v>3708</v>
+        <v>39</v>
+      </c>
+      <c r="B161" s="3" t="s">
+        <v>413</v>
       </c>
       <c r="C161" t="s">
         <v>3575</v>
@@ -56070,10 +56076,10 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>43</v>
+        <v>3705</v>
       </c>
       <c r="B162" t="s">
-        <v>3702</v>
+        <v>3708</v>
       </c>
       <c r="C162" t="s">
         <v>3575</v>
@@ -56081,10 +56087,10 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B163" t="s">
-        <v>175</v>
+        <v>3702</v>
       </c>
       <c r="C163" t="s">
         <v>3575</v>
@@ -56092,10 +56098,10 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>3670</v>
+        <v>41</v>
       </c>
       <c r="B164" t="s">
-        <v>3679</v>
+        <v>175</v>
       </c>
       <c r="C164" t="s">
         <v>3575</v>
@@ -56103,10 +56109,10 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>3669</v>
+        <v>3670</v>
       </c>
       <c r="B165" t="s">
-        <v>3678</v>
+        <v>3679</v>
       </c>
       <c r="C165" t="s">
         <v>3575</v>
@@ -56114,10 +56120,10 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>3668</v>
+        <v>3669</v>
       </c>
       <c r="B166" t="s">
-        <v>3677</v>
+        <v>3678</v>
       </c>
       <c r="C166" t="s">
         <v>3575</v>
@@ -56125,10 +56131,10 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>3667</v>
+        <v>3668</v>
       </c>
       <c r="B167" t="s">
-        <v>3676</v>
+        <v>3677</v>
       </c>
       <c r="C167" t="s">
         <v>3575</v>
@@ -56136,10 +56142,10 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>3666</v>
+        <v>3667</v>
       </c>
       <c r="B168" t="s">
-        <v>3675</v>
+        <v>3676</v>
       </c>
       <c r="C168" t="s">
         <v>3575</v>
@@ -56147,10 +56153,10 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>3665</v>
+        <v>3666</v>
       </c>
       <c r="B169" t="s">
-        <v>3674</v>
+        <v>3675</v>
       </c>
       <c r="C169" t="s">
         <v>3575</v>
@@ -56158,10 +56164,10 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>3704</v>
+        <v>3665</v>
       </c>
       <c r="B170" t="s">
-        <v>3707</v>
+        <v>3674</v>
       </c>
       <c r="C170" t="s">
         <v>3575</v>
@@ -56169,10 +56175,10 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>3673</v>
+        <v>3704</v>
       </c>
       <c r="B171" t="s">
-        <v>3682</v>
+        <v>3707</v>
       </c>
       <c r="C171" t="s">
         <v>3575</v>
@@ -56180,10 +56186,10 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>3672</v>
+        <v>3673</v>
       </c>
       <c r="B172" t="s">
-        <v>3681</v>
+        <v>3682</v>
       </c>
       <c r="C172" t="s">
         <v>3575</v>
@@ -56191,10 +56197,10 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>3671</v>
+        <v>3672</v>
       </c>
       <c r="B173" t="s">
-        <v>3680</v>
+        <v>3681</v>
       </c>
       <c r="C173" t="s">
         <v>3575</v>
@@ -56202,10 +56208,10 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>3658</v>
+        <v>3671</v>
       </c>
       <c r="B174" t="s">
-        <v>3659</v>
+        <v>3680</v>
       </c>
       <c r="C174" t="s">
         <v>3575</v>
@@ -56213,10 +56219,10 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>3655</v>
+        <v>3658</v>
       </c>
       <c r="B175" t="s">
-        <v>3657</v>
+        <v>3659</v>
       </c>
       <c r="C175" t="s">
         <v>3575</v>
@@ -56224,10 +56230,10 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>3654</v>
+        <v>3655</v>
       </c>
       <c r="B176" t="s">
-        <v>3652</v>
+        <v>3657</v>
       </c>
       <c r="C176" t="s">
         <v>3575</v>
@@ -56235,10 +56241,10 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>3651</v>
+        <v>3654</v>
       </c>
       <c r="B177" t="s">
-        <v>3653</v>
+        <v>3652</v>
       </c>
       <c r="C177" t="s">
         <v>3575</v>
@@ -56246,10 +56252,10 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>3655</v>
+        <v>3651</v>
       </c>
       <c r="B178" t="s">
-        <v>3656</v>
+        <v>3653</v>
       </c>
       <c r="C178" t="s">
         <v>3575</v>
@@ -56257,10 +56263,10 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>3479</v>
+        <v>3655</v>
       </c>
       <c r="B179" t="s">
-        <v>3480</v>
+        <v>3656</v>
       </c>
       <c r="C179" t="s">
         <v>3575</v>
@@ -56268,10 +56274,10 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>3461</v>
+        <v>3479</v>
       </c>
       <c r="B180" t="s">
-        <v>3476</v>
+        <v>3480</v>
       </c>
       <c r="C180" t="s">
         <v>3575</v>
@@ -56279,10 +56285,10 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>3478</v>
+        <v>3461</v>
       </c>
       <c r="B181" t="s">
-        <v>3474</v>
+        <v>3476</v>
       </c>
       <c r="C181" t="s">
         <v>3575</v>
@@ -56290,10 +56296,10 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>36</v>
+        <v>3478</v>
       </c>
       <c r="B182" t="s">
-        <v>411</v>
+        <v>3474</v>
       </c>
       <c r="C182" t="s">
         <v>3575</v>
@@ -56301,10 +56307,10 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>357</v>
+        <v>36</v>
       </c>
       <c r="B183" t="s">
-        <v>355</v>
+        <v>411</v>
       </c>
       <c r="C183" t="s">
         <v>3575</v>
@@ -56312,10 +56318,10 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B184" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="C184" t="s">
         <v>3575</v>
@@ -56323,10 +56329,10 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>3711</v>
+        <v>358</v>
       </c>
       <c r="B185" t="s">
-        <v>3712</v>
+        <v>356</v>
       </c>
       <c r="C185" t="s">
         <v>3575</v>
@@ -56334,10 +56340,10 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>3710</v>
+        <v>3711</v>
       </c>
       <c r="B186" t="s">
-        <v>3714</v>
+        <v>3712</v>
       </c>
       <c r="C186" t="s">
         <v>3575</v>
@@ -56345,10 +56351,10 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>3835</v>
+        <v>3710</v>
       </c>
       <c r="B187" t="s">
-        <v>3836</v>
+        <v>3714</v>
       </c>
       <c r="C187" t="s">
         <v>3575</v>
@@ -56356,10 +56362,10 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>3838</v>
+        <v>3835</v>
       </c>
       <c r="B188" t="s">
-        <v>3837</v>
+        <v>3836</v>
       </c>
       <c r="C188" t="s">
         <v>3575</v>
@@ -56367,10 +56373,10 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>3709</v>
+        <v>3838</v>
       </c>
       <c r="B189" t="s">
-        <v>3713</v>
+        <v>3837</v>
       </c>
       <c r="C189" t="s">
         <v>3575</v>
@@ -56378,10 +56384,10 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>3925</v>
+        <v>3709</v>
       </c>
       <c r="B190" t="s">
-        <v>3922</v>
+        <v>3713</v>
       </c>
       <c r="C190" t="s">
         <v>3575</v>
@@ -56389,10 +56395,10 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>3927</v>
+        <v>3925</v>
       </c>
       <c r="B191" t="s">
-        <v>3924</v>
+        <v>3922</v>
       </c>
       <c r="C191" t="s">
         <v>3575</v>
@@ -56400,10 +56406,10 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>3928</v>
+        <v>3927</v>
       </c>
       <c r="B192" t="s">
-        <v>3923</v>
+        <v>3924</v>
       </c>
       <c r="C192" t="s">
         <v>3575</v>
@@ -56411,10 +56417,10 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>3717</v>
+        <v>3928</v>
       </c>
       <c r="B193" t="s">
-        <v>3720</v>
+        <v>3923</v>
       </c>
       <c r="C193" t="s">
         <v>3575</v>
@@ -56422,10 +56428,10 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>3718</v>
+        <v>3717</v>
       </c>
       <c r="B194" t="s">
-        <v>3721</v>
+        <v>3720</v>
       </c>
       <c r="C194" t="s">
         <v>3575</v>
@@ -56433,10 +56439,10 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>3719</v>
+        <v>3718</v>
       </c>
       <c r="B195" t="s">
-        <v>3722</v>
+        <v>3721</v>
       </c>
       <c r="C195" t="s">
         <v>3575</v>
@@ -56444,10 +56450,10 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>3926</v>
+        <v>3719</v>
       </c>
       <c r="B196" t="s">
-        <v>3931</v>
+        <v>3722</v>
       </c>
       <c r="C196" t="s">
         <v>3575</v>
@@ -56455,10 +56461,10 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>3930</v>
+        <v>3926</v>
       </c>
       <c r="B197" t="s">
-        <v>3932</v>
+        <v>3931</v>
       </c>
       <c r="C197" t="s">
         <v>3575</v>
@@ -56466,10 +56472,10 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>3929</v>
+        <v>3930</v>
       </c>
       <c r="B198" t="s">
-        <v>3933</v>
+        <v>3932</v>
       </c>
       <c r="C198" t="s">
         <v>3575</v>
@@ -56477,10 +56483,10 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>3529</v>
+        <v>3929</v>
       </c>
       <c r="B199" t="s">
-        <v>3530</v>
+        <v>3933</v>
       </c>
       <c r="C199" t="s">
         <v>3575</v>
@@ -56488,10 +56494,10 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>3532</v>
+        <v>3529</v>
       </c>
       <c r="B200" t="s">
-        <v>3531</v>
+        <v>3530</v>
       </c>
       <c r="C200" t="s">
         <v>3575</v>
@@ -56499,10 +56505,10 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>3940</v>
+        <v>3532</v>
       </c>
       <c r="B201" t="s">
-        <v>3943</v>
+        <v>3531</v>
       </c>
       <c r="C201" t="s">
         <v>3575</v>
@@ -56510,10 +56516,10 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>3941</v>
+        <v>3940</v>
       </c>
       <c r="B202" t="s">
-        <v>3944</v>
+        <v>3943</v>
       </c>
       <c r="C202" t="s">
         <v>3575</v>
@@ -56521,10 +56527,10 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>3942</v>
+        <v>3941</v>
       </c>
       <c r="B203" t="s">
-        <v>3945</v>
+        <v>3944</v>
       </c>
       <c r="C203" t="s">
         <v>3575</v>
@@ -56532,10 +56538,10 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>3934</v>
+        <v>3942</v>
       </c>
       <c r="B204" t="s">
-        <v>3937</v>
+        <v>3945</v>
       </c>
       <c r="C204" t="s">
         <v>3575</v>
@@ -56543,10 +56549,10 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>3935</v>
+        <v>3934</v>
       </c>
       <c r="B205" t="s">
-        <v>3938</v>
+        <v>3937</v>
       </c>
       <c r="C205" t="s">
         <v>3575</v>
@@ -56554,10 +56560,10 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>3936</v>
+        <v>3935</v>
       </c>
       <c r="B206" t="s">
-        <v>3939</v>
+        <v>3938</v>
       </c>
       <c r="C206" t="s">
         <v>3575</v>
@@ -56565,10 +56571,10 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>27</v>
-      </c>
-      <c r="B207" s="3" t="s">
-        <v>128</v>
+        <v>3936</v>
+      </c>
+      <c r="B207" t="s">
+        <v>3939</v>
       </c>
       <c r="C207" t="s">
         <v>3575</v>
@@ -56576,10 +56582,10 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>3867</v>
-      </c>
-      <c r="B208" t="s">
-        <v>3895</v>
+        <v>27</v>
+      </c>
+      <c r="B208" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="C208" t="s">
         <v>3575</v>
@@ -56587,10 +56593,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>3865</v>
+        <v>3867</v>
       </c>
       <c r="B209" t="s">
-        <v>3896</v>
+        <v>3895</v>
       </c>
       <c r="C209" t="s">
         <v>3575</v>
@@ -56598,10 +56604,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>3868</v>
+        <v>3865</v>
       </c>
       <c r="B210" t="s">
-        <v>3897</v>
+        <v>3896</v>
       </c>
       <c r="C210" t="s">
         <v>3575</v>
@@ -56609,10 +56615,10 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>3869</v>
+        <v>3868</v>
       </c>
       <c r="B211" t="s">
-        <v>3898</v>
+        <v>3897</v>
       </c>
       <c r="C211" t="s">
         <v>3575</v>
@@ -56620,10 +56626,10 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>3857</v>
+        <v>3869</v>
       </c>
       <c r="B212" t="s">
-        <v>3899</v>
+        <v>3898</v>
       </c>
       <c r="C212" t="s">
         <v>3575</v>
@@ -56631,10 +56637,10 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>3870</v>
+        <v>3857</v>
       </c>
       <c r="B213" t="s">
-        <v>3900</v>
+        <v>3899</v>
       </c>
       <c r="C213" t="s">
         <v>3575</v>
@@ -56642,10 +56648,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>3871</v>
+        <v>3870</v>
       </c>
       <c r="B214" t="s">
-        <v>3901</v>
+        <v>3900</v>
       </c>
       <c r="C214" t="s">
         <v>3575</v>
@@ -56653,10 +56659,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>3872</v>
+        <v>3871</v>
       </c>
       <c r="B215" t="s">
-        <v>3902</v>
+        <v>3901</v>
       </c>
       <c r="C215" t="s">
         <v>3575</v>
@@ -56664,32 +56670,32 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>3873</v>
+        <v>3872</v>
       </c>
       <c r="B216" t="s">
-        <v>3903</v>
+        <v>3902</v>
       </c>
       <c r="C216" t="s">
         <v>3575</v>
       </c>
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A217" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B217" s="3" t="s">
-        <v>124</v>
+      <c r="A217" t="s">
+        <v>3873</v>
+      </c>
+      <c r="B217" t="s">
+        <v>3903</v>
       </c>
       <c r="C217" t="s">
         <v>3575</v>
       </c>
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>3861</v>
-      </c>
-      <c r="B218" t="s">
-        <v>3904</v>
+      <c r="A218" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B218" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="C218" t="s">
         <v>3575</v>
@@ -56697,10 +56703,10 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>3874</v>
+        <v>3861</v>
       </c>
       <c r="B219" t="s">
-        <v>3905</v>
+        <v>3904</v>
       </c>
       <c r="C219" t="s">
         <v>3575</v>
@@ -56708,10 +56714,10 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>3875</v>
+        <v>3874</v>
       </c>
       <c r="B220" t="s">
-        <v>3906</v>
+        <v>3905</v>
       </c>
       <c r="C220" t="s">
         <v>3575</v>
@@ -56719,10 +56725,10 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>3876</v>
+        <v>3875</v>
       </c>
       <c r="B221" t="s">
-        <v>3907</v>
+        <v>3906</v>
       </c>
       <c r="C221" t="s">
         <v>3575</v>
@@ -56730,10 +56736,10 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>3877</v>
+        <v>3876</v>
       </c>
       <c r="B222" t="s">
-        <v>3908</v>
+        <v>3907</v>
       </c>
       <c r="C222" t="s">
         <v>3575</v>
@@ -56741,10 +56747,10 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>3866</v>
+        <v>3877</v>
       </c>
       <c r="B223" t="s">
-        <v>3909</v>
+        <v>3908</v>
       </c>
       <c r="C223" t="s">
         <v>3575</v>
@@ -56752,10 +56758,10 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>3859</v>
+        <v>3866</v>
       </c>
       <c r="B224" t="s">
-        <v>3910</v>
+        <v>3909</v>
       </c>
       <c r="C224" t="s">
         <v>3575</v>
@@ -56763,10 +56769,10 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>3878</v>
+        <v>3859</v>
       </c>
       <c r="B225" t="s">
-        <v>3911</v>
+        <v>3910</v>
       </c>
       <c r="C225" t="s">
         <v>3575</v>
@@ -56774,10 +56780,10 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>3879</v>
+        <v>3878</v>
       </c>
       <c r="B226" t="s">
-        <v>3912</v>
+        <v>3911</v>
       </c>
       <c r="C226" t="s">
         <v>3575</v>
@@ -56785,32 +56791,32 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>3863</v>
+        <v>3879</v>
       </c>
       <c r="B227" t="s">
-        <v>3913</v>
+        <v>3912</v>
       </c>
       <c r="C227" t="s">
         <v>3575</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A228" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B228" s="3" t="s">
-        <v>125</v>
+      <c r="A228" t="s">
+        <v>3863</v>
+      </c>
+      <c r="B228" t="s">
+        <v>3913</v>
       </c>
       <c r="C228" t="s">
         <v>3575</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A229" t="s">
-        <v>3856</v>
-      </c>
-      <c r="B229" t="s">
-        <v>3914</v>
+      <c r="A229" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B229" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="C229" t="s">
         <v>3575</v>
@@ -56818,10 +56824,10 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>3880</v>
+        <v>3856</v>
       </c>
       <c r="B230" t="s">
-        <v>3915</v>
+        <v>3914</v>
       </c>
       <c r="C230" t="s">
         <v>3575</v>
@@ -56829,10 +56835,10 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>3881</v>
+        <v>3880</v>
       </c>
       <c r="B231" t="s">
-        <v>3916</v>
+        <v>3915</v>
       </c>
       <c r="C231" t="s">
         <v>3575</v>
@@ -56840,10 +56846,10 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>3882</v>
+        <v>3881</v>
       </c>
       <c r="B232" t="s">
-        <v>3917</v>
+        <v>3916</v>
       </c>
       <c r="C232" t="s">
         <v>3575</v>
@@ -56851,10 +56857,10 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>3883</v>
+        <v>3882</v>
       </c>
       <c r="B233" t="s">
-        <v>3918</v>
+        <v>3917</v>
       </c>
       <c r="C233" t="s">
         <v>3575</v>
@@ -56862,10 +56868,10 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>28</v>
-      </c>
-      <c r="B234" s="3" t="s">
-        <v>129</v>
+        <v>3883</v>
+      </c>
+      <c r="B234" t="s">
+        <v>3918</v>
       </c>
       <c r="C234" t="s">
         <v>3575</v>
@@ -56873,10 +56879,10 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>3884</v>
-      </c>
-      <c r="B235" t="s">
-        <v>3919</v>
+        <v>28</v>
+      </c>
+      <c r="B235" s="3" t="s">
+        <v>129</v>
       </c>
       <c r="C235" t="s">
         <v>3575</v>
@@ -56884,10 +56890,10 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>3885</v>
+        <v>3884</v>
       </c>
       <c r="B236" t="s">
-        <v>3920</v>
+        <v>3919</v>
       </c>
       <c r="C236" t="s">
         <v>3575</v>
@@ -56895,10 +56901,10 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>3886</v>
+        <v>3885</v>
       </c>
       <c r="B237" t="s">
-        <v>3921</v>
+        <v>3920</v>
       </c>
       <c r="C237" t="s">
         <v>3575</v>
@@ -56906,10 +56912,10 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>25</v>
-      </c>
-      <c r="B238" s="3" t="s">
-        <v>126</v>
+        <v>3886</v>
+      </c>
+      <c r="B238" t="s">
+        <v>3921</v>
       </c>
       <c r="C238" t="s">
         <v>3575</v>
@@ -56917,10 +56923,10 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>3862</v>
-      </c>
-      <c r="B239" t="s">
-        <v>3890</v>
+        <v>25</v>
+      </c>
+      <c r="B239" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C239" t="s">
         <v>3575</v>
@@ -56928,10 +56934,10 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>26</v>
-      </c>
-      <c r="B240" s="3" t="s">
-        <v>127</v>
+        <v>3862</v>
+      </c>
+      <c r="B240" t="s">
+        <v>3890</v>
       </c>
       <c r="C240" t="s">
         <v>3575</v>
@@ -56939,10 +56945,10 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>3860</v>
-      </c>
-      <c r="B241" t="s">
-        <v>3891</v>
+        <v>26</v>
+      </c>
+      <c r="B241" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="C241" t="s">
         <v>3575</v>
@@ -56950,10 +56956,10 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>3858</v>
+        <v>3860</v>
       </c>
       <c r="B242" t="s">
-        <v>3892</v>
+        <v>3891</v>
       </c>
       <c r="C242" t="s">
         <v>3575</v>
@@ -56961,10 +56967,10 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>3887</v>
+        <v>3858</v>
       </c>
       <c r="B243" t="s">
-        <v>3893</v>
+        <v>3892</v>
       </c>
       <c r="C243" t="s">
         <v>3575</v>
@@ -56972,10 +56978,10 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>3888</v>
+        <v>3887</v>
       </c>
       <c r="B244" t="s">
-        <v>3894</v>
+        <v>3893</v>
       </c>
       <c r="C244" t="s">
         <v>3575</v>
@@ -56983,10 +56989,10 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>3472</v>
+        <v>3888</v>
       </c>
       <c r="B245" t="s">
-        <v>3470</v>
+        <v>3894</v>
       </c>
       <c r="C245" t="s">
         <v>3575</v>
@@ -56994,10 +57000,10 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>3467</v>
+        <v>3472</v>
       </c>
       <c r="B246" t="s">
-        <v>3471</v>
+        <v>3470</v>
       </c>
       <c r="C246" t="s">
         <v>3575</v>
@@ -57005,10 +57011,10 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>3469</v>
+        <v>3467</v>
       </c>
       <c r="B247" t="s">
-        <v>3468</v>
+        <v>3471</v>
       </c>
       <c r="C247" t="s">
         <v>3575</v>
@@ -57016,10 +57022,10 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>3528</v>
+        <v>3469</v>
       </c>
       <c r="B248" t="s">
-        <v>3569</v>
+        <v>3468</v>
       </c>
       <c r="C248" t="s">
         <v>3575</v>
@@ -57027,10 +57033,10 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>40</v>
-      </c>
-      <c r="B249" s="3" t="s">
-        <v>3834</v>
+        <v>3528</v>
+      </c>
+      <c r="B249" t="s">
+        <v>3569</v>
       </c>
       <c r="C249" t="s">
         <v>3575</v>
@@ -57038,10 +57044,10 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>3715</v>
-      </c>
-      <c r="B250" t="s">
-        <v>3716</v>
+        <v>40</v>
+      </c>
+      <c r="B250" s="3" t="s">
+        <v>3834</v>
       </c>
       <c r="C250" t="s">
         <v>3575</v>
@@ -57049,10 +57055,10 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>33</v>
-      </c>
-      <c r="B251" s="3" t="s">
-        <v>134</v>
+        <v>3715</v>
+      </c>
+      <c r="B251" t="s">
+        <v>3716</v>
       </c>
       <c r="C251" t="s">
         <v>3575</v>
@@ -57060,10 +57066,10 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="B252" s="3" t="s">
-        <v>130</v>
+        <v>134</v>
       </c>
       <c r="C252" t="s">
         <v>3575</v>
@@ -57071,10 +57077,10 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B253" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C253" t="s">
         <v>3575</v>
@@ -57082,10 +57088,10 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B254" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C254" t="s">
         <v>3575</v>
@@ -57093,10 +57099,10 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>3864</v>
+        <v>31</v>
       </c>
       <c r="B255" s="3" t="s">
-        <v>3889</v>
+        <v>132</v>
       </c>
       <c r="C255" t="s">
         <v>3575</v>
@@ -57104,10 +57110,10 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>32</v>
+        <v>3864</v>
       </c>
       <c r="B256" s="3" t="s">
-        <v>133</v>
+        <v>3889</v>
       </c>
       <c r="C256" t="s">
         <v>3575</v>
@@ -57115,10 +57121,10 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>3698</v>
-      </c>
-      <c r="B257" t="s">
-        <v>3699</v>
+        <v>32</v>
+      </c>
+      <c r="B257" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="C257" t="s">
         <v>3575</v>
@@ -57126,10 +57132,10 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>3697</v>
+        <v>3698</v>
       </c>
       <c r="B258" t="s">
-        <v>3700</v>
+        <v>3699</v>
       </c>
       <c r="C258" t="s">
         <v>3575</v>
@@ -57137,10 +57143,10 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>42</v>
+        <v>3697</v>
       </c>
       <c r="B259" t="s">
-        <v>3701</v>
+        <v>3700</v>
       </c>
       <c r="C259" t="s">
         <v>3575</v>
@@ -57148,10 +57154,10 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>375</v>
+        <v>42</v>
       </c>
       <c r="B260" t="s">
-        <v>376</v>
+        <v>3701</v>
       </c>
       <c r="C260" t="s">
         <v>3575</v>
@@ -57159,10 +57165,10 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>285</v>
+        <v>375</v>
       </c>
       <c r="B261" t="s">
-        <v>283</v>
+        <v>376</v>
       </c>
       <c r="C261" t="s">
         <v>3575</v>
@@ -57170,10 +57176,10 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="B262" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="C262" t="s">
         <v>3575</v>
@@ -57181,10 +57187,10 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>395</v>
+        <v>286</v>
       </c>
       <c r="B263" t="s">
-        <v>396</v>
+        <v>284</v>
       </c>
       <c r="C263" t="s">
         <v>3575</v>
@@ -57192,10 +57198,10 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>325</v>
+        <v>395</v>
       </c>
       <c r="B264" t="s">
-        <v>323</v>
+        <v>396</v>
       </c>
       <c r="C264" t="s">
         <v>3575</v>
@@ -57203,10 +57209,10 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B265" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C265" t="s">
         <v>3575</v>
@@ -57214,10 +57220,10 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>387</v>
+        <v>326</v>
       </c>
       <c r="B266" t="s">
-        <v>388</v>
+        <v>324</v>
       </c>
       <c r="C266" t="s">
         <v>3575</v>
@@ -57225,10 +57231,10 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>309</v>
+        <v>387</v>
       </c>
       <c r="B267" t="s">
-        <v>307</v>
+        <v>388</v>
       </c>
       <c r="C267" t="s">
         <v>3575</v>
@@ -57236,10 +57242,10 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B268" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="C268" t="s">
         <v>3575</v>
@@ -57247,10 +57253,10 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>403</v>
+        <v>310</v>
       </c>
       <c r="B269" t="s">
-        <v>404</v>
+        <v>308</v>
       </c>
       <c r="C269" t="s">
         <v>3575</v>
@@ -57258,10 +57264,10 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>343</v>
+        <v>403</v>
       </c>
       <c r="B270" t="s">
-        <v>339</v>
+        <v>404</v>
       </c>
       <c r="C270" t="s">
         <v>3575</v>
@@ -57269,10 +57275,10 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B271" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C271" t="s">
         <v>3575</v>
@@ -57280,10 +57286,10 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>368</v>
+        <v>344</v>
       </c>
       <c r="B272" t="s">
-        <v>369</v>
+        <v>340</v>
       </c>
       <c r="C272" t="s">
         <v>3575</v>
@@ -57291,10 +57297,10 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>269</v>
+        <v>368</v>
       </c>
       <c r="B273" t="s">
-        <v>271</v>
+        <v>369</v>
       </c>
       <c r="C273" t="s">
         <v>3575</v>
@@ -57302,10 +57308,10 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B274" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C274" t="s">
         <v>3575</v>
@@ -57313,10 +57319,10 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>364</v>
+        <v>270</v>
       </c>
       <c r="B275" t="s">
-        <v>365</v>
+        <v>272</v>
       </c>
       <c r="C275" t="s">
         <v>3575</v>
@@ -57324,10 +57330,10 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>267</v>
+        <v>364</v>
       </c>
       <c r="B276" t="s">
-        <v>261</v>
+        <v>365</v>
       </c>
       <c r="C276" t="s">
         <v>3575</v>
@@ -57335,10 +57341,10 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B277" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C277" t="s">
         <v>3575</v>
@@ -57346,10 +57352,10 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>405</v>
+        <v>268</v>
       </c>
       <c r="B278" t="s">
-        <v>406</v>
+        <v>262</v>
       </c>
       <c r="C278" t="s">
         <v>3575</v>
@@ -57357,10 +57363,10 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>345</v>
+        <v>405</v>
       </c>
       <c r="B279" t="s">
-        <v>341</v>
+        <v>406</v>
       </c>
       <c r="C279" t="s">
         <v>3575</v>
@@ -57368,10 +57374,10 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B280" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C280" t="s">
         <v>3575</v>
@@ -57379,10 +57385,10 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>399</v>
+        <v>346</v>
       </c>
       <c r="B281" t="s">
-        <v>400</v>
+        <v>342</v>
       </c>
       <c r="C281" t="s">
         <v>3575</v>
@@ -57390,10 +57396,10 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>335</v>
+        <v>399</v>
       </c>
       <c r="B282" t="s">
-        <v>331</v>
+        <v>400</v>
       </c>
       <c r="C282" t="s">
         <v>3575</v>
@@ -57401,10 +57407,10 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B283" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C283" t="s">
         <v>3575</v>
@@ -57412,10 +57418,10 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>401</v>
+        <v>336</v>
       </c>
       <c r="B284" t="s">
-        <v>402</v>
+        <v>332</v>
       </c>
       <c r="C284" t="s">
         <v>3575</v>
@@ -57423,10 +57429,10 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>337</v>
+        <v>401</v>
       </c>
       <c r="B285" t="s">
-        <v>333</v>
+        <v>402</v>
       </c>
       <c r="C285" t="s">
         <v>3575</v>
@@ -57434,10 +57440,10 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B286" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C286" t="s">
         <v>3575</v>
@@ -57445,10 +57451,10 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>370</v>
+        <v>338</v>
       </c>
       <c r="B287" t="s">
-        <v>371</v>
+        <v>334</v>
       </c>
       <c r="C287" t="s">
         <v>3575</v>
@@ -57456,10 +57462,10 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>275</v>
+        <v>370</v>
       </c>
       <c r="B288" t="s">
-        <v>273</v>
+        <v>371</v>
       </c>
       <c r="C288" t="s">
         <v>3575</v>
@@ -57467,10 +57473,10 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B289" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="C289" t="s">
         <v>3575</v>
@@ -57478,10 +57484,10 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>379</v>
+        <v>276</v>
       </c>
       <c r="B290" t="s">
-        <v>380</v>
+        <v>274</v>
       </c>
       <c r="C290" t="s">
         <v>3575</v>
@@ -57489,10 +57495,10 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>293</v>
+        <v>379</v>
       </c>
       <c r="B291" t="s">
-        <v>291</v>
+        <v>380</v>
       </c>
       <c r="C291" t="s">
         <v>3575</v>
@@ -57500,10 +57506,10 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B292" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="C292" t="s">
         <v>3575</v>
@@ -57511,10 +57517,10 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>397</v>
+        <v>294</v>
       </c>
       <c r="B293" t="s">
-        <v>398</v>
+        <v>292</v>
       </c>
       <c r="C293" t="s">
         <v>3575</v>
@@ -57522,10 +57528,10 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>329</v>
+        <v>397</v>
       </c>
       <c r="B294" t="s">
-        <v>327</v>
+        <v>398</v>
       </c>
       <c r="C294" t="s">
         <v>3575</v>
@@ -57533,10 +57539,10 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B295" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C295" t="s">
         <v>3575</v>
@@ -57544,10 +57550,10 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>372</v>
+        <v>330</v>
       </c>
       <c r="B296" t="s">
-        <v>3448</v>
+        <v>328</v>
       </c>
       <c r="C296" t="s">
         <v>3575</v>
@@ -57555,10 +57561,10 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>277</v>
+        <v>372</v>
       </c>
       <c r="B297" t="s">
-        <v>3449</v>
+        <v>3448</v>
       </c>
       <c r="C297" t="s">
         <v>3575</v>
@@ -57566,10 +57572,10 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B298" t="s">
-        <v>3450</v>
+        <v>3449</v>
       </c>
       <c r="C298" t="s">
         <v>3575</v>
@@ -57577,10 +57583,10 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>377</v>
+        <v>278</v>
       </c>
       <c r="B299" t="s">
-        <v>378</v>
+        <v>3450</v>
       </c>
       <c r="C299" t="s">
         <v>3575</v>
@@ -57588,10 +57594,10 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>289</v>
+        <v>377</v>
       </c>
       <c r="B300" t="s">
-        <v>287</v>
+        <v>378</v>
       </c>
       <c r="C300" t="s">
         <v>3575</v>
@@ -57599,10 +57605,10 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B301" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="C301" t="s">
         <v>3575</v>
@@ -57610,10 +57616,10 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>409</v>
+        <v>290</v>
       </c>
       <c r="B302" t="s">
-        <v>410</v>
+        <v>288</v>
       </c>
       <c r="C302" t="s">
         <v>3575</v>
@@ -57621,10 +57627,10 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>353</v>
+        <v>409</v>
       </c>
       <c r="B303" t="s">
-        <v>349</v>
+        <v>410</v>
       </c>
       <c r="C303" t="s">
         <v>3575</v>
@@ -57632,10 +57638,10 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B304" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="C304" t="s">
         <v>3575</v>
@@ -57643,10 +57649,10 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>407</v>
+        <v>354</v>
       </c>
       <c r="B305" t="s">
-        <v>408</v>
+        <v>350</v>
       </c>
       <c r="C305" t="s">
         <v>3575</v>
@@ -57654,10 +57660,10 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>351</v>
+        <v>407</v>
       </c>
       <c r="B306" t="s">
-        <v>347</v>
+        <v>408</v>
       </c>
       <c r="C306" t="s">
         <v>3575</v>
@@ -57665,10 +57671,10 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B307" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="C307" t="s">
         <v>3575</v>
@@ -57676,10 +57682,10 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>391</v>
+        <v>352</v>
       </c>
       <c r="B308" t="s">
-        <v>392</v>
+        <v>348</v>
       </c>
       <c r="C308" t="s">
         <v>3575</v>
@@ -57687,10 +57693,10 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>321</v>
+        <v>391</v>
       </c>
       <c r="B309" t="s">
-        <v>315</v>
+        <v>392</v>
       </c>
       <c r="C309" t="s">
         <v>3575</v>
@@ -57698,10 +57704,10 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B310" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="C310" t="s">
         <v>3575</v>
@@ -57709,10 +57715,10 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>389</v>
+        <v>322</v>
       </c>
       <c r="B311" t="s">
-        <v>390</v>
+        <v>316</v>
       </c>
       <c r="C311" t="s">
         <v>3575</v>
@@ -57720,10 +57726,10 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>311</v>
+        <v>389</v>
       </c>
       <c r="B312" t="s">
-        <v>313</v>
+        <v>390</v>
       </c>
       <c r="C312" t="s">
         <v>3575</v>
@@ -57731,10 +57737,10 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B313" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C313" t="s">
         <v>3575</v>
@@ -57742,10 +57748,10 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>366</v>
+        <v>312</v>
       </c>
       <c r="B314" t="s">
-        <v>367</v>
+        <v>314</v>
       </c>
       <c r="C314" t="s">
         <v>3575</v>
@@ -57753,10 +57759,10 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>263</v>
+        <v>366</v>
       </c>
       <c r="B315" t="s">
-        <v>264</v>
+        <v>367</v>
       </c>
       <c r="C315" t="s">
         <v>3575</v>
@@ -57764,10 +57770,10 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>266</v>
+        <v>263</v>
       </c>
       <c r="B316" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C316" t="s">
         <v>3575</v>
@@ -57775,10 +57781,10 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>385</v>
+        <v>266</v>
       </c>
       <c r="B317" t="s">
-        <v>386</v>
+        <v>265</v>
       </c>
       <c r="C317" t="s">
         <v>3575</v>
@@ -57786,10 +57792,10 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>305</v>
+        <v>385</v>
       </c>
       <c r="B318" t="s">
-        <v>303</v>
+        <v>386</v>
       </c>
       <c r="C318" t="s">
         <v>3575</v>
@@ -57797,10 +57803,10 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B319" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C319" t="s">
         <v>3575</v>
@@ -57808,10 +57814,10 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>381</v>
+        <v>306</v>
       </c>
       <c r="B320" t="s">
-        <v>382</v>
+        <v>304</v>
       </c>
       <c r="C320" t="s">
         <v>3575</v>
@@ -57819,10 +57825,10 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>297</v>
+        <v>381</v>
       </c>
       <c r="B321" t="s">
-        <v>295</v>
+        <v>382</v>
       </c>
       <c r="C321" t="s">
         <v>3575</v>
@@ -57830,10 +57836,10 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="B322" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="C322" t="s">
         <v>3575</v>
@@ -57841,10 +57847,10 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>393</v>
+        <v>298</v>
       </c>
       <c r="B323" t="s">
-        <v>394</v>
+        <v>296</v>
       </c>
       <c r="C323" t="s">
         <v>3575</v>
@@ -57852,10 +57858,10 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>319</v>
+        <v>393</v>
       </c>
       <c r="B324" t="s">
-        <v>317</v>
+        <v>394</v>
       </c>
       <c r="C324" t="s">
         <v>3575</v>
@@ -57863,10 +57869,10 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B325" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C325" t="s">
         <v>3575</v>
@@ -57874,10 +57880,10 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>383</v>
+        <v>320</v>
       </c>
       <c r="B326" t="s">
-        <v>384</v>
+        <v>318</v>
       </c>
       <c r="C326" t="s">
         <v>3575</v>
@@ -57885,10 +57891,10 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>301</v>
+        <v>383</v>
       </c>
       <c r="B327" t="s">
-        <v>299</v>
+        <v>384</v>
       </c>
       <c r="C327" t="s">
         <v>3575</v>
@@ -57896,10 +57902,10 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B328" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="C328" t="s">
         <v>3575</v>
@@ -57907,10 +57913,10 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>19</v>
-      </c>
-      <c r="B329" s="3" t="s">
-        <v>164</v>
+        <v>302</v>
+      </c>
+      <c r="B329" t="s">
+        <v>300</v>
       </c>
       <c r="C329" t="s">
         <v>3575</v>
@@ -57918,10 +57924,10 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B330" s="3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C330" t="s">
         <v>3575</v>
@@ -57929,10 +57935,10 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B331" s="3" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C331" t="s">
         <v>3575</v>
@@ -57940,10 +57946,10 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="B332" s="3" t="s">
-        <v>161</v>
+        <v>166</v>
       </c>
       <c r="C332" t="s">
         <v>3575</v>
@@ -57951,10 +57957,10 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B333" s="3" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C333" t="s">
         <v>3575</v>
@@ -57962,10 +57968,10 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C334" t="s">
         <v>3575</v>
@@ -57973,10 +57979,10 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C335" t="s">
         <v>3575</v>
@@ -57984,10 +57990,10 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C336" t="s">
         <v>3575</v>
@@ -57995,10 +58001,10 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C337" t="s">
         <v>3575</v>
@@ -58006,10 +58012,10 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C338" t="s">
         <v>3575</v>
@@ -58017,10 +58023,10 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C339" t="s">
         <v>3575</v>
@@ -58028,10 +58034,10 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>3466</v>
-      </c>
-      <c r="B340" t="s">
-        <v>3465</v>
+        <v>11</v>
+      </c>
+      <c r="B340" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="C340" t="s">
         <v>3575</v>
@@ -58039,10 +58045,10 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>3459</v>
+        <v>3466</v>
       </c>
       <c r="B341" t="s">
-        <v>3462</v>
+        <v>3465</v>
       </c>
       <c r="C341" t="s">
         <v>3575</v>
@@ -58050,10 +58056,10 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>3463</v>
+        <v>3459</v>
       </c>
       <c r="B342" t="s">
-        <v>3464</v>
+        <v>3462</v>
       </c>
       <c r="C342" t="s">
         <v>3575</v>
@@ -58061,10 +58067,10 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>415</v>
+        <v>3463</v>
       </c>
       <c r="B343" t="s">
-        <v>227</v>
+        <v>3464</v>
       </c>
       <c r="C343" t="s">
         <v>3575</v>
@@ -58072,10 +58078,10 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>118</v>
+        <v>415</v>
       </c>
       <c r="B344" t="s">
-        <v>3445</v>
+        <v>227</v>
       </c>
       <c r="C344" t="s">
         <v>3575</v>
@@ -58083,10 +58089,10 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>416</v>
+        <v>118</v>
       </c>
       <c r="B345" t="s">
-        <v>226</v>
+        <v>3445</v>
       </c>
       <c r="C345" t="s">
         <v>3575</v>
@@ -58094,32 +58100,32 @@
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>117</v>
+        <v>416</v>
       </c>
       <c r="B346" t="s">
-        <v>3444</v>
+        <v>226</v>
       </c>
       <c r="C346" t="s">
         <v>3575</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A347" s="2" t="s">
-        <v>417</v>
+      <c r="A347" t="s">
+        <v>117</v>
       </c>
       <c r="B347" t="s">
-        <v>225</v>
+        <v>3444</v>
       </c>
       <c r="C347" t="s">
         <v>3575</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A348" t="s">
-        <v>116</v>
+      <c r="A348" s="2" t="s">
+        <v>417</v>
       </c>
       <c r="B348" t="s">
-        <v>3447</v>
+        <v>225</v>
       </c>
       <c r="C348" t="s">
         <v>3575</v>
@@ -58127,10 +58133,10 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>418</v>
+        <v>116</v>
       </c>
       <c r="B349" t="s">
-        <v>224</v>
+        <v>3447</v>
       </c>
       <c r="C349" t="s">
         <v>3575</v>
@@ -58138,10 +58144,10 @@
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>115</v>
+        <v>418</v>
       </c>
       <c r="B350" t="s">
-        <v>3446</v>
+        <v>224</v>
       </c>
       <c r="C350" t="s">
         <v>3575</v>
@@ -58149,10 +58155,10 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>3547</v>
+        <v>115</v>
       </c>
       <c r="B351" t="s">
-        <v>3549</v>
+        <v>3446</v>
       </c>
       <c r="C351" t="s">
         <v>3575</v>
@@ -58160,10 +58166,10 @@
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>3455</v>
+        <v>3547</v>
       </c>
       <c r="B352" t="s">
-        <v>3456</v>
+        <v>3549</v>
       </c>
       <c r="C352" t="s">
         <v>3575</v>
@@ -58171,10 +58177,10 @@
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>3454</v>
+        <v>3455</v>
       </c>
       <c r="B353" t="s">
-        <v>3453</v>
+        <v>3456</v>
       </c>
       <c r="C353" t="s">
         <v>3575</v>
@@ -58182,10 +58188,10 @@
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>3451</v>
+        <v>3454</v>
       </c>
       <c r="B354" t="s">
-        <v>3452</v>
+        <v>3453</v>
       </c>
       <c r="C354" t="s">
         <v>3575</v>
@@ -58193,10 +58199,10 @@
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>3660</v>
-      </c>
-      <c r="B355" s="3" t="s">
-        <v>3661</v>
+        <v>3451</v>
+      </c>
+      <c r="B355" t="s">
+        <v>3452</v>
       </c>
       <c r="C355" t="s">
         <v>3575</v>
@@ -58204,10 +58210,10 @@
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>22</v>
+        <v>3660</v>
       </c>
       <c r="B356" s="3" t="s">
-        <v>412</v>
+        <v>3661</v>
       </c>
       <c r="C356" t="s">
         <v>3575</v>
@@ -58215,10 +58221,10 @@
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>3833</v>
-      </c>
-      <c r="B357" t="s">
-        <v>3662</v>
+        <v>22</v>
+      </c>
+      <c r="B357" s="3" t="s">
+        <v>412</v>
       </c>
       <c r="C357" t="s">
         <v>3575</v>
@@ -58226,10 +58232,10 @@
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>3460</v>
+        <v>3833</v>
       </c>
       <c r="B358" t="s">
-        <v>3475</v>
+        <v>3662</v>
       </c>
       <c r="C358" t="s">
         <v>3575</v>
@@ -58237,10 +58243,10 @@
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>3477</v>
+        <v>3460</v>
       </c>
       <c r="B359" t="s">
-        <v>3473</v>
+        <v>3475</v>
       </c>
       <c r="C359" t="s">
         <v>3575</v>
@@ -58248,10 +58254,10 @@
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>17</v>
-      </c>
-      <c r="B360" s="3" t="s">
-        <v>359</v>
+        <v>3477</v>
+      </c>
+      <c r="B360" t="s">
+        <v>3473</v>
       </c>
       <c r="C360" t="s">
         <v>3575</v>
@@ -58259,10 +58265,10 @@
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>414</v>
+        <v>17</v>
       </c>
       <c r="B361" s="3" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="C361" t="s">
         <v>3575</v>
@@ -58270,10 +58276,10 @@
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>15</v>
+        <v>414</v>
       </c>
       <c r="B362" s="3" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="C362" t="s">
         <v>3575</v>
@@ -58281,10 +58287,10 @@
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="C363" t="s">
         <v>3575</v>
@@ -58292,10 +58298,10 @@
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="C364" t="s">
         <v>3575</v>
@@ -58303,10 +58309,10 @@
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>419</v>
+        <v>362</v>
       </c>
       <c r="C365" t="s">
         <v>3575</v>
@@ -58314,10 +58320,10 @@
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="C366" t="s">
         <v>3575</v>
@@ -58325,10 +58331,10 @@
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C367" t="s">
         <v>3575</v>
@@ -58336,10 +58342,10 @@
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C368" t="s">
         <v>3575</v>
@@ -58347,10 +58353,10 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>3639</v>
-      </c>
-      <c r="B369" t="s">
-        <v>3640</v>
+        <v>2</v>
+      </c>
+      <c r="B369" s="3" t="s">
+        <v>422</v>
       </c>
       <c r="C369" t="s">
         <v>3575</v>
@@ -58358,10 +58364,10 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>3643</v>
+        <v>3639</v>
       </c>
       <c r="B370" t="s">
-        <v>3644</v>
+        <v>3640</v>
       </c>
       <c r="C370" t="s">
         <v>3575</v>
@@ -58369,10 +58375,10 @@
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>3641</v>
+        <v>3643</v>
       </c>
       <c r="B371" t="s">
-        <v>3642</v>
+        <v>3644</v>
       </c>
       <c r="C371" t="s">
         <v>3575</v>
@@ -58380,10 +58386,10 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>3457</v>
+        <v>3641</v>
       </c>
       <c r="B372" t="s">
-        <v>3458</v>
+        <v>3642</v>
       </c>
       <c r="C372" t="s">
         <v>3575</v>
@@ -58391,10 +58397,10 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>3649</v>
-      </c>
-      <c r="B373" s="3" t="s">
-        <v>3650</v>
+        <v>3457</v>
+      </c>
+      <c r="B373" t="s">
+        <v>3458</v>
       </c>
       <c r="C373" t="s">
         <v>3575</v>
@@ -58402,10 +58408,10 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>3648</v>
+        <v>3649</v>
       </c>
       <c r="B374" s="3" t="s">
-        <v>3646</v>
+        <v>3650</v>
       </c>
       <c r="C374" t="s">
         <v>3575</v>
@@ -58413,10 +58419,10 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>3647</v>
+        <v>3648</v>
       </c>
       <c r="B375" s="3" t="s">
-        <v>3645</v>
+        <v>3646</v>
       </c>
       <c r="C375" t="s">
         <v>3575</v>
@@ -58424,10 +58430,10 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>3546</v>
-      </c>
-      <c r="B376" t="s">
-        <v>3548</v>
+        <v>3647</v>
+      </c>
+      <c r="B376" s="3" t="s">
+        <v>3645</v>
       </c>
       <c r="C376" t="s">
         <v>3575</v>
@@ -58435,10 +58441,10 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>14</v>
-      </c>
-      <c r="B377" s="3" t="s">
-        <v>163</v>
+        <v>3546</v>
+      </c>
+      <c r="B377" t="s">
+        <v>3548</v>
       </c>
       <c r="C377" t="s">
         <v>3575</v>
@@ -58446,21 +58452,21 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>112</v>
-      </c>
-      <c r="B378" t="s">
-        <v>194</v>
+        <v>14</v>
+      </c>
+      <c r="B378" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="C378" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>108</v>
+        <v>112</v>
       </c>
       <c r="B379" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="C379" t="s">
         <v>3576</v>
@@ -58468,10 +58474,10 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B380" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C380" t="s">
         <v>3576</v>
@@ -58479,10 +58485,10 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B381" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C381" t="s">
         <v>3576</v>
@@ -58490,10 +58496,10 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B382" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="C382" t="s">
         <v>3576</v>
@@ -58501,10 +58507,10 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="B383" t="s">
-        <v>179</v>
+        <v>199</v>
       </c>
       <c r="C383" t="s">
         <v>3576</v>
@@ -58512,10 +58518,10 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="B384" t="s">
-        <v>186</v>
+        <v>179</v>
       </c>
       <c r="C384" t="s">
         <v>3576</v>
@@ -58523,10 +58529,10 @@
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>96</v>
+        <v>103</v>
       </c>
       <c r="B385" t="s">
-        <v>180</v>
+        <v>186</v>
       </c>
       <c r="C385" t="s">
         <v>3576</v>
@@ -58534,10 +58540,10 @@
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B386" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C386" t="s">
         <v>3576</v>
@@ -58545,10 +58551,10 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>93</v>
+        <v>97</v>
       </c>
       <c r="B387" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="C387" t="s">
         <v>3576</v>
@@ -58556,10 +58562,10 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B388" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C388" t="s">
         <v>3576</v>
@@ -58567,10 +58573,10 @@
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="B389" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="C389" t="s">
         <v>3576</v>
@@ -58578,10 +58584,10 @@
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B390" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C390" t="s">
         <v>3576</v>
@@ -58589,10 +58595,10 @@
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>121</v>
+        <v>99</v>
       </c>
       <c r="B391" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C391" t="s">
         <v>3576</v>
@@ -58600,10 +58606,10 @@
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>111</v>
+        <v>121</v>
       </c>
       <c r="B392" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C392" t="s">
         <v>3576</v>
@@ -58611,10 +58617,10 @@
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="B393" t="s">
-        <v>185</v>
+        <v>192</v>
       </c>
       <c r="C393" t="s">
         <v>3576</v>
@@ -58622,10 +58628,10 @@
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B394" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C394" t="s">
         <v>3576</v>
@@ -58633,10 +58639,10 @@
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>122</v>
+        <v>102</v>
       </c>
       <c r="B395" t="s">
-        <v>3723</v>
+        <v>187</v>
       </c>
       <c r="C395" t="s">
         <v>3576</v>
@@ -58644,10 +58650,10 @@
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="B396" t="s">
-        <v>193</v>
+        <v>3723</v>
       </c>
       <c r="C396" t="s">
         <v>3576</v>
@@ -58655,10 +58661,10 @@
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
       <c r="B397" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
       <c r="C397" t="s">
         <v>3576</v>
@@ -58666,10 +58672,10 @@
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="B398" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="C398" t="s">
         <v>3576</v>
@@ -58677,10 +58683,10 @@
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>104</v>
+        <v>119</v>
       </c>
       <c r="B399" t="s">
-        <v>188</v>
+        <v>190</v>
       </c>
       <c r="C399" t="s">
         <v>3576</v>
@@ -58688,10 +58694,10 @@
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B400" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C400" t="s">
         <v>3576</v>
@@ -58699,23 +58705,34 @@
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="B401" t="s">
-        <v>195</v>
+        <v>189</v>
       </c>
       <c r="C401" t="s">
         <v>3576</v>
       </c>
     </row>
+    <row r="402" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A402" t="s">
+        <v>120</v>
+      </c>
+      <c r="B402" t="s">
+        <v>195</v>
+      </c>
+      <c r="C402" t="s">
+        <v>3576</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C389" xr:uid="{00000000-0009-0000-0000-000007000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C401">
-      <sortCondition ref="C1:C389"/>
+  <autoFilter ref="A1:C390" xr:uid="{00000000-0009-0000-0000-000007000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C402">
+      <sortCondition ref="C1:C390"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A358:B444">
-    <sortCondition ref="A358:A444"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A359:B445">
+    <sortCondition ref="A359:A445"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Inclusão de melhorias @202405201008
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,45 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98EE2F09-BF02-475B-922B-D51F182CDEAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AD1572-EE57-4FF7-9E3E-999CCA207668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="3280" windowWidth="19420" windowHeight="10300" tabRatio="699" firstSheet="6" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="3280" windowWidth="19420" windowHeight="10300" tabRatio="699" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="market" sheetId="8" r:id="rId1"/>
-    <sheet name="consensus" sheetId="7" r:id="rId2"/>
-    <sheet name="income_cashflow" sheetId="5" r:id="rId3"/>
-    <sheet name="dividend" sheetId="16" r:id="rId4"/>
-    <sheet name="short_interest" sheetId="17" r:id="rId5"/>
-    <sheet name="technicals" sheetId="18" r:id="rId6"/>
-    <sheet name="leverage" sheetId="15" r:id="rId7"/>
-    <sheet name="balance_sheet" sheetId="11" r:id="rId8"/>
-    <sheet name="ratios" sheetId="12" r:id="rId9"/>
-    <sheet name="options" sheetId="10" r:id="rId10"/>
-    <sheet name="index_fundamentals" sheetId="14" r:id="rId11"/>
-    <sheet name="&gt;" sheetId="9" r:id="rId12"/>
-    <sheet name="equities" sheetId="3" r:id="rId13"/>
-    <sheet name="macro" sheetId="1" r:id="rId14"/>
-    <sheet name="anbima" sheetId="13" r:id="rId15"/>
-    <sheet name="Planilha4" sheetId="4" r:id="rId16"/>
+    <sheet name="daily" sheetId="19" r:id="rId1"/>
+    <sheet name="quarterly" sheetId="20" r:id="rId2"/>
+    <sheet name="index_fundamentals" sheetId="14" r:id="rId3"/>
+    <sheet name="&gt;" sheetId="9" r:id="rId4"/>
+    <sheet name="equities" sheetId="3" r:id="rId5"/>
+    <sheet name="macro" sheetId="1" r:id="rId6"/>
+    <sheet name="anbima" sheetId="13" r:id="rId7"/>
+    <sheet name="Planilha4" sheetId="4" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId17"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">balance_sheet!$A$1:$B$181</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">consensus!$A$1:$B$191</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">dividend!$A$1:$B$170</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">equities!$A$1:$L$1268</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">income_cashflow!$A$1:$B$169</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">index_fundamentals!$A$1:$B$195</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">leverage!$A$1:$B$180</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">macro!$A$1:$C$358</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">market!$A$1:$B$195</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">options!$A$1:$B$195</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">ratios!$A$1:$B$177</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">short_interest!$A$1:$B$169</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">technicals!$A$1:$B$170</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">daily!$C$1:$C$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">equities!$A$1:$L$1268</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">index_fundamentals!$A$1:$B$195</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">macro!$A$1:$C$358</definedName>
   </definedNames>
   <calcPr calcId="191029" calcMode="manual"/>
   <extLst>
@@ -69,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11381" uniqueCount="3948">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11444" uniqueCount="3978">
   <si>
     <t>bbgTicker</t>
   </si>
@@ -11913,6 +11896,96 @@
   </si>
   <si>
     <t>us_utilities_xlu</t>
+  </si>
+  <si>
+    <t>INJCSP Index</t>
+  </si>
+  <si>
+    <t>us_continuing_jobless_claims</t>
+  </si>
+  <si>
+    <t>SHORT_SELL_NUM_SHARES</t>
+  </si>
+  <si>
+    <t>short_interest</t>
+  </si>
+  <si>
+    <t>market</t>
+  </si>
+  <si>
+    <t>consensus</t>
+  </si>
+  <si>
+    <t>dividend</t>
+  </si>
+  <si>
+    <t>technicals</t>
+  </si>
+  <si>
+    <t>options</t>
+  </si>
+  <si>
+    <t>leverage</t>
+  </si>
+  <si>
+    <t>balance_sheet</t>
+  </si>
+  <si>
+    <t>ratios</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>income_statement</t>
+  </si>
+  <si>
+    <t>cash_flow</t>
+  </si>
+  <si>
+    <t>num_of_shares</t>
+  </si>
+  <si>
+    <t>TOTAL_INVESTED_CAPITAL</t>
+  </si>
+  <si>
+    <t>invested_capital</t>
+  </si>
+  <si>
+    <t>CAPITAL_EMPLOYED</t>
+  </si>
+  <si>
+    <t>capital_employed</t>
+  </si>
+  <si>
+    <t>JOLTQUIS Index</t>
+  </si>
+  <si>
+    <t>us_quits_rate</t>
+  </si>
+  <si>
+    <t>us_quits_rate_nsa</t>
+  </si>
+  <si>
+    <t>JOLTQUIT Index</t>
+  </si>
+  <si>
+    <t>AHE YOY% Index</t>
+  </si>
+  <si>
+    <t>us_average_hourly_earnings_yoy</t>
+  </si>
+  <si>
+    <t>USURTOT  Index</t>
+  </si>
+  <si>
+    <t>us_unemployment_rate</t>
+  </si>
+  <si>
+    <t>NFP TYOY Index</t>
+  </si>
+  <si>
+    <t>us_employees_nonfarm_payrolls_yoy</t>
   </si>
 </sst>
 </file>
@@ -12490,13 +12563,821 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr codeName="Planilha1"/>
-  <dimension ref="A1:B77"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AF12734-6CD2-4763-A89F-68BEE8262926}">
+  <dimension ref="A1:C77"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3357</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3427</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3371</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3375</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3952</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3810</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3813</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3952</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3811</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3814</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3952</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3812</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3815</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3952</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3372</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3376</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3952</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3373</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3377</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3952</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3374</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3378</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3952</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3413</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3411</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3952</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3839</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3840</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3952</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3380</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3384</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3381</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3385</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3382</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3386</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3383</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3387</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3394</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3395</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3388</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3390</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3397</v>
+      </c>
+      <c r="B17" t="s">
+        <v>3787</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3389</v>
+      </c>
+      <c r="B18" t="s">
+        <v>3391</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3392</v>
+      </c>
+      <c r="B19" t="s">
+        <v>3393</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3398</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3399</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="4" t="s">
+        <v>3400</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3401</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3402</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3403</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3816</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3817</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3953</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3796</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3855</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3954</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3797</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3854</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3954</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3798</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3799</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3951</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>3800</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3801</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3951</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>3950</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>3951</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3951</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3802</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3806</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3955</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>3803</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3809</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3955</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>3804</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3807</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3955</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3805</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3808</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3955</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>3420</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3423</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3956</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>3421</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3424</v>
+      </c>
+      <c r="C34" t="s">
+        <v>3956</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>3422</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3425</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3956</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>3368</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3405</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3963</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="3"/>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{122C3747-39A0-4581-8089-8AF8AFD16A06}">
+  <dimension ref="A1:C91"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3357</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3427</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3358</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3361</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3960</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3841</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3847</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3961</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>3844</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3848</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3961</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3842</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3849</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3961</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3846</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3850</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3961</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3843</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3851</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3961</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3435</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3853</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3961</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3845</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>3852</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3962</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3788</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3792</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3957</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3789</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3793</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3957</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3359</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3363</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3360</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3364</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3366</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3418</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3369</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3417</v>
+      </c>
+      <c r="C15" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3367</v>
+      </c>
+      <c r="B16" t="s">
+        <v>3404</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3419</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>3437</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3436</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>3428</v>
+      </c>
+      <c r="C18" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3964</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>3965</v>
+      </c>
+      <c r="C19" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3966</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>3967</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3958</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3415</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3408</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3959</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="4" t="s">
+        <v>3414</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>3409</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3959</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3416</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>3410</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3959</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B52" s="3"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="3"/>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="3"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="3"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B57" s="3"/>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B58" s="3"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B59" s="3"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B60" s="3"/>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B61" s="3"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B62" s="3"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B63" s="3"/>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B64" s="3"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" s="3"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" s="3"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" s="3"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B68" s="3"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B69" s="3"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" s="3"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" s="3"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" s="3"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" s="3"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" s="3"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" s="3"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" s="3"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" s="3"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" s="3"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" s="3"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" s="3"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" s="3"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" s="3"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" s="3"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5233DC-DA50-4AF6-A52B-C110073B56A9}">
+  <sheetPr codeName="Planilha7"/>
+  <dimension ref="A1:B115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12515,144 +13396,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3371</v>
+        <v>3388</v>
       </c>
       <c r="B2" t="s">
-        <v>3375</v>
+        <v>3390</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3810</v>
+        <v>3781</v>
       </c>
       <c r="B3" t="s">
-        <v>3813</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3811</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3814</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3812</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3815</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3372</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3376</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3373</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3377</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3374</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3378</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3413</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3411</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3839</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3840</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="3"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B234" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <sheetPr codeName="Planilha6"/>
-  <dimension ref="A1:B115"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J14" sqref="J14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3357</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3427</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3420</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3423</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3421</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3424</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3422</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3425</v>
+        <v>3782</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -12790,182 +13545,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5233DC-DA50-4AF6-A52B-C110073B56A9}">
-  <sheetPr codeName="Planilha7"/>
-  <dimension ref="A1:B115"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3357</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3427</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3388</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3390</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3781</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3782</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B17" s="4"/>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B28" s="4"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A30" s="4"/>
-      <c r="B30" s="4"/>
-    </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
-      <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="3"/>
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="3"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="3"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="3"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="3"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="3"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="3"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="3"/>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B95" s="3"/>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="3"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="3"/>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B98" s="3"/>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="3"/>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="3"/>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="3"/>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B102" s="3"/>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B103" s="3"/>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B104" s="3"/>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B105" s="3"/>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B106" s="3"/>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B107" s="3"/>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B108" s="3"/>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B114" s="3"/>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B115" s="3"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B234" xr:uid="{00000000-0009-0000-0000-000005000000}"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Planilha8">
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -12973,7 +13553,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="K28" sqref="K28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12982,7 +13562,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr codeName="Planilha10"/>
   <dimension ref="A1:N1269"/>
@@ -54286,14 +54866,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Planilha9"/>
-  <dimension ref="A1:C402"/>
+  <dimension ref="A1:C408"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I134" sqref="I134"/>
+      <pane ySplit="1" topLeftCell="A391" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55757,10 +56337,10 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>3946</v>
+        <v>3820</v>
       </c>
       <c r="B133" t="s">
-        <v>3947</v>
+        <v>3823</v>
       </c>
       <c r="C133" t="s">
         <v>3574</v>
@@ -55768,10 +56348,10 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>3820</v>
+        <v>3346</v>
       </c>
       <c r="B134" t="s">
-        <v>3823</v>
+        <v>3539</v>
       </c>
       <c r="C134" t="s">
         <v>3574</v>
@@ -55779,10 +56359,10 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>3346</v>
+        <v>3541</v>
       </c>
       <c r="B135" t="s">
-        <v>3539</v>
+        <v>3540</v>
       </c>
       <c r="C135" t="s">
         <v>3574</v>
@@ -55790,10 +56370,10 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>3541</v>
+        <v>3824</v>
       </c>
       <c r="B136" t="s">
-        <v>3540</v>
+        <v>3825</v>
       </c>
       <c r="C136" t="s">
         <v>3574</v>
@@ -55801,10 +56381,10 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>3824</v>
+        <v>3356</v>
       </c>
       <c r="B137" t="s">
-        <v>3825</v>
+        <v>3509</v>
       </c>
       <c r="C137" t="s">
         <v>3574</v>
@@ -55812,10 +56392,10 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>3356</v>
+        <v>3819</v>
       </c>
       <c r="B138" t="s">
-        <v>3509</v>
+        <v>3818</v>
       </c>
       <c r="C138" t="s">
         <v>3574</v>
@@ -55823,10 +56403,10 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>3819</v>
+        <v>38</v>
       </c>
       <c r="B139" t="s">
-        <v>3818</v>
+        <v>3511</v>
       </c>
       <c r="C139" t="s">
         <v>3574</v>
@@ -55834,10 +56414,10 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>38</v>
+        <v>3946</v>
       </c>
       <c r="B140" t="s">
-        <v>3511</v>
+        <v>3947</v>
       </c>
       <c r="C140" t="s">
         <v>3574</v>
@@ -57957,10 +58537,10 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>12</v>
-      </c>
-      <c r="B333" s="3" t="s">
-        <v>161</v>
+        <v>3972</v>
+      </c>
+      <c r="B333" t="s">
+        <v>3973</v>
       </c>
       <c r="C333" t="s">
         <v>3575</v>
@@ -57968,10 +58548,10 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="B334" s="3" t="s">
-        <v>155</v>
+        <v>161</v>
       </c>
       <c r="C334" t="s">
         <v>3575</v>
@@ -57979,10 +58559,10 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>13</v>
+        <v>6</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C335" t="s">
         <v>3575</v>
@@ -57990,10 +58570,10 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>156</v>
+        <v>162</v>
       </c>
       <c r="C336" t="s">
         <v>3575</v>
@@ -58001,10 +58581,10 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C337" t="s">
         <v>3575</v>
@@ -58012,10 +58592,10 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B338" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C338" t="s">
         <v>3575</v>
@@ -58023,10 +58603,10 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B339" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C339" t="s">
         <v>3575</v>
@@ -58034,10 +58614,10 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B340" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C340" t="s">
         <v>3575</v>
@@ -58045,10 +58625,10 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>3466</v>
-      </c>
-      <c r="B341" t="s">
-        <v>3465</v>
+        <v>11</v>
+      </c>
+      <c r="B341" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="C341" t="s">
         <v>3575</v>
@@ -58056,10 +58636,10 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>3459</v>
+        <v>3948</v>
       </c>
       <c r="B342" t="s">
-        <v>3462</v>
+        <v>3949</v>
       </c>
       <c r="C342" t="s">
         <v>3575</v>
@@ -58067,10 +58647,10 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>3463</v>
+        <v>3466</v>
       </c>
       <c r="B343" t="s">
-        <v>3464</v>
+        <v>3465</v>
       </c>
       <c r="C343" t="s">
         <v>3575</v>
@@ -58078,10 +58658,10 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>415</v>
+        <v>3459</v>
       </c>
       <c r="B344" t="s">
-        <v>227</v>
+        <v>3462</v>
       </c>
       <c r="C344" t="s">
         <v>3575</v>
@@ -58089,10 +58669,10 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>118</v>
+        <v>3463</v>
       </c>
       <c r="B345" t="s">
-        <v>3445</v>
+        <v>3464</v>
       </c>
       <c r="C345" t="s">
         <v>3575</v>
@@ -58100,10 +58680,10 @@
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B346" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C346" t="s">
         <v>3575</v>
@@ -58111,21 +58691,21 @@
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B347" t="s">
-        <v>3444</v>
+        <v>3445</v>
       </c>
       <c r="C347" t="s">
         <v>3575</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A348" s="2" t="s">
-        <v>417</v>
+      <c r="A348" t="s">
+        <v>416</v>
       </c>
       <c r="B348" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C348" t="s">
         <v>3575</v>
@@ -58133,21 +58713,21 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B349" t="s">
-        <v>3447</v>
+        <v>3444</v>
       </c>
       <c r="C349" t="s">
         <v>3575</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A350" t="s">
-        <v>418</v>
+      <c r="A350" s="2" t="s">
+        <v>417</v>
       </c>
       <c r="B350" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="C350" t="s">
         <v>3575</v>
@@ -58155,10 +58735,10 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B351" t="s">
-        <v>3446</v>
+        <v>3447</v>
       </c>
       <c r="C351" t="s">
         <v>3575</v>
@@ -58166,10 +58746,10 @@
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>3547</v>
+        <v>418</v>
       </c>
       <c r="B352" t="s">
-        <v>3549</v>
+        <v>224</v>
       </c>
       <c r="C352" t="s">
         <v>3575</v>
@@ -58177,10 +58757,10 @@
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>3455</v>
+        <v>115</v>
       </c>
       <c r="B353" t="s">
-        <v>3456</v>
+        <v>3446</v>
       </c>
       <c r="C353" t="s">
         <v>3575</v>
@@ -58188,10 +58768,10 @@
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>3454</v>
+        <v>3547</v>
       </c>
       <c r="B354" t="s">
-        <v>3453</v>
+        <v>3549</v>
       </c>
       <c r="C354" t="s">
         <v>3575</v>
@@ -58199,10 +58779,10 @@
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>3451</v>
+        <v>3455</v>
       </c>
       <c r="B355" t="s">
-        <v>3452</v>
+        <v>3456</v>
       </c>
       <c r="C355" t="s">
         <v>3575</v>
@@ -58210,10 +58790,10 @@
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>3660</v>
-      </c>
-      <c r="B356" s="3" t="s">
-        <v>3661</v>
+        <v>3454</v>
+      </c>
+      <c r="B356" t="s">
+        <v>3453</v>
       </c>
       <c r="C356" t="s">
         <v>3575</v>
@@ -58221,10 +58801,10 @@
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>22</v>
-      </c>
-      <c r="B357" s="3" t="s">
-        <v>412</v>
+        <v>3451</v>
+      </c>
+      <c r="B357" t="s">
+        <v>3452</v>
       </c>
       <c r="C357" t="s">
         <v>3575</v>
@@ -58232,10 +58812,10 @@
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>3833</v>
-      </c>
-      <c r="B358" t="s">
-        <v>3662</v>
+        <v>3660</v>
+      </c>
+      <c r="B358" s="3" t="s">
+        <v>3661</v>
       </c>
       <c r="C358" t="s">
         <v>3575</v>
@@ -58243,10 +58823,10 @@
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>3460</v>
-      </c>
-      <c r="B359" t="s">
-        <v>3475</v>
+        <v>3976</v>
+      </c>
+      <c r="B359" s="3" t="s">
+        <v>3977</v>
       </c>
       <c r="C359" t="s">
         <v>3575</v>
@@ -58254,10 +58834,10 @@
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>3477</v>
-      </c>
-      <c r="B360" t="s">
-        <v>3473</v>
+        <v>22</v>
+      </c>
+      <c r="B360" s="3" t="s">
+        <v>412</v>
       </c>
       <c r="C360" t="s">
         <v>3575</v>
@@ -58265,10 +58845,10 @@
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>17</v>
-      </c>
-      <c r="B361" s="3" t="s">
-        <v>359</v>
+        <v>3833</v>
+      </c>
+      <c r="B361" t="s">
+        <v>3662</v>
       </c>
       <c r="C361" t="s">
         <v>3575</v>
@@ -58276,10 +58856,10 @@
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>414</v>
-      </c>
-      <c r="B362" s="3" t="s">
-        <v>363</v>
+        <v>3460</v>
+      </c>
+      <c r="B362" t="s">
+        <v>3475</v>
       </c>
       <c r="C362" t="s">
         <v>3575</v>
@@ -58287,10 +58867,10 @@
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>15</v>
-      </c>
-      <c r="B363" s="3" t="s">
-        <v>360</v>
+        <v>3477</v>
+      </c>
+      <c r="B363" t="s">
+        <v>3473</v>
       </c>
       <c r="C363" t="s">
         <v>3575</v>
@@ -58298,10 +58878,10 @@
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C364" t="s">
         <v>3575</v>
@@ -58309,10 +58889,10 @@
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>16</v>
+        <v>414</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="C365" t="s">
         <v>3575</v>
@@ -58320,10 +58900,10 @@
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="B366" s="3" t="s">
-        <v>419</v>
+        <v>360</v>
       </c>
       <c r="C366" t="s">
         <v>3575</v>
@@ -58331,10 +58911,10 @@
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B367" s="3" t="s">
-        <v>420</v>
+        <v>361</v>
       </c>
       <c r="C367" t="s">
         <v>3575</v>
@@ -58342,10 +58922,10 @@
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>5</v>
+        <v>16</v>
       </c>
       <c r="B368" s="3" t="s">
-        <v>421</v>
+        <v>362</v>
       </c>
       <c r="C368" t="s">
         <v>3575</v>
@@ -58353,10 +58933,10 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B369" s="3" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="C369" t="s">
         <v>3575</v>
@@ -58364,10 +58944,10 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>3639</v>
-      </c>
-      <c r="B370" t="s">
-        <v>3640</v>
+        <v>4</v>
+      </c>
+      <c r="B370" s="3" t="s">
+        <v>420</v>
       </c>
       <c r="C370" t="s">
         <v>3575</v>
@@ -58375,10 +58955,10 @@
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>3643</v>
-      </c>
-      <c r="B371" t="s">
-        <v>3644</v>
+        <v>5</v>
+      </c>
+      <c r="B371" s="3" t="s">
+        <v>421</v>
       </c>
       <c r="C371" t="s">
         <v>3575</v>
@@ -58386,10 +58966,10 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>3641</v>
-      </c>
-      <c r="B372" t="s">
-        <v>3642</v>
+        <v>2</v>
+      </c>
+      <c r="B372" s="3" t="s">
+        <v>422</v>
       </c>
       <c r="C372" t="s">
         <v>3575</v>
@@ -58397,10 +58977,10 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>3457</v>
+        <v>3639</v>
       </c>
       <c r="B373" t="s">
-        <v>3458</v>
+        <v>3640</v>
       </c>
       <c r="C373" t="s">
         <v>3575</v>
@@ -58408,10 +58988,10 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>3649</v>
-      </c>
-      <c r="B374" s="3" t="s">
-        <v>3650</v>
+        <v>3643</v>
+      </c>
+      <c r="B374" t="s">
+        <v>3644</v>
       </c>
       <c r="C374" t="s">
         <v>3575</v>
@@ -58419,10 +58999,10 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>3648</v>
-      </c>
-      <c r="B375" s="3" t="s">
-        <v>3646</v>
+        <v>3641</v>
+      </c>
+      <c r="B375" t="s">
+        <v>3642</v>
       </c>
       <c r="C375" t="s">
         <v>3575</v>
@@ -58430,10 +59010,10 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>3647</v>
-      </c>
-      <c r="B376" s="3" t="s">
-        <v>3645</v>
+        <v>3457</v>
+      </c>
+      <c r="B376" t="s">
+        <v>3458</v>
       </c>
       <c r="C376" t="s">
         <v>3575</v>
@@ -58441,10 +59021,10 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>3546</v>
+        <v>3968</v>
       </c>
       <c r="B377" t="s">
-        <v>3548</v>
+        <v>3969</v>
       </c>
       <c r="C377" t="s">
         <v>3575</v>
@@ -58452,10 +59032,10 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>14</v>
-      </c>
-      <c r="B378" s="3" t="s">
-        <v>163</v>
+        <v>3971</v>
+      </c>
+      <c r="B378" t="s">
+        <v>3970</v>
       </c>
       <c r="C378" t="s">
         <v>3575</v>
@@ -58463,76 +59043,76 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>112</v>
-      </c>
-      <c r="B379" t="s">
-        <v>194</v>
+        <v>3649</v>
+      </c>
+      <c r="B379" s="3" t="s">
+        <v>3650</v>
       </c>
       <c r="C379" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>108</v>
-      </c>
-      <c r="B380" t="s">
-        <v>198</v>
+        <v>3648</v>
+      </c>
+      <c r="B380" s="3" t="s">
+        <v>3646</v>
       </c>
       <c r="C380" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>106</v>
-      </c>
-      <c r="B381" t="s">
-        <v>196</v>
+        <v>3647</v>
+      </c>
+      <c r="B381" s="3" t="s">
+        <v>3645</v>
       </c>
       <c r="C381" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>107</v>
+        <v>3546</v>
       </c>
       <c r="B382" t="s">
-        <v>197</v>
+        <v>3548</v>
       </c>
       <c r="C382" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>109</v>
+        <v>3974</v>
       </c>
       <c r="B383" t="s">
-        <v>199</v>
+        <v>3975</v>
       </c>
       <c r="C383" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>95</v>
-      </c>
-      <c r="B384" t="s">
-        <v>179</v>
+        <v>14</v>
+      </c>
+      <c r="B384" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="C384" t="s">
-        <v>3576</v>
+        <v>3575</v>
       </c>
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
       <c r="B385" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C385" t="s">
         <v>3576</v>
@@ -58540,10 +59120,10 @@
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>96</v>
+        <v>108</v>
       </c>
       <c r="B386" t="s">
-        <v>180</v>
+        <v>198</v>
       </c>
       <c r="C386" t="s">
         <v>3576</v>
@@ -58551,10 +59131,10 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="B387" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="C387" t="s">
         <v>3576</v>
@@ -58562,10 +59142,10 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>93</v>
+        <v>107</v>
       </c>
       <c r="B388" t="s">
-        <v>177</v>
+        <v>197</v>
       </c>
       <c r="C388" t="s">
         <v>3576</v>
@@ -58573,10 +59153,10 @@
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="B389" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="C389" t="s">
         <v>3576</v>
@@ -58584,10 +59164,10 @@
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B390" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C390" t="s">
         <v>3576</v>
@@ -58595,10 +59175,10 @@
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B391" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="C391" t="s">
         <v>3576</v>
@@ -58606,10 +59186,10 @@
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>121</v>
+        <v>96</v>
       </c>
       <c r="B392" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="C392" t="s">
         <v>3576</v>
@@ -58617,10 +59197,10 @@
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B393" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C393" t="s">
         <v>3576</v>
@@ -58628,10 +59208,10 @@
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="B394" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C394" t="s">
         <v>3576</v>
@@ -58639,10 +59219,10 @@
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="B395" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C395" t="s">
         <v>3576</v>
@@ -58650,10 +59230,10 @@
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>122</v>
+        <v>98</v>
       </c>
       <c r="B396" t="s">
-        <v>3723</v>
+        <v>182</v>
       </c>
       <c r="C396" t="s">
         <v>3576</v>
@@ -58661,10 +59241,10 @@
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
       <c r="B397" t="s">
-        <v>193</v>
+        <v>183</v>
       </c>
       <c r="C397" t="s">
         <v>3576</v>
@@ -58672,10 +59252,10 @@
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>100</v>
+        <v>121</v>
       </c>
       <c r="B398" t="s">
-        <v>184</v>
+        <v>191</v>
       </c>
       <c r="C398" t="s">
         <v>3576</v>
@@ -58683,10 +59263,10 @@
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="B399" t="s">
-        <v>190</v>
+        <v>192</v>
       </c>
       <c r="C399" t="s">
         <v>3576</v>
@@ -58694,10 +59274,10 @@
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B400" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C400" t="s">
         <v>3576</v>
@@ -58705,10 +59285,10 @@
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B401" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C401" t="s">
         <v>3576</v>
@@ -58716,18 +59296,84 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B402" t="s">
-        <v>195</v>
+        <v>3723</v>
       </c>
       <c r="C402" t="s">
         <v>3576</v>
       </c>
     </row>
+    <row r="403" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A403" t="s">
+        <v>110</v>
+      </c>
+      <c r="B403" t="s">
+        <v>193</v>
+      </c>
+      <c r="C403" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="404" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A404" t="s">
+        <v>100</v>
+      </c>
+      <c r="B404" t="s">
+        <v>184</v>
+      </c>
+      <c r="C404" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="405" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A405" t="s">
+        <v>119</v>
+      </c>
+      <c r="B405" t="s">
+        <v>190</v>
+      </c>
+      <c r="C405" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="406" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A406" t="s">
+        <v>104</v>
+      </c>
+      <c r="B406" t="s">
+        <v>188</v>
+      </c>
+      <c r="C406" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="407" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A407" t="s">
+        <v>105</v>
+      </c>
+      <c r="B407" t="s">
+        <v>189</v>
+      </c>
+      <c r="C407" t="s">
+        <v>3576</v>
+      </c>
+    </row>
+    <row r="408" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A408" t="s">
+        <v>120</v>
+      </c>
+      <c r="B408" t="s">
+        <v>195</v>
+      </c>
+      <c r="C408" t="s">
+        <v>3576</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C390" xr:uid="{00000000-0009-0000-0000-000007000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C402">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C408">
       <sortCondition ref="C1:C390"/>
     </sortState>
   </autoFilter>
@@ -58739,7 +59385,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr codeName="Planilha11"/>
   <dimension ref="A1:B34"/>
@@ -59031,7 +59677,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr codeName="Planilha12"/>
   <dimension ref="A1:D19"/>
@@ -59193,1314 +59839,4 @@
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr codeName="Planilha2"/>
-  <dimension ref="A1:B73"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3357</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3427</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3380</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3384</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3381</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3385</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3382</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3386</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3383</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3387</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3394</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3395</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3388</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3390</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3397</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3787</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3389</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3391</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3392</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3393</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3398</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3399</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
-        <v>3400</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3401</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>3402</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3403</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>3816</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3817</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A26" s="4"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A71" s="3"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A73" s="3"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B230" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <sheetPr codeName="Planilha3"/>
-  <dimension ref="A1:B89"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3357</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3427</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3358</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3361</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3841</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3847</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3844</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3848</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3842</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3849</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3846</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3850</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3843</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3851</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3845</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>3852</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3435</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3853</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="3"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="3"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="3"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="3"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="3"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="3"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="3"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B208" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C9DCE0E7-0088-4A2B-A337-2E9F71FCD182}">
-  <sheetPr codeName="Planilha14"/>
-  <dimension ref="A1:B90"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3357</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3427</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3796</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3855</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3797</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3854</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="3"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="3"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="3"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="3"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="3"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="3"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="3"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="3"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B209" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475AAE06-8F25-42D5-A7FC-7E45A1549051}">
-  <sheetPr codeName="Planilha15"/>
-  <dimension ref="A1:B89"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E20" sqref="E20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3357</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3427</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3798</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3799</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3800</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3801</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B50" s="3"/>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3"/>
-      <c r="B51" s="3"/>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B52" s="3"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B53" s="3"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B54" s="3"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B55" s="3"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B56" s="3"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="3"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="3"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="3"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="3"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B208" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB2BF224-0D55-4A1C-AEF3-DC9AF5D3B568}">
-  <sheetPr codeName="Planilha16"/>
-  <dimension ref="A1:B52"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C17" sqref="C17"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3357</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3427</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3802</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3806</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3803</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3809</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3804</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3807</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3805</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3808</v>
-      </c>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" s="3"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B209" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B802DFDF-DAA6-46CB-9B07-61A1C1D16372}">
-  <sheetPr codeName="Planilha13"/>
-  <dimension ref="A1:B100"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F34" sqref="F34"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3357</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3427</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3358</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3361</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3788</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3792</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3789</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3793</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="4"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B13" s="4"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="3"/>
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="3"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="3"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="3"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="3"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="3"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="3"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="3"/>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B99" s="3"/>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="3"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B219" xr:uid="{00000000-0009-0000-0000-000002000000}"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <sheetPr codeName="Planilha4"/>
-  <dimension ref="A1:B101"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B10" sqref="B10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3357</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3427</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3358</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3361</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3359</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3363</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3360</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3364</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3366</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3418</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3369</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3417</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3367</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3404</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3419</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>3437</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>3436</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>3428</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B14" s="4"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" s="4"/>
-      <c r="B16" s="4"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="3"/>
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="3"/>
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="3"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="3"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="3"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="3"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="3"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="3"/>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B91" s="3"/>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B92" s="3"/>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B93" s="3"/>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B94" s="3"/>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B100" s="3"/>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B101" s="3"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B220" xr:uid="{00000000-0009-0000-0000-000003000000}"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <sheetPr codeName="Planilha5"/>
-  <dimension ref="A1:B97"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B13" sqref="B13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3357</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3427</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3358</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3361</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3415</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3408</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
-        <v>3414</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>3409</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3416</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>3410</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B10" s="4"/>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="3"/>
-      <c r="B57" s="3"/>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B58" s="3"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="3"/>
-      <c r="B59" s="3"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B60" s="3"/>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B61" s="3"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B62" s="3"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B63" s="3"/>
-    </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B64" s="3"/>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B65" s="3"/>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B66" s="3"/>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B67" s="3"/>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B68" s="3"/>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B69" s="3"/>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B70" s="3"/>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B71" s="3"/>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B72" s="3"/>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B73" s="3"/>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B74" s="3"/>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B75" s="3"/>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B76" s="3"/>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B77" s="3"/>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B78" s="3"/>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B79" s="3"/>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B80" s="3"/>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B81" s="3"/>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B82" s="3"/>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B83" s="3"/>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B84" s="3"/>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B85" s="3"/>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B86" s="3"/>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B87" s="3"/>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B88" s="3"/>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B89" s="3"/>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B90" s="3"/>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B96" s="3"/>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.25">
-      <c r="B97" s="3"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:B216" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Inclusão de melhorias @202405201256
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AD1572-EE57-4FF7-9E3E-999CCA207668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B409A7C-0783-4B14-869F-FC2E53030D53}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="3280" windowWidth="19420" windowHeight="10300" tabRatio="699" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="7740" windowWidth="19410" windowHeight="7845" tabRatio="699" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="daily" sheetId="19" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11444" uniqueCount="3978">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11588" uniqueCount="4072">
   <si>
     <t>bbgTicker</t>
   </si>
@@ -11986,6 +11986,288 @@
   </si>
   <si>
     <t>us_employees_nonfarm_payrolls_yoy</t>
+  </si>
+  <si>
+    <t>IP       Index</t>
+  </si>
+  <si>
+    <t>IP  YOY Index</t>
+  </si>
+  <si>
+    <t>us_industrial_production_yoy</t>
+  </si>
+  <si>
+    <t>IP  CHNG Index</t>
+  </si>
+  <si>
+    <t>us_industrial_production_mom</t>
+  </si>
+  <si>
+    <t>NHSLTOT Index</t>
+  </si>
+  <si>
+    <t>NHSPSTOT Index</t>
+  </si>
+  <si>
+    <t>NHSPATOT Index</t>
+  </si>
+  <si>
+    <t>SPCSUSA  Index</t>
+  </si>
+  <si>
+    <t>SPCS20SA Index</t>
+  </si>
+  <si>
+    <t>us_case_shiller_home_price_national</t>
+  </si>
+  <si>
+    <t>SPCS20SY Index</t>
+  </si>
+  <si>
+    <t>us_case_shiller_home_price_20_city_index</t>
+  </si>
+  <si>
+    <t>us_case_shiller_home_price_20_city_yoy</t>
+  </si>
+  <si>
+    <t>us_case_shiller_home_price_national_yoy</t>
+  </si>
+  <si>
+    <t>SPCSUSYS Index</t>
+  </si>
+  <si>
+    <t>us_industrial_production_index</t>
+  </si>
+  <si>
+    <t>us_new_home_sales_index</t>
+  </si>
+  <si>
+    <t>us_housing_starts_index</t>
+  </si>
+  <si>
+    <t>us_building_permits_index</t>
+  </si>
+  <si>
+    <t>us_new_home_sales_yoy</t>
+  </si>
+  <si>
+    <t>us_housing_starts_yoy</t>
+  </si>
+  <si>
+    <t>us_building_permits_yoy</t>
+  </si>
+  <si>
+    <t>NHSLYOY Index</t>
+  </si>
+  <si>
+    <t>NHSPSTY% Index</t>
+  </si>
+  <si>
+    <t>NHSPATY% Index</t>
+  </si>
+  <si>
+    <t>us_delinquency_rates_consumer_loans</t>
+  </si>
+  <si>
+    <t>USDECNLN Index</t>
+  </si>
+  <si>
+    <t>USDECRED Index</t>
+  </si>
+  <si>
+    <t>us_delinquency_rates_credit_cards</t>
+  </si>
+  <si>
+    <t>us_delinquency_rates_business_loans</t>
+  </si>
+  <si>
+    <t>USDEC&amp;IL Index</t>
+  </si>
+  <si>
+    <t>NAPMPMI Index</t>
+  </si>
+  <si>
+    <t>NAPMNMI Index</t>
+  </si>
+  <si>
+    <t>NAPMNEWO Index</t>
+  </si>
+  <si>
+    <t>NAPMINV Index</t>
+  </si>
+  <si>
+    <t>NAPMPRIC Index</t>
+  </si>
+  <si>
+    <t>NAPMEMPL Index</t>
+  </si>
+  <si>
+    <t>NAPMNNO Index</t>
+  </si>
+  <si>
+    <t>NAPMNPRC Index</t>
+  </si>
+  <si>
+    <t>NAPMNEMP Index</t>
+  </si>
+  <si>
+    <t>us_ism_manufacting</t>
+  </si>
+  <si>
+    <t>us_ism_services</t>
+  </si>
+  <si>
+    <t>us_ism_manufacturing_new_orders</t>
+  </si>
+  <si>
+    <t>us_ism_manufacturing_inventories</t>
+  </si>
+  <si>
+    <t>us_ism_manufacturing_prices_paid</t>
+  </si>
+  <si>
+    <t>us_ism_manufacturing_employment</t>
+  </si>
+  <si>
+    <t>us_ism_services_new_orders</t>
+  </si>
+  <si>
+    <t>us_ism_services_prices_paid</t>
+  </si>
+  <si>
+    <t>us_ism_services_employment</t>
+  </si>
+  <si>
+    <t>CONSSENT Index</t>
+  </si>
+  <si>
+    <t>us_university_michigan_consumer_sentiment_index</t>
+  </si>
+  <si>
+    <t>CONSEXP  Index</t>
+  </si>
+  <si>
+    <t>us_university_michigan_consumer_expectations_index</t>
+  </si>
+  <si>
+    <t>BRSRTTSV Index</t>
+  </si>
+  <si>
+    <t>BRSRTTVY Index</t>
+  </si>
+  <si>
+    <t>br_pms_services_volume_total_index</t>
+  </si>
+  <si>
+    <t>br_pms_services_volume_total_yoy</t>
+  </si>
+  <si>
+    <t>br_pms_services_volume_total_mom</t>
+  </si>
+  <si>
+    <t>br_pms_services_volume_administrative_index</t>
+  </si>
+  <si>
+    <t>BRSRTRSV Index</t>
+  </si>
+  <si>
+    <t>br_pms_services_volume_transport_index</t>
+  </si>
+  <si>
+    <t>br_pms_services_volume_individual_and_family_index</t>
+  </si>
+  <si>
+    <t>BRSRICSV Index</t>
+  </si>
+  <si>
+    <t>br_pms_services_volume_information_communication_index</t>
+  </si>
+  <si>
+    <t>BRSRPASV Index</t>
+  </si>
+  <si>
+    <t>BRSROSSV Index</t>
+  </si>
+  <si>
+    <t>br_pms_services_volume_others_index</t>
+  </si>
+  <si>
+    <t>br_pmc_retail_sales_volume_total_index</t>
+  </si>
+  <si>
+    <t>br_pmc_retail_sales_volume_total_amplified_index</t>
+  </si>
+  <si>
+    <t>BZRTRYOY Index</t>
+  </si>
+  <si>
+    <t>BZRTAMPY Index</t>
+  </si>
+  <si>
+    <t>BZRTAVSA Index</t>
+  </si>
+  <si>
+    <t>BZRTRTSA Index</t>
+  </si>
+  <si>
+    <t>br_pmc_retail_sales_volume_total_yoy</t>
+  </si>
+  <si>
+    <t>br_pmc_retail_sales_volume_total_amplified_yoy</t>
+  </si>
+  <si>
+    <t>BZRTFLSA Index</t>
+  </si>
+  <si>
+    <t>BZRTFDSA Index</t>
+  </si>
+  <si>
+    <t>BZRTSMSA Index</t>
+  </si>
+  <si>
+    <t>BZRTCLSA Index</t>
+  </si>
+  <si>
+    <t>BZRTFUSA Index</t>
+  </si>
+  <si>
+    <t>BZRTPHSA Index</t>
+  </si>
+  <si>
+    <t>BZRTBKSA Index</t>
+  </si>
+  <si>
+    <t>BZRTEQSA Index</t>
+  </si>
+  <si>
+    <t>BZRTOHSA Index</t>
+  </si>
+  <si>
+    <t>br_pmc_retail_sales_volume_fuels_lubrificants_index</t>
+  </si>
+  <si>
+    <t>br_pmc_retail_sales_volume_food_beverage_index</t>
+  </si>
+  <si>
+    <t>br_pmc_retail_sales_volume_supermarkets_index</t>
+  </si>
+  <si>
+    <t>br_pmc_retail_sales_volume_textiles_clothing_index</t>
+  </si>
+  <si>
+    <t>br_pmc_retail_sales_volume_furniture_index</t>
+  </si>
+  <si>
+    <t>br_pmc_retail_sales_volume_pharma_cosmetics_index</t>
+  </si>
+  <si>
+    <t>br_pmc_retail_sales_volume_books_magazines_index</t>
+  </si>
+  <si>
+    <t>br_pmc_retail_sales_volume_office_materials_index</t>
+  </si>
+  <si>
+    <t>br_pmc_retail_sales_volume_others_index</t>
   </si>
 </sst>
 </file>
@@ -54869,17 +55151,17 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Planilha9"/>
-  <dimension ref="A1:C408"/>
+  <dimension ref="A1:C456"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A391" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A443" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C457" sqref="C457"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="44.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="56.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -59371,14 +59653,542 @@
         <v>3576</v>
       </c>
     </row>
+    <row r="409" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A409" t="s">
+        <v>3978</v>
+      </c>
+      <c r="B409" t="s">
+        <v>3994</v>
+      </c>
+      <c r="C409" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="410" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A410" t="s">
+        <v>3979</v>
+      </c>
+      <c r="B410" t="s">
+        <v>3980</v>
+      </c>
+      <c r="C410" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="411" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A411" t="s">
+        <v>3981</v>
+      </c>
+      <c r="B411" t="s">
+        <v>3982</v>
+      </c>
+      <c r="C411" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="412" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A412" t="s">
+        <v>3983</v>
+      </c>
+      <c r="B412" t="s">
+        <v>3995</v>
+      </c>
+      <c r="C412" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="413" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A413" t="s">
+        <v>4001</v>
+      </c>
+      <c r="B413" t="s">
+        <v>3998</v>
+      </c>
+      <c r="C413" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="414" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A414" t="s">
+        <v>3984</v>
+      </c>
+      <c r="B414" t="s">
+        <v>3996</v>
+      </c>
+      <c r="C414" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="415" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A415" t="s">
+        <v>4002</v>
+      </c>
+      <c r="B415" t="s">
+        <v>3999</v>
+      </c>
+      <c r="C415" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="416" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A416" t="s">
+        <v>3985</v>
+      </c>
+      <c r="B416" t="s">
+        <v>3997</v>
+      </c>
+      <c r="C416" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="417" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A417" t="s">
+        <v>4003</v>
+      </c>
+      <c r="B417" t="s">
+        <v>4000</v>
+      </c>
+      <c r="C417" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="418" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A418" t="s">
+        <v>3986</v>
+      </c>
+      <c r="B418" t="s">
+        <v>3988</v>
+      </c>
+      <c r="C418" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="419" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A419" t="s">
+        <v>3993</v>
+      </c>
+      <c r="B419" t="s">
+        <v>3992</v>
+      </c>
+      <c r="C419" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="420" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A420" t="s">
+        <v>3987</v>
+      </c>
+      <c r="B420" t="s">
+        <v>3990</v>
+      </c>
+      <c r="C420" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="421" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A421" t="s">
+        <v>3989</v>
+      </c>
+      <c r="B421" t="s">
+        <v>3991</v>
+      </c>
+      <c r="C421" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="422" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A422" t="s">
+        <v>4005</v>
+      </c>
+      <c r="B422" t="s">
+        <v>4004</v>
+      </c>
+      <c r="C422" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="423" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A423" t="s">
+        <v>4006</v>
+      </c>
+      <c r="B423" t="s">
+        <v>4007</v>
+      </c>
+      <c r="C423" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="424" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A424" t="s">
+        <v>4009</v>
+      </c>
+      <c r="B424" t="s">
+        <v>4008</v>
+      </c>
+      <c r="C424" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="425" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A425" t="s">
+        <v>4010</v>
+      </c>
+      <c r="B425" t="s">
+        <v>4019</v>
+      </c>
+      <c r="C425" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="426" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A426" t="s">
+        <v>4011</v>
+      </c>
+      <c r="B426" t="s">
+        <v>4020</v>
+      </c>
+      <c r="C426" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="427" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A427" t="s">
+        <v>4012</v>
+      </c>
+      <c r="B427" t="s">
+        <v>4021</v>
+      </c>
+      <c r="C427" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="428" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A428" t="s">
+        <v>4013</v>
+      </c>
+      <c r="B428" t="s">
+        <v>4022</v>
+      </c>
+      <c r="C428" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="429" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A429" t="s">
+        <v>4014</v>
+      </c>
+      <c r="B429" t="s">
+        <v>4023</v>
+      </c>
+      <c r="C429" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="430" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A430" t="s">
+        <v>4015</v>
+      </c>
+      <c r="B430" t="s">
+        <v>4024</v>
+      </c>
+      <c r="C430" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="431" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A431" t="s">
+        <v>4016</v>
+      </c>
+      <c r="B431" t="s">
+        <v>4025</v>
+      </c>
+      <c r="C431" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="432" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A432" t="s">
+        <v>4017</v>
+      </c>
+      <c r="B432" t="s">
+        <v>4026</v>
+      </c>
+      <c r="C432" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="433" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A433" t="s">
+        <v>4018</v>
+      </c>
+      <c r="B433" t="s">
+        <v>4027</v>
+      </c>
+      <c r="C433" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="434" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A434" t="s">
+        <v>4028</v>
+      </c>
+      <c r="B434" t="s">
+        <v>4029</v>
+      </c>
+      <c r="C434" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="435" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A435" t="s">
+        <v>4030</v>
+      </c>
+      <c r="B435" t="s">
+        <v>4031</v>
+      </c>
+      <c r="C435" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="436" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A436" t="s">
+        <v>4032</v>
+      </c>
+      <c r="B436" t="s">
+        <v>4034</v>
+      </c>
+      <c r="C436" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="437" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A437" t="s">
+        <v>4033</v>
+      </c>
+      <c r="B437" t="s">
+        <v>4035</v>
+      </c>
+      <c r="C437" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="438" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A438" t="s">
+        <v>4033</v>
+      </c>
+      <c r="B438" t="s">
+        <v>4036</v>
+      </c>
+      <c r="C438" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="439" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A439" t="s">
+        <v>4043</v>
+      </c>
+      <c r="B439" t="s">
+        <v>4037</v>
+      </c>
+      <c r="C439" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="440" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A440" t="s">
+        <v>4038</v>
+      </c>
+      <c r="B440" t="s">
+        <v>4039</v>
+      </c>
+      <c r="C440" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="441" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A441" t="s">
+        <v>4038</v>
+      </c>
+      <c r="B441" t="s">
+        <v>4040</v>
+      </c>
+      <c r="C441" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="442" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A442" t="s">
+        <v>4041</v>
+      </c>
+      <c r="B442" t="s">
+        <v>4042</v>
+      </c>
+      <c r="C442" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="443" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A443" t="s">
+        <v>4044</v>
+      </c>
+      <c r="B443" t="s">
+        <v>4045</v>
+      </c>
+      <c r="C443" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="444" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A444" t="s">
+        <v>4051</v>
+      </c>
+      <c r="B444" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C444" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="445" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A445" t="s">
+        <v>4048</v>
+      </c>
+      <c r="B445" t="s">
+        <v>4052</v>
+      </c>
+      <c r="C445" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="446" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A446" t="s">
+        <v>4050</v>
+      </c>
+      <c r="B446" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C446" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="447" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A447" t="s">
+        <v>4049</v>
+      </c>
+      <c r="B447" t="s">
+        <v>4053</v>
+      </c>
+      <c r="C447" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="448" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A448" t="s">
+        <v>4054</v>
+      </c>
+      <c r="B448" t="s">
+        <v>4063</v>
+      </c>
+      <c r="C448" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="449" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A449" t="s">
+        <v>4055</v>
+      </c>
+      <c r="B449" t="s">
+        <v>4064</v>
+      </c>
+      <c r="C449" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="450" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A450" t="s">
+        <v>4056</v>
+      </c>
+      <c r="B450" t="s">
+        <v>4065</v>
+      </c>
+      <c r="C450" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="451" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A451" t="s">
+        <v>4057</v>
+      </c>
+      <c r="B451" t="s">
+        <v>4066</v>
+      </c>
+      <c r="C451" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="452" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A452" t="s">
+        <v>4058</v>
+      </c>
+      <c r="B452" t="s">
+        <v>4067</v>
+      </c>
+      <c r="C452" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="453" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A453" t="s">
+        <v>4059</v>
+      </c>
+      <c r="B453" t="s">
+        <v>4068</v>
+      </c>
+      <c r="C453" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="454" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A454" t="s">
+        <v>4060</v>
+      </c>
+      <c r="B454" t="s">
+        <v>4069</v>
+      </c>
+      <c r="C454" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="455" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A455" t="s">
+        <v>4061</v>
+      </c>
+      <c r="B455" t="s">
+        <v>4070</v>
+      </c>
+      <c r="C455" t="s">
+        <v>3575</v>
+      </c>
+    </row>
+    <row r="456" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A456" t="s">
+        <v>4062</v>
+      </c>
+      <c r="B456" t="s">
+        <v>4071</v>
+      </c>
+      <c r="C456" t="s">
+        <v>3575</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C390" xr:uid="{00000000-0009-0000-0000-000007000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C408">
       <sortCondition ref="C1:C390"/>
     </sortState>
   </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A359:B445">
-    <sortCondition ref="A359:A445"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A359:B461">
+    <sortCondition ref="A359:A461"/>
   </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Inclusão de melhorias @202405240906
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -13553,7 +13553,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -55014,8 +55014,8 @@
   <dimension ref="A1:C464"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A453" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B471" sqref="B471"/>
+      <pane ySplit="1" topLeftCell="A435" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B488" sqref="B488"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>

</xml_diff>

<commit_message>
Inclusão de melhorias @202405281007
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10756736-0500-4D63-B625-9CB19B9DF614}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E548D0F-1C95-4F1C-9C84-B5D035234627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="699" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="699" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="equity_signals" sheetId="19" r:id="rId1"/>
@@ -27,7 +27,7 @@
   </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">equities!$A$1:$L$1268</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">equity_signals!$C$1:$C$77</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">equity_signals!$C$1:$C$79</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">macro!$A$1:$C$360</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11627" uniqueCount="4097">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11633" uniqueCount="4101">
   <si>
     <t>bbgTicker</t>
   </si>
@@ -12342,6 +12342,18 @@
   </si>
   <si>
     <t>bcb_code</t>
+  </si>
+  <si>
+    <t>BEST_TARGET_PRICE</t>
+  </si>
+  <si>
+    <t>BEST_ANALYST_RATING</t>
+  </si>
+  <si>
+    <t>analyst_rating</t>
+  </si>
+  <si>
+    <t>price_target</t>
   </si>
 </sst>
 </file>
@@ -12920,11 +12932,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C77"/>
+  <dimension ref="A1:C79"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13189,54 +13201,54 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>3788</v>
+        <v>4098</v>
       </c>
       <c r="B24" t="s">
-        <v>3847</v>
+        <v>4099</v>
       </c>
       <c r="C24" t="s">
-        <v>3946</v>
+        <v>3945</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>3789</v>
+        <v>4097</v>
       </c>
       <c r="B25" t="s">
-        <v>3846</v>
+        <v>4100</v>
       </c>
       <c r="C25" t="s">
-        <v>3946</v>
+        <v>3945</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>3790</v>
+        <v>3788</v>
       </c>
       <c r="B26" t="s">
-        <v>3791</v>
+        <v>3847</v>
       </c>
       <c r="C26" t="s">
-        <v>3943</v>
+        <v>3946</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>3792</v>
+        <v>3789</v>
       </c>
       <c r="B27" t="s">
-        <v>3793</v>
+        <v>3846</v>
       </c>
       <c r="C27" t="s">
-        <v>3943</v>
+        <v>3946</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
-        <v>3942</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>3943</v>
+      <c r="A28" t="s">
+        <v>3790</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3791</v>
       </c>
       <c r="C28" t="s">
         <v>3943</v>
@@ -13244,32 +13256,32 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>3794</v>
+        <v>3792</v>
       </c>
       <c r="B29" t="s">
-        <v>3798</v>
+        <v>3793</v>
       </c>
       <c r="C29" t="s">
-        <v>3947</v>
+        <v>3943</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>3795</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3801</v>
+      <c r="A30" s="4" t="s">
+        <v>3942</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>3943</v>
       </c>
       <c r="C30" t="s">
-        <v>3947</v>
+        <v>3943</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>3796</v>
+        <v>3794</v>
       </c>
       <c r="B31" t="s">
-        <v>3799</v>
+        <v>3798</v>
       </c>
       <c r="C31" t="s">
         <v>3947</v>
@@ -13277,10 +13289,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>3797</v>
+        <v>3795</v>
       </c>
       <c r="B32" t="s">
-        <v>3800</v>
+        <v>3801</v>
       </c>
       <c r="C32" t="s">
         <v>3947</v>
@@ -13288,32 +13300,32 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>3412</v>
+        <v>3796</v>
       </c>
       <c r="B33" t="s">
-        <v>3415</v>
+        <v>3799</v>
       </c>
       <c r="C33" t="s">
-        <v>3948</v>
+        <v>3947</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>3413</v>
+        <v>3797</v>
       </c>
       <c r="B34" t="s">
-        <v>3416</v>
+        <v>3800</v>
       </c>
       <c r="C34" t="s">
-        <v>3948</v>
+        <v>3947</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>3414</v>
+        <v>3412</v>
       </c>
       <c r="B35" t="s">
-        <v>3417</v>
+        <v>3415</v>
       </c>
       <c r="C35" t="s">
         <v>3948</v>
@@ -13321,54 +13333,54 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>3366</v>
+        <v>3413</v>
       </c>
       <c r="B36" t="s">
-        <v>3403</v>
+        <v>3416</v>
       </c>
       <c r="C36" t="s">
-        <v>3953</v>
+        <v>3948</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>3833</v>
+        <v>3414</v>
       </c>
       <c r="B37" t="s">
-        <v>3839</v>
+        <v>3417</v>
       </c>
       <c r="C37" t="s">
-        <v>3951</v>
+        <v>3948</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="4" t="s">
-        <v>3836</v>
+      <c r="A38" t="s">
+        <v>3366</v>
       </c>
       <c r="B38" t="s">
-        <v>3840</v>
+        <v>3403</v>
       </c>
       <c r="C38" t="s">
-        <v>3951</v>
+        <v>3953</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>3834</v>
+        <v>3833</v>
       </c>
       <c r="B39" t="s">
-        <v>3841</v>
+        <v>3839</v>
       </c>
       <c r="C39" t="s">
         <v>3951</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>3838</v>
+      <c r="A40" s="4" t="s">
+        <v>3836</v>
       </c>
       <c r="B40" t="s">
-        <v>3842</v>
+        <v>3840</v>
       </c>
       <c r="C40" t="s">
         <v>3951</v>
@@ -13376,10 +13388,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>3835</v>
+        <v>3834</v>
       </c>
       <c r="B41" t="s">
-        <v>3843</v>
+        <v>3841</v>
       </c>
       <c r="C41" t="s">
         <v>3951</v>
@@ -13387,10 +13399,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>3427</v>
+        <v>3838</v>
       </c>
       <c r="B42" t="s">
-        <v>3845</v>
+        <v>3842</v>
       </c>
       <c r="C42" t="s">
         <v>3951</v>
@@ -13398,76 +13410,76 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>3837</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>3844</v>
+        <v>3835</v>
+      </c>
+      <c r="B43" t="s">
+        <v>3843</v>
       </c>
       <c r="C43" t="s">
-        <v>3952</v>
+        <v>3951</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>4080</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>4079</v>
+        <v>3427</v>
+      </c>
+      <c r="B44" t="s">
+        <v>3845</v>
       </c>
       <c r="C44" t="s">
-        <v>3952</v>
+        <v>3951</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>3780</v>
-      </c>
-      <c r="B45" t="s">
-        <v>3784</v>
+        <v>3837</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>3844</v>
       </c>
       <c r="C45" t="s">
-        <v>3949</v>
+        <v>3952</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>3781</v>
-      </c>
-      <c r="B46" t="s">
-        <v>3785</v>
+        <v>4080</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>4079</v>
       </c>
       <c r="C46" t="s">
-        <v>3949</v>
+        <v>3952</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>3358</v>
+        <v>3780</v>
       </c>
       <c r="B47" t="s">
-        <v>3361</v>
+        <v>3784</v>
       </c>
       <c r="C47" t="s">
-        <v>3950</v>
+        <v>3949</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>3359</v>
+        <v>3781</v>
       </c>
       <c r="B48" t="s">
-        <v>3362</v>
+        <v>3785</v>
       </c>
       <c r="C48" t="s">
-        <v>3950</v>
+        <v>3949</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>3364</v>
+        <v>3358</v>
       </c>
       <c r="B49" t="s">
-        <v>3410</v>
+        <v>3361</v>
       </c>
       <c r="C49" t="s">
         <v>3950</v>
@@ -13475,10 +13487,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>3367</v>
+        <v>3359</v>
       </c>
       <c r="B50" t="s">
-        <v>3409</v>
+        <v>3362</v>
       </c>
       <c r="C50" t="s">
         <v>3950</v>
@@ -13486,10 +13498,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>3365</v>
+        <v>3364</v>
       </c>
       <c r="B51" t="s">
-        <v>3402</v>
+        <v>3410</v>
       </c>
       <c r="C51" t="s">
         <v>3950</v>
@@ -13497,10 +13509,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>3411</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>3429</v>
+        <v>3367</v>
+      </c>
+      <c r="B52" t="s">
+        <v>3409</v>
       </c>
       <c r="C52" t="s">
         <v>3950</v>
@@ -13508,10 +13520,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>3428</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>3420</v>
+        <v>3365</v>
+      </c>
+      <c r="B53" t="s">
+        <v>3402</v>
       </c>
       <c r="C53" t="s">
         <v>3950</v>
@@ -13519,10 +13531,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>3954</v>
+        <v>3411</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>3955</v>
+        <v>3429</v>
       </c>
       <c r="C54" t="s">
         <v>3950</v>
@@ -13530,20 +13542,42 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>3956</v>
+        <v>3428</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>3957</v>
+        <v>3420</v>
       </c>
       <c r="C55" t="s">
         <v>3950</v>
       </c>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A75" s="3"/>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>3954</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>3955</v>
+      </c>
+      <c r="C56" t="s">
+        <v>3950</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>3956</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>3957</v>
+      </c>
+      <c r="C57" t="s">
+        <v>3950</v>
+      </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="3"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -60152,8 +60186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0CFEF5EF-AE24-41AB-8D64-46525708C7D6}">
   <dimension ref="A1:C437"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X7" sqref="X7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Inclusão de melhorias @202405281324
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E548D0F-1C95-4F1C-9C84-B5D035234627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CA3B8ED-6BB2-49B8-9755-2A2F6FF99BE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" tabRatio="699" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6765" yWindow="2790" windowWidth="23445" windowHeight="11970" tabRatio="699" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="equity_signals" sheetId="19" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11633" uniqueCount="4101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11633" uniqueCount="4102">
   <si>
     <t>bbgTicker</t>
   </si>
@@ -12354,6 +12354,9 @@
   </si>
   <si>
     <t>price_target</t>
+  </si>
+  <si>
+    <t>analyst_sentiment</t>
   </si>
 </sst>
 </file>
@@ -12935,15 +12938,15 @@
   <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
@@ -13207,7 +13210,7 @@
         <v>4099</v>
       </c>
       <c r="C24" t="s">
-        <v>3945</v>
+        <v>4101</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -13218,7 +13221,7 @@
         <v>4100</v>
       </c>
       <c r="C25" t="s">
-        <v>3945</v>
+        <v>4101</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Inclusão de melhorias @202406051156
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3F13A42-8831-4088-941E-F98BCBA881D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A21D021-05A2-48A8-B7E9-9A906CDA2742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19310" yWindow="3280" windowWidth="19420" windowHeight="10300" tabRatio="699" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11717" uniqueCount="4158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11729" uniqueCount="4166">
   <si>
     <t>bbgTicker</t>
   </si>
@@ -12525,6 +12525,30 @@
   </si>
   <si>
     <t>us_university_michigan_expected_inflation_fwd_12m_yoy</t>
+  </si>
+  <si>
+    <t>BZIPTLSA Index</t>
+  </si>
+  <si>
+    <t>br_industrial_production</t>
+  </si>
+  <si>
+    <t>BZIPYOY% Index</t>
+  </si>
+  <si>
+    <t>br_industrial_production_yoy</t>
+  </si>
+  <si>
+    <t>BZIPV12P Index</t>
+  </si>
+  <si>
+    <t>br_industrial_production_12m_yoy</t>
+  </si>
+  <si>
+    <t>BZIPTL% Index</t>
+  </si>
+  <si>
+    <t>br_industrial_production_mom</t>
   </si>
 </sst>
 </file>
@@ -55247,11 +55271,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Planilha9"/>
-  <dimension ref="A1:C481"/>
+  <dimension ref="A1:C485"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E6" sqref="E6"/>
+      <pane ySplit="1" topLeftCell="A469" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D478" sqref="D478"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60550,6 +60574,50 @@
       </c>
       <c r="C481" t="s">
         <v>3568</v>
+      </c>
+    </row>
+    <row r="482" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A482" t="s">
+        <v>4158</v>
+      </c>
+      <c r="B482" t="s">
+        <v>4159</v>
+      </c>
+      <c r="C482" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="483" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A483" t="s">
+        <v>4160</v>
+      </c>
+      <c r="B483" t="s">
+        <v>4161</v>
+      </c>
+      <c r="C483" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="484" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A484" t="s">
+        <v>4162</v>
+      </c>
+      <c r="B484" t="s">
+        <v>4163</v>
+      </c>
+      <c r="C484" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="485" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A485" t="s">
+        <v>4164</v>
+      </c>
+      <c r="B485" t="s">
+        <v>4165</v>
+      </c>
+      <c r="C485" t="s">
+        <v>3567</v>
       </c>
     </row>
   </sheetData>
@@ -60572,7 +60640,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Inclusão de melhorias @202406051344
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A21D021-05A2-48A8-B7E9-9A906CDA2742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA04F0F-8C17-4085-8873-DDBCC02BD776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="3280" windowWidth="19420" windowHeight="10300" tabRatio="699" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="3280" windowWidth="19420" windowHeight="10300" tabRatio="699" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="equity_signals" sheetId="19" r:id="rId1"/>
@@ -51,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11729" uniqueCount="4166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11735" uniqueCount="4169">
   <si>
     <t>bbgTicker</t>
   </si>
@@ -12549,6 +12549,15 @@
   </si>
   <si>
     <t>br_industrial_production_mom</t>
+  </si>
+  <si>
+    <t>br_bcb_net_public_sector_debt_to_gdp</t>
+  </si>
+  <si>
+    <t>br_bcb_nominal_result_12m_to_gdp</t>
+  </si>
+  <si>
+    <t>br_bcb_primary_result_12m_to_gdp</t>
   </si>
 </sst>
 </file>
@@ -55273,9 +55282,9 @@
   <sheetPr codeName="Planilha9"/>
   <dimension ref="A1:C485"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A469" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D478" sqref="D478"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57564,10 +57573,10 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>3916</v>
+        <v>4158</v>
       </c>
       <c r="B208" t="s">
-        <v>3919</v>
+        <v>4159</v>
       </c>
       <c r="C208" t="s">
         <v>3567</v>
@@ -57575,10 +57584,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>3917</v>
+        <v>4162</v>
       </c>
       <c r="B209" t="s">
-        <v>3920</v>
+        <v>4163</v>
       </c>
       <c r="C209" t="s">
         <v>3567</v>
@@ -57586,10 +57595,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>3918</v>
+        <v>4164</v>
       </c>
       <c r="B210" t="s">
-        <v>3921</v>
+        <v>4165</v>
       </c>
       <c r="C210" t="s">
         <v>3567</v>
@@ -57597,10 +57606,10 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>27</v>
-      </c>
-      <c r="B211" s="3" t="s">
-        <v>128</v>
+        <v>4160</v>
+      </c>
+      <c r="B211" t="s">
+        <v>4161</v>
       </c>
       <c r="C211" t="s">
         <v>3567</v>
@@ -57608,10 +57617,10 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>3849</v>
+        <v>3916</v>
       </c>
       <c r="B212" t="s">
-        <v>3877</v>
+        <v>3919</v>
       </c>
       <c r="C212" t="s">
         <v>3567</v>
@@ -57619,10 +57628,10 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>3847</v>
+        <v>3917</v>
       </c>
       <c r="B213" t="s">
-        <v>3878</v>
+        <v>3920</v>
       </c>
       <c r="C213" t="s">
         <v>3567</v>
@@ -57630,10 +57639,10 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>3850</v>
+        <v>3918</v>
       </c>
       <c r="B214" t="s">
-        <v>3879</v>
+        <v>3921</v>
       </c>
       <c r="C214" t="s">
         <v>3567</v>
@@ -57641,10 +57650,10 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>3851</v>
-      </c>
-      <c r="B215" t="s">
-        <v>3880</v>
+        <v>27</v>
+      </c>
+      <c r="B215" s="3" t="s">
+        <v>128</v>
       </c>
       <c r="C215" t="s">
         <v>3567</v>
@@ -57652,10 +57661,10 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>3839</v>
+        <v>3849</v>
       </c>
       <c r="B216" t="s">
-        <v>3881</v>
+        <v>3877</v>
       </c>
       <c r="C216" t="s">
         <v>3567</v>
@@ -57663,10 +57672,10 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>3852</v>
+        <v>3847</v>
       </c>
       <c r="B217" t="s">
-        <v>3882</v>
+        <v>3878</v>
       </c>
       <c r="C217" t="s">
         <v>3567</v>
@@ -57674,10 +57683,10 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>3853</v>
+        <v>3850</v>
       </c>
       <c r="B218" t="s">
-        <v>3883</v>
+        <v>3879</v>
       </c>
       <c r="C218" t="s">
         <v>3567</v>
@@ -57685,10 +57694,10 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>3854</v>
+        <v>3851</v>
       </c>
       <c r="B219" t="s">
-        <v>3884</v>
+        <v>3880</v>
       </c>
       <c r="C219" t="s">
         <v>3567</v>
@@ -57696,21 +57705,21 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>3855</v>
+        <v>3839</v>
       </c>
       <c r="B220" t="s">
-        <v>3885</v>
+        <v>3881</v>
       </c>
       <c r="C220" t="s">
         <v>3567</v>
       </c>
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A221" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B221" s="3" t="s">
-        <v>124</v>
+      <c r="A221" t="s">
+        <v>3852</v>
+      </c>
+      <c r="B221" t="s">
+        <v>3882</v>
       </c>
       <c r="C221" t="s">
         <v>3567</v>
@@ -57718,10 +57727,10 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>3843</v>
+        <v>3853</v>
       </c>
       <c r="B222" t="s">
-        <v>3886</v>
+        <v>3883</v>
       </c>
       <c r="C222" t="s">
         <v>3567</v>
@@ -57729,10 +57738,10 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>3856</v>
+        <v>3854</v>
       </c>
       <c r="B223" t="s">
-        <v>3887</v>
+        <v>3884</v>
       </c>
       <c r="C223" t="s">
         <v>3567</v>
@@ -57740,21 +57749,21 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>3857</v>
+        <v>3855</v>
       </c>
       <c r="B224" t="s">
-        <v>3888</v>
+        <v>3885</v>
       </c>
       <c r="C224" t="s">
         <v>3567</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
-        <v>3858</v>
-      </c>
-      <c r="B225" t="s">
-        <v>3889</v>
+      <c r="A225" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B225" s="3" t="s">
+        <v>124</v>
       </c>
       <c r="C225" t="s">
         <v>3567</v>
@@ -57762,10 +57771,10 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>3859</v>
+        <v>3843</v>
       </c>
       <c r="B226" t="s">
-        <v>3890</v>
+        <v>3886</v>
       </c>
       <c r="C226" t="s">
         <v>3567</v>
@@ -57773,10 +57782,10 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>3848</v>
+        <v>3856</v>
       </c>
       <c r="B227" t="s">
-        <v>3891</v>
+        <v>3887</v>
       </c>
       <c r="C227" t="s">
         <v>3567</v>
@@ -57784,10 +57793,10 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>3841</v>
+        <v>3857</v>
       </c>
       <c r="B228" t="s">
-        <v>3892</v>
+        <v>3888</v>
       </c>
       <c r="C228" t="s">
         <v>3567</v>
@@ -57795,10 +57804,10 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>3860</v>
+        <v>3858</v>
       </c>
       <c r="B229" t="s">
-        <v>3893</v>
+        <v>3889</v>
       </c>
       <c r="C229" t="s">
         <v>3567</v>
@@ -57806,10 +57815,10 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>3861</v>
+        <v>3859</v>
       </c>
       <c r="B230" t="s">
-        <v>3894</v>
+        <v>3890</v>
       </c>
       <c r="C230" t="s">
         <v>3567</v>
@@ -57817,21 +57826,21 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>3845</v>
+        <v>3848</v>
       </c>
       <c r="B231" t="s">
-        <v>3895</v>
+        <v>3891</v>
       </c>
       <c r="C231" t="s">
         <v>3567</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A232" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B232" s="3" t="s">
-        <v>125</v>
+      <c r="A232" t="s">
+        <v>3841</v>
+      </c>
+      <c r="B232" t="s">
+        <v>3892</v>
       </c>
       <c r="C232" t="s">
         <v>3567</v>
@@ -57839,10 +57848,10 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>3838</v>
+        <v>3860</v>
       </c>
       <c r="B233" t="s">
-        <v>3896</v>
+        <v>3893</v>
       </c>
       <c r="C233" t="s">
         <v>3567</v>
@@ -57850,10 +57859,10 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>3862</v>
+        <v>3861</v>
       </c>
       <c r="B234" t="s">
-        <v>3897</v>
+        <v>3894</v>
       </c>
       <c r="C234" t="s">
         <v>3567</v>
@@ -57861,21 +57870,21 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>3863</v>
+        <v>3845</v>
       </c>
       <c r="B235" t="s">
-        <v>3898</v>
+        <v>3895</v>
       </c>
       <c r="C235" t="s">
         <v>3567</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A236" t="s">
-        <v>3864</v>
-      </c>
-      <c r="B236" t="s">
-        <v>3899</v>
+      <c r="A236" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B236" s="3" t="s">
+        <v>125</v>
       </c>
       <c r="C236" t="s">
         <v>3567</v>
@@ -57883,10 +57892,10 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>3865</v>
+        <v>3838</v>
       </c>
       <c r="B237" t="s">
-        <v>3900</v>
+        <v>3896</v>
       </c>
       <c r="C237" t="s">
         <v>3567</v>
@@ -57894,10 +57903,10 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>28</v>
-      </c>
-      <c r="B238" s="3" t="s">
-        <v>129</v>
+        <v>3862</v>
+      </c>
+      <c r="B238" t="s">
+        <v>3897</v>
       </c>
       <c r="C238" t="s">
         <v>3567</v>
@@ -57905,10 +57914,10 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>3866</v>
+        <v>3863</v>
       </c>
       <c r="B239" t="s">
-        <v>3901</v>
+        <v>3898</v>
       </c>
       <c r="C239" t="s">
         <v>3567</v>
@@ -57916,10 +57925,10 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>3867</v>
+        <v>3864</v>
       </c>
       <c r="B240" t="s">
-        <v>3902</v>
+        <v>3899</v>
       </c>
       <c r="C240" t="s">
         <v>3567</v>
@@ -57927,10 +57936,10 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>3868</v>
+        <v>3865</v>
       </c>
       <c r="B241" t="s">
-        <v>3903</v>
+        <v>3900</v>
       </c>
       <c r="C241" t="s">
         <v>3567</v>
@@ -57938,10 +57947,10 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B242" s="3" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="C242" t="s">
         <v>3567</v>
@@ -57949,10 +57958,10 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>3844</v>
+        <v>3866</v>
       </c>
       <c r="B243" t="s">
-        <v>3872</v>
+        <v>3901</v>
       </c>
       <c r="C243" t="s">
         <v>3567</v>
@@ -57960,10 +57969,10 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>26</v>
-      </c>
-      <c r="B244" s="3" t="s">
-        <v>127</v>
+        <v>3867</v>
+      </c>
+      <c r="B244" t="s">
+        <v>3902</v>
       </c>
       <c r="C244" t="s">
         <v>3567</v>
@@ -57971,10 +57980,10 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>3842</v>
+        <v>3868</v>
       </c>
       <c r="B245" t="s">
-        <v>3873</v>
+        <v>3903</v>
       </c>
       <c r="C245" t="s">
         <v>3567</v>
@@ -57982,10 +57991,10 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>3840</v>
-      </c>
-      <c r="B246" t="s">
-        <v>3874</v>
+        <v>25</v>
+      </c>
+      <c r="B246" s="3" t="s">
+        <v>126</v>
       </c>
       <c r="C246" t="s">
         <v>3567</v>
@@ -57993,10 +58002,10 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>3869</v>
+        <v>3844</v>
       </c>
       <c r="B247" t="s">
-        <v>3875</v>
+        <v>3872</v>
       </c>
       <c r="C247" t="s">
         <v>3567</v>
@@ -58004,10 +58013,10 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>3870</v>
-      </c>
-      <c r="B248" t="s">
-        <v>3876</v>
+        <v>26</v>
+      </c>
+      <c r="B248" s="3" t="s">
+        <v>127</v>
       </c>
       <c r="C248" t="s">
         <v>3567</v>
@@ -58015,10 +58024,10 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>3464</v>
+        <v>3842</v>
       </c>
       <c r="B249" t="s">
-        <v>3462</v>
+        <v>3873</v>
       </c>
       <c r="C249" t="s">
         <v>3567</v>
@@ -58026,10 +58035,10 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>3459</v>
+        <v>3840</v>
       </c>
       <c r="B250" t="s">
-        <v>3463</v>
+        <v>3874</v>
       </c>
       <c r="C250" t="s">
         <v>3567</v>
@@ -58037,10 +58046,10 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>3461</v>
+        <v>3869</v>
       </c>
       <c r="B251" t="s">
-        <v>3460</v>
+        <v>3875</v>
       </c>
       <c r="C251" t="s">
         <v>3567</v>
@@ -58048,10 +58057,10 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>3520</v>
+        <v>3870</v>
       </c>
       <c r="B252" t="s">
-        <v>3561</v>
+        <v>3876</v>
       </c>
       <c r="C252" t="s">
         <v>3567</v>
@@ -58059,10 +58068,10 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>40</v>
-      </c>
-      <c r="B253" s="3" t="s">
-        <v>3816</v>
+        <v>3464</v>
+      </c>
+      <c r="B253" t="s">
+        <v>3462</v>
       </c>
       <c r="C253" t="s">
         <v>3567</v>
@@ -58070,10 +58079,10 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>4037</v>
+        <v>3459</v>
       </c>
       <c r="B254" t="s">
-        <v>4046</v>
+        <v>3463</v>
       </c>
       <c r="C254" t="s">
         <v>3567</v>
@@ -58081,10 +58090,10 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>4032</v>
+        <v>3461</v>
       </c>
       <c r="B255" t="s">
-        <v>4041</v>
+        <v>3460</v>
       </c>
       <c r="C255" t="s">
         <v>3567</v>
@@ -58092,10 +58101,10 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>4031</v>
+        <v>3520</v>
       </c>
       <c r="B256" t="s">
-        <v>4040</v>
+        <v>3561</v>
       </c>
       <c r="C256" t="s">
         <v>3567</v>
@@ -58103,10 +58112,10 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>4035</v>
-      </c>
-      <c r="B257" t="s">
-        <v>4044</v>
+        <v>40</v>
+      </c>
+      <c r="B257" s="3" t="s">
+        <v>3816</v>
       </c>
       <c r="C257" t="s">
         <v>3567</v>
@@ -58114,10 +58123,10 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>4038</v>
+        <v>4037</v>
       </c>
       <c r="B258" t="s">
-        <v>4047</v>
+        <v>4046</v>
       </c>
       <c r="C258" t="s">
         <v>3567</v>
@@ -58125,10 +58134,10 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>4039</v>
+        <v>4032</v>
       </c>
       <c r="B259" t="s">
-        <v>4048</v>
+        <v>4041</v>
       </c>
       <c r="C259" t="s">
         <v>3567</v>
@@ -58136,10 +58145,10 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>4036</v>
+        <v>4031</v>
       </c>
       <c r="B260" t="s">
-        <v>4045</v>
+        <v>4040</v>
       </c>
       <c r="C260" t="s">
         <v>3567</v>
@@ -58147,10 +58156,10 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>4033</v>
+        <v>4035</v>
       </c>
       <c r="B261" t="s">
-        <v>4042</v>
+        <v>4044</v>
       </c>
       <c r="C261" t="s">
         <v>3567</v>
@@ -58158,10 +58167,10 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>4034</v>
+        <v>4038</v>
       </c>
       <c r="B262" t="s">
-        <v>4043</v>
+        <v>4047</v>
       </c>
       <c r="C262" t="s">
         <v>3567</v>
@@ -58169,10 +58178,10 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>4027</v>
+        <v>4039</v>
       </c>
       <c r="B263" t="s">
-        <v>4024</v>
+        <v>4048</v>
       </c>
       <c r="C263" t="s">
         <v>3567</v>
@@ -58180,10 +58189,10 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>4026</v>
+        <v>4036</v>
       </c>
       <c r="B264" t="s">
-        <v>4030</v>
+        <v>4045</v>
       </c>
       <c r="C264" t="s">
         <v>3567</v>
@@ -58191,10 +58200,10 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>4028</v>
+        <v>4033</v>
       </c>
       <c r="B265" t="s">
-        <v>4023</v>
+        <v>4042</v>
       </c>
       <c r="C265" t="s">
         <v>3567</v>
@@ -58202,10 +58211,10 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>4025</v>
+        <v>4034</v>
       </c>
       <c r="B266" t="s">
-        <v>4029</v>
+        <v>4043</v>
       </c>
       <c r="C266" t="s">
         <v>3567</v>
@@ -58213,10 +58222,10 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>4020</v>
+        <v>4027</v>
       </c>
       <c r="B267" t="s">
-        <v>4014</v>
+        <v>4024</v>
       </c>
       <c r="C267" t="s">
         <v>3567</v>
@@ -58224,10 +58233,10 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>4015</v>
+        <v>4026</v>
       </c>
       <c r="B268" t="s">
-        <v>4017</v>
+        <v>4030</v>
       </c>
       <c r="C268" t="s">
         <v>3567</v>
@@ -58235,10 +58244,10 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>4018</v>
+        <v>4028</v>
       </c>
       <c r="B269" t="s">
-        <v>4019</v>
+        <v>4023</v>
       </c>
       <c r="C269" t="s">
         <v>3567</v>
@@ -58246,10 +58255,10 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>4021</v>
+        <v>4025</v>
       </c>
       <c r="B270" t="s">
-        <v>4022</v>
+        <v>4029</v>
       </c>
       <c r="C270" t="s">
         <v>3567</v>
@@ -58257,10 +58266,10 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>4009</v>
+        <v>4020</v>
       </c>
       <c r="B271" t="s">
-        <v>4011</v>
+        <v>4014</v>
       </c>
       <c r="C271" t="s">
         <v>3567</v>
@@ -58268,10 +58277,10 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>4049</v>
+        <v>4015</v>
       </c>
       <c r="B272" t="s">
-        <v>4013</v>
+        <v>4017</v>
       </c>
       <c r="C272" t="s">
         <v>3567</v>
@@ -58279,10 +58288,10 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>4010</v>
+        <v>4018</v>
       </c>
       <c r="B273" t="s">
-        <v>4012</v>
+        <v>4019</v>
       </c>
       <c r="C273" t="s">
         <v>3567</v>
@@ -58290,10 +58299,10 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>4015</v>
+        <v>4021</v>
       </c>
       <c r="B274" t="s">
-        <v>4016</v>
+        <v>4022</v>
       </c>
       <c r="C274" t="s">
         <v>3567</v>
@@ -58301,10 +58310,10 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>3697</v>
+        <v>4009</v>
       </c>
       <c r="B275" t="s">
-        <v>3698</v>
+        <v>4011</v>
       </c>
       <c r="C275" t="s">
         <v>3567</v>
@@ -58312,10 +58321,10 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>33</v>
-      </c>
-      <c r="B276" s="3" t="s">
-        <v>134</v>
+        <v>4049</v>
+      </c>
+      <c r="B276" t="s">
+        <v>4013</v>
       </c>
       <c r="C276" t="s">
         <v>3567</v>
@@ -58323,10 +58332,10 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>29</v>
-      </c>
-      <c r="B277" s="3" t="s">
-        <v>130</v>
+        <v>4010</v>
+      </c>
+      <c r="B277" t="s">
+        <v>4012</v>
       </c>
       <c r="C277" t="s">
         <v>3567</v>
@@ -58334,10 +58343,10 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>30</v>
-      </c>
-      <c r="B278" s="3" t="s">
-        <v>131</v>
+        <v>4015</v>
+      </c>
+      <c r="B278" t="s">
+        <v>4016</v>
       </c>
       <c r="C278" t="s">
         <v>3567</v>
@@ -58345,10 +58354,10 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>31</v>
-      </c>
-      <c r="B279" s="3" t="s">
-        <v>132</v>
+        <v>3697</v>
+      </c>
+      <c r="B279" t="s">
+        <v>3698</v>
       </c>
       <c r="C279" t="s">
         <v>3567</v>
@@ -58356,10 +58365,10 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>3846</v>
+        <v>33</v>
       </c>
       <c r="B280" s="3" t="s">
-        <v>3871</v>
+        <v>134</v>
       </c>
       <c r="C280" t="s">
         <v>3567</v>
@@ -58367,10 +58376,10 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B281" s="3" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C281" t="s">
         <v>3567</v>
@@ -58378,10 +58387,10 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>4055</v>
-      </c>
-      <c r="B282" t="s">
-        <v>4054</v>
+        <v>30</v>
+      </c>
+      <c r="B282" s="3" t="s">
+        <v>131</v>
       </c>
       <c r="C282" t="s">
         <v>3567</v>
@@ -58389,10 +58398,10 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>3680</v>
-      </c>
-      <c r="B283" t="s">
-        <v>3681</v>
+        <v>31</v>
+      </c>
+      <c r="B283" s="3" t="s">
+        <v>132</v>
       </c>
       <c r="C283" t="s">
         <v>3567</v>
@@ -58400,10 +58409,10 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>3679</v>
-      </c>
-      <c r="B284" t="s">
-        <v>3682</v>
+        <v>3846</v>
+      </c>
+      <c r="B284" s="3" t="s">
+        <v>3871</v>
       </c>
       <c r="C284" t="s">
         <v>3567</v>
@@ -58411,10 +58420,10 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>42</v>
-      </c>
-      <c r="B285" t="s">
-        <v>3683</v>
+        <v>32</v>
+      </c>
+      <c r="B285" s="3" t="s">
+        <v>133</v>
       </c>
       <c r="C285" t="s">
         <v>3567</v>
@@ -58422,10 +58431,10 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>375</v>
+        <v>4055</v>
       </c>
       <c r="B286" t="s">
-        <v>376</v>
+        <v>4054</v>
       </c>
       <c r="C286" t="s">
         <v>3567</v>
@@ -58433,10 +58442,10 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>285</v>
+        <v>3680</v>
       </c>
       <c r="B287" t="s">
-        <v>283</v>
+        <v>3681</v>
       </c>
       <c r="C287" t="s">
         <v>3567</v>
@@ -58444,10 +58453,10 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>286</v>
+        <v>3679</v>
       </c>
       <c r="B288" t="s">
-        <v>284</v>
+        <v>3682</v>
       </c>
       <c r="C288" t="s">
         <v>3567</v>
@@ -58455,10 +58464,10 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>395</v>
+        <v>42</v>
       </c>
       <c r="B289" t="s">
-        <v>396</v>
+        <v>3683</v>
       </c>
       <c r="C289" t="s">
         <v>3567</v>
@@ -58466,10 +58475,10 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>325</v>
+        <v>375</v>
       </c>
       <c r="B290" t="s">
-        <v>323</v>
+        <v>376</v>
       </c>
       <c r="C290" t="s">
         <v>3567</v>
@@ -58477,10 +58486,10 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
-        <v>326</v>
+        <v>285</v>
       </c>
       <c r="B291" t="s">
-        <v>324</v>
+        <v>283</v>
       </c>
       <c r="C291" t="s">
         <v>3567</v>
@@ -58488,10 +58497,10 @@
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
-        <v>4112</v>
+        <v>286</v>
       </c>
       <c r="B292" t="s">
-        <v>4111</v>
+        <v>284</v>
       </c>
       <c r="C292" t="s">
         <v>3567</v>
@@ -58499,10 +58508,10 @@
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
-        <v>4113</v>
+        <v>395</v>
       </c>
       <c r="B293" t="s">
-        <v>4114</v>
+        <v>396</v>
       </c>
       <c r="C293" t="s">
         <v>3567</v>
@@ -58510,10 +58519,10 @@
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
-        <v>387</v>
+        <v>325</v>
       </c>
       <c r="B294" t="s">
-        <v>388</v>
+        <v>323</v>
       </c>
       <c r="C294" t="s">
         <v>3567</v>
@@ -58521,10 +58530,10 @@
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
-        <v>309</v>
+        <v>326</v>
       </c>
       <c r="B295" t="s">
-        <v>307</v>
+        <v>324</v>
       </c>
       <c r="C295" t="s">
         <v>3567</v>
@@ -58532,10 +58541,10 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>310</v>
+        <v>4112</v>
       </c>
       <c r="B296" t="s">
-        <v>308</v>
+        <v>4111</v>
       </c>
       <c r="C296" t="s">
         <v>3567</v>
@@ -58543,10 +58552,10 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>4117</v>
+        <v>4113</v>
       </c>
       <c r="B297" t="s">
-        <v>4115</v>
+        <v>4114</v>
       </c>
       <c r="C297" t="s">
         <v>3567</v>
@@ -58554,10 +58563,10 @@
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
-        <v>4118</v>
+        <v>387</v>
       </c>
       <c r="B298" t="s">
-        <v>4116</v>
+        <v>388</v>
       </c>
       <c r="C298" t="s">
         <v>3567</v>
@@ -58565,10 +58574,10 @@
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
-        <v>4124</v>
+        <v>309</v>
       </c>
       <c r="B299" t="s">
-        <v>4119</v>
+        <v>307</v>
       </c>
       <c r="C299" t="s">
         <v>3567</v>
@@ -58576,10 +58585,10 @@
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
-        <v>4120</v>
+        <v>310</v>
       </c>
       <c r="B300" t="s">
-        <v>4121</v>
+        <v>308</v>
       </c>
       <c r="C300" t="s">
         <v>3567</v>
@@ -58587,10 +58596,10 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>4122</v>
+        <v>4117</v>
       </c>
       <c r="B301" t="s">
-        <v>4123</v>
+        <v>4115</v>
       </c>
       <c r="C301" t="s">
         <v>3567</v>
@@ -58598,10 +58607,10 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>403</v>
+        <v>4118</v>
       </c>
       <c r="B302" t="s">
-        <v>404</v>
+        <v>4116</v>
       </c>
       <c r="C302" t="s">
         <v>3567</v>
@@ -58609,10 +58618,10 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>343</v>
+        <v>4124</v>
       </c>
       <c r="B303" t="s">
-        <v>339</v>
+        <v>4119</v>
       </c>
       <c r="C303" t="s">
         <v>3567</v>
@@ -58620,10 +58629,10 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>344</v>
+        <v>4120</v>
       </c>
       <c r="B304" t="s">
-        <v>340</v>
+        <v>4121</v>
       </c>
       <c r="C304" t="s">
         <v>3567</v>
@@ -58631,10 +58640,10 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>368</v>
+        <v>4122</v>
       </c>
       <c r="B305" t="s">
-        <v>369</v>
+        <v>4123</v>
       </c>
       <c r="C305" t="s">
         <v>3567</v>
@@ -58642,10 +58651,10 @@
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
-        <v>269</v>
+        <v>403</v>
       </c>
       <c r="B306" t="s">
-        <v>271</v>
+        <v>404</v>
       </c>
       <c r="C306" t="s">
         <v>3567</v>
@@ -58653,10 +58662,10 @@
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
-        <v>270</v>
+        <v>343</v>
       </c>
       <c r="B307" t="s">
-        <v>272</v>
+        <v>339</v>
       </c>
       <c r="C307" t="s">
         <v>3567</v>
@@ -58664,10 +58673,10 @@
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
-        <v>364</v>
+        <v>344</v>
       </c>
       <c r="B308" t="s">
-        <v>365</v>
+        <v>340</v>
       </c>
       <c r="C308" t="s">
         <v>3567</v>
@@ -58675,10 +58684,10 @@
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
-        <v>267</v>
+        <v>368</v>
       </c>
       <c r="B309" t="s">
-        <v>261</v>
+        <v>369</v>
       </c>
       <c r="C309" t="s">
         <v>3567</v>
@@ -58686,10 +58695,10 @@
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B310" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="C310" t="s">
         <v>3567</v>
@@ -58697,10 +58706,10 @@
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
-        <v>405</v>
+        <v>270</v>
       </c>
       <c r="B311" t="s">
-        <v>406</v>
+        <v>272</v>
       </c>
       <c r="C311" t="s">
         <v>3567</v>
@@ -58708,10 +58717,10 @@
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
-        <v>345</v>
+        <v>364</v>
       </c>
       <c r="B312" t="s">
-        <v>341</v>
+        <v>365</v>
       </c>
       <c r="C312" t="s">
         <v>3567</v>
@@ -58719,10 +58728,10 @@
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
-        <v>346</v>
+        <v>267</v>
       </c>
       <c r="B313" t="s">
-        <v>342</v>
+        <v>261</v>
       </c>
       <c r="C313" t="s">
         <v>3567</v>
@@ -58730,10 +58739,10 @@
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
-        <v>399</v>
+        <v>268</v>
       </c>
       <c r="B314" t="s">
-        <v>400</v>
+        <v>262</v>
       </c>
       <c r="C314" t="s">
         <v>3567</v>
@@ -58741,10 +58750,10 @@
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
-        <v>335</v>
+        <v>405</v>
       </c>
       <c r="B315" t="s">
-        <v>331</v>
+        <v>406</v>
       </c>
       <c r="C315" t="s">
         <v>3567</v>
@@ -58752,10 +58761,10 @@
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
       <c r="B316" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="C316" t="s">
         <v>3567</v>
@@ -58763,10 +58772,10 @@
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
-        <v>401</v>
+        <v>346</v>
       </c>
       <c r="B317" t="s">
-        <v>402</v>
+        <v>342</v>
       </c>
       <c r="C317" t="s">
         <v>3567</v>
@@ -58774,10 +58783,10 @@
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
-        <v>337</v>
+        <v>399</v>
       </c>
       <c r="B318" t="s">
-        <v>333</v>
+        <v>400</v>
       </c>
       <c r="C318" t="s">
         <v>3567</v>
@@ -58785,10 +58794,10 @@
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B319" t="s">
-        <v>334</v>
+        <v>331</v>
       </c>
       <c r="C319" t="s">
         <v>3567</v>
@@ -58796,10 +58805,10 @@
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
-        <v>370</v>
+        <v>336</v>
       </c>
       <c r="B320" t="s">
-        <v>371</v>
+        <v>332</v>
       </c>
       <c r="C320" t="s">
         <v>3567</v>
@@ -58807,10 +58816,10 @@
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
-        <v>275</v>
+        <v>401</v>
       </c>
       <c r="B321" t="s">
-        <v>273</v>
+        <v>402</v>
       </c>
       <c r="C321" t="s">
         <v>3567</v>
@@ -58818,10 +58827,10 @@
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
-        <v>276</v>
+        <v>337</v>
       </c>
       <c r="B322" t="s">
-        <v>274</v>
+        <v>333</v>
       </c>
       <c r="C322" t="s">
         <v>3567</v>
@@ -58829,10 +58838,10 @@
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
-        <v>379</v>
+        <v>338</v>
       </c>
       <c r="B323" t="s">
-        <v>380</v>
+        <v>334</v>
       </c>
       <c r="C323" t="s">
         <v>3567</v>
@@ -58840,10 +58849,10 @@
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
-        <v>293</v>
+        <v>370</v>
       </c>
       <c r="B324" t="s">
-        <v>291</v>
+        <v>371</v>
       </c>
       <c r="C324" t="s">
         <v>3567</v>
@@ -58851,10 +58860,10 @@
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
-        <v>294</v>
+        <v>275</v>
       </c>
       <c r="B325" t="s">
-        <v>292</v>
+        <v>273</v>
       </c>
       <c r="C325" t="s">
         <v>3567</v>
@@ -58862,10 +58871,10 @@
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
-        <v>397</v>
+        <v>276</v>
       </c>
       <c r="B326" t="s">
-        <v>398</v>
+        <v>274</v>
       </c>
       <c r="C326" t="s">
         <v>3567</v>
@@ -58873,10 +58882,10 @@
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
-        <v>329</v>
+        <v>379</v>
       </c>
       <c r="B327" t="s">
-        <v>327</v>
+        <v>380</v>
       </c>
       <c r="C327" t="s">
         <v>3567</v>
@@ -58884,10 +58893,10 @@
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
-        <v>330</v>
+        <v>293</v>
       </c>
       <c r="B328" t="s">
-        <v>328</v>
+        <v>291</v>
       </c>
       <c r="C328" t="s">
         <v>3567</v>
@@ -58895,10 +58904,10 @@
     </row>
     <row r="329" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
-        <v>372</v>
+        <v>294</v>
       </c>
       <c r="B329" t="s">
-        <v>3440</v>
+        <v>292</v>
       </c>
       <c r="C329" t="s">
         <v>3567</v>
@@ -58906,10 +58915,10 @@
     </row>
     <row r="330" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
-        <v>277</v>
+        <v>397</v>
       </c>
       <c r="B330" t="s">
-        <v>3441</v>
+        <v>398</v>
       </c>
       <c r="C330" t="s">
         <v>3567</v>
@@ -58917,10 +58926,10 @@
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
-        <v>278</v>
+        <v>329</v>
       </c>
       <c r="B331" t="s">
-        <v>3442</v>
+        <v>327</v>
       </c>
       <c r="C331" t="s">
         <v>3567</v>
@@ -58928,10 +58937,10 @@
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
-        <v>377</v>
+        <v>330</v>
       </c>
       <c r="B332" t="s">
-        <v>378</v>
+        <v>328</v>
       </c>
       <c r="C332" t="s">
         <v>3567</v>
@@ -58939,10 +58948,10 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
-        <v>289</v>
+        <v>372</v>
       </c>
       <c r="B333" t="s">
-        <v>287</v>
+        <v>3440</v>
       </c>
       <c r="C333" t="s">
         <v>3567</v>
@@ -58950,10 +58959,10 @@
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
-        <v>290</v>
+        <v>277</v>
       </c>
       <c r="B334" t="s">
-        <v>288</v>
+        <v>3441</v>
       </c>
       <c r="C334" t="s">
         <v>3567</v>
@@ -58961,10 +58970,10 @@
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
-        <v>409</v>
+        <v>278</v>
       </c>
       <c r="B335" t="s">
-        <v>410</v>
+        <v>3442</v>
       </c>
       <c r="C335" t="s">
         <v>3567</v>
@@ -58972,10 +58981,10 @@
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
-        <v>353</v>
+        <v>377</v>
       </c>
       <c r="B336" t="s">
-        <v>349</v>
+        <v>378</v>
       </c>
       <c r="C336" t="s">
         <v>3567</v>
@@ -58983,10 +58992,10 @@
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
-        <v>354</v>
+        <v>289</v>
       </c>
       <c r="B337" t="s">
-        <v>350</v>
+        <v>287</v>
       </c>
       <c r="C337" t="s">
         <v>3567</v>
@@ -58994,10 +59003,10 @@
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
-        <v>407</v>
+        <v>290</v>
       </c>
       <c r="B338" t="s">
-        <v>408</v>
+        <v>288</v>
       </c>
       <c r="C338" t="s">
         <v>3567</v>
@@ -59005,10 +59014,10 @@
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
-        <v>351</v>
+        <v>409</v>
       </c>
       <c r="B339" t="s">
-        <v>347</v>
+        <v>410</v>
       </c>
       <c r="C339" t="s">
         <v>3567</v>
@@ -59016,10 +59025,10 @@
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B340" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="C340" t="s">
         <v>3567</v>
@@ -59027,10 +59036,10 @@
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
-        <v>391</v>
+        <v>354</v>
       </c>
       <c r="B341" t="s">
-        <v>392</v>
+        <v>350</v>
       </c>
       <c r="C341" t="s">
         <v>3567</v>
@@ -59038,10 +59047,10 @@
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
-        <v>321</v>
+        <v>407</v>
       </c>
       <c r="B342" t="s">
-        <v>315</v>
+        <v>408</v>
       </c>
       <c r="C342" t="s">
         <v>3567</v>
@@ -59049,10 +59058,10 @@
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
-        <v>322</v>
+        <v>351</v>
       </c>
       <c r="B343" t="s">
-        <v>316</v>
+        <v>347</v>
       </c>
       <c r="C343" t="s">
         <v>3567</v>
@@ -59060,10 +59069,10 @@
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
-        <v>389</v>
+        <v>352</v>
       </c>
       <c r="B344" t="s">
-        <v>390</v>
+        <v>348</v>
       </c>
       <c r="C344" t="s">
         <v>3567</v>
@@ -59071,10 +59080,10 @@
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
-        <v>311</v>
+        <v>391</v>
       </c>
       <c r="B345" t="s">
-        <v>313</v>
+        <v>392</v>
       </c>
       <c r="C345" t="s">
         <v>3567</v>
@@ -59082,10 +59091,10 @@
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="B346" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C346" t="s">
         <v>3567</v>
@@ -59093,10 +59102,10 @@
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
-        <v>366</v>
+        <v>322</v>
       </c>
       <c r="B347" t="s">
-        <v>367</v>
+        <v>316</v>
       </c>
       <c r="C347" t="s">
         <v>3567</v>
@@ -59104,10 +59113,10 @@
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
-        <v>263</v>
+        <v>389</v>
       </c>
       <c r="B348" t="s">
-        <v>264</v>
+        <v>390</v>
       </c>
       <c r="C348" t="s">
         <v>3567</v>
@@ -59115,10 +59124,10 @@
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
-        <v>266</v>
+        <v>311</v>
       </c>
       <c r="B349" t="s">
-        <v>265</v>
+        <v>313</v>
       </c>
       <c r="C349" t="s">
         <v>3567</v>
@@ -59126,10 +59135,10 @@
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
-        <v>385</v>
+        <v>312</v>
       </c>
       <c r="B350" t="s">
-        <v>386</v>
+        <v>314</v>
       </c>
       <c r="C350" t="s">
         <v>3567</v>
@@ -59137,10 +59146,10 @@
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
-        <v>305</v>
+        <v>366</v>
       </c>
       <c r="B351" t="s">
-        <v>303</v>
+        <v>367</v>
       </c>
       <c r="C351" t="s">
         <v>3567</v>
@@ -59148,10 +59157,10 @@
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
-        <v>306</v>
+        <v>263</v>
       </c>
       <c r="B352" t="s">
-        <v>304</v>
+        <v>264</v>
       </c>
       <c r="C352" t="s">
         <v>3567</v>
@@ -59159,10 +59168,10 @@
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
-        <v>381</v>
+        <v>266</v>
       </c>
       <c r="B353" t="s">
-        <v>382</v>
+        <v>265</v>
       </c>
       <c r="C353" t="s">
         <v>3567</v>
@@ -59170,10 +59179,10 @@
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
-        <v>297</v>
+        <v>385</v>
       </c>
       <c r="B354" t="s">
-        <v>295</v>
+        <v>386</v>
       </c>
       <c r="C354" t="s">
         <v>3567</v>
@@ -59181,10 +59190,10 @@
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="B355" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="C355" t="s">
         <v>3567</v>
@@ -59192,10 +59201,10 @@
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
-        <v>393</v>
+        <v>306</v>
       </c>
       <c r="B356" t="s">
-        <v>394</v>
+        <v>304</v>
       </c>
       <c r="C356" t="s">
         <v>3567</v>
@@ -59203,10 +59212,10 @@
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
-        <v>319</v>
+        <v>381</v>
       </c>
       <c r="B357" t="s">
-        <v>317</v>
+        <v>382</v>
       </c>
       <c r="C357" t="s">
         <v>3567</v>
@@ -59214,10 +59223,10 @@
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
-        <v>320</v>
+        <v>297</v>
       </c>
       <c r="B358" t="s">
-        <v>318</v>
+        <v>295</v>
       </c>
       <c r="C358" t="s">
         <v>3567</v>
@@ -59225,10 +59234,10 @@
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
-        <v>383</v>
+        <v>298</v>
       </c>
       <c r="B359" t="s">
-        <v>384</v>
+        <v>296</v>
       </c>
       <c r="C359" t="s">
         <v>3567</v>
@@ -59236,10 +59245,10 @@
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
-        <v>301</v>
+        <v>393</v>
       </c>
       <c r="B360" t="s">
-        <v>299</v>
+        <v>394</v>
       </c>
       <c r="C360" t="s">
         <v>3567</v>
@@ -59247,10 +59256,10 @@
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
-        <v>302</v>
+        <v>319</v>
       </c>
       <c r="B361" t="s">
-        <v>300</v>
+        <v>317</v>
       </c>
       <c r="C361" t="s">
         <v>3567</v>
@@ -59258,10 +59267,10 @@
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
-        <v>19</v>
-      </c>
-      <c r="B362" s="3" t="s">
-        <v>164</v>
+        <v>320</v>
+      </c>
+      <c r="B362" t="s">
+        <v>318</v>
       </c>
       <c r="C362" t="s">
         <v>3567</v>
@@ -59269,10 +59278,10 @@
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
-        <v>20</v>
-      </c>
-      <c r="B363" s="3" t="s">
-        <v>165</v>
+        <v>383</v>
+      </c>
+      <c r="B363" t="s">
+        <v>384</v>
       </c>
       <c r="C363" t="s">
         <v>3567</v>
@@ -59280,10 +59289,10 @@
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
-        <v>21</v>
-      </c>
-      <c r="B364" s="3" t="s">
-        <v>166</v>
+        <v>301</v>
+      </c>
+      <c r="B364" t="s">
+        <v>299</v>
       </c>
       <c r="C364" t="s">
         <v>3567</v>
@@ -59291,10 +59300,10 @@
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
-        <v>4130</v>
+        <v>302</v>
       </c>
       <c r="B365" t="s">
-        <v>4129</v>
+        <v>300</v>
       </c>
       <c r="C365" t="s">
         <v>3567</v>
@@ -59302,10 +59311,10 @@
     </row>
     <row r="366" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
-        <v>4131</v>
-      </c>
-      <c r="B366" t="s">
-        <v>4133</v>
+        <v>19</v>
+      </c>
+      <c r="B366" s="3" t="s">
+        <v>164</v>
       </c>
       <c r="C366" t="s">
         <v>3567</v>
@@ -59313,10 +59322,10 @@
     </row>
     <row r="367" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
-        <v>4132</v>
-      </c>
-      <c r="B367" t="s">
-        <v>4134</v>
+        <v>20</v>
+      </c>
+      <c r="B367" s="3" t="s">
+        <v>165</v>
       </c>
       <c r="C367" t="s">
         <v>3567</v>
@@ -59324,10 +59333,10 @@
     </row>
     <row r="368" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
-        <v>4135</v>
-      </c>
-      <c r="B368" t="s">
-        <v>4136</v>
+        <v>21</v>
+      </c>
+      <c r="B368" s="3" t="s">
+        <v>166</v>
       </c>
       <c r="C368" t="s">
         <v>3567</v>
@@ -59335,10 +59344,10 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>4140</v>
+        <v>4130</v>
       </c>
       <c r="B369" t="s">
-        <v>4139</v>
+        <v>4129</v>
       </c>
       <c r="C369" t="s">
         <v>3567</v>
@@ -59346,10 +59355,10 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
-        <v>4137</v>
+        <v>4131</v>
       </c>
       <c r="B370" t="s">
-        <v>4138</v>
+        <v>4133</v>
       </c>
       <c r="C370" t="s">
         <v>3567</v>
@@ -59357,10 +59366,10 @@
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
-        <v>4142</v>
+        <v>4132</v>
       </c>
       <c r="B371" t="s">
-        <v>4141</v>
+        <v>4134</v>
       </c>
       <c r="C371" t="s">
         <v>3567</v>
@@ -59368,10 +59377,10 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>3949</v>
+        <v>4135</v>
       </c>
       <c r="B372" t="s">
-        <v>3950</v>
+        <v>4136</v>
       </c>
       <c r="C372" t="s">
         <v>3567</v>
@@ -59379,10 +59388,10 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>12</v>
-      </c>
-      <c r="B373" s="3" t="s">
-        <v>161</v>
+        <v>4140</v>
+      </c>
+      <c r="B373" t="s">
+        <v>4139</v>
       </c>
       <c r="C373" t="s">
         <v>3567</v>
@@ -59390,10 +59399,10 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>6</v>
-      </c>
-      <c r="B374" s="3" t="s">
-        <v>155</v>
+        <v>4137</v>
+      </c>
+      <c r="B374" t="s">
+        <v>4138</v>
       </c>
       <c r="C374" t="s">
         <v>3567</v>
@@ -59401,10 +59410,10 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>13</v>
-      </c>
-      <c r="B375" s="3" t="s">
-        <v>162</v>
+        <v>4142</v>
+      </c>
+      <c r="B375" t="s">
+        <v>4141</v>
       </c>
       <c r="C375" t="s">
         <v>3567</v>
@@ -59412,10 +59421,10 @@
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
-        <v>7</v>
-      </c>
-      <c r="B376" s="3" t="s">
-        <v>156</v>
+        <v>3949</v>
+      </c>
+      <c r="B376" t="s">
+        <v>3950</v>
       </c>
       <c r="C376" t="s">
         <v>3567</v>
@@ -59423,10 +59432,10 @@
     </row>
     <row r="377" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B377" s="3" t="s">
-        <v>157</v>
+        <v>161</v>
       </c>
       <c r="C377" t="s">
         <v>3567</v>
@@ -59434,10 +59443,10 @@
     </row>
     <row r="378" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B378" s="3" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C378" t="s">
         <v>3567</v>
@@ -59445,10 +59454,10 @@
     </row>
     <row r="379" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B379" s="3" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="C379" t="s">
         <v>3567</v>
@@ -59456,10 +59465,10 @@
     </row>
     <row r="380" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B380" s="3" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C380" t="s">
         <v>3567</v>
@@ -59467,10 +59476,10 @@
     </row>
     <row r="381" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
-        <v>3962</v>
-      </c>
-      <c r="B381" t="s">
-        <v>3974</v>
+        <v>8</v>
+      </c>
+      <c r="B381" s="3" t="s">
+        <v>157</v>
       </c>
       <c r="C381" t="s">
         <v>3567</v>
@@ -59478,10 +59487,10 @@
     </row>
     <row r="382" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
-        <v>3980</v>
-      </c>
-      <c r="B382" t="s">
-        <v>3977</v>
+        <v>9</v>
+      </c>
+      <c r="B382" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="C382" t="s">
         <v>3567</v>
@@ -59489,10 +59498,10 @@
     </row>
     <row r="383" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
-        <v>3964</v>
-      </c>
-      <c r="B383" t="s">
-        <v>3967</v>
+        <v>10</v>
+      </c>
+      <c r="B383" s="3" t="s">
+        <v>159</v>
       </c>
       <c r="C383" t="s">
         <v>3567</v>
@@ -59500,10 +59509,10 @@
     </row>
     <row r="384" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
-        <v>3966</v>
-      </c>
-      <c r="B384" t="s">
-        <v>3968</v>
+        <v>11</v>
+      </c>
+      <c r="B384" s="3" t="s">
+        <v>160</v>
       </c>
       <c r="C384" t="s">
         <v>3567</v>
@@ -59511,10 +59520,10 @@
     </row>
     <row r="385" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
-        <v>3963</v>
+        <v>3962</v>
       </c>
       <c r="B385" t="s">
-        <v>3965</v>
+        <v>3974</v>
       </c>
       <c r="C385" t="s">
         <v>3567</v>
@@ -59522,10 +59531,10 @@
     </row>
     <row r="386" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
-        <v>3970</v>
+        <v>3980</v>
       </c>
       <c r="B386" t="s">
-        <v>3969</v>
+        <v>3977</v>
       </c>
       <c r="C386" t="s">
         <v>3567</v>
@@ -59533,10 +59542,10 @@
     </row>
     <row r="387" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
-        <v>3930</v>
+        <v>3964</v>
       </c>
       <c r="B387" t="s">
-        <v>3931</v>
+        <v>3967</v>
       </c>
       <c r="C387" t="s">
         <v>3567</v>
@@ -59544,10 +59553,10 @@
     </row>
     <row r="388" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
-        <v>3458</v>
+        <v>3966</v>
       </c>
       <c r="B388" t="s">
-        <v>3457</v>
+        <v>3968</v>
       </c>
       <c r="C388" t="s">
         <v>3567</v>
@@ -59555,10 +59564,10 @@
     </row>
     <row r="389" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
-        <v>3451</v>
+        <v>3963</v>
       </c>
       <c r="B389" t="s">
-        <v>3454</v>
+        <v>3965</v>
       </c>
       <c r="C389" t="s">
         <v>3567</v>
@@ -59566,10 +59575,10 @@
     </row>
     <row r="390" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
-        <v>3455</v>
+        <v>3970</v>
       </c>
       <c r="B390" t="s">
-        <v>3456</v>
+        <v>3969</v>
       </c>
       <c r="C390" t="s">
         <v>3567</v>
@@ -59577,10 +59586,10 @@
     </row>
     <row r="391" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>3449</v>
+        <v>3930</v>
       </c>
       <c r="B391" t="s">
-        <v>4148</v>
+        <v>3931</v>
       </c>
       <c r="C391" t="s">
         <v>3567</v>
@@ -59588,10 +59597,10 @@
     </row>
     <row r="392" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
-        <v>415</v>
+        <v>3458</v>
       </c>
       <c r="B392" t="s">
-        <v>227</v>
+        <v>3457</v>
       </c>
       <c r="C392" t="s">
         <v>3567</v>
@@ -59599,10 +59608,10 @@
     </row>
     <row r="393" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
-        <v>118</v>
+        <v>3451</v>
       </c>
       <c r="B393" t="s">
-        <v>3437</v>
+        <v>3454</v>
       </c>
       <c r="C393" t="s">
         <v>3567</v>
@@ -59610,10 +59619,10 @@
     </row>
     <row r="394" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
-        <v>416</v>
+        <v>3455</v>
       </c>
       <c r="B394" t="s">
-        <v>226</v>
+        <v>3456</v>
       </c>
       <c r="C394" t="s">
         <v>3567</v>
@@ -59621,21 +59630,21 @@
     </row>
     <row r="395" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
-        <v>117</v>
+        <v>3449</v>
       </c>
       <c r="B395" t="s">
-        <v>3436</v>
+        <v>4148</v>
       </c>
       <c r="C395" t="s">
         <v>3567</v>
       </c>
     </row>
     <row r="396" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A396" s="2" t="s">
-        <v>417</v>
+      <c r="A396" t="s">
+        <v>415</v>
       </c>
       <c r="B396" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="C396" t="s">
         <v>3567</v>
@@ -59643,10 +59652,10 @@
     </row>
     <row r="397" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B397" t="s">
-        <v>3439</v>
+        <v>3437</v>
       </c>
       <c r="C397" t="s">
         <v>3567</v>
@@ -59654,10 +59663,10 @@
     </row>
     <row r="398" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="B398" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C398" t="s">
         <v>3567</v>
@@ -59665,21 +59674,21 @@
     </row>
     <row r="399" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B399" t="s">
-        <v>3438</v>
+        <v>3436</v>
       </c>
       <c r="C399" t="s">
         <v>3567</v>
       </c>
     </row>
     <row r="400" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A400" t="s">
-        <v>3539</v>
+      <c r="A400" s="2" t="s">
+        <v>417</v>
       </c>
       <c r="B400" t="s">
-        <v>3541</v>
+        <v>225</v>
       </c>
       <c r="C400" t="s">
         <v>3567</v>
@@ -59687,10 +59696,10 @@
     </row>
     <row r="401" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>3447</v>
+        <v>116</v>
       </c>
       <c r="B401" t="s">
-        <v>3448</v>
+        <v>3439</v>
       </c>
       <c r="C401" t="s">
         <v>3567</v>
@@ -59698,10 +59707,10 @@
     </row>
     <row r="402" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>3446</v>
+        <v>418</v>
       </c>
       <c r="B402" t="s">
-        <v>3445</v>
+        <v>224</v>
       </c>
       <c r="C402" t="s">
         <v>3567</v>
@@ -59709,10 +59718,10 @@
     </row>
     <row r="403" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>3443</v>
+        <v>115</v>
       </c>
       <c r="B403" t="s">
-        <v>3444</v>
+        <v>3438</v>
       </c>
       <c r="C403" t="s">
         <v>3567</v>
@@ -59720,10 +59729,10 @@
     </row>
     <row r="404" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>3986</v>
+        <v>3539</v>
       </c>
       <c r="B404" t="s">
-        <v>3985</v>
+        <v>3541</v>
       </c>
       <c r="C404" t="s">
         <v>3567</v>
@@ -59731,10 +59740,10 @@
     </row>
     <row r="405" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>3982</v>
+        <v>3447</v>
       </c>
       <c r="B405" t="s">
-        <v>3981</v>
+        <v>3448</v>
       </c>
       <c r="C405" t="s">
         <v>3567</v>
@@ -59742,10 +59751,10 @@
     </row>
     <row r="406" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>3983</v>
+        <v>3446</v>
       </c>
       <c r="B406" t="s">
-        <v>3984</v>
+        <v>3445</v>
       </c>
       <c r="C406" t="s">
         <v>3567</v>
@@ -59753,10 +59762,10 @@
     </row>
     <row r="407" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>3652</v>
-      </c>
-      <c r="B407" s="3" t="s">
-        <v>3653</v>
+        <v>3443</v>
+      </c>
+      <c r="B407" t="s">
+        <v>3444</v>
       </c>
       <c r="C407" t="s">
         <v>3567</v>
@@ -59764,10 +59773,10 @@
     </row>
     <row r="408" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>3953</v>
-      </c>
-      <c r="B408" s="3" t="s">
-        <v>3954</v>
+        <v>3986</v>
+      </c>
+      <c r="B408" t="s">
+        <v>3985</v>
       </c>
       <c r="C408" t="s">
         <v>3567</v>
@@ -59775,10 +59784,10 @@
     </row>
     <row r="409" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>22</v>
-      </c>
-      <c r="B409" s="3" t="s">
-        <v>412</v>
+        <v>3982</v>
+      </c>
+      <c r="B409" t="s">
+        <v>3981</v>
       </c>
       <c r="C409" t="s">
         <v>3567</v>
@@ -59786,10 +59795,10 @@
     </row>
     <row r="410" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>3815</v>
+        <v>3983</v>
       </c>
       <c r="B410" t="s">
-        <v>3654</v>
+        <v>3984</v>
       </c>
       <c r="C410" t="s">
         <v>3567</v>
@@ -59797,10 +59806,10 @@
     </row>
     <row r="411" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>3452</v>
-      </c>
-      <c r="B411" t="s">
-        <v>3467</v>
+        <v>3652</v>
+      </c>
+      <c r="B411" s="3" t="s">
+        <v>3653</v>
       </c>
       <c r="C411" t="s">
         <v>3567</v>
@@ -59808,10 +59817,10 @@
     </row>
     <row r="412" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>3469</v>
-      </c>
-      <c r="B412" t="s">
-        <v>3465</v>
+        <v>3953</v>
+      </c>
+      <c r="B412" s="3" t="s">
+        <v>3954</v>
       </c>
       <c r="C412" t="s">
         <v>3567</v>
@@ -59819,10 +59828,10 @@
     </row>
     <row r="413" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B413" s="3" t="s">
-        <v>359</v>
+        <v>412</v>
       </c>
       <c r="C413" t="s">
         <v>3567</v>
@@ -59830,10 +59839,10 @@
     </row>
     <row r="414" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>414</v>
-      </c>
-      <c r="B414" s="3" t="s">
-        <v>363</v>
+        <v>3815</v>
+      </c>
+      <c r="B414" t="s">
+        <v>3654</v>
       </c>
       <c r="C414" t="s">
         <v>3567</v>
@@ -59841,10 +59850,10 @@
     </row>
     <row r="415" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>15</v>
-      </c>
-      <c r="B415" s="3" t="s">
-        <v>360</v>
+        <v>3452</v>
+      </c>
+      <c r="B415" t="s">
+        <v>3467</v>
       </c>
       <c r="C415" t="s">
         <v>3567</v>
@@ -59852,10 +59861,10 @@
     </row>
     <row r="416" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>18</v>
-      </c>
-      <c r="B416" s="3" t="s">
-        <v>361</v>
+        <v>3469</v>
+      </c>
+      <c r="B416" t="s">
+        <v>3465</v>
       </c>
       <c r="C416" t="s">
         <v>3567</v>
@@ -59863,10 +59872,10 @@
     </row>
     <row r="417" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B417" s="3" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="C417" t="s">
         <v>3567</v>
@@ -59874,10 +59883,10 @@
     </row>
     <row r="418" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>3</v>
+        <v>414</v>
       </c>
       <c r="B418" s="3" t="s">
-        <v>419</v>
+        <v>363</v>
       </c>
       <c r="C418" t="s">
         <v>3567</v>
@@ -59885,10 +59894,10 @@
     </row>
     <row r="419" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B419" s="3" t="s">
-        <v>420</v>
+        <v>360</v>
       </c>
       <c r="C419" t="s">
         <v>3567</v>
@@ -59896,10 +59905,10 @@
     </row>
     <row r="420" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="B420" s="3" t="s">
-        <v>421</v>
+        <v>361</v>
       </c>
       <c r="C420" t="s">
         <v>3567</v>
@@ -59907,10 +59916,10 @@
     </row>
     <row r="421" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
-        <v>2</v>
+        <v>16</v>
       </c>
       <c r="B421" s="3" t="s">
-        <v>422</v>
+        <v>362</v>
       </c>
       <c r="C421" t="s">
         <v>3567</v>
@@ -59918,10 +59927,10 @@
     </row>
     <row r="422" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>3961</v>
-      </c>
-      <c r="B422" t="s">
-        <v>3973</v>
+        <v>3</v>
+      </c>
+      <c r="B422" s="3" t="s">
+        <v>419</v>
       </c>
       <c r="C422" t="s">
         <v>3567</v>
@@ -59929,10 +59938,10 @@
     </row>
     <row r="423" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>3979</v>
-      </c>
-      <c r="B423" t="s">
-        <v>3976</v>
+        <v>4</v>
+      </c>
+      <c r="B423" s="3" t="s">
+        <v>420</v>
       </c>
       <c r="C423" t="s">
         <v>3567</v>
@@ -59940,10 +59949,10 @@
     </row>
     <row r="424" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
-        <v>3955</v>
-      </c>
-      <c r="B424" t="s">
-        <v>3971</v>
+        <v>5</v>
+      </c>
+      <c r="B424" s="3" t="s">
+        <v>421</v>
       </c>
       <c r="C424" t="s">
         <v>3567</v>
@@ -59951,10 +59960,10 @@
     </row>
     <row r="425" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>3958</v>
-      </c>
-      <c r="B425" t="s">
-        <v>3959</v>
+        <v>2</v>
+      </c>
+      <c r="B425" s="3" t="s">
+        <v>422</v>
       </c>
       <c r="C425" t="s">
         <v>3567</v>
@@ -59962,10 +59971,10 @@
     </row>
     <row r="426" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>3956</v>
+        <v>3961</v>
       </c>
       <c r="B426" t="s">
-        <v>3957</v>
+        <v>3973</v>
       </c>
       <c r="C426" t="s">
         <v>3567</v>
@@ -59973,10 +59982,10 @@
     </row>
     <row r="427" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>3631</v>
+        <v>3979</v>
       </c>
       <c r="B427" t="s">
-        <v>3632</v>
+        <v>3976</v>
       </c>
       <c r="C427" t="s">
         <v>3567</v>
@@ -59984,10 +59993,10 @@
     </row>
     <row r="428" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>3635</v>
+        <v>3955</v>
       </c>
       <c r="B428" t="s">
-        <v>3636</v>
+        <v>3971</v>
       </c>
       <c r="C428" t="s">
         <v>3567</v>
@@ -59995,10 +60004,10 @@
     </row>
     <row r="429" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>3633</v>
+        <v>3958</v>
       </c>
       <c r="B429" t="s">
-        <v>3634</v>
+        <v>3959</v>
       </c>
       <c r="C429" t="s">
         <v>3567</v>
@@ -60006,10 +60015,10 @@
     </row>
     <row r="430" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>3987</v>
+        <v>3956</v>
       </c>
       <c r="B430" t="s">
-        <v>3996</v>
+        <v>3957</v>
       </c>
       <c r="C430" t="s">
         <v>3567</v>
@@ -60017,10 +60026,10 @@
     </row>
     <row r="431" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>3992</v>
+        <v>3631</v>
       </c>
       <c r="B431" t="s">
-        <v>4001</v>
+        <v>3632</v>
       </c>
       <c r="C431" t="s">
         <v>3567</v>
@@ -60028,10 +60037,10 @@
     </row>
     <row r="432" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>3990</v>
+        <v>3635</v>
       </c>
       <c r="B432" t="s">
-        <v>3999</v>
+        <v>3636</v>
       </c>
       <c r="C432" t="s">
         <v>3567</v>
@@ -60039,10 +60048,10 @@
     </row>
     <row r="433" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>3989</v>
+        <v>3633</v>
       </c>
       <c r="B433" t="s">
-        <v>3998</v>
+        <v>3634</v>
       </c>
       <c r="C433" t="s">
         <v>3567</v>
@@ -60050,10 +60059,10 @@
     </row>
     <row r="434" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>3991</v>
+        <v>3987</v>
       </c>
       <c r="B434" t="s">
-        <v>4000</v>
+        <v>3996</v>
       </c>
       <c r="C434" t="s">
         <v>3567</v>
@@ -60061,10 +60070,10 @@
     </row>
     <row r="435" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>3988</v>
+        <v>3992</v>
       </c>
       <c r="B435" t="s">
-        <v>3997</v>
+        <v>4001</v>
       </c>
       <c r="C435" t="s">
         <v>3567</v>
@@ -60072,10 +60081,10 @@
     </row>
     <row r="436" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>3995</v>
+        <v>3990</v>
       </c>
       <c r="B436" t="s">
-        <v>4004</v>
+        <v>3999</v>
       </c>
       <c r="C436" t="s">
         <v>3567</v>
@@ -60083,10 +60092,10 @@
     </row>
     <row r="437" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>3993</v>
+        <v>3989</v>
       </c>
       <c r="B437" t="s">
-        <v>4002</v>
+        <v>3998</v>
       </c>
       <c r="C437" t="s">
         <v>3567</v>
@@ -60094,10 +60103,10 @@
     </row>
     <row r="438" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>3994</v>
+        <v>3991</v>
       </c>
       <c r="B438" t="s">
-        <v>4003</v>
+        <v>4000</v>
       </c>
       <c r="C438" t="s">
         <v>3567</v>
@@ -60105,10 +60114,10 @@
     </row>
     <row r="439" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>4128</v>
+        <v>3988</v>
       </c>
       <c r="B439" t="s">
-        <v>4146</v>
+        <v>3997</v>
       </c>
       <c r="C439" t="s">
         <v>3567</v>
@@ -60116,10 +60125,10 @@
     </row>
     <row r="440" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>4127</v>
+        <v>3995</v>
       </c>
       <c r="B440" t="s">
-        <v>4145</v>
+        <v>4004</v>
       </c>
       <c r="C440" t="s">
         <v>3567</v>
@@ -60127,10 +60136,10 @@
     </row>
     <row r="441" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>3948</v>
+        <v>3993</v>
       </c>
       <c r="B441" t="s">
-        <v>4147</v>
+        <v>4002</v>
       </c>
       <c r="C441" t="s">
         <v>3567</v>
@@ -60138,10 +60147,10 @@
     </row>
     <row r="442" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>3960</v>
+        <v>3994</v>
       </c>
       <c r="B442" t="s">
-        <v>3972</v>
+        <v>4003</v>
       </c>
       <c r="C442" t="s">
         <v>3567</v>
@@ -60149,10 +60158,10 @@
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>3978</v>
+        <v>4128</v>
       </c>
       <c r="B443" t="s">
-        <v>3975</v>
+        <v>4146</v>
       </c>
       <c r="C443" t="s">
         <v>3567</v>
@@ -60160,10 +60169,10 @@
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>4152</v>
+        <v>4127</v>
       </c>
       <c r="B444" t="s">
-        <v>3450</v>
+        <v>4145</v>
       </c>
       <c r="C444" t="s">
         <v>3567</v>
@@ -60171,10 +60180,10 @@
     </row>
     <row r="445" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>4153</v>
+        <v>3948</v>
       </c>
       <c r="B445" t="s">
-        <v>4149</v>
+        <v>4147</v>
       </c>
       <c r="C445" t="s">
         <v>3567</v>
@@ -60182,10 +60191,10 @@
     </row>
     <row r="446" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>4154</v>
+        <v>3960</v>
       </c>
       <c r="B446" t="s">
-        <v>4150</v>
+        <v>3972</v>
       </c>
       <c r="C446" t="s">
         <v>3567</v>
@@ -60193,10 +60202,10 @@
     </row>
     <row r="447" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>4155</v>
+        <v>3978</v>
       </c>
       <c r="B447" t="s">
-        <v>4151</v>
+        <v>3975</v>
       </c>
       <c r="C447" t="s">
         <v>3567</v>
@@ -60204,10 +60213,10 @@
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>3641</v>
-      </c>
-      <c r="B448" s="3" t="s">
-        <v>3642</v>
+        <v>4152</v>
+      </c>
+      <c r="B448" t="s">
+        <v>3450</v>
       </c>
       <c r="C448" t="s">
         <v>3567</v>
@@ -60215,10 +60224,10 @@
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>3640</v>
-      </c>
-      <c r="B449" s="3" t="s">
-        <v>3638</v>
+        <v>4153</v>
+      </c>
+      <c r="B449" t="s">
+        <v>4149</v>
       </c>
       <c r="C449" t="s">
         <v>3567</v>
@@ -60226,10 +60235,10 @@
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>3639</v>
-      </c>
-      <c r="B450" s="3" t="s">
-        <v>3637</v>
+        <v>4154</v>
+      </c>
+      <c r="B450" t="s">
+        <v>4150</v>
       </c>
       <c r="C450" t="s">
         <v>3567</v>
@@ -60237,10 +60246,10 @@
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>3538</v>
+        <v>4155</v>
       </c>
       <c r="B451" t="s">
-        <v>3540</v>
+        <v>4151</v>
       </c>
       <c r="C451" t="s">
         <v>3567</v>
@@ -60248,10 +60257,10 @@
     </row>
     <row r="452" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>3951</v>
-      </c>
-      <c r="B452" t="s">
-        <v>3952</v>
+        <v>3641</v>
+      </c>
+      <c r="B452" s="3" t="s">
+        <v>3642</v>
       </c>
       <c r="C452" t="s">
         <v>3567</v>
@@ -60259,10 +60268,10 @@
     </row>
     <row r="453" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>4144</v>
-      </c>
-      <c r="B453" t="s">
-        <v>4143</v>
+        <v>3640</v>
+      </c>
+      <c r="B453" s="3" t="s">
+        <v>3638</v>
       </c>
       <c r="C453" t="s">
         <v>3567</v>
@@ -60270,10 +60279,10 @@
     </row>
     <row r="454" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>4007</v>
-      </c>
-      <c r="B454" t="s">
-        <v>4008</v>
+        <v>3639</v>
+      </c>
+      <c r="B454" s="3" t="s">
+        <v>3637</v>
       </c>
       <c r="C454" t="s">
         <v>3567</v>
@@ -60281,10 +60290,10 @@
     </row>
     <row r="455" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>4005</v>
+        <v>3538</v>
       </c>
       <c r="B455" t="s">
-        <v>4006</v>
+        <v>3540</v>
       </c>
       <c r="C455" t="s">
         <v>3567</v>
@@ -60292,10 +60301,10 @@
     </row>
     <row r="456" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>4156</v>
+        <v>3951</v>
       </c>
       <c r="B456" t="s">
-        <v>4157</v>
+        <v>3952</v>
       </c>
       <c r="C456" t="s">
         <v>3567</v>
@@ -60303,10 +60312,10 @@
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>14</v>
-      </c>
-      <c r="B457" s="3" t="s">
-        <v>163</v>
+        <v>4144</v>
+      </c>
+      <c r="B457" t="s">
+        <v>4143</v>
       </c>
       <c r="C457" t="s">
         <v>3567</v>
@@ -60314,54 +60323,54 @@
     </row>
     <row r="458" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>112</v>
+        <v>4007</v>
       </c>
       <c r="B458" t="s">
-        <v>194</v>
+        <v>4008</v>
       </c>
       <c r="C458" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
     </row>
     <row r="459" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>108</v>
+        <v>4005</v>
       </c>
       <c r="B459" t="s">
-        <v>198</v>
+        <v>4006</v>
       </c>
       <c r="C459" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>106</v>
+        <v>4156</v>
       </c>
       <c r="B460" t="s">
-        <v>196</v>
+        <v>4157</v>
       </c>
       <c r="C460" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
     </row>
     <row r="461" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>107</v>
-      </c>
-      <c r="B461" t="s">
-        <v>197</v>
+        <v>14</v>
+      </c>
+      <c r="B461" s="3" t="s">
+        <v>163</v>
       </c>
       <c r="C461" t="s">
-        <v>3568</v>
+        <v>3567</v>
       </c>
     </row>
     <row r="462" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B462" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="C462" t="s">
         <v>3568</v>
@@ -60369,10 +60378,10 @@
     </row>
     <row r="463" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>95</v>
+        <v>108</v>
       </c>
       <c r="B463" t="s">
-        <v>179</v>
+        <v>198</v>
       </c>
       <c r="C463" t="s">
         <v>3568</v>
@@ -60380,10 +60389,10 @@
     </row>
     <row r="464" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="B464" t="s">
-        <v>186</v>
+        <v>196</v>
       </c>
       <c r="C464" t="s">
         <v>3568</v>
@@ -60391,10 +60400,10 @@
     </row>
     <row r="465" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>96</v>
+        <v>107</v>
       </c>
       <c r="B465" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="C465" t="s">
         <v>3568</v>
@@ -60402,10 +60411,10 @@
     </row>
     <row r="466" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B466" t="s">
-        <v>181</v>
+        <v>199</v>
       </c>
       <c r="C466" t="s">
         <v>3568</v>
@@ -60413,10 +60422,10 @@
     </row>
     <row r="467" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B467" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="C467" t="s">
         <v>3568</v>
@@ -60424,10 +60433,10 @@
     </row>
     <row r="468" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="B468" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="C468" t="s">
         <v>3568</v>
@@ -60435,10 +60444,10 @@
     </row>
     <row r="469" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B469" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="C469" t="s">
         <v>3568</v>
@@ -60446,10 +60455,10 @@
     </row>
     <row r="470" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B470" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C470" t="s">
         <v>3568</v>
@@ -60457,10 +60466,10 @@
     </row>
     <row r="471" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>121</v>
+        <v>93</v>
       </c>
       <c r="B471" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="C471" t="s">
         <v>3568</v>
@@ -60468,10 +60477,10 @@
     </row>
     <row r="472" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>111</v>
+        <v>94</v>
       </c>
       <c r="B472" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="C472" t="s">
         <v>3568</v>
@@ -60479,10 +60488,10 @@
     </row>
     <row r="473" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B473" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C473" t="s">
         <v>3568</v>
@@ -60490,10 +60499,10 @@
     </row>
     <row r="474" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B474" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="C474" t="s">
         <v>3568</v>
@@ -60501,10 +60510,10 @@
     </row>
     <row r="475" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B475" t="s">
-        <v>3705</v>
+        <v>191</v>
       </c>
       <c r="C475" t="s">
         <v>3568</v>
@@ -60512,10 +60521,10 @@
     </row>
     <row r="476" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B476" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C476" t="s">
         <v>3568</v>
@@ -60523,10 +60532,10 @@
     </row>
     <row r="477" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B477" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="C477" t="s">
         <v>3568</v>
@@ -60534,10 +60543,10 @@
     </row>
     <row r="478" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>119</v>
+        <v>102</v>
       </c>
       <c r="B478" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C478" t="s">
         <v>3568</v>
@@ -60545,10 +60554,10 @@
     </row>
     <row r="479" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>104</v>
+        <v>122</v>
       </c>
       <c r="B479" t="s">
-        <v>188</v>
+        <v>3705</v>
       </c>
       <c r="C479" t="s">
         <v>3568</v>
@@ -60556,10 +60565,10 @@
     </row>
     <row r="480" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B480" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C480" t="s">
         <v>3568</v>
@@ -60567,10 +60576,10 @@
     </row>
     <row r="481" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>120</v>
+        <v>100</v>
       </c>
       <c r="B481" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C481" t="s">
         <v>3568</v>
@@ -60578,51 +60587,51 @@
     </row>
     <row r="482" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>4158</v>
+        <v>119</v>
       </c>
       <c r="B482" t="s">
-        <v>4159</v>
+        <v>190</v>
       </c>
       <c r="C482" t="s">
-        <v>3567</v>
+        <v>3568</v>
       </c>
     </row>
     <row r="483" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>4160</v>
+        <v>104</v>
       </c>
       <c r="B483" t="s">
-        <v>4161</v>
+        <v>188</v>
       </c>
       <c r="C483" t="s">
-        <v>3567</v>
+        <v>3568</v>
       </c>
     </row>
     <row r="484" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>4162</v>
+        <v>105</v>
       </c>
       <c r="B484" t="s">
-        <v>4163</v>
+        <v>189</v>
       </c>
       <c r="C484" t="s">
-        <v>3567</v>
+        <v>3568</v>
       </c>
     </row>
     <row r="485" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>4164</v>
+        <v>120</v>
       </c>
       <c r="B485" t="s">
-        <v>4165</v>
+        <v>195</v>
       </c>
       <c r="C485" t="s">
-        <v>3567</v>
+        <v>3568</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C387" xr:uid="{00000000-0009-0000-0000-000004000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C481">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C485">
       <sortCondition ref="C1:C387"/>
     </sortState>
   </autoFilter>
@@ -60638,9 +60647,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C435"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60826,14 +60835,47 @@
         <v>4110</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="15">
+        <v>4513</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>4166</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="15">
+        <v>5793</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>4168</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="15">
+        <v>5727</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>4167</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4099</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B30" s="4"/>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
       <c r="B31" s="4"/>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="16"/>
       <c r="B32" s="4"/>
     </row>

</xml_diff>

<commit_message>
Inclusão de melhorias @202406051435
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAA04F0F-8C17-4085-8873-DDBCC02BD776}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C1F350-4E15-4F16-A04D-333069524851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="3280" windowWidth="19420" windowHeight="10300" tabRatio="699" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19290" yWindow="3390" windowWidth="9780" windowHeight="10170" tabRatio="699" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="equity_signals" sheetId="19" r:id="rId1"/>
@@ -29,6 +29,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">equities!$A$1:$L$1268</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">equity_signals!$C$1:$C$79</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">macro!$A$1:$C$355</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">sgs!$A$1:$C$19</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11735" uniqueCount="4169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11780" uniqueCount="4199">
   <si>
     <t>bbgTicker</t>
   </si>
@@ -12558,6 +12559,96 @@
   </si>
   <si>
     <t>br_bcb_primary_result_12m_to_gdp</t>
+  </si>
+  <si>
+    <t>br_ipca_non_regulated_yoy</t>
+  </si>
+  <si>
+    <t>IPTNNRGT Index</t>
+  </si>
+  <si>
+    <t>IPTNRITW Index</t>
+  </si>
+  <si>
+    <t>br_ipca_regulated_yoy</t>
+  </si>
+  <si>
+    <t>IPTNSRVT Index</t>
+  </si>
+  <si>
+    <t>br_ipca_services_yoy</t>
+  </si>
+  <si>
+    <t>IPTNDURT Index</t>
+  </si>
+  <si>
+    <t>br_ipca_durable_yoy</t>
+  </si>
+  <si>
+    <t>br_ipca_semi_durable_yoy</t>
+  </si>
+  <si>
+    <t>IPTNSDUT Index</t>
+  </si>
+  <si>
+    <t>IPTNNDUT Index</t>
+  </si>
+  <si>
+    <t>br_ipca_non_durable_yoy</t>
+  </si>
+  <si>
+    <t>BRYAFDBV Index</t>
+  </si>
+  <si>
+    <t>BRYAHSIN Index</t>
+  </si>
+  <si>
+    <t>BRYAHITM Index</t>
+  </si>
+  <si>
+    <t>BRYACLTH Index</t>
+  </si>
+  <si>
+    <t>BRYATRPT Index</t>
+  </si>
+  <si>
+    <t>BRYAPERH Index</t>
+  </si>
+  <si>
+    <t>BRYAPERX Index</t>
+  </si>
+  <si>
+    <t>BRYAEDUC Index</t>
+  </si>
+  <si>
+    <t>BRYACOMN Index</t>
+  </si>
+  <si>
+    <t>br_ipca_food_beverages_yoy</t>
+  </si>
+  <si>
+    <t>br_ipca_housing_yoy</t>
+  </si>
+  <si>
+    <t>br_ipca_household_goods_yoy</t>
+  </si>
+  <si>
+    <t>br_ipca_clothing_yoy</t>
+  </si>
+  <si>
+    <t>br_ipca_transport_yoy</t>
+  </si>
+  <si>
+    <t>br_ipca_health_yoy</t>
+  </si>
+  <si>
+    <t>br_ipca_personal_expenses_yoy</t>
+  </si>
+  <si>
+    <t>br_ipca_education_yoy</t>
+  </si>
+  <si>
+    <t>br_ipca_communications_yoy</t>
   </si>
 </sst>
 </file>
@@ -55280,11 +55371,11 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Planilha9"/>
-  <dimension ref="A1:C485"/>
+  <dimension ref="A1:C500"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B198" sqref="B198"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57499,7 +57590,7 @@
         <v>3912</v>
       </c>
       <c r="B201" t="s">
-        <v>3914</v>
+        <v>3915</v>
       </c>
       <c r="C201" t="s">
         <v>3567</v>
@@ -57510,7 +57601,7 @@
         <v>3911</v>
       </c>
       <c r="B202" t="s">
-        <v>3915</v>
+        <v>3914</v>
       </c>
       <c r="C202" t="s">
         <v>3567</v>
@@ -60627,6 +60718,171 @@
       </c>
       <c r="C485" t="s">
         <v>3568</v>
+      </c>
+    </row>
+    <row r="486" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A486" t="s">
+        <v>4170</v>
+      </c>
+      <c r="B486" t="s">
+        <v>4169</v>
+      </c>
+      <c r="C486" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="487" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A487" t="s">
+        <v>4171</v>
+      </c>
+      <c r="B487" t="s">
+        <v>4172</v>
+      </c>
+      <c r="C487" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="488" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A488" t="s">
+        <v>4173</v>
+      </c>
+      <c r="B488" t="s">
+        <v>4174</v>
+      </c>
+      <c r="C488" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="489" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A489" t="s">
+        <v>4175</v>
+      </c>
+      <c r="B489" t="s">
+        <v>4176</v>
+      </c>
+      <c r="C489" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="490" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A490" t="s">
+        <v>4178</v>
+      </c>
+      <c r="B490" t="s">
+        <v>4177</v>
+      </c>
+      <c r="C490" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="491" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A491" t="s">
+        <v>4179</v>
+      </c>
+      <c r="B491" t="s">
+        <v>4180</v>
+      </c>
+      <c r="C491" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="492" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A492" t="s">
+        <v>4181</v>
+      </c>
+      <c r="B492" t="s">
+        <v>4190</v>
+      </c>
+      <c r="C492" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="493" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A493" t="s">
+        <v>4182</v>
+      </c>
+      <c r="B493" t="s">
+        <v>4191</v>
+      </c>
+      <c r="C493" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="494" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A494" t="s">
+        <v>4183</v>
+      </c>
+      <c r="B494" t="s">
+        <v>4192</v>
+      </c>
+      <c r="C494" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="495" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A495" t="s">
+        <v>4184</v>
+      </c>
+      <c r="B495" t="s">
+        <v>4193</v>
+      </c>
+      <c r="C495" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="496" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A496" t="s">
+        <v>4185</v>
+      </c>
+      <c r="B496" t="s">
+        <v>4194</v>
+      </c>
+      <c r="C496" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="497" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A497" t="s">
+        <v>4186</v>
+      </c>
+      <c r="B497" t="s">
+        <v>4195</v>
+      </c>
+      <c r="C497" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="498" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A498" t="s">
+        <v>4187</v>
+      </c>
+      <c r="B498" t="s">
+        <v>4196</v>
+      </c>
+      <c r="C498" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="499" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A499" t="s">
+        <v>4188</v>
+      </c>
+      <c r="B499" t="s">
+        <v>4197</v>
+      </c>
+      <c r="C499" t="s">
+        <v>3567</v>
+      </c>
+    </row>
+    <row r="500" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A500" t="s">
+        <v>4189</v>
+      </c>
+      <c r="B500" t="s">
+        <v>4198</v>
+      </c>
+      <c r="C500" t="s">
+        <v>3567</v>
       </c>
     </row>
   </sheetData>
@@ -60647,9 +60903,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C435"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60672,175 +60928,175 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
-        <v>28784</v>
+        <v>1376</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4091</v>
+        <v>4104</v>
       </c>
       <c r="C2" t="s">
-        <v>4090</v>
+        <v>4108</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="15">
-        <v>25359</v>
+        <v>1374</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4092</v>
+        <v>4102</v>
       </c>
       <c r="C3" t="s">
-        <v>4096</v>
+        <v>4108</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
-        <v>20716</v>
+        <v>1375</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>4093</v>
+        <v>4103</v>
       </c>
       <c r="C4" t="s">
-        <v>4096</v>
+        <v>4108</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
-        <v>20715</v>
+        <v>1373</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>4094</v>
+        <v>4101</v>
       </c>
       <c r="C5" t="s">
-        <v>4096</v>
+        <v>4108</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
-        <v>20714</v>
+        <v>1379</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>4095</v>
+        <v>4107</v>
       </c>
       <c r="C6" t="s">
-        <v>4096</v>
+        <v>4108</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="15">
-        <v>13762</v>
+        <v>1380</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>4097</v>
+        <v>4106</v>
       </c>
       <c r="C7" t="s">
-        <v>4099</v>
+        <v>4108</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="15">
-        <v>4536</v>
+        <v>1378</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>4098</v>
+        <v>4105</v>
       </c>
       <c r="C8" t="s">
-        <v>4099</v>
+        <v>4108</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="15">
-        <v>1373</v>
+        <v>20716</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>4101</v>
+        <v>4093</v>
       </c>
       <c r="C9" t="s">
-        <v>4108</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="15">
-        <v>1374</v>
+        <v>20715</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>4102</v>
+        <v>4094</v>
       </c>
       <c r="C10" t="s">
-        <v>4108</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="15">
-        <v>1375</v>
+        <v>20714</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>4103</v>
+        <v>4095</v>
       </c>
       <c r="C11" t="s">
-        <v>4108</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
-        <v>1376</v>
+        <v>25359</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>4104</v>
+        <v>4092</v>
       </c>
       <c r="C12" t="s">
-        <v>4108</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
-        <v>1378</v>
+        <v>13762</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>4105</v>
+        <v>4097</v>
       </c>
       <c r="C13" t="s">
-        <v>4108</v>
+        <v>4099</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
-        <v>1379</v>
+        <v>4536</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>4107</v>
+        <v>4098</v>
       </c>
       <c r="C14" t="s">
-        <v>4108</v>
+        <v>4099</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
-        <v>1380</v>
+        <v>4513</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>4106</v>
+        <v>4166</v>
       </c>
       <c r="C15" t="s">
-        <v>4108</v>
+        <v>4099</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
-        <v>13521</v>
+        <v>5727</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>4109</v>
+        <v>4167</v>
       </c>
       <c r="C16" t="s">
-        <v>4110</v>
+        <v>4099</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
-        <v>4513</v>
+        <v>5793</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>4166</v>
+        <v>4168</v>
       </c>
       <c r="C17" t="s">
         <v>4099</v>
@@ -60848,24 +61104,24 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
-        <v>5793</v>
+        <v>13521</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>4168</v>
+        <v>4109</v>
       </c>
       <c r="C18" t="s">
-        <v>4099</v>
+        <v>4110</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
-        <v>5727</v>
+        <v>28784</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>4167</v>
+        <v>4091</v>
       </c>
       <c r="C19" t="s">
-        <v>4099</v>
+        <v>4090</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -61038,6 +61294,11 @@
       <c r="B435" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C19" xr:uid="{00000000-0001-0000-0500-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C19">
+      <sortCondition ref="C1:C19"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Inclusão de melhorias @202406051509
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75C1F350-4E15-4F16-A04D-333069524851}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDA43844-7F3A-4E2A-8058-1B594BB2BBD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19290" yWindow="3390" windowWidth="9780" windowHeight="10170" tabRatio="699" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19290" yWindow="3390" windowWidth="9780" windowHeight="10170" tabRatio="699" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="equity_signals" sheetId="19" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11780" uniqueCount="4199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11802" uniqueCount="4210">
   <si>
     <t>bbgTicker</t>
   </si>
@@ -12333,12 +12333,6 @@
     <t>br_bcb_icc_earmarked_individuals</t>
   </si>
   <si>
-    <t>br_bcb_average_interest_rate_individuals</t>
-  </si>
-  <si>
-    <t>br_bcb_average_interest_rate_nonfinancial</t>
-  </si>
-  <si>
     <t>br_bcb_average_interest_rate_total</t>
   </si>
   <si>
@@ -12649,6 +12643,45 @@
   </si>
   <si>
     <t>br_ipca_communications_yoy</t>
+  </si>
+  <si>
+    <t>br_bcb_credit_outstanding_pj</t>
+  </si>
+  <si>
+    <t>br_bcb_credit_outstanding_pf</t>
+  </si>
+  <si>
+    <t>br_bcb_average_interest_rate_pf</t>
+  </si>
+  <si>
+    <t>br_bcb_average_interest_rate_pj</t>
+  </si>
+  <si>
+    <t>br_bcb_nonearmarked_credit_outstanding_pj</t>
+  </si>
+  <si>
+    <t>br_bcb_earmarked_credit_outstanding_pj</t>
+  </si>
+  <si>
+    <t>br_bcb_nonearmarked_credit_outstanding_pf</t>
+  </si>
+  <si>
+    <t>br_bcb_earmarked_credit_outstanding_pf</t>
+  </si>
+  <si>
+    <t>br_bcb_credit_outstanding_msme</t>
+  </si>
+  <si>
+    <t>br_bcb_credit_outstanding_corporate</t>
+  </si>
+  <si>
+    <t>br_bcb_credit_outstanding_total</t>
+  </si>
+  <si>
+    <t>br_bcb_past_due_loans_pf</t>
+  </si>
+  <si>
+    <t>br_bcb_past_due_loans_pj</t>
   </si>
 </sst>
 </file>
@@ -55373,9 +55406,9 @@
   <sheetPr codeName="Planilha9"/>
   <dimension ref="A1:C500"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B198" sqref="B198"/>
+      <selection pane="bottomLeft" activeCell="B202" sqref="B202"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56652,10 +56685,10 @@
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>4125</v>
+        <v>4123</v>
       </c>
       <c r="B116" t="s">
-        <v>4126</v>
+        <v>4124</v>
       </c>
       <c r="C116" t="s">
         <v>3566</v>
@@ -57664,10 +57697,10 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>4158</v>
+        <v>4156</v>
       </c>
       <c r="B208" t="s">
-        <v>4159</v>
+        <v>4157</v>
       </c>
       <c r="C208" t="s">
         <v>3567</v>
@@ -57675,10 +57708,10 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>4162</v>
+        <v>4160</v>
       </c>
       <c r="B209" t="s">
-        <v>4163</v>
+        <v>4161</v>
       </c>
       <c r="C209" t="s">
         <v>3567</v>
@@ -57686,10 +57719,10 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>4164</v>
+        <v>4162</v>
       </c>
       <c r="B210" t="s">
-        <v>4165</v>
+        <v>4163</v>
       </c>
       <c r="C210" t="s">
         <v>3567</v>
@@ -57697,10 +57730,10 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>4160</v>
+        <v>4158</v>
       </c>
       <c r="B211" t="s">
-        <v>4161</v>
+        <v>4159</v>
       </c>
       <c r="C211" t="s">
         <v>3567</v>
@@ -58632,10 +58665,10 @@
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
-        <v>4112</v>
+        <v>4110</v>
       </c>
       <c r="B296" t="s">
-        <v>4111</v>
+        <v>4109</v>
       </c>
       <c r="C296" t="s">
         <v>3567</v>
@@ -58643,10 +58676,10 @@
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
-        <v>4113</v>
+        <v>4111</v>
       </c>
       <c r="B297" t="s">
-        <v>4114</v>
+        <v>4112</v>
       </c>
       <c r="C297" t="s">
         <v>3567</v>
@@ -58687,10 +58720,10 @@
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
-        <v>4117</v>
+        <v>4115</v>
       </c>
       <c r="B301" t="s">
-        <v>4115</v>
+        <v>4113</v>
       </c>
       <c r="C301" t="s">
         <v>3567</v>
@@ -58698,10 +58731,10 @@
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
-        <v>4118</v>
+        <v>4116</v>
       </c>
       <c r="B302" t="s">
-        <v>4116</v>
+        <v>4114</v>
       </c>
       <c r="C302" t="s">
         <v>3567</v>
@@ -58709,10 +58742,10 @@
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
-        <v>4124</v>
+        <v>4122</v>
       </c>
       <c r="B303" t="s">
-        <v>4119</v>
+        <v>4117</v>
       </c>
       <c r="C303" t="s">
         <v>3567</v>
@@ -58720,10 +58753,10 @@
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
-        <v>4120</v>
+        <v>4118</v>
       </c>
       <c r="B304" t="s">
-        <v>4121</v>
+        <v>4119</v>
       </c>
       <c r="C304" t="s">
         <v>3567</v>
@@ -58731,10 +58764,10 @@
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
-        <v>4122</v>
+        <v>4120</v>
       </c>
       <c r="B305" t="s">
-        <v>4123</v>
+        <v>4121</v>
       </c>
       <c r="C305" t="s">
         <v>3567</v>
@@ -59435,10 +59468,10 @@
     </row>
     <row r="369" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
-        <v>4130</v>
+        <v>4128</v>
       </c>
       <c r="B369" t="s">
-        <v>4129</v>
+        <v>4127</v>
       </c>
       <c r="C369" t="s">
         <v>3567</v>
@@ -59446,10 +59479,10 @@
     </row>
     <row r="370" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
+        <v>4129</v>
+      </c>
+      <c r="B370" t="s">
         <v>4131</v>
-      </c>
-      <c r="B370" t="s">
-        <v>4133</v>
       </c>
       <c r="C370" t="s">
         <v>3567</v>
@@ -59457,10 +59490,10 @@
     </row>
     <row r="371" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
+        <v>4130</v>
+      </c>
+      <c r="B371" t="s">
         <v>4132</v>
-      </c>
-      <c r="B371" t="s">
-        <v>4134</v>
       </c>
       <c r="C371" t="s">
         <v>3567</v>
@@ -59468,10 +59501,10 @@
     </row>
     <row r="372" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
-        <v>4135</v>
+        <v>4133</v>
       </c>
       <c r="B372" t="s">
-        <v>4136</v>
+        <v>4134</v>
       </c>
       <c r="C372" t="s">
         <v>3567</v>
@@ -59479,10 +59512,10 @@
     </row>
     <row r="373" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
-        <v>4140</v>
+        <v>4138</v>
       </c>
       <c r="B373" t="s">
-        <v>4139</v>
+        <v>4137</v>
       </c>
       <c r="C373" t="s">
         <v>3567</v>
@@ -59490,10 +59523,10 @@
     </row>
     <row r="374" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
-        <v>4137</v>
+        <v>4135</v>
       </c>
       <c r="B374" t="s">
-        <v>4138</v>
+        <v>4136</v>
       </c>
       <c r="C374" t="s">
         <v>3567</v>
@@ -59501,10 +59534,10 @@
     </row>
     <row r="375" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
-        <v>4142</v>
+        <v>4140</v>
       </c>
       <c r="B375" t="s">
-        <v>4141</v>
+        <v>4139</v>
       </c>
       <c r="C375" t="s">
         <v>3567</v>
@@ -59724,7 +59757,7 @@
         <v>3449</v>
       </c>
       <c r="B395" t="s">
-        <v>4148</v>
+        <v>4146</v>
       </c>
       <c r="C395" t="s">
         <v>3567</v>
@@ -60249,10 +60282,10 @@
     </row>
     <row r="443" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>4128</v>
+        <v>4126</v>
       </c>
       <c r="B443" t="s">
-        <v>4146</v>
+        <v>4144</v>
       </c>
       <c r="C443" t="s">
         <v>3567</v>
@@ -60260,10 +60293,10 @@
     </row>
     <row r="444" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>4127</v>
+        <v>4125</v>
       </c>
       <c r="B444" t="s">
-        <v>4145</v>
+        <v>4143</v>
       </c>
       <c r="C444" t="s">
         <v>3567</v>
@@ -60274,7 +60307,7 @@
         <v>3948</v>
       </c>
       <c r="B445" t="s">
-        <v>4147</v>
+        <v>4145</v>
       </c>
       <c r="C445" t="s">
         <v>3567</v>
@@ -60304,7 +60337,7 @@
     </row>
     <row r="448" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>4152</v>
+        <v>4150</v>
       </c>
       <c r="B448" t="s">
         <v>3450</v>
@@ -60315,10 +60348,10 @@
     </row>
     <row r="449" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>4153</v>
+        <v>4151</v>
       </c>
       <c r="B449" t="s">
-        <v>4149</v>
+        <v>4147</v>
       </c>
       <c r="C449" t="s">
         <v>3567</v>
@@ -60326,10 +60359,10 @@
     </row>
     <row r="450" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>4154</v>
+        <v>4152</v>
       </c>
       <c r="B450" t="s">
-        <v>4150</v>
+        <v>4148</v>
       </c>
       <c r="C450" t="s">
         <v>3567</v>
@@ -60337,10 +60370,10 @@
     </row>
     <row r="451" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>4155</v>
+        <v>4153</v>
       </c>
       <c r="B451" t="s">
-        <v>4151</v>
+        <v>4149</v>
       </c>
       <c r="C451" t="s">
         <v>3567</v>
@@ -60403,10 +60436,10 @@
     </row>
     <row r="457" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>4144</v>
+        <v>4142</v>
       </c>
       <c r="B457" t="s">
-        <v>4143</v>
+        <v>4141</v>
       </c>
       <c r="C457" t="s">
         <v>3567</v>
@@ -60436,10 +60469,10 @@
     </row>
     <row r="460" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>4156</v>
+        <v>4154</v>
       </c>
       <c r="B460" t="s">
-        <v>4157</v>
+        <v>4155</v>
       </c>
       <c r="C460" t="s">
         <v>3567</v>
@@ -60722,10 +60755,10 @@
     </row>
     <row r="486" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>4170</v>
+        <v>4168</v>
       </c>
       <c r="B486" t="s">
-        <v>4169</v>
+        <v>4167</v>
       </c>
       <c r="C486" t="s">
         <v>3567</v>
@@ -60733,10 +60766,10 @@
     </row>
     <row r="487" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>4171</v>
+        <v>4169</v>
       </c>
       <c r="B487" t="s">
-        <v>4172</v>
+        <v>4170</v>
       </c>
       <c r="C487" t="s">
         <v>3567</v>
@@ -60744,10 +60777,10 @@
     </row>
     <row r="488" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>4173</v>
+        <v>4171</v>
       </c>
       <c r="B488" t="s">
-        <v>4174</v>
+        <v>4172</v>
       </c>
       <c r="C488" t="s">
         <v>3567</v>
@@ -60755,10 +60788,10 @@
     </row>
     <row r="489" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>4175</v>
+        <v>4173</v>
       </c>
       <c r="B489" t="s">
-        <v>4176</v>
+        <v>4174</v>
       </c>
       <c r="C489" t="s">
         <v>3567</v>
@@ -60766,10 +60799,10 @@
     </row>
     <row r="490" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>4178</v>
+        <v>4176</v>
       </c>
       <c r="B490" t="s">
-        <v>4177</v>
+        <v>4175</v>
       </c>
       <c r="C490" t="s">
         <v>3567</v>
@@ -60777,10 +60810,10 @@
     </row>
     <row r="491" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>4179</v>
+        <v>4177</v>
       </c>
       <c r="B491" t="s">
-        <v>4180</v>
+        <v>4178</v>
       </c>
       <c r="C491" t="s">
         <v>3567</v>
@@ -60788,10 +60821,10 @@
     </row>
     <row r="492" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>4181</v>
+        <v>4179</v>
       </c>
       <c r="B492" t="s">
-        <v>4190</v>
+        <v>4188</v>
       </c>
       <c r="C492" t="s">
         <v>3567</v>
@@ -60799,10 +60832,10 @@
     </row>
     <row r="493" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>4182</v>
+        <v>4180</v>
       </c>
       <c r="B493" t="s">
-        <v>4191</v>
+        <v>4189</v>
       </c>
       <c r="C493" t="s">
         <v>3567</v>
@@ -60810,10 +60843,10 @@
     </row>
     <row r="494" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>4183</v>
+        <v>4181</v>
       </c>
       <c r="B494" t="s">
-        <v>4192</v>
+        <v>4190</v>
       </c>
       <c r="C494" t="s">
         <v>3567</v>
@@ -60821,10 +60854,10 @@
     </row>
     <row r="495" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>4184</v>
+        <v>4182</v>
       </c>
       <c r="B495" t="s">
-        <v>4193</v>
+        <v>4191</v>
       </c>
       <c r="C495" t="s">
         <v>3567</v>
@@ -60832,10 +60865,10 @@
     </row>
     <row r="496" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>4185</v>
+        <v>4183</v>
       </c>
       <c r="B496" t="s">
-        <v>4194</v>
+        <v>4192</v>
       </c>
       <c r="C496" t="s">
         <v>3567</v>
@@ -60843,10 +60876,10 @@
     </row>
     <row r="497" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>4186</v>
+        <v>4184</v>
       </c>
       <c r="B497" t="s">
-        <v>4195</v>
+        <v>4193</v>
       </c>
       <c r="C497" t="s">
         <v>3567</v>
@@ -60854,10 +60887,10 @@
     </row>
     <row r="498" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>4187</v>
+        <v>4185</v>
       </c>
       <c r="B498" t="s">
-        <v>4196</v>
+        <v>4194</v>
       </c>
       <c r="C498" t="s">
         <v>3567</v>
@@ -60865,10 +60898,10 @@
     </row>
     <row r="499" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>4188</v>
+        <v>4186</v>
       </c>
       <c r="B499" t="s">
-        <v>4197</v>
+        <v>4195</v>
       </c>
       <c r="C499" t="s">
         <v>3567</v>
@@ -60876,10 +60909,10 @@
     </row>
     <row r="500" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>4189</v>
+        <v>4187</v>
       </c>
       <c r="B500" t="s">
-        <v>4198</v>
+        <v>4196</v>
       </c>
       <c r="C500" t="s">
         <v>3567</v>
@@ -60903,9 +60936,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C435"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60917,7 +60950,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
-        <v>4100</v>
+        <v>4098</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>3368</v>
@@ -60931,10 +60964,10 @@
         <v>1376</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4104</v>
+        <v>4102</v>
       </c>
       <c r="C2" t="s">
-        <v>4108</v>
+        <v>4106</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -60942,10 +60975,10 @@
         <v>1374</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>4102</v>
+        <v>4100</v>
       </c>
       <c r="C3" t="s">
-        <v>4108</v>
+        <v>4106</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -60953,10 +60986,10 @@
         <v>1375</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>4103</v>
+        <v>4101</v>
       </c>
       <c r="C4" t="s">
-        <v>4108</v>
+        <v>4106</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -60964,10 +60997,10 @@
         <v>1373</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>4101</v>
+        <v>4099</v>
       </c>
       <c r="C5" t="s">
-        <v>4108</v>
+        <v>4106</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -60975,10 +61008,10 @@
         <v>1379</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>4107</v>
+        <v>4105</v>
       </c>
       <c r="C6" t="s">
-        <v>4108</v>
+        <v>4106</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -60986,10 +61019,10 @@
         <v>1380</v>
       </c>
       <c r="B7" s="4" t="s">
+        <v>4104</v>
+      </c>
+      <c r="C7" t="s">
         <v>4106</v>
-      </c>
-      <c r="C7" t="s">
-        <v>4108</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -60997,10 +61030,10 @@
         <v>1378</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>4105</v>
+        <v>4103</v>
       </c>
       <c r="C8" t="s">
-        <v>4108</v>
+        <v>4106</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -61008,10 +61041,10 @@
         <v>20716</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>4093</v>
+        <v>4199</v>
       </c>
       <c r="C9" t="s">
-        <v>4096</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -61019,10 +61052,10 @@
         <v>20715</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>4200</v>
+      </c>
+      <c r="C10" t="s">
         <v>4094</v>
-      </c>
-      <c r="C10" t="s">
-        <v>4096</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -61030,102 +61063,220 @@
         <v>20714</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>4095</v>
+        <v>4093</v>
       </c>
       <c r="C11" t="s">
-        <v>4096</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="15">
-        <v>25359</v>
+        <v>27702</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>4092</v>
+        <v>4206</v>
       </c>
       <c r="C12" t="s">
-        <v>4096</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="15">
-        <v>13762</v>
+        <v>27701</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>4097</v>
+        <v>4205</v>
       </c>
       <c r="C13" t="s">
-        <v>4099</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="15">
-        <v>4536</v>
+        <v>20541</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>4098</v>
+        <v>4198</v>
       </c>
       <c r="C14" t="s">
-        <v>4099</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="15">
-        <v>4513</v>
+        <v>20540</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>4166</v>
+        <v>4197</v>
       </c>
       <c r="C15" t="s">
-        <v>4099</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="15">
-        <v>5727</v>
+        <v>20540</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>4167</v>
+        <v>4207</v>
       </c>
       <c r="C16" t="s">
-        <v>4099</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="15">
-        <v>5793</v>
+        <v>20606</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>4168</v>
+        <v>4204</v>
       </c>
       <c r="C17" t="s">
-        <v>4099</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="15">
-        <v>13521</v>
+        <v>20594</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>4109</v>
+        <v>4202</v>
       </c>
       <c r="C18" t="s">
-        <v>4110</v>
+        <v>4094</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="15">
+        <v>25359</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>4092</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4094</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="15">
+        <v>20570</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>4203</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4094</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="15">
+        <v>20543</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>4201</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4094</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="15">
+        <v>21084</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>4208</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4094</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="15">
+        <v>21083</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>4209</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4094</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="15">
+        <v>13762</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>4095</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4097</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
+        <v>4536</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>4096</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4097</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
+        <v>4513</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>4164</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4097</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
+        <v>5727</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>4165</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4097</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="15">
+        <v>5793</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>4166</v>
+      </c>
+      <c r="C28" t="s">
+        <v>4097</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="15">
+        <v>13521</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>4107</v>
+      </c>
+      <c r="C29" t="s">
+        <v>4108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="15">
         <v>28784</v>
       </c>
-      <c r="B19" s="4" t="s">
+      <c r="B30" s="4" t="s">
         <v>4091</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C30" t="s">
         <v>4090</v>
       </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B30" s="4"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="16"/>
@@ -61295,7 +61446,7 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:C19" xr:uid="{00000000-0001-0000-0500-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C19">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C30">
       <sortCondition ref="C1:C19"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
Inclusão de melhorias @202406071543
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1407B623-17C3-4C1F-B4CD-95D33174D6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E92C30E7-E33D-4960-8799-785E398890F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="3280" windowWidth="19420" windowHeight="10300" tabRatio="699" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3870" yWindow="3450" windowWidth="19155" windowHeight="10065" tabRatio="699" firstSheet="2" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="equity_signals" sheetId="19" r:id="rId1"/>
@@ -54761,8 +54761,8 @@
   <dimension ref="A1:D553"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A454" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L458" sqref="L458"/>
+      <pane ySplit="1" topLeftCell="A511" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G520" sqref="G520"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61857,266 +61857,266 @@
       </c>
     </row>
     <row r="507" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A507" s="15" t="s">
+      <c r="A507" t="s">
+        <v>4242</v>
+      </c>
+      <c r="B507" t="s">
+        <v>4232</v>
+      </c>
+      <c r="C507" t="s">
+        <v>3566</v>
+      </c>
+      <c r="D507" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="508" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A508" t="s">
+        <v>4243</v>
+      </c>
+      <c r="B508" t="s">
+        <v>4233</v>
+      </c>
+      <c r="C508" t="s">
+        <v>3566</v>
+      </c>
+      <c r="D508" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="509" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A509" t="s">
+        <v>4244</v>
+      </c>
+      <c r="B509" t="s">
+        <v>4234</v>
+      </c>
+      <c r="C509" t="s">
+        <v>3566</v>
+      </c>
+      <c r="D509" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="510" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A510" t="s">
+        <v>4245</v>
+      </c>
+      <c r="B510" t="s">
+        <v>4235</v>
+      </c>
+      <c r="C510" t="s">
+        <v>3566</v>
+      </c>
+      <c r="D510" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="511" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A511" t="s">
+        <v>4246</v>
+      </c>
+      <c r="B511" t="s">
+        <v>4236</v>
+      </c>
+      <c r="C511" t="s">
+        <v>3566</v>
+      </c>
+      <c r="D511" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="512" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A512" t="s">
+        <v>4247</v>
+      </c>
+      <c r="B512" t="s">
+        <v>4237</v>
+      </c>
+      <c r="C512" t="s">
+        <v>3566</v>
+      </c>
+      <c r="D512" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="513" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A513" t="s">
+        <v>4248</v>
+      </c>
+      <c r="B513" t="s">
+        <v>4238</v>
+      </c>
+      <c r="C513" t="s">
+        <v>3566</v>
+      </c>
+      <c r="D513" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="514" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A514" t="s">
+        <v>4249</v>
+      </c>
+      <c r="B514" t="s">
+        <v>4239</v>
+      </c>
+      <c r="C514" t="s">
+        <v>3566</v>
+      </c>
+      <c r="D514" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="515" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A515" t="s">
+        <v>4250</v>
+      </c>
+      <c r="B515" t="s">
+        <v>4240</v>
+      </c>
+      <c r="C515" t="s">
+        <v>3566</v>
+      </c>
+      <c r="D515" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="516" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A516" t="s">
+        <v>4251</v>
+      </c>
+      <c r="B516" t="s">
+        <v>4241</v>
+      </c>
+      <c r="C516" t="s">
+        <v>3566</v>
+      </c>
+      <c r="D516" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="517" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A517" t="s">
+        <v>4257</v>
+      </c>
+      <c r="B517" t="s">
+        <v>4258</v>
+      </c>
+      <c r="C517" t="s">
+        <v>3566</v>
+      </c>
+      <c r="D517" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="518" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A518" t="s">
+        <v>4259</v>
+      </c>
+      <c r="B518" t="s">
+        <v>4260</v>
+      </c>
+      <c r="C518" t="s">
+        <v>3567</v>
+      </c>
+      <c r="D518" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="519" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A519" t="s">
+        <v>4261</v>
+      </c>
+      <c r="B519" t="s">
+        <v>4264</v>
+      </c>
+      <c r="C519" t="s">
+        <v>3567</v>
+      </c>
+      <c r="D519" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="520" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A520" t="s">
+        <v>4262</v>
+      </c>
+      <c r="B520" t="s">
+        <v>4263</v>
+      </c>
+      <c r="C520" t="s">
+        <v>3567</v>
+      </c>
+      <c r="D520" t="s">
+        <v>4216</v>
+      </c>
+    </row>
+    <row r="521" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A521" s="15" t="s">
         <v>4213</v>
       </c>
-      <c r="B507" s="4" t="s">
+      <c r="B521" s="4" t="s">
         <v>4214</v>
       </c>
-      <c r="C507" t="s">
+      <c r="C521" t="s">
         <v>4097</v>
       </c>
-      <c r="D507" t="s">
+      <c r="D521" t="s">
         <v>4217</v>
       </c>
     </row>
-    <row r="508" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A508" s="15" t="s">
+    <row r="522" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A522" s="15" t="s">
         <v>4211</v>
       </c>
-      <c r="B508" s="4" t="s">
+      <c r="B522" s="4" t="s">
         <v>4212</v>
       </c>
-      <c r="C508" t="s">
+      <c r="C522" t="s">
         <v>4090</v>
       </c>
-      <c r="D508" t="s">
+      <c r="D522" t="s">
         <v>4217</v>
       </c>
     </row>
-    <row r="509" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A509" s="15">
-        <v>1376</v>
-      </c>
-      <c r="B509" s="4" t="s">
-        <v>4102</v>
-      </c>
-      <c r="C509" t="s">
-        <v>4106</v>
-      </c>
-      <c r="D509" t="s">
-        <v>4219</v>
-      </c>
-    </row>
-    <row r="510" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A510" s="15">
-        <v>1374</v>
-      </c>
-      <c r="B510" s="4" t="s">
-        <v>4100</v>
-      </c>
-      <c r="C510" t="s">
-        <v>4106</v>
-      </c>
-      <c r="D510" t="s">
-        <v>4219</v>
-      </c>
-    </row>
-    <row r="511" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A511" s="15">
-        <v>1375</v>
-      </c>
-      <c r="B511" s="4" t="s">
-        <v>4101</v>
-      </c>
-      <c r="C511" t="s">
-        <v>4106</v>
-      </c>
-      <c r="D511" t="s">
-        <v>4219</v>
-      </c>
-    </row>
-    <row r="512" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A512" s="15">
-        <v>1373</v>
-      </c>
-      <c r="B512" s="4" t="s">
-        <v>4099</v>
-      </c>
-      <c r="C512" t="s">
-        <v>4106</v>
-      </c>
-      <c r="D512" t="s">
-        <v>4219</v>
-      </c>
-    </row>
-    <row r="513" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A513" s="15">
-        <v>1379</v>
-      </c>
-      <c r="B513" s="4" t="s">
-        <v>4105</v>
-      </c>
-      <c r="C513" t="s">
-        <v>4106</v>
-      </c>
-      <c r="D513" t="s">
-        <v>4219</v>
-      </c>
-    </row>
-    <row r="514" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A514" s="15">
-        <v>1380</v>
-      </c>
-      <c r="B514" s="4" t="s">
-        <v>4104</v>
-      </c>
-      <c r="C514" t="s">
-        <v>4106</v>
-      </c>
-      <c r="D514" t="s">
-        <v>4219</v>
-      </c>
-    </row>
-    <row r="515" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A515" s="15">
-        <v>1378</v>
-      </c>
-      <c r="B515" s="4" t="s">
-        <v>4103</v>
-      </c>
-      <c r="C515" t="s">
-        <v>4106</v>
-      </c>
-      <c r="D515" t="s">
-        <v>4219</v>
-      </c>
-    </row>
-    <row r="516" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A516" s="15">
-        <v>20716</v>
-      </c>
-      <c r="B516" s="4" t="s">
-        <v>4199</v>
-      </c>
-      <c r="C516" t="s">
-        <v>4094</v>
-      </c>
-      <c r="D516" t="s">
-        <v>4219</v>
-      </c>
-    </row>
-    <row r="517" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A517" s="15">
-        <v>20715</v>
-      </c>
-      <c r="B517" s="4" t="s">
-        <v>4200</v>
-      </c>
-      <c r="C517" t="s">
-        <v>4094</v>
-      </c>
-      <c r="D517" t="s">
-        <v>4219</v>
-      </c>
-    </row>
-    <row r="518" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A518" s="15">
-        <v>20714</v>
-      </c>
-      <c r="B518" s="4" t="s">
-        <v>4093</v>
-      </c>
-      <c r="C518" t="s">
-        <v>4094</v>
-      </c>
-      <c r="D518" t="s">
-        <v>4219</v>
-      </c>
-    </row>
-    <row r="519" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A519" s="15">
-        <v>27702</v>
-      </c>
-      <c r="B519" s="4" t="s">
-        <v>4206</v>
-      </c>
-      <c r="C519" t="s">
-        <v>4094</v>
-      </c>
-      <c r="D519" t="s">
-        <v>4219</v>
-      </c>
-    </row>
-    <row r="520" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A520" s="15">
-        <v>27701</v>
-      </c>
-      <c r="B520" s="4" t="s">
-        <v>4205</v>
-      </c>
-      <c r="C520" t="s">
-        <v>4094</v>
-      </c>
-      <c r="D520" t="s">
-        <v>4219</v>
-      </c>
-    </row>
-    <row r="521" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A521" s="15">
-        <v>20541</v>
-      </c>
-      <c r="B521" s="4" t="s">
-        <v>4198</v>
-      </c>
-      <c r="C521" t="s">
-        <v>4094</v>
-      </c>
-      <c r="D521" t="s">
-        <v>4219</v>
-      </c>
-    </row>
-    <row r="522" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A522" s="15">
-        <v>20540</v>
-      </c>
-      <c r="B522" s="4" t="s">
-        <v>4197</v>
-      </c>
-      <c r="C522" t="s">
-        <v>4094</v>
-      </c>
-      <c r="D522" t="s">
-        <v>4219</v>
-      </c>
-    </row>
     <row r="523" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A523" s="15">
-        <v>20540</v>
-      </c>
-      <c r="B523" s="4" t="s">
-        <v>4207</v>
+      <c r="A523" t="s">
+        <v>4265</v>
+      </c>
+      <c r="B523" t="s">
+        <v>4266</v>
       </c>
       <c r="C523" t="s">
-        <v>4094</v>
+        <v>4090</v>
       </c>
       <c r="D523" t="s">
-        <v>4219</v>
+        <v>4217</v>
       </c>
     </row>
     <row r="524" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A524" s="15">
-        <v>20606</v>
-      </c>
-      <c r="B524" s="4" t="s">
-        <v>4204</v>
+      <c r="A524" t="s">
+        <v>4268</v>
+      </c>
+      <c r="B524" t="s">
+        <v>4267</v>
       </c>
       <c r="C524" t="s">
-        <v>4094</v>
+        <v>4090</v>
       </c>
       <c r="D524" t="s">
-        <v>4219</v>
+        <v>4217</v>
       </c>
     </row>
     <row r="525" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A525" s="15">
-        <v>20594</v>
+        <v>1376</v>
       </c>
       <c r="B525" s="4" t="s">
-        <v>4202</v>
+        <v>4102</v>
       </c>
       <c r="C525" t="s">
-        <v>4094</v>
+        <v>4106</v>
       </c>
       <c r="D525" t="s">
         <v>4219</v>
@@ -62124,13 +62124,13 @@
     </row>
     <row r="526" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A526" s="15">
-        <v>25359</v>
+        <v>1374</v>
       </c>
       <c r="B526" s="4" t="s">
-        <v>4092</v>
+        <v>4100</v>
       </c>
       <c r="C526" t="s">
-        <v>4094</v>
+        <v>4106</v>
       </c>
       <c r="D526" t="s">
         <v>4219</v>
@@ -62138,13 +62138,13 @@
     </row>
     <row r="527" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A527" s="15">
-        <v>20570</v>
+        <v>1375</v>
       </c>
       <c r="B527" s="4" t="s">
-        <v>4203</v>
+        <v>4101</v>
       </c>
       <c r="C527" t="s">
-        <v>4094</v>
+        <v>4106</v>
       </c>
       <c r="D527" t="s">
         <v>4219</v>
@@ -62152,13 +62152,13 @@
     </row>
     <row r="528" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A528" s="15">
-        <v>20543</v>
+        <v>1373</v>
       </c>
       <c r="B528" s="4" t="s">
-        <v>4201</v>
+        <v>4099</v>
       </c>
       <c r="C528" t="s">
-        <v>4094</v>
+        <v>4106</v>
       </c>
       <c r="D528" t="s">
         <v>4219</v>
@@ -62166,13 +62166,13 @@
     </row>
     <row r="529" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A529" s="15">
-        <v>21084</v>
+        <v>1379</v>
       </c>
       <c r="B529" s="4" t="s">
-        <v>4208</v>
+        <v>4105</v>
       </c>
       <c r="C529" t="s">
-        <v>4094</v>
+        <v>4106</v>
       </c>
       <c r="D529" t="s">
         <v>4219</v>
@@ -62180,13 +62180,13 @@
     </row>
     <row r="530" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A530" s="15">
-        <v>21083</v>
+        <v>1380</v>
       </c>
       <c r="B530" s="4" t="s">
-        <v>4209</v>
+        <v>4104</v>
       </c>
       <c r="C530" t="s">
-        <v>4094</v>
+        <v>4106</v>
       </c>
       <c r="D530" t="s">
         <v>4219</v>
@@ -62194,13 +62194,13 @@
     </row>
     <row r="531" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A531" s="15">
-        <v>13762</v>
+        <v>1378</v>
       </c>
       <c r="B531" s="4" t="s">
-        <v>4095</v>
+        <v>4103</v>
       </c>
       <c r="C531" t="s">
-        <v>4097</v>
+        <v>4106</v>
       </c>
       <c r="D531" t="s">
         <v>4219</v>
@@ -62208,13 +62208,13 @@
     </row>
     <row r="532" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A532" s="15">
-        <v>4536</v>
+        <v>20716</v>
       </c>
       <c r="B532" s="4" t="s">
-        <v>4096</v>
+        <v>4199</v>
       </c>
       <c r="C532" t="s">
-        <v>4097</v>
+        <v>4094</v>
       </c>
       <c r="D532" t="s">
         <v>4219</v>
@@ -62222,13 +62222,13 @@
     </row>
     <row r="533" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A533" s="15">
-        <v>4513</v>
+        <v>20715</v>
       </c>
       <c r="B533" s="4" t="s">
-        <v>4164</v>
+        <v>4200</v>
       </c>
       <c r="C533" t="s">
-        <v>4097</v>
+        <v>4094</v>
       </c>
       <c r="D533" t="s">
         <v>4219</v>
@@ -62236,13 +62236,13 @@
     </row>
     <row r="534" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A534" s="15">
-        <v>5727</v>
+        <v>20714</v>
       </c>
       <c r="B534" s="4" t="s">
-        <v>4165</v>
+        <v>4093</v>
       </c>
       <c r="C534" t="s">
-        <v>4097</v>
+        <v>4094</v>
       </c>
       <c r="D534" t="s">
         <v>4219</v>
@@ -62250,13 +62250,13 @@
     </row>
     <row r="535" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A535" s="15">
-        <v>5793</v>
+        <v>27702</v>
       </c>
       <c r="B535" s="4" t="s">
-        <v>4166</v>
+        <v>4206</v>
       </c>
       <c r="C535" t="s">
-        <v>4097</v>
+        <v>4094</v>
       </c>
       <c r="D535" t="s">
         <v>4219</v>
@@ -62264,13 +62264,13 @@
     </row>
     <row r="536" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A536" s="15">
-        <v>13521</v>
+        <v>27701</v>
       </c>
       <c r="B536" s="4" t="s">
-        <v>4107</v>
+        <v>4205</v>
       </c>
       <c r="C536" t="s">
-        <v>4108</v>
+        <v>4094</v>
       </c>
       <c r="D536" t="s">
         <v>4219</v>
@@ -62278,249 +62278,250 @@
     </row>
     <row r="537" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A537" s="15">
-        <v>28784</v>
+        <v>20541</v>
       </c>
       <c r="B537" s="4" t="s">
-        <v>4091</v>
+        <v>4198</v>
       </c>
       <c r="C537" t="s">
-        <v>4090</v>
+        <v>4094</v>
       </c>
       <c r="D537" t="s">
         <v>4219</v>
       </c>
     </row>
     <row r="538" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A538" t="s">
-        <v>4242</v>
-      </c>
-      <c r="B538" t="s">
-        <v>4232</v>
+      <c r="A538" s="15">
+        <v>20540</v>
+      </c>
+      <c r="B538" s="4" t="s">
+        <v>4197</v>
       </c>
       <c r="C538" t="s">
-        <v>3566</v>
+        <v>4094</v>
       </c>
       <c r="D538" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="539" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A539" t="s">
-        <v>4243</v>
-      </c>
-      <c r="B539" t="s">
-        <v>4233</v>
+      <c r="A539" s="15">
+        <v>20540</v>
+      </c>
+      <c r="B539" s="4" t="s">
+        <v>4207</v>
       </c>
       <c r="C539" t="s">
-        <v>3566</v>
+        <v>4094</v>
       </c>
       <c r="D539" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="540" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A540" t="s">
-        <v>4244</v>
-      </c>
-      <c r="B540" t="s">
-        <v>4234</v>
+      <c r="A540" s="15">
+        <v>20606</v>
+      </c>
+      <c r="B540" s="4" t="s">
+        <v>4204</v>
       </c>
       <c r="C540" t="s">
-        <v>3566</v>
+        <v>4094</v>
       </c>
       <c r="D540" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="541" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A541" t="s">
-        <v>4245</v>
-      </c>
-      <c r="B541" t="s">
-        <v>4235</v>
+      <c r="A541" s="15">
+        <v>20594</v>
+      </c>
+      <c r="B541" s="4" t="s">
+        <v>4202</v>
       </c>
       <c r="C541" t="s">
-        <v>3566</v>
+        <v>4094</v>
       </c>
       <c r="D541" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="542" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A542" t="s">
-        <v>4246</v>
-      </c>
-      <c r="B542" t="s">
-        <v>4236</v>
+      <c r="A542" s="15">
+        <v>25359</v>
+      </c>
+      <c r="B542" s="4" t="s">
+        <v>4092</v>
       </c>
       <c r="C542" t="s">
-        <v>3566</v>
+        <v>4094</v>
       </c>
       <c r="D542" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="543" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A543" t="s">
-        <v>4247</v>
-      </c>
-      <c r="B543" t="s">
-        <v>4237</v>
+      <c r="A543" s="15">
+        <v>20570</v>
+      </c>
+      <c r="B543" s="4" t="s">
+        <v>4203</v>
       </c>
       <c r="C543" t="s">
-        <v>3566</v>
+        <v>4094</v>
       </c>
       <c r="D543" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="544" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A544" t="s">
-        <v>4248</v>
-      </c>
-      <c r="B544" t="s">
-        <v>4238</v>
+      <c r="A544" s="15">
+        <v>20543</v>
+      </c>
+      <c r="B544" s="4" t="s">
+        <v>4201</v>
       </c>
       <c r="C544" t="s">
-        <v>3566</v>
+        <v>4094</v>
       </c>
       <c r="D544" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="545" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A545" t="s">
-        <v>4249</v>
-      </c>
-      <c r="B545" t="s">
-        <v>4239</v>
+      <c r="A545" s="15">
+        <v>21084</v>
+      </c>
+      <c r="B545" s="4" t="s">
+        <v>4208</v>
       </c>
       <c r="C545" t="s">
-        <v>3566</v>
+        <v>4094</v>
       </c>
       <c r="D545" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="546" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A546" t="s">
-        <v>4250</v>
-      </c>
-      <c r="B546" t="s">
-        <v>4240</v>
+      <c r="A546" s="15">
+        <v>21083</v>
+      </c>
+      <c r="B546" s="4" t="s">
+        <v>4209</v>
       </c>
       <c r="C546" t="s">
-        <v>3566</v>
+        <v>4094</v>
       </c>
       <c r="D546" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="547" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A547" t="s">
-        <v>4251</v>
-      </c>
-      <c r="B547" t="s">
-        <v>4241</v>
+      <c r="A547" s="15">
+        <v>13762</v>
+      </c>
+      <c r="B547" s="4" t="s">
+        <v>4095</v>
       </c>
       <c r="C547" t="s">
-        <v>3566</v>
+        <v>4097</v>
       </c>
       <c r="D547" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="548" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A548" t="s">
-        <v>4257</v>
-      </c>
-      <c r="B548" t="s">
-        <v>4258</v>
+      <c r="A548" s="15">
+        <v>4536</v>
+      </c>
+      <c r="B548" s="4" t="s">
+        <v>4096</v>
       </c>
       <c r="C548" t="s">
-        <v>3566</v>
+        <v>4097</v>
       </c>
       <c r="D548" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="549" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A549" t="s">
-        <v>4259</v>
-      </c>
-      <c r="B549" t="s">
-        <v>4260</v>
+      <c r="A549" s="15">
+        <v>4513</v>
+      </c>
+      <c r="B549" s="4" t="s">
+        <v>4164</v>
       </c>
       <c r="C549" t="s">
-        <v>3567</v>
+        <v>4097</v>
       </c>
       <c r="D549" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="550" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A550" t="s">
-        <v>4261</v>
-      </c>
-      <c r="B550" t="s">
-        <v>4264</v>
+      <c r="A550" s="15">
+        <v>5727</v>
+      </c>
+      <c r="B550" s="4" t="s">
+        <v>4165</v>
       </c>
       <c r="C550" t="s">
-        <v>3567</v>
+        <v>4097</v>
       </c>
       <c r="D550" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="551" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A551" t="s">
-        <v>4262</v>
-      </c>
-      <c r="B551" t="s">
-        <v>4263</v>
+      <c r="A551" s="15">
+        <v>5793</v>
+      </c>
+      <c r="B551" s="4" t="s">
+        <v>4166</v>
       </c>
       <c r="C551" t="s">
-        <v>3567</v>
+        <v>4097</v>
       </c>
       <c r="D551" t="s">
-        <v>4216</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="552" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A552" t="s">
-        <v>4265</v>
-      </c>
-      <c r="B552" t="s">
-        <v>4266</v>
+      <c r="A552" s="15">
+        <v>13521</v>
+      </c>
+      <c r="B552" s="4" t="s">
+        <v>4107</v>
       </c>
       <c r="C552" t="s">
-        <v>4090</v>
+        <v>4108</v>
       </c>
       <c r="D552" t="s">
-        <v>4217</v>
+        <v>4219</v>
       </c>
     </row>
     <row r="553" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A553" t="s">
-        <v>4268</v>
-      </c>
-      <c r="B553" t="s">
-        <v>4267</v>
+      <c r="A553" s="15">
+        <v>28784</v>
+      </c>
+      <c r="B553" s="4" t="s">
+        <v>4091</v>
       </c>
       <c r="C553" t="s">
         <v>4090</v>
       </c>
       <c r="D553" t="s">
-        <v>4217</v>
+        <v>4219</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D537" xr:uid="{F2CB12C5-8725-4AAE-9F74-FA739078C419}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D537">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D553">
       <sortCondition ref="D1:D537"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Inclusão de melhorias @202406111729
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A85007A-882A-4105-A1D9-364EF8E2A73F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51289D5A-0863-4315-B848-018707D59B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" tabRatio="699" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13936" uniqueCount="4474">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14087" uniqueCount="4615">
   <si>
     <t>bbgTicker</t>
   </si>
@@ -13141,9 +13141,6 @@
     <t>S&amp;P 500</t>
   </si>
   <si>
-    <t>IFRM</t>
-  </si>
-  <si>
     <t>IPCA (% YoY)</t>
   </si>
   <si>
@@ -13469,6 +13466,432 @@
   </si>
   <si>
     <t>Austrália (5Y)</t>
+  </si>
+  <si>
+    <t>Café Arábica</t>
+  </si>
+  <si>
+    <t>Frango</t>
+  </si>
+  <si>
+    <t>Etanol</t>
+  </si>
+  <si>
+    <t>Suíno</t>
+  </si>
+  <si>
+    <t>Trigo</t>
+  </si>
+  <si>
+    <t>Dianteiro (boi)</t>
+  </si>
+  <si>
+    <t>Traseiro (boi)</t>
+  </si>
+  <si>
+    <t>Flanco (boi)</t>
+  </si>
+  <si>
+    <t>Carcaça (boi)</t>
+  </si>
+  <si>
+    <t>Boi Gordo</t>
+  </si>
+  <si>
+    <t>IPSA (Chile)</t>
+  </si>
+  <si>
+    <t>CSI1000 (China)</t>
+  </si>
+  <si>
+    <t>OBX (Norway)</t>
+  </si>
+  <si>
+    <t>CSI300 (China)</t>
+  </si>
+  <si>
+    <t>SSE (China)</t>
+  </si>
+  <si>
+    <t>MSCI China</t>
+  </si>
+  <si>
+    <t>Stoxx 50 (Europa)</t>
+  </si>
+  <si>
+    <t>FTSE MIB (Itália)</t>
+  </si>
+  <si>
+    <t>JCI (Indonésia)</t>
+  </si>
+  <si>
+    <t>Nifty 50 (Índia)</t>
+  </si>
+  <si>
+    <t>DAX 40 (Alemanha)</t>
+  </si>
+  <si>
+    <t>MSCI ACWI</t>
+  </si>
+  <si>
+    <t>BMV (México)</t>
+  </si>
+  <si>
+    <t>Nikkei 225 (Japão)</t>
+  </si>
+  <si>
+    <t>MSCI Emerging Markets</t>
+  </si>
+  <si>
+    <t>MSCI Europe</t>
+  </si>
+  <si>
+    <t>NZX 50 (Nova Zelândia)</t>
+  </si>
+  <si>
+    <t>Top 40 (África do Sul)</t>
+  </si>
+  <si>
+    <t>OMX (Suécia)</t>
+  </si>
+  <si>
+    <t>SMI (Suíça)</t>
+  </si>
+  <si>
+    <t>UKX (UK)</t>
+  </si>
+  <si>
+    <t>Nasdaq Composite (US)</t>
+  </si>
+  <si>
+    <t>Nasdaq 100 (US)</t>
+  </si>
+  <si>
+    <t>Russell 2000 (US)</t>
+  </si>
+  <si>
+    <t>XLU Utilities (US)</t>
+  </si>
+  <si>
+    <t>SOXX Semiconductor (US)</t>
+  </si>
+  <si>
+    <t>IMA-B</t>
+  </si>
+  <si>
+    <t>IMA-S</t>
+  </si>
+  <si>
+    <t>IRF-M</t>
+  </si>
+  <si>
+    <t>Credit Impulse (China)</t>
+  </si>
+  <si>
+    <t>Credit Impulse 12M (China)</t>
+  </si>
+  <si>
+    <t>Treasury 10Y</t>
+  </si>
+  <si>
+    <t>Treasury 2Y</t>
+  </si>
+  <si>
+    <t>Treasury 5Y</t>
+  </si>
+  <si>
+    <t>Treasury Bonds</t>
+  </si>
+  <si>
+    <t>EWZ (Brasil)</t>
+  </si>
+  <si>
+    <t>XLK Info Tech (US)</t>
+  </si>
+  <si>
+    <t>XLF Financials (US)</t>
+  </si>
+  <si>
+    <t>XLC Comm Services (US)</t>
+  </si>
+  <si>
+    <t>XLY Consumer Discretionary (US)</t>
+  </si>
+  <si>
+    <t>XLP Consumer Staples (US)</t>
+  </si>
+  <si>
+    <t>XLV Healthcare (US)</t>
+  </si>
+  <si>
+    <t>XLE Energy (US)</t>
+  </si>
+  <si>
+    <t>XLI Industrials (US)</t>
+  </si>
+  <si>
+    <t>XLRE Real Estate (US)</t>
+  </si>
+  <si>
+    <t>XLB Materials (US)</t>
+  </si>
+  <si>
+    <t>Índice de Surpresas Econômicas (Citi)</t>
+  </si>
+  <si>
+    <t>Índice de Surpresas Econômicas (Bloomberg)</t>
+  </si>
+  <si>
+    <t>Õnibus</t>
+  </si>
+  <si>
+    <t>Caminhões</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Meta</t>
+  </si>
+  <si>
+    <t>Dívida Bruta / PIB</t>
+  </si>
+  <si>
+    <t>Dívida Líquida / PIB</t>
+  </si>
+  <si>
+    <t>Dívida Líquida do Setor Público / PIB</t>
+  </si>
+  <si>
+    <t>Resultado Primário / PIB</t>
+  </si>
+  <si>
+    <t>Resultado Nominal / PIB</t>
+  </si>
+  <si>
+    <t>Pequenas e Médias Empresas (PME)</t>
+  </si>
+  <si>
+    <t>Grandes</t>
+  </si>
+  <si>
+    <t>PF</t>
+  </si>
+  <si>
+    <t>PJ</t>
+  </si>
+  <si>
+    <t>Selic</t>
+  </si>
+  <si>
+    <t>Taxa de Desemprego</t>
+  </si>
+  <si>
+    <t>IBC-Br (Índice)</t>
+  </si>
+  <si>
+    <t>IBC-Br (% MoM)</t>
+  </si>
+  <si>
+    <t>IBC-Br (% YoY)</t>
+  </si>
+  <si>
+    <t>IBC-Br (% QoQ)</t>
+  </si>
+  <si>
+    <t>IBC-Br (Índice NSA)</t>
+  </si>
+  <si>
+    <t>IGP-10 (Índice)</t>
+  </si>
+  <si>
+    <t>IGP-10 (% MoM)</t>
+  </si>
+  <si>
+    <t>IGP-10 (% YoY)</t>
+  </si>
+  <si>
+    <t>IGP-DI (Índice)</t>
+  </si>
+  <si>
+    <t>IGP-DI (% MoM)</t>
+  </si>
+  <si>
+    <t>IGP-DI (% YoY)</t>
+  </si>
+  <si>
+    <t>IGP-M (Índice)</t>
+  </si>
+  <si>
+    <t>IGP-M (% MoM)</t>
+  </si>
+  <si>
+    <t>IGP-M (% YoY)</t>
+  </si>
+  <si>
+    <t>INCC-10 (Índice)</t>
+  </si>
+  <si>
+    <t>INCC-10 (% MoM)</t>
+  </si>
+  <si>
+    <t>INCC-10 (% YoY)</t>
+  </si>
+  <si>
+    <t>IPA-10 (Índice)</t>
+  </si>
+  <si>
+    <t>IPA-10 (% MoM)</t>
+  </si>
+  <si>
+    <t>IPA-10 (% YoY)</t>
+  </si>
+  <si>
+    <t>Índice de Termos de Troca (MDIC)</t>
+  </si>
+  <si>
+    <t>Produção Industrial (% YoY)</t>
+  </si>
+  <si>
+    <t>Produção Industrial (% MoM)</t>
+  </si>
+  <si>
+    <t>Produção Industrial</t>
+  </si>
+  <si>
+    <t>Produção Industrial (12m % YoY)</t>
+  </si>
+  <si>
+    <t>Pré (10Y)</t>
+  </si>
+  <si>
+    <t>Pré (1Y)</t>
+  </si>
+  <si>
+    <t>Pré (2Y)</t>
+  </si>
+  <si>
+    <t>Pré (3Y)</t>
+  </si>
+  <si>
+    <t>Pré (4Y)</t>
+  </si>
+  <si>
+    <t>Pré (5Y)</t>
+  </si>
+  <si>
+    <t>IPCA (10Y)</t>
+  </si>
+  <si>
+    <t>IPCA (15Y)</t>
+  </si>
+  <si>
+    <t>IPCA (2Y)</t>
+  </si>
+  <si>
+    <t>IPCA (3Y)</t>
+  </si>
+  <si>
+    <t>IPCA (5Y)</t>
+  </si>
+  <si>
+    <t>IPCA (12Y)</t>
+  </si>
+  <si>
+    <t>IPCA (11Y)</t>
+  </si>
+  <si>
+    <t>IPCA (13Y)</t>
+  </si>
+  <si>
+    <t>IPCA (14Y)</t>
+  </si>
+  <si>
+    <t>IPCA (16Y)</t>
+  </si>
+  <si>
+    <t>IPCA (17Y)</t>
+  </si>
+  <si>
+    <t>IPCA (18Y)</t>
+  </si>
+  <si>
+    <t>IPCA (19Y)</t>
+  </si>
+  <si>
+    <t>IPCA (20Y)</t>
+  </si>
+  <si>
+    <t>IPCA (21Y)</t>
+  </si>
+  <si>
+    <t>IPCA (22Y)</t>
+  </si>
+  <si>
+    <t>IPCA (23Y)</t>
+  </si>
+  <si>
+    <t>IPCA (24Y)</t>
+  </si>
+  <si>
+    <t>IPCA (25Y)</t>
+  </si>
+  <si>
+    <t>IPCA (26Y)</t>
+  </si>
+  <si>
+    <t>IPCA (27Y)</t>
+  </si>
+  <si>
+    <t>IPCA (28Y)</t>
+  </si>
+  <si>
+    <t>IPCA (29Y)</t>
+  </si>
+  <si>
+    <t>IPCA (30Y)</t>
+  </si>
+  <si>
+    <t>IPCA (31Y)</t>
+  </si>
+  <si>
+    <t>IPCA (32Y)</t>
+  </si>
+  <si>
+    <t>IPCA (33Y)</t>
+  </si>
+  <si>
+    <t>IPCA (34Y)</t>
+  </si>
+  <si>
+    <t>IPCA (35Y)</t>
+  </si>
+  <si>
+    <t>IPCA (36Y)</t>
+  </si>
+  <si>
+    <t>IPCA (37Y)</t>
+  </si>
+  <si>
+    <t>IPCA (38Y)</t>
+  </si>
+  <si>
+    <t>IPCA (1Y)</t>
+  </si>
+  <si>
+    <t>IPCA (4Y)</t>
+  </si>
+  <si>
+    <t>IPCA (6Y)</t>
+  </si>
+  <si>
+    <t>IPCA (7Y)</t>
+  </si>
+  <si>
+    <t>IPCA (8Y)</t>
+  </si>
+  <si>
+    <t>IPCA (9Y)</t>
   </si>
 </sst>
 </file>
@@ -55072,8 +55495,8 @@
   <dimension ref="A1:E564"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <pane ySplit="1" topLeftCell="A477" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B492" sqref="B492"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55199,6 +55622,9 @@
       <c r="D7" t="s">
         <v>4214</v>
       </c>
+      <c r="E7" t="s">
+        <v>4473</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -55213,6 +55639,9 @@
       <c r="D8" t="s">
         <v>4214</v>
       </c>
+      <c r="E8" t="s">
+        <v>4481</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -55227,6 +55656,9 @@
       <c r="D9" t="s">
         <v>4214</v>
       </c>
+      <c r="E9" t="s">
+        <v>4478</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -55241,6 +55673,9 @@
       <c r="D10" t="s">
         <v>4214</v>
       </c>
+      <c r="E10" t="s">
+        <v>4479</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -55255,6 +55690,9 @@
       <c r="D11" t="s">
         <v>4214</v>
       </c>
+      <c r="E11" t="s">
+        <v>4480</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -55269,6 +55707,9 @@
       <c r="D12" t="s">
         <v>4214</v>
       </c>
+      <c r="E12" t="s">
+        <v>4474</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -55283,6 +55724,9 @@
       <c r="D13" t="s">
         <v>4214</v>
       </c>
+      <c r="E13" t="s">
+        <v>4275</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -55297,6 +55741,9 @@
       <c r="D14" t="s">
         <v>4214</v>
       </c>
+      <c r="E14" t="s">
+        <v>4283</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -55311,6 +55758,9 @@
       <c r="D15" t="s">
         <v>4214</v>
       </c>
+      <c r="E15" t="s">
+        <v>4475</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -55325,6 +55775,9 @@
       <c r="D16" t="s">
         <v>4214</v>
       </c>
+      <c r="E16" t="s">
+        <v>4482</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -55339,6 +55792,9 @@
       <c r="D17" t="s">
         <v>4214</v>
       </c>
+      <c r="E17" t="s">
+        <v>4296</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -55353,6 +55809,9 @@
       <c r="D18" t="s">
         <v>4214</v>
       </c>
+      <c r="E18" t="s">
+        <v>4476</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
@@ -55367,6 +55826,9 @@
       <c r="D19" t="s">
         <v>4214</v>
       </c>
+      <c r="E19" t="s">
+        <v>4477</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
@@ -55381,6 +55843,9 @@
       <c r="D20" t="s">
         <v>4214</v>
       </c>
+      <c r="E20" t="s">
+        <v>4343</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
@@ -55395,6 +55860,9 @@
       <c r="D21" t="s">
         <v>4214</v>
       </c>
+      <c r="E21" t="s">
+        <v>4276</v>
+      </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
@@ -55805,6 +56273,9 @@
       <c r="D46" t="s">
         <v>4214</v>
       </c>
+      <c r="E46" t="s">
+        <v>4482</v>
+      </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
@@ -56136,6 +56607,9 @@
       <c r="D66" t="s">
         <v>4214</v>
       </c>
+      <c r="E66" t="s">
+        <v>4343</v>
+      </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
@@ -56151,7 +56625,7 @@
         <v>4214</v>
       </c>
       <c r="E67" t="s">
-        <v>4343</v>
+        <v>4477</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -56946,6 +57420,9 @@
       <c r="D114" t="s">
         <v>4214</v>
       </c>
+      <c r="E114" t="s">
+        <v>4483</v>
+      </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
@@ -56960,6 +57437,9 @@
       <c r="D115" t="s">
         <v>4214</v>
       </c>
+      <c r="E115" t="s">
+        <v>4484</v>
+      </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
@@ -56974,6 +57454,9 @@
       <c r="D116" t="s">
         <v>4214</v>
       </c>
+      <c r="E116" t="s">
+        <v>4486</v>
+      </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
@@ -56988,6 +57471,9 @@
       <c r="D117" t="s">
         <v>4214</v>
       </c>
+      <c r="E117" t="s">
+        <v>4488</v>
+      </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
@@ -57002,6 +57488,9 @@
       <c r="D118" t="s">
         <v>4214</v>
       </c>
+      <c r="E118" t="s">
+        <v>4487</v>
+      </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
@@ -57016,6 +57505,9 @@
       <c r="D119" t="s">
         <v>4214</v>
       </c>
+      <c r="E119" t="s">
+        <v>4489</v>
+      </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
@@ -57030,6 +57522,9 @@
       <c r="D120" t="s">
         <v>4214</v>
       </c>
+      <c r="E120" t="s">
+        <v>4493</v>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
@@ -57044,6 +57539,9 @@
       <c r="D121" t="s">
         <v>4214</v>
       </c>
+      <c r="E121" t="s">
+        <v>4492</v>
+      </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
@@ -57058,6 +57556,9 @@
       <c r="D122" t="s">
         <v>4214</v>
       </c>
+      <c r="E122" t="s">
+        <v>4491</v>
+      </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
@@ -57072,6 +57573,9 @@
       <c r="D123" t="s">
         <v>4214</v>
       </c>
+      <c r="E123" t="s">
+        <v>4490</v>
+      </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
@@ -57086,6 +57590,9 @@
       <c r="D124" t="s">
         <v>4214</v>
       </c>
+      <c r="E124" t="s">
+        <v>4496</v>
+      </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
@@ -57100,6 +57607,9 @@
       <c r="D125" t="s">
         <v>4214</v>
       </c>
+      <c r="E125" t="s">
+        <v>4495</v>
+      </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
@@ -57114,6 +57624,9 @@
       <c r="D126" t="s">
         <v>4214</v>
       </c>
+      <c r="E126" t="s">
+        <v>4494</v>
+      </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
@@ -57128,6 +57641,9 @@
       <c r="D127" t="s">
         <v>4214</v>
       </c>
+      <c r="E127" t="s">
+        <v>4497</v>
+      </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
@@ -57142,8 +57658,11 @@
       <c r="D128" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E128" t="s">
+        <v>4498</v>
+      </c>
+    </row>
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>3474</v>
       </c>
@@ -57156,8 +57675,11 @@
       <c r="D129" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E129" t="s">
+        <v>4499</v>
+      </c>
+    </row>
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>3477</v>
       </c>
@@ -57170,8 +57692,11 @@
       <c r="D130" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E130" t="s">
+        <v>4485</v>
+      </c>
+    </row>
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>3482</v>
       </c>
@@ -57184,8 +57709,11 @@
       <c r="D131" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E131" t="s">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>3480</v>
       </c>
@@ -57198,8 +57726,11 @@
       <c r="D132" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E132" t="s">
+        <v>4501</v>
+      </c>
+    </row>
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>3478</v>
       </c>
@@ -57212,8 +57743,11 @@
       <c r="D133" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E133" t="s">
+        <v>4502</v>
+      </c>
+    </row>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>3479</v>
       </c>
@@ -57226,8 +57760,11 @@
       <c r="D134" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E134" t="s">
+        <v>4503</v>
+      </c>
+    </row>
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>3808</v>
       </c>
@@ -57241,7 +57778,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>3810</v>
       </c>
@@ -57255,7 +57792,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>3803</v>
       </c>
@@ -57269,7 +57806,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>4225</v>
       </c>
@@ -57283,7 +57820,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>4224</v>
       </c>
@@ -57297,7 +57834,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>3802</v>
       </c>
@@ -57311,7 +57848,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>3346</v>
       </c>
@@ -57324,8 +57861,11 @@
       <c r="D141" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E141" t="s">
+        <v>4504</v>
+      </c>
+    </row>
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>3533</v>
       </c>
@@ -57338,8 +57878,11 @@
       <c r="D142" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E142" t="s">
+        <v>4505</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>3806</v>
       </c>
@@ -57353,7 +57896,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>3356</v>
       </c>
@@ -57365,6 +57908,9 @@
       </c>
       <c r="D144" t="s">
         <v>4214</v>
+      </c>
+      <c r="E144" t="s">
+        <v>4506</v>
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.25">
@@ -57380,6 +57926,9 @@
       <c r="D145" t="s">
         <v>4214</v>
       </c>
+      <c r="E145" t="s">
+        <v>4508</v>
+      </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
@@ -57411,6 +57960,9 @@
       <c r="D147" t="s">
         <v>4214</v>
       </c>
+      <c r="E147" t="s">
+        <v>4507</v>
+      </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
@@ -57502,7 +58054,7 @@
         <v>4214</v>
       </c>
       <c r="E153" t="s">
-        <v>4471</v>
+        <v>4470</v>
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.25">
@@ -57519,7 +58071,7 @@
         <v>4214</v>
       </c>
       <c r="E154" t="s">
-        <v>4472</v>
+        <v>4471</v>
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.25">
@@ -57536,7 +58088,7 @@
         <v>4214</v>
       </c>
       <c r="E155" t="s">
-        <v>4473</v>
+        <v>4472</v>
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.25">
@@ -58081,7 +58633,7 @@
         <v>4214</v>
       </c>
       <c r="E192" t="s">
-        <v>4468</v>
+        <v>4467</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
@@ -58098,7 +58650,7 @@
         <v>4214</v>
       </c>
       <c r="E193" t="s">
-        <v>4469</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
@@ -58115,7 +58667,7 @@
         <v>4214</v>
       </c>
       <c r="E194" t="s">
-        <v>4470</v>
+        <v>4469</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
@@ -58131,6 +58683,9 @@
       <c r="D195" t="s">
         <v>4214</v>
       </c>
+      <c r="E195" t="s">
+        <v>4546</v>
+      </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
@@ -58145,6 +58700,9 @@
       <c r="D196" t="s">
         <v>4214</v>
       </c>
+      <c r="E196" t="s">
+        <v>4547</v>
+      </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
@@ -58159,6 +58717,9 @@
       <c r="D197" t="s">
         <v>4214</v>
       </c>
+      <c r="E197" t="s">
+        <v>4550</v>
+      </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
@@ -58173,6 +58734,9 @@
       <c r="D198" t="s">
         <v>4214</v>
       </c>
+      <c r="E198" t="s">
+        <v>4549</v>
+      </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
@@ -58187,6 +58751,9 @@
       <c r="D199" t="s">
         <v>4214</v>
       </c>
+      <c r="E199" t="s">
+        <v>4548</v>
+      </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
@@ -58201,6 +58768,9 @@
       <c r="D200" t="s">
         <v>4214</v>
       </c>
+      <c r="E200" t="s">
+        <v>4551</v>
+      </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
@@ -58215,6 +58785,9 @@
       <c r="D201" t="s">
         <v>4214</v>
       </c>
+      <c r="E201" t="s">
+        <v>4552</v>
+      </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
@@ -58229,6 +58802,9 @@
       <c r="D202" t="s">
         <v>4214</v>
       </c>
+      <c r="E202" t="s">
+        <v>4553</v>
+      </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
@@ -58243,6 +58819,9 @@
       <c r="D203" t="s">
         <v>4214</v>
       </c>
+      <c r="E203" t="s">
+        <v>4554</v>
+      </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
@@ -58257,6 +58836,9 @@
       <c r="D204" t="s">
         <v>4214</v>
       </c>
+      <c r="E204" t="s">
+        <v>4555</v>
+      </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
@@ -58271,6 +58853,9 @@
       <c r="D205" t="s">
         <v>4214</v>
       </c>
+      <c r="E205" t="s">
+        <v>4556</v>
+      </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
@@ -58285,6 +58870,9 @@
       <c r="D206" t="s">
         <v>4214</v>
       </c>
+      <c r="E206" t="s">
+        <v>4557</v>
+      </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
@@ -58299,6 +58887,9 @@
       <c r="D207" t="s">
         <v>4214</v>
       </c>
+      <c r="E207" t="s">
+        <v>4558</v>
+      </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
@@ -58313,8 +58904,11 @@
       <c r="D208" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="209" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E208" t="s">
+        <v>4559</v>
+      </c>
+    </row>
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>3521</v>
       </c>
@@ -58327,8 +58921,11 @@
       <c r="D209" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="210" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E209" t="s">
+        <v>4509</v>
+      </c>
+    </row>
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>3524</v>
       </c>
@@ -58341,8 +58938,11 @@
       <c r="D210" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="211" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E210" t="s">
+        <v>4510</v>
+      </c>
+    </row>
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>3922</v>
       </c>
@@ -58355,8 +58955,11 @@
       <c r="D211" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="212" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E211" t="s">
+        <v>4560</v>
+      </c>
+    </row>
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>3923</v>
       </c>
@@ -58369,8 +58972,11 @@
       <c r="D212" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="213" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E212" t="s">
+        <v>4561</v>
+      </c>
+    </row>
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>3924</v>
       </c>
@@ -58383,8 +58989,11 @@
       <c r="D213" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="214" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E213" t="s">
+        <v>4562</v>
+      </c>
+    </row>
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>4155</v>
       </c>
@@ -58397,8 +59006,11 @@
       <c r="D214" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="215" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E214" t="s">
+        <v>4569</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>4159</v>
       </c>
@@ -58411,8 +59023,11 @@
       <c r="D215" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="216" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E215" t="s">
+        <v>4570</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>4161</v>
       </c>
@@ -58425,8 +59040,11 @@
       <c r="D216" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="217" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E216" t="s">
+        <v>4568</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>4157</v>
       </c>
@@ -58439,8 +59057,11 @@
       <c r="D217" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="218" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E217" t="s">
+        <v>4567</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>3916</v>
       </c>
@@ -58453,8 +59074,11 @@
       <c r="D218" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="219" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E218" t="s">
+        <v>4563</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>3917</v>
       </c>
@@ -58467,8 +59091,11 @@
       <c r="D219" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="220" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E219" t="s">
+        <v>4564</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>3918</v>
       </c>
@@ -58481,8 +59108,11 @@
       <c r="D220" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="221" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E220" t="s">
+        <v>4565</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>27</v>
       </c>
@@ -58495,8 +59125,11 @@
       <c r="D221" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="222" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E221" t="s">
+        <v>4577</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>3849</v>
       </c>
@@ -58509,8 +59142,11 @@
       <c r="D222" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="223" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E222" t="s">
+        <v>4583</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>3847</v>
       </c>
@@ -58523,8 +59159,11 @@
       <c r="D223" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="224" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E223" t="s">
+        <v>4582</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>3850</v>
       </c>
@@ -58537,8 +59176,11 @@
       <c r="D224" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="225" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E224" t="s">
+        <v>4584</v>
+      </c>
+    </row>
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>3851</v>
       </c>
@@ -58551,8 +59193,11 @@
       <c r="D225" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="226" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E225" t="s">
+        <v>4585</v>
+      </c>
+    </row>
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>3839</v>
       </c>
@@ -58565,8 +59210,11 @@
       <c r="D226" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="227" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E226" t="s">
+        <v>4578</v>
+      </c>
+    </row>
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>3852</v>
       </c>
@@ -58579,8 +59227,11 @@
       <c r="D227" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="228" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E227" t="s">
+        <v>4586</v>
+      </c>
+    </row>
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>3853</v>
       </c>
@@ -58593,8 +59244,11 @@
       <c r="D228" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="229" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E228" t="s">
+        <v>4587</v>
+      </c>
+    </row>
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>3854</v>
       </c>
@@ -58607,8 +59261,11 @@
       <c r="D229" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="230" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E229" t="s">
+        <v>4588</v>
+      </c>
+    </row>
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>3855</v>
       </c>
@@ -58621,8 +59278,11 @@
       <c r="D230" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="231" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E230" t="s">
+        <v>4589</v>
+      </c>
+    </row>
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" s="3" t="s">
         <v>23</v>
       </c>
@@ -58635,8 +59295,11 @@
       <c r="D231" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="232" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E231" t="s">
+        <v>4609</v>
+      </c>
+    </row>
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>3843</v>
       </c>
@@ -58649,8 +59312,11 @@
       <c r="D232" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="233" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E232" t="s">
+        <v>4590</v>
+      </c>
+    </row>
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>3856</v>
       </c>
@@ -58663,8 +59329,11 @@
       <c r="D233" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="234" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E233" t="s">
+        <v>4591</v>
+      </c>
+    </row>
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>3857</v>
       </c>
@@ -58677,8 +59346,11 @@
       <c r="D234" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="235" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E234" t="s">
+        <v>4592</v>
+      </c>
+    </row>
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>3858</v>
       </c>
@@ -58691,8 +59363,11 @@
       <c r="D235" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="236" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E235" t="s">
+        <v>4593</v>
+      </c>
+    </row>
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>3859</v>
       </c>
@@ -58705,8 +59380,11 @@
       <c r="D236" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="237" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E236" t="s">
+        <v>4594</v>
+      </c>
+    </row>
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>3848</v>
       </c>
@@ -58719,8 +59397,11 @@
       <c r="D237" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="238" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E237" t="s">
+        <v>4595</v>
+      </c>
+    </row>
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>3841</v>
       </c>
@@ -58733,8 +59414,11 @@
       <c r="D238" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="239" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E238" t="s">
+        <v>4596</v>
+      </c>
+    </row>
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>3860</v>
       </c>
@@ -58747,8 +59431,11 @@
       <c r="D239" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="240" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E239" t="s">
+        <v>4597</v>
+      </c>
+    </row>
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>3861</v>
       </c>
@@ -58761,8 +59448,11 @@
       <c r="D240" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="241" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E240" t="s">
+        <v>4598</v>
+      </c>
+    </row>
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>3845</v>
       </c>
@@ -58775,8 +59465,11 @@
       <c r="D241" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="242" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E241" t="s">
+        <v>4599</v>
+      </c>
+    </row>
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" s="3" t="s">
         <v>24</v>
       </c>
@@ -58789,8 +59482,11 @@
       <c r="D242" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="243" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E242" t="s">
+        <v>4579</v>
+      </c>
+    </row>
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>3838</v>
       </c>
@@ -58803,8 +59499,11 @@
       <c r="D243" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="244" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E243" t="s">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>3862</v>
       </c>
@@ -58817,8 +59516,11 @@
       <c r="D244" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="245" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E244" t="s">
+        <v>4601</v>
+      </c>
+    </row>
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>3863</v>
       </c>
@@ -58831,8 +59533,11 @@
       <c r="D245" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="246" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E245" t="s">
+        <v>4602</v>
+      </c>
+    </row>
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>3864</v>
       </c>
@@ -58845,8 +59550,11 @@
       <c r="D246" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="247" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E246" t="s">
+        <v>4603</v>
+      </c>
+    </row>
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>3865</v>
       </c>
@@ -58859,8 +59567,11 @@
       <c r="D247" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="248" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E247" t="s">
+        <v>4604</v>
+      </c>
+    </row>
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>28</v>
       </c>
@@ -58873,8 +59584,11 @@
       <c r="D248" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="249" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E248" t="s">
+        <v>4605</v>
+      </c>
+    </row>
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>3866</v>
       </c>
@@ -58887,8 +59601,11 @@
       <c r="D249" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="250" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E249" t="s">
+        <v>4606</v>
+      </c>
+    </row>
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>3867</v>
       </c>
@@ -58901,8 +59618,11 @@
       <c r="D250" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="251" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E250" t="s">
+        <v>4607</v>
+      </c>
+    </row>
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>3868</v>
       </c>
@@ -58915,8 +59635,11 @@
       <c r="D251" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="252" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E251" t="s">
+        <v>4608</v>
+      </c>
+    </row>
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>25</v>
       </c>
@@ -58929,8 +59652,11 @@
       <c r="D252" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="253" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E252" t="s">
+        <v>4580</v>
+      </c>
+    </row>
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>3844</v>
       </c>
@@ -58943,8 +59669,11 @@
       <c r="D253" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="254" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E253" t="s">
+        <v>4610</v>
+      </c>
+    </row>
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>26</v>
       </c>
@@ -58957,8 +59686,11 @@
       <c r="D254" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="255" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E254" t="s">
+        <v>4581</v>
+      </c>
+    </row>
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>3842</v>
       </c>
@@ -58971,8 +59703,11 @@
       <c r="D255" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="256" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E255" t="s">
+        <v>4611</v>
+      </c>
+    </row>
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>3840</v>
       </c>
@@ -58984,6 +59719,9 @@
       </c>
       <c r="D256" t="s">
         <v>4214</v>
+      </c>
+      <c r="E256" t="s">
+        <v>4612</v>
       </c>
     </row>
     <row r="257" spans="1:5" x14ac:dyDescent="0.25">
@@ -58999,6 +59737,9 @@
       <c r="D257" t="s">
         <v>4214</v>
       </c>
+      <c r="E257" t="s">
+        <v>4613</v>
+      </c>
     </row>
     <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
@@ -59013,6 +59754,9 @@
       <c r="D258" t="s">
         <v>4214</v>
       </c>
+      <c r="E258" t="s">
+        <v>4614</v>
+      </c>
     </row>
     <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
@@ -59140,7 +59884,7 @@
         <v>4214</v>
       </c>
       <c r="E267" t="s">
-        <v>4367</v>
+        <v>4366</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
@@ -59157,7 +59901,7 @@
         <v>4214</v>
       </c>
       <c r="E268" t="s">
-        <v>4366</v>
+        <v>4365</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -59272,7 +60016,7 @@
         <v>4214</v>
       </c>
       <c r="E276" t="s">
-        <v>4365</v>
+        <v>4364</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
@@ -59289,7 +60033,7 @@
         <v>4214</v>
       </c>
       <c r="E277" t="s">
-        <v>4364</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="278" spans="1:5" x14ac:dyDescent="0.25">
@@ -59305,6 +60049,9 @@
       <c r="D278" t="s">
         <v>4214</v>
       </c>
+      <c r="E278" t="s">
+        <v>4566</v>
+      </c>
     </row>
     <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
@@ -59446,7 +60193,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="289" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>4026</v>
       </c>
@@ -59460,7 +60207,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="290" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>4028</v>
       </c>
@@ -59474,7 +60221,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="291" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>4025</v>
       </c>
@@ -59488,7 +60235,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="292" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>4020</v>
       </c>
@@ -59502,7 +60249,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="293" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>4015</v>
       </c>
@@ -59516,7 +60263,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="294" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>4018</v>
       </c>
@@ -59530,7 +60277,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="295" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>4021</v>
       </c>
@@ -59544,7 +60291,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="296" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>4009</v>
       </c>
@@ -59558,7 +60305,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="297" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>4049</v>
       </c>
@@ -59572,7 +60319,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="298" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>4010</v>
       </c>
@@ -59586,7 +60333,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="299" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>4015</v>
       </c>
@@ -59600,7 +60347,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="300" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>3697</v>
       </c>
@@ -59613,8 +60360,11 @@
       <c r="D300" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="301" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E300" t="s">
+        <v>4545</v>
+      </c>
+    </row>
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>33</v>
       </c>
@@ -59627,8 +60377,11 @@
       <c r="D301" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="302" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E301" t="s">
+        <v>4571</v>
+      </c>
+    </row>
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>29</v>
       </c>
@@ -59641,8 +60394,11 @@
       <c r="D302" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="303" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E302" t="s">
+        <v>4572</v>
+      </c>
+    </row>
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>30</v>
       </c>
@@ -59655,8 +60411,11 @@
       <c r="D303" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="304" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E303" t="s">
+        <v>4573</v>
+      </c>
+    </row>
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>31</v>
       </c>
@@ -59668,6 +60427,9 @@
       </c>
       <c r="D304" t="s">
         <v>4214</v>
+      </c>
+      <c r="E304" t="s">
+        <v>4574</v>
       </c>
     </row>
     <row r="305" spans="1:5" x14ac:dyDescent="0.25">
@@ -59683,6 +60445,9 @@
       <c r="D305" t="s">
         <v>4214</v>
       </c>
+      <c r="E305" t="s">
+        <v>4575</v>
+      </c>
     </row>
     <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
@@ -59697,6 +60462,9 @@
       <c r="D306" t="s">
         <v>4214</v>
       </c>
+      <c r="E306" t="s">
+        <v>4576</v>
+      </c>
     </row>
     <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
@@ -59711,6 +60479,9 @@
       <c r="D307" t="s">
         <v>4214</v>
       </c>
+      <c r="E307" t="s">
+        <v>4544</v>
+      </c>
     </row>
     <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
@@ -59768,7 +60539,7 @@
         <v>4214</v>
       </c>
       <c r="E311" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="312" spans="1:5" x14ac:dyDescent="0.25">
@@ -59785,7 +60556,7 @@
         <v>4214</v>
       </c>
       <c r="E312" t="s">
-        <v>4463</v>
+        <v>4462</v>
       </c>
     </row>
     <row r="313" spans="1:5" x14ac:dyDescent="0.25">
@@ -59802,7 +60573,7 @@
         <v>4214</v>
       </c>
       <c r="E313" t="s">
-        <v>4464</v>
+        <v>4463</v>
       </c>
     </row>
     <row r="314" spans="1:5" x14ac:dyDescent="0.25">
@@ -59819,7 +60590,7 @@
         <v>4214</v>
       </c>
       <c r="E314" t="s">
-        <v>4465</v>
+        <v>4464</v>
       </c>
     </row>
     <row r="315" spans="1:5" x14ac:dyDescent="0.25">
@@ -59836,7 +60607,7 @@
         <v>4214</v>
       </c>
       <c r="E315" t="s">
-        <v>4466</v>
+        <v>4465</v>
       </c>
     </row>
     <row r="316" spans="1:5" x14ac:dyDescent="0.25">
@@ -59853,7 +60624,7 @@
         <v>4214</v>
       </c>
       <c r="E316" t="s">
-        <v>4467</v>
+        <v>4466</v>
       </c>
     </row>
     <row r="317" spans="1:5" x14ac:dyDescent="0.25">
@@ -59869,6 +60640,9 @@
       <c r="D317" t="s">
         <v>4214</v>
       </c>
+      <c r="E317" t="s">
+        <v>4512</v>
+      </c>
     </row>
     <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
@@ -59883,6 +60657,9 @@
       <c r="D318" t="s">
         <v>4214</v>
       </c>
+      <c r="E318" t="s">
+        <v>4513</v>
+      </c>
     </row>
     <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
@@ -59898,7 +60675,7 @@
         <v>4214</v>
       </c>
       <c r="E319" t="s">
-        <v>4459</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="320" spans="1:5" x14ac:dyDescent="0.25">
@@ -59915,7 +60692,7 @@
         <v>4214</v>
       </c>
       <c r="E320" t="s">
-        <v>4460</v>
+        <v>4459</v>
       </c>
     </row>
     <row r="321" spans="1:5" x14ac:dyDescent="0.25">
@@ -59932,7 +60709,7 @@
         <v>4214</v>
       </c>
       <c r="E321" t="s">
-        <v>4461</v>
+        <v>4460</v>
       </c>
     </row>
     <row r="322" spans="1:5" x14ac:dyDescent="0.25">
@@ -60019,7 +60796,7 @@
         <v>4214</v>
       </c>
       <c r="E327" t="s">
-        <v>4399</v>
+        <v>4398</v>
       </c>
     </row>
     <row r="328" spans="1:5" x14ac:dyDescent="0.25">
@@ -60036,7 +60813,7 @@
         <v>4214</v>
       </c>
       <c r="E328" t="s">
-        <v>4400</v>
+        <v>4399</v>
       </c>
     </row>
     <row r="329" spans="1:5" x14ac:dyDescent="0.25">
@@ -60053,7 +60830,7 @@
         <v>4214</v>
       </c>
       <c r="E329" t="s">
-        <v>4401</v>
+        <v>4400</v>
       </c>
     </row>
     <row r="330" spans="1:5" x14ac:dyDescent="0.25">
@@ -60070,7 +60847,7 @@
         <v>4214</v>
       </c>
       <c r="E330" t="s">
-        <v>4402</v>
+        <v>4401</v>
       </c>
     </row>
     <row r="331" spans="1:5" x14ac:dyDescent="0.25">
@@ -60087,7 +60864,7 @@
         <v>4214</v>
       </c>
       <c r="E331" t="s">
-        <v>4403</v>
+        <v>4402</v>
       </c>
     </row>
     <row r="332" spans="1:5" x14ac:dyDescent="0.25">
@@ -60104,7 +60881,7 @@
         <v>4214</v>
       </c>
       <c r="E332" t="s">
-        <v>4404</v>
+        <v>4403</v>
       </c>
     </row>
     <row r="333" spans="1:5" x14ac:dyDescent="0.25">
@@ -60121,7 +60898,7 @@
         <v>4214</v>
       </c>
       <c r="E333" t="s">
-        <v>4405</v>
+        <v>4404</v>
       </c>
     </row>
     <row r="334" spans="1:5" x14ac:dyDescent="0.25">
@@ -60138,7 +60915,7 @@
         <v>4214</v>
       </c>
       <c r="E334" t="s">
-        <v>4406</v>
+        <v>4405</v>
       </c>
     </row>
     <row r="335" spans="1:5" x14ac:dyDescent="0.25">
@@ -60155,7 +60932,7 @@
         <v>4214</v>
       </c>
       <c r="E335" t="s">
-        <v>4407</v>
+        <v>4406</v>
       </c>
     </row>
     <row r="336" spans="1:5" x14ac:dyDescent="0.25">
@@ -60172,7 +60949,7 @@
         <v>4214</v>
       </c>
       <c r="E336" t="s">
-        <v>4408</v>
+        <v>4407</v>
       </c>
     </row>
     <row r="337" spans="1:5" x14ac:dyDescent="0.25">
@@ -60189,7 +60966,7 @@
         <v>4214</v>
       </c>
       <c r="E337" t="s">
-        <v>4409</v>
+        <v>4408</v>
       </c>
     </row>
     <row r="338" spans="1:5" x14ac:dyDescent="0.25">
@@ -60206,7 +60983,7 @@
         <v>4214</v>
       </c>
       <c r="E338" t="s">
-        <v>4410</v>
+        <v>4409</v>
       </c>
     </row>
     <row r="339" spans="1:5" x14ac:dyDescent="0.25">
@@ -60223,7 +61000,7 @@
         <v>4214</v>
       </c>
       <c r="E339" t="s">
-        <v>4411</v>
+        <v>4410</v>
       </c>
     </row>
     <row r="340" spans="1:5" x14ac:dyDescent="0.25">
@@ -60240,7 +61017,7 @@
         <v>4214</v>
       </c>
       <c r="E340" t="s">
-        <v>4412</v>
+        <v>4411</v>
       </c>
     </row>
     <row r="341" spans="1:5" x14ac:dyDescent="0.25">
@@ -60257,7 +61034,7 @@
         <v>4214</v>
       </c>
       <c r="E341" t="s">
-        <v>4413</v>
+        <v>4412</v>
       </c>
     </row>
     <row r="342" spans="1:5" x14ac:dyDescent="0.25">
@@ -60274,7 +61051,7 @@
         <v>4214</v>
       </c>
       <c r="E342" t="s">
-        <v>4414</v>
+        <v>4413</v>
       </c>
     </row>
     <row r="343" spans="1:5" x14ac:dyDescent="0.25">
@@ -60291,7 +61068,7 @@
         <v>4214</v>
       </c>
       <c r="E343" t="s">
-        <v>4415</v>
+        <v>4414</v>
       </c>
     </row>
     <row r="344" spans="1:5" x14ac:dyDescent="0.25">
@@ -60308,7 +61085,7 @@
         <v>4214</v>
       </c>
       <c r="E344" t="s">
-        <v>4416</v>
+        <v>4415</v>
       </c>
     </row>
     <row r="345" spans="1:5" x14ac:dyDescent="0.25">
@@ -60325,7 +61102,7 @@
         <v>4214</v>
       </c>
       <c r="E345" t="s">
-        <v>4417</v>
+        <v>4416</v>
       </c>
     </row>
     <row r="346" spans="1:5" x14ac:dyDescent="0.25">
@@ -60342,7 +61119,7 @@
         <v>4214</v>
       </c>
       <c r="E346" t="s">
-        <v>4418</v>
+        <v>4417</v>
       </c>
     </row>
     <row r="347" spans="1:5" x14ac:dyDescent="0.25">
@@ -60359,7 +61136,7 @@
         <v>4214</v>
       </c>
       <c r="E347" t="s">
-        <v>4419</v>
+        <v>4418</v>
       </c>
     </row>
     <row r="348" spans="1:5" x14ac:dyDescent="0.25">
@@ -60376,7 +61153,7 @@
         <v>4214</v>
       </c>
       <c r="E348" t="s">
-        <v>4420</v>
+        <v>4419</v>
       </c>
     </row>
     <row r="349" spans="1:5" x14ac:dyDescent="0.25">
@@ -60393,7 +61170,7 @@
         <v>4214</v>
       </c>
       <c r="E349" t="s">
-        <v>4421</v>
+        <v>4420</v>
       </c>
     </row>
     <row r="350" spans="1:5" x14ac:dyDescent="0.25">
@@ -60410,7 +61187,7 @@
         <v>4214</v>
       </c>
       <c r="E350" t="s">
-        <v>4422</v>
+        <v>4421</v>
       </c>
     </row>
     <row r="351" spans="1:5" x14ac:dyDescent="0.25">
@@ -60427,7 +61204,7 @@
         <v>4214</v>
       </c>
       <c r="E351" t="s">
-        <v>4423</v>
+        <v>4422</v>
       </c>
     </row>
     <row r="352" spans="1:5" x14ac:dyDescent="0.25">
@@ -60444,7 +61221,7 @@
         <v>4214</v>
       </c>
       <c r="E352" t="s">
-        <v>4424</v>
+        <v>4423</v>
       </c>
     </row>
     <row r="353" spans="1:5" x14ac:dyDescent="0.25">
@@ -60461,7 +61238,7 @@
         <v>4214</v>
       </c>
       <c r="E353" t="s">
-        <v>4425</v>
+        <v>4424</v>
       </c>
     </row>
     <row r="354" spans="1:5" x14ac:dyDescent="0.25">
@@ -60478,7 +61255,7 @@
         <v>4214</v>
       </c>
       <c r="E354" t="s">
-        <v>4426</v>
+        <v>4425</v>
       </c>
     </row>
     <row r="355" spans="1:5" x14ac:dyDescent="0.25">
@@ -60495,7 +61272,7 @@
         <v>4214</v>
       </c>
       <c r="E355" t="s">
-        <v>4427</v>
+        <v>4426</v>
       </c>
     </row>
     <row r="356" spans="1:5" x14ac:dyDescent="0.25">
@@ -60512,7 +61289,7 @@
         <v>4214</v>
       </c>
       <c r="E356" t="s">
-        <v>4428</v>
+        <v>4427</v>
       </c>
     </row>
     <row r="357" spans="1:5" x14ac:dyDescent="0.25">
@@ -60529,7 +61306,7 @@
         <v>4214</v>
       </c>
       <c r="E357" t="s">
-        <v>4429</v>
+        <v>4428</v>
       </c>
     </row>
     <row r="358" spans="1:5" x14ac:dyDescent="0.25">
@@ -60546,7 +61323,7 @@
         <v>4214</v>
       </c>
       <c r="E358" t="s">
-        <v>4430</v>
+        <v>4429</v>
       </c>
     </row>
     <row r="359" spans="1:5" x14ac:dyDescent="0.25">
@@ -60563,7 +61340,7 @@
         <v>4214</v>
       </c>
       <c r="E359" t="s">
-        <v>4431</v>
+        <v>4430</v>
       </c>
     </row>
     <row r="360" spans="1:5" x14ac:dyDescent="0.25">
@@ -60580,7 +61357,7 @@
         <v>4214</v>
       </c>
       <c r="E360" t="s">
-        <v>4432</v>
+        <v>4431</v>
       </c>
     </row>
     <row r="361" spans="1:5" x14ac:dyDescent="0.25">
@@ -60597,7 +61374,7 @@
         <v>4214</v>
       </c>
       <c r="E361" t="s">
-        <v>4433</v>
+        <v>4432</v>
       </c>
     </row>
     <row r="362" spans="1:5" x14ac:dyDescent="0.25">
@@ -60614,7 +61391,7 @@
         <v>4214</v>
       </c>
       <c r="E362" t="s">
-        <v>4434</v>
+        <v>4433</v>
       </c>
     </row>
     <row r="363" spans="1:5" x14ac:dyDescent="0.25">
@@ -60631,7 +61408,7 @@
         <v>4214</v>
       </c>
       <c r="E363" t="s">
-        <v>4435</v>
+        <v>4434</v>
       </c>
     </row>
     <row r="364" spans="1:5" x14ac:dyDescent="0.25">
@@ -60648,7 +61425,7 @@
         <v>4214</v>
       </c>
       <c r="E364" t="s">
-        <v>4436</v>
+        <v>4435</v>
       </c>
     </row>
     <row r="365" spans="1:5" x14ac:dyDescent="0.25">
@@ -60665,7 +61442,7 @@
         <v>4214</v>
       </c>
       <c r="E365" t="s">
-        <v>4437</v>
+        <v>4436</v>
       </c>
     </row>
     <row r="366" spans="1:5" x14ac:dyDescent="0.25">
@@ -60682,7 +61459,7 @@
         <v>4214</v>
       </c>
       <c r="E366" t="s">
-        <v>4438</v>
+        <v>4437</v>
       </c>
     </row>
     <row r="367" spans="1:5" x14ac:dyDescent="0.25">
@@ -60699,7 +61476,7 @@
         <v>4214</v>
       </c>
       <c r="E367" t="s">
-        <v>4439</v>
+        <v>4438</v>
       </c>
     </row>
     <row r="368" spans="1:5" x14ac:dyDescent="0.25">
@@ -60716,7 +61493,7 @@
         <v>4214</v>
       </c>
       <c r="E368" t="s">
-        <v>4440</v>
+        <v>4439</v>
       </c>
     </row>
     <row r="369" spans="1:5" x14ac:dyDescent="0.25">
@@ -60733,7 +61510,7 @@
         <v>4214</v>
       </c>
       <c r="E369" t="s">
-        <v>4441</v>
+        <v>4440</v>
       </c>
     </row>
     <row r="370" spans="1:5" x14ac:dyDescent="0.25">
@@ -60750,7 +61527,7 @@
         <v>4214</v>
       </c>
       <c r="E370" t="s">
-        <v>4442</v>
+        <v>4441</v>
       </c>
     </row>
     <row r="371" spans="1:5" x14ac:dyDescent="0.25">
@@ -60767,7 +61544,7 @@
         <v>4214</v>
       </c>
       <c r="E371" t="s">
-        <v>4443</v>
+        <v>4442</v>
       </c>
     </row>
     <row r="372" spans="1:5" x14ac:dyDescent="0.25">
@@ -60784,7 +61561,7 @@
         <v>4214</v>
       </c>
       <c r="E372" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="373" spans="1:5" x14ac:dyDescent="0.25">
@@ -60801,7 +61578,7 @@
         <v>4214</v>
       </c>
       <c r="E373" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="374" spans="1:5" x14ac:dyDescent="0.25">
@@ -60818,7 +61595,7 @@
         <v>4214</v>
       </c>
       <c r="E374" t="s">
-        <v>4446</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="375" spans="1:5" x14ac:dyDescent="0.25">
@@ -60835,7 +61612,7 @@
         <v>4214</v>
       </c>
       <c r="E375" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="376" spans="1:5" x14ac:dyDescent="0.25">
@@ -60852,7 +61629,7 @@
         <v>4214</v>
       </c>
       <c r="E376" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="377" spans="1:5" x14ac:dyDescent="0.25">
@@ -60869,7 +61646,7 @@
         <v>4214</v>
       </c>
       <c r="E377" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="378" spans="1:5" x14ac:dyDescent="0.25">
@@ -60886,7 +61663,7 @@
         <v>4214</v>
       </c>
       <c r="E378" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="379" spans="1:5" x14ac:dyDescent="0.25">
@@ -60903,7 +61680,7 @@
         <v>4214</v>
       </c>
       <c r="E379" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="380" spans="1:5" x14ac:dyDescent="0.25">
@@ -60920,7 +61697,7 @@
         <v>4214</v>
       </c>
       <c r="E380" t="s">
-        <v>4452</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="381" spans="1:5" x14ac:dyDescent="0.25">
@@ -60937,7 +61714,7 @@
         <v>4214</v>
       </c>
       <c r="E381" t="s">
-        <v>4453</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="382" spans="1:5" x14ac:dyDescent="0.25">
@@ -60954,7 +61731,7 @@
         <v>4214</v>
       </c>
       <c r="E382" t="s">
-        <v>4454</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="383" spans="1:5" x14ac:dyDescent="0.25">
@@ -60971,7 +61748,7 @@
         <v>4214</v>
       </c>
       <c r="E383" t="s">
-        <v>4455</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="384" spans="1:5" x14ac:dyDescent="0.25">
@@ -60988,7 +61765,7 @@
         <v>4214</v>
       </c>
       <c r="E384" t="s">
-        <v>4456</v>
+        <v>4455</v>
       </c>
     </row>
     <row r="385" spans="1:5" x14ac:dyDescent="0.25">
@@ -61005,7 +61782,7 @@
         <v>4214</v>
       </c>
       <c r="E385" t="s">
-        <v>4457</v>
+        <v>4456</v>
       </c>
     </row>
     <row r="386" spans="1:5" x14ac:dyDescent="0.25">
@@ -61022,7 +61799,7 @@
         <v>4214</v>
       </c>
       <c r="E386" t="s">
-        <v>4458</v>
+        <v>4457</v>
       </c>
     </row>
     <row r="387" spans="1:5" x14ac:dyDescent="0.25">
@@ -61753,7 +62530,7 @@
         <v>4214</v>
       </c>
       <c r="E438" t="s">
-        <v>4394</v>
+        <v>4393</v>
       </c>
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.25">
@@ -61770,7 +62547,7 @@
         <v>4214</v>
       </c>
       <c r="E439" t="s">
-        <v>4395</v>
+        <v>4394</v>
       </c>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.25">
@@ -61787,7 +62564,7 @@
         <v>4214</v>
       </c>
       <c r="E440" t="s">
-        <v>4396</v>
+        <v>4395</v>
       </c>
     </row>
     <row r="441" spans="1:5" x14ac:dyDescent="0.25">
@@ -61804,7 +62581,7 @@
         <v>4214</v>
       </c>
       <c r="E441" t="s">
-        <v>4397</v>
+        <v>4396</v>
       </c>
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.25">
@@ -61821,7 +62598,7 @@
         <v>4214</v>
       </c>
       <c r="E442" t="s">
-        <v>4398</v>
+        <v>4397</v>
       </c>
     </row>
     <row r="443" spans="1:5" x14ac:dyDescent="0.25">
@@ -62397,6 +63174,9 @@
       <c r="D483" t="s">
         <v>4214</v>
       </c>
+      <c r="E483" t="s">
+        <v>4361</v>
+      </c>
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
@@ -62411,6 +63191,9 @@
       <c r="D484" t="s">
         <v>4214</v>
       </c>
+      <c r="E484" t="s">
+        <v>4514</v>
+      </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
@@ -62425,6 +63208,9 @@
       <c r="D485" t="s">
         <v>4214</v>
       </c>
+      <c r="E485" t="s">
+        <v>4515</v>
+      </c>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
@@ -62439,6 +63225,9 @@
       <c r="D486" t="s">
         <v>4214</v>
       </c>
+      <c r="E486" t="s">
+        <v>4516</v>
+      </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
@@ -62453,6 +63242,9 @@
       <c r="D487" t="s">
         <v>4214</v>
       </c>
+      <c r="E487" t="s">
+        <v>4517</v>
+      </c>
     </row>
     <row r="488" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
@@ -62604,7 +63396,7 @@
         <v>4214</v>
       </c>
       <c r="E496" t="s">
-        <v>4368</v>
+        <v>4367</v>
       </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.25">
@@ -62621,7 +63413,7 @@
         <v>4214</v>
       </c>
       <c r="E497" t="s">
-        <v>4369</v>
+        <v>4368</v>
       </c>
     </row>
     <row r="498" spans="1:5" x14ac:dyDescent="0.25">
@@ -62672,7 +63464,7 @@
         <v>4214</v>
       </c>
       <c r="E500" t="s">
-        <v>4370</v>
+        <v>4369</v>
       </c>
     </row>
     <row r="501" spans="1:5" x14ac:dyDescent="0.25">
@@ -62774,7 +63566,7 @@
         <v>4214</v>
       </c>
       <c r="E506" t="s">
-        <v>4371</v>
+        <v>4370</v>
       </c>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.25">
@@ -62790,6 +63582,9 @@
       <c r="D507" t="s">
         <v>4214</v>
       </c>
+      <c r="E507" s="4" t="s">
+        <v>4519</v>
+      </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
@@ -62804,6 +63599,9 @@
       <c r="D508" t="s">
         <v>4214</v>
       </c>
+      <c r="E508" s="4" t="s">
+        <v>4520</v>
+      </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
@@ -62818,6 +63616,9 @@
       <c r="D509" t="s">
         <v>4214</v>
       </c>
+      <c r="E509" s="4" t="s">
+        <v>4521</v>
+      </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
@@ -62832,6 +63633,9 @@
       <c r="D510" t="s">
         <v>4214</v>
       </c>
+      <c r="E510" s="4" t="s">
+        <v>4522</v>
+      </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
@@ -62846,6 +63650,9 @@
       <c r="D511" t="s">
         <v>4214</v>
       </c>
+      <c r="E511" s="4" t="s">
+        <v>4523</v>
+      </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
@@ -62860,8 +63667,11 @@
       <c r="D512" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="513" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E512" s="4" t="s">
+        <v>4524</v>
+      </c>
+    </row>
+    <row r="513" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
         <v>4246</v>
       </c>
@@ -62874,8 +63684,11 @@
       <c r="D513" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="514" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E513" s="4" t="s">
+        <v>4525</v>
+      </c>
+    </row>
+    <row r="514" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
         <v>4247</v>
       </c>
@@ -62888,8 +63701,11 @@
       <c r="D514" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="515" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E514" s="4" t="s">
+        <v>4526</v>
+      </c>
+    </row>
+    <row r="515" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
         <v>4248</v>
       </c>
@@ -62902,8 +63718,11 @@
       <c r="D515" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="516" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E515" s="4" t="s">
+        <v>4527</v>
+      </c>
+    </row>
+    <row r="516" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
         <v>4249</v>
       </c>
@@ -62916,8 +63735,11 @@
       <c r="D516" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="517" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E516" s="4" t="s">
+        <v>4528</v>
+      </c>
+    </row>
+    <row r="517" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
         <v>4255</v>
       </c>
@@ -62930,8 +63752,11 @@
       <c r="D517" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="518" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E517" s="4" t="s">
+        <v>4518</v>
+      </c>
+    </row>
+    <row r="518" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
         <v>4257</v>
       </c>
@@ -62945,7 +63770,7 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="519" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="519" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
         <v>4259</v>
       </c>
@@ -62958,8 +63783,11 @@
       <c r="D519" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="520" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E519" s="4" t="s">
+        <v>4529</v>
+      </c>
+    </row>
+    <row r="520" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
         <v>4260</v>
       </c>
@@ -62972,8 +63800,11 @@
       <c r="D520" t="s">
         <v>4214</v>
       </c>
-    </row>
-    <row r="521" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E520" s="4" t="s">
+        <v>4530</v>
+      </c>
+    </row>
+    <row r="521" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A521" s="14" t="s">
         <v>4211</v>
       </c>
@@ -62987,7 +63818,7 @@
         <v>4215</v>
       </c>
     </row>
-    <row r="522" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="522" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A522" s="14" t="s">
         <v>4209</v>
       </c>
@@ -63001,7 +63832,7 @@
         <v>4215</v>
       </c>
     </row>
-    <row r="523" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="523" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
         <v>4263</v>
       </c>
@@ -63015,7 +63846,7 @@
         <v>4215</v>
       </c>
     </row>
-    <row r="524" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="524" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A524" t="s">
         <v>4266</v>
       </c>
@@ -63029,7 +63860,7 @@
         <v>4215</v>
       </c>
     </row>
-    <row r="525" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="525" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A525" s="14">
         <v>1376</v>
       </c>
@@ -63042,8 +63873,11 @@
       <c r="D525" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="526" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E525" t="s">
+        <v>4531</v>
+      </c>
+    </row>
+    <row r="526" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A526" s="14">
         <v>1374</v>
       </c>
@@ -63057,7 +63891,7 @@
         <v>4217</v>
       </c>
     </row>
-    <row r="527" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="527" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A527" s="14">
         <v>1375</v>
       </c>
@@ -63070,8 +63904,11 @@
       <c r="D527" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="528" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E527" t="s">
+        <v>4532</v>
+      </c>
+    </row>
+    <row r="528" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A528" s="14">
         <v>1373</v>
       </c>
@@ -63084,8 +63921,11 @@
       <c r="D528" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="529" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E528" t="s">
+        <v>4533</v>
+      </c>
+    </row>
+    <row r="529" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A529" s="14">
         <v>1379</v>
       </c>
@@ -63099,7 +63939,7 @@
         <v>4217</v>
       </c>
     </row>
-    <row r="530" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="530" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A530" s="14">
         <v>1380</v>
       </c>
@@ -63113,7 +63953,7 @@
         <v>4217</v>
       </c>
     </row>
-    <row r="531" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="531" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A531" s="14">
         <v>1378</v>
       </c>
@@ -63127,7 +63967,7 @@
         <v>4217</v>
       </c>
     </row>
-    <row r="532" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="532" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A532" s="14">
         <v>20716</v>
       </c>
@@ -63141,7 +63981,7 @@
         <v>4217</v>
       </c>
     </row>
-    <row r="533" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="533" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A533" s="14">
         <v>20715</v>
       </c>
@@ -63155,7 +63995,7 @@
         <v>4217</v>
       </c>
     </row>
-    <row r="534" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="534" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A534" s="14">
         <v>20714</v>
       </c>
@@ -63169,7 +64009,7 @@
         <v>4217</v>
       </c>
     </row>
-    <row r="535" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="535" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A535" s="14">
         <v>27702</v>
       </c>
@@ -63182,8 +64022,11 @@
       <c r="D535" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="536" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E535" t="s">
+        <v>4541</v>
+      </c>
+    </row>
+    <row r="536" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A536" s="14">
         <v>27701</v>
       </c>
@@ -63196,8 +64039,11 @@
       <c r="D536" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="537" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E536" t="s">
+        <v>4540</v>
+      </c>
+    </row>
+    <row r="537" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A537" s="14">
         <v>20541</v>
       </c>
@@ -63210,8 +64056,11 @@
       <c r="D537" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="538" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E537" t="s">
+        <v>4542</v>
+      </c>
+    </row>
+    <row r="538" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A538" s="14">
         <v>20540</v>
       </c>
@@ -63224,8 +64073,11 @@
       <c r="D538" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="539" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E538" t="s">
+        <v>4543</v>
+      </c>
+    </row>
+    <row r="539" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A539" s="14">
         <v>20540</v>
       </c>
@@ -63238,8 +64090,11 @@
       <c r="D539" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="540" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E539" t="s">
+        <v>4533</v>
+      </c>
+    </row>
+    <row r="540" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A540" s="14">
         <v>20606</v>
       </c>
@@ -63253,7 +64108,7 @@
         <v>4217</v>
       </c>
     </row>
-    <row r="541" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="541" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A541" s="14">
         <v>20594</v>
       </c>
@@ -63267,7 +64122,7 @@
         <v>4217</v>
       </c>
     </row>
-    <row r="542" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="542" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A542" s="14">
         <v>25359</v>
       </c>
@@ -63281,7 +64136,7 @@
         <v>4217</v>
       </c>
     </row>
-    <row r="543" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="543" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A543" s="14">
         <v>20570</v>
       </c>
@@ -63295,7 +64150,7 @@
         <v>4217</v>
       </c>
     </row>
-    <row r="544" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="544" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A544" s="14">
         <v>20543</v>
       </c>
@@ -63309,7 +64164,7 @@
         <v>4217</v>
       </c>
     </row>
-    <row r="545" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="545" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A545" s="14">
         <v>21084</v>
       </c>
@@ -63323,7 +64178,7 @@
         <v>4217</v>
       </c>
     </row>
-    <row r="546" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A546" s="14">
         <v>21083</v>
       </c>
@@ -63337,7 +64192,7 @@
         <v>4217</v>
       </c>
     </row>
-    <row r="547" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="547" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A547" s="14">
         <v>13762</v>
       </c>
@@ -63350,8 +64205,11 @@
       <c r="D547" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="548" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E547" t="s">
+        <v>4535</v>
+      </c>
+    </row>
+    <row r="548" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A548" s="14">
         <v>4536</v>
       </c>
@@ -63364,8 +64222,11 @@
       <c r="D548" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="549" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E548" t="s">
+        <v>4536</v>
+      </c>
+    </row>
+    <row r="549" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A549" s="14">
         <v>4513</v>
       </c>
@@ -63378,8 +64239,11 @@
       <c r="D549" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="550" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E549" t="s">
+        <v>4537</v>
+      </c>
+    </row>
+    <row r="550" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A550" s="14">
         <v>5727</v>
       </c>
@@ -63392,8 +64256,11 @@
       <c r="D550" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="551" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E550" t="s">
+        <v>4539</v>
+      </c>
+    </row>
+    <row r="551" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A551" s="14">
         <v>5793</v>
       </c>
@@ -63406,8 +64273,11 @@
       <c r="D551" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="552" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E551" t="s">
+        <v>4538</v>
+      </c>
+    </row>
+    <row r="552" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A552" s="14">
         <v>13521</v>
       </c>
@@ -63420,8 +64290,11 @@
       <c r="D552" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="553" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E552" t="s">
+        <v>4534</v>
+      </c>
+    </row>
+    <row r="553" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A553" s="14">
         <v>28784</v>
       </c>
@@ -63434,13 +64307,16 @@
       <c r="D553" t="s">
         <v>4217</v>
       </c>
-    </row>
-    <row r="554" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E553" t="s">
+        <v>4533</v>
+      </c>
+    </row>
+    <row r="554" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A554" t="s">
-        <v>4374</v>
+        <v>4373</v>
       </c>
       <c r="B554" t="s">
-        <v>4381</v>
+        <v>4380</v>
       </c>
       <c r="C554" t="s">
         <v>3567</v>
@@ -63449,12 +64325,12 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="555" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="555" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A555" t="s">
-        <v>4375</v>
+        <v>4374</v>
       </c>
       <c r="B555" t="s">
-        <v>4382</v>
+        <v>4381</v>
       </c>
       <c r="C555" t="s">
         <v>3567</v>
@@ -63463,12 +64339,12 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="556" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="556" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A556" t="s">
-        <v>4373</v>
+        <v>4372</v>
       </c>
       <c r="B556" t="s">
-        <v>4383</v>
+        <v>4382</v>
       </c>
       <c r="C556" t="s">
         <v>3567</v>
@@ -63477,12 +64353,12 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="557" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="557" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A557" t="s">
-        <v>4372</v>
+        <v>4371</v>
       </c>
       <c r="B557" t="s">
-        <v>4384</v>
+        <v>4383</v>
       </c>
       <c r="C557" t="s">
         <v>3567</v>
@@ -63491,12 +64367,12 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="558" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="558" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A558" t="s">
-        <v>4376</v>
+        <v>4375</v>
       </c>
       <c r="B558" t="s">
-        <v>4385</v>
+        <v>4384</v>
       </c>
       <c r="C558" t="s">
         <v>3567</v>
@@ -63505,12 +64381,12 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="559" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="559" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
-        <v>4377</v>
+        <v>4376</v>
       </c>
       <c r="B559" t="s">
-        <v>4386</v>
+        <v>4385</v>
       </c>
       <c r="C559" t="s">
         <v>3567</v>
@@ -63519,12 +64395,12 @@
         <v>4214</v>
       </c>
     </row>
-    <row r="560" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="560" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
-        <v>4378</v>
+        <v>4377</v>
       </c>
       <c r="B560" t="s">
-        <v>4387</v>
+        <v>4386</v>
       </c>
       <c r="C560" t="s">
         <v>3567</v>
@@ -63535,10 +64411,10 @@
     </row>
     <row r="561" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
-        <v>4379</v>
+        <v>4378</v>
       </c>
       <c r="B561" t="s">
-        <v>4388</v>
+        <v>4387</v>
       </c>
       <c r="C561" t="s">
         <v>3567</v>
@@ -63549,10 +64425,10 @@
     </row>
     <row r="562" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
-        <v>4380</v>
+        <v>4379</v>
       </c>
       <c r="B562" t="s">
-        <v>4389</v>
+        <v>4388</v>
       </c>
       <c r="C562" t="s">
         <v>3567</v>
@@ -63563,10 +64439,10 @@
     </row>
     <row r="563" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
+        <v>4389</v>
+      </c>
+      <c r="B563" t="s">
         <v>4390</v>
-      </c>
-      <c r="B563" t="s">
-        <v>4391</v>
       </c>
       <c r="C563" t="s">
         <v>3567</v>
@@ -63577,10 +64453,10 @@
     </row>
     <row r="564" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
+        <v>4391</v>
+      </c>
+      <c r="B564" t="s">
         <v>4392</v>
-      </c>
-      <c r="B564" t="s">
-        <v>4393</v>
       </c>
       <c r="C564" t="s">
         <v>3567</v>

</xml_diff>

<commit_message>
Inclusão de melhorias @202406120932
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,23 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51289D5A-0863-4315-B848-018707D59B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A8989DD-76F2-4C92-B9EC-19797B625A7D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" tabRatio="699" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" tabRatio="699" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="equity_signals" sheetId="19" r:id="rId1"/>
-    <sheet name="index_signals" sheetId="14" r:id="rId2"/>
-    <sheet name="&gt;" sheetId="9" r:id="rId3"/>
-    <sheet name="equities" sheetId="3" r:id="rId4"/>
-    <sheet name="anbima" sheetId="13" r:id="rId5"/>
-    <sheet name="indicators" sheetId="22" r:id="rId6"/>
-    <sheet name="Planilha4" sheetId="4" r:id="rId7"/>
+    <sheet name="fixed_income_signals" sheetId="23" r:id="rId1"/>
+    <sheet name="equity_signals" sheetId="19" r:id="rId2"/>
+    <sheet name="index_signals" sheetId="14" r:id="rId3"/>
+    <sheet name="&gt;" sheetId="9" r:id="rId4"/>
+    <sheet name="equities" sheetId="3" r:id="rId5"/>
+    <sheet name="anbima" sheetId="13" r:id="rId6"/>
+    <sheet name="indicators" sheetId="22" r:id="rId7"/>
+    <sheet name="Planilha4" sheetId="4" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">equities!$A$1:$L$1268</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">equity_signals!$C$1:$C$79</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">indicators!$A$1:$E$564</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">equities!$A$1:$L$1268</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">equity_signals!$C$1:$C$79</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fixed_income_signals!$A$1:$C$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">indicators!$A$1:$E$564</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14087" uniqueCount="4615">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14132" uniqueCount="4643">
   <si>
     <t>bbgTicker</t>
   </si>
@@ -13892,6 +13894,90 @@
   </si>
   <si>
     <t>IPCA (9Y)</t>
+  </si>
+  <si>
+    <t>ISSUER</t>
+  </si>
+  <si>
+    <t>issuer</t>
+  </si>
+  <si>
+    <t>ISSUER_PARENT_EQY_TICKER</t>
+  </si>
+  <si>
+    <t>ISSUE_DT</t>
+  </si>
+  <si>
+    <t>AMT_ISSUED</t>
+  </si>
+  <si>
+    <t>amount_issued</t>
+  </si>
+  <si>
+    <t>issue_date</t>
+  </si>
+  <si>
+    <t>issuer_equity_code</t>
+  </si>
+  <si>
+    <t>CPN</t>
+  </si>
+  <si>
+    <t>coupon</t>
+  </si>
+  <si>
+    <t>coupon_frequency</t>
+  </si>
+  <si>
+    <t>CPN_FREQ</t>
+  </si>
+  <si>
+    <t>maturity</t>
+  </si>
+  <si>
+    <t>CRNCY</t>
+  </si>
+  <si>
+    <t>MATURITY</t>
+  </si>
+  <si>
+    <t>market_issue</t>
+  </si>
+  <si>
+    <t>MARKET_ISSUE</t>
+  </si>
+  <si>
+    <t>static</t>
+  </si>
+  <si>
+    <t>history</t>
+  </si>
+  <si>
+    <t>DUR_MID</t>
+  </si>
+  <si>
+    <t>DUR_ADJ_MID</t>
+  </si>
+  <si>
+    <t>modified_duration</t>
+  </si>
+  <si>
+    <t>macauley_duration</t>
+  </si>
+  <si>
+    <t>YLD_YTM_MID</t>
+  </si>
+  <si>
+    <t>yield_to_maturity</t>
+  </si>
+  <si>
+    <t>CALC_TYP_DES</t>
+  </si>
+  <si>
+    <t>index_type</t>
+  </si>
+  <si>
+    <t>PX_CLEAN_MID</t>
   </si>
 </sst>
 </file>
@@ -14336,11 +14422,233 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE9BFA3A-A372-440F-86E1-C70EDC1063D4}">
+  <dimension ref="A1:C78"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3357</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3419</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4615</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4616</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>4617</v>
+      </c>
+      <c r="B3" t="s">
+        <v>4622</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4618</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4621</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4619</v>
+      </c>
+      <c r="B5" t="s">
+        <v>4620</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>4623</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4624</v>
+      </c>
+      <c r="C6" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4626</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4625</v>
+      </c>
+      <c r="C7" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>4629</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4627</v>
+      </c>
+      <c r="C8" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4628</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3565</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4631</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4630</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>4634</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4636</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4633</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>4635</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4637</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4633</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4638</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4639</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4633</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>4640</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4641</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4632</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4642</v>
+      </c>
+      <c r="B15" t="s">
+        <v>3373</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4633</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="4"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B44" s="4"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B45" s="4"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B53" s="4"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B54" s="4"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B55" s="4"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B56" s="4"/>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="3"/>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="3"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:C14" xr:uid="{FE9BFA3A-A372-440F-86E1-C70EDC1063D4}"/>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A53" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
     </sheetView>
   </sheetViews>
@@ -15001,7 +15309,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr codeName="Planilha7"/>
   <dimension ref="A1:C16"/>
@@ -15142,7 +15450,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Planilha8">
     <tabColor theme="9" tint="0.79998168889431442"/>
@@ -15159,7 +15467,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Planilha10"/>
   <dimension ref="A1:N1269"/>
@@ -55198,7 +55506,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr codeName="Planilha11"/>
   <dimension ref="A1:B34"/>
@@ -55490,13 +55798,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2CB12C5-8725-4AAE-9F74-FA739078C419}">
   <dimension ref="A1:E564"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A477" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B492" sqref="B492"/>
+      <selection pane="bottomLeft" activeCell="B480" sqref="B480"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64472,7 +64780,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr codeName="Planilha12"/>
   <dimension ref="A1:D19"/>

</xml_diff>

<commit_message>
Inclusão de melhorias @202406131219
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D74E18CB-9FB6-4E0B-9988-D6767D1C6587}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB22F36F-8736-475A-AF9C-689B237BDAB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" tabRatio="699" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,6 +29,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">indicators!$A$1:$E$566</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -49,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14172" uniqueCount="4666">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14286" uniqueCount="4763">
   <si>
     <t>bbgTicker</t>
   </si>
@@ -14047,6 +14048,297 @@
   </si>
   <si>
     <t>PJ (Direcionados)</t>
+  </si>
+  <si>
+    <t>Expectativas</t>
+  </si>
+  <si>
+    <t>Atual</t>
+  </si>
+  <si>
+    <t>Índice de Incerteza Econômica</t>
+  </si>
+  <si>
+    <t>FIPE (Índice)</t>
+  </si>
+  <si>
+    <t>FIPE (% MoM)</t>
+  </si>
+  <si>
+    <t>FIPE (% YoY)</t>
+  </si>
+  <si>
+    <t>IPCA Expectativas Focus (12m % YoY)</t>
+  </si>
+  <si>
+    <t>IPCA Expectativas Focus (12m % YoY) - Suavizado</t>
+  </si>
+  <si>
+    <t>IPCA Livres (% YoY)</t>
+  </si>
+  <si>
+    <t>IPCA Administrados (% YoY)</t>
+  </si>
+  <si>
+    <t>Alimentação e Bebidas</t>
+  </si>
+  <si>
+    <t>Educação</t>
+  </si>
+  <si>
+    <t>Vestuário</t>
+  </si>
+  <si>
+    <t>Saúde e Cuidados Pessoais</t>
+  </si>
+  <si>
+    <t>Habitação</t>
+  </si>
+  <si>
+    <t>Artigos de Residência</t>
+  </si>
+  <si>
+    <t>Transportes</t>
+  </si>
+  <si>
+    <t>Comunicação</t>
+  </si>
+  <si>
+    <t>Duráveis</t>
+  </si>
+  <si>
+    <t>Não-Duráveis</t>
+  </si>
+  <si>
+    <t>Despesas Pessoais</t>
+  </si>
+  <si>
+    <t>Serviços</t>
+  </si>
+  <si>
+    <t>Semi-Duráveis</t>
+  </si>
+  <si>
+    <t>Conta Corrente  / PIB</t>
+  </si>
+  <si>
+    <t>Conta Corrente  (12m)</t>
+  </si>
+  <si>
+    <t>Exportação</t>
+  </si>
+  <si>
+    <t>Importação</t>
+  </si>
+  <si>
+    <t>Índice (% YoY)</t>
+  </si>
+  <si>
+    <t>Índice Ampliado</t>
+  </si>
+  <si>
+    <t>Índice Ampliado (% YoY)</t>
+  </si>
+  <si>
+    <t>Combustíveis</t>
+  </si>
+  <si>
+    <t>Farmácias</t>
+  </si>
+  <si>
+    <t>Vestuário e calçados</t>
+  </si>
+  <si>
+    <t>Outros</t>
+  </si>
+  <si>
+    <t>Livros e Revistas</t>
+  </si>
+  <si>
+    <t>Móveis e Eletrodomésticos</t>
+  </si>
+  <si>
+    <t>Atacado de Produtos Alimentícios</t>
+  </si>
+  <si>
+    <t>Mmateriais para Escritório</t>
+  </si>
+  <si>
+    <t>Supermercados</t>
+  </si>
+  <si>
+    <t>Cartão de Crédito</t>
+  </si>
+  <si>
+    <t>Empresas</t>
+  </si>
+  <si>
+    <t>Consumidor</t>
+  </si>
+  <si>
+    <t>CPI (Índice)</t>
+  </si>
+  <si>
+    <t>CPI (% MoM)</t>
+  </si>
+  <si>
+    <t>CPI (% YoY)</t>
+  </si>
+  <si>
+    <t>Core CPI (Índice)</t>
+  </si>
+  <si>
+    <t>Core CPI (% MoM)</t>
+  </si>
+  <si>
+    <t>Core CPI (% YoY)</t>
+  </si>
+  <si>
+    <t>Core PCE (% YoY)</t>
+  </si>
+  <si>
+    <t>ISM Services</t>
+  </si>
+  <si>
+    <t>New Orders</t>
+  </si>
+  <si>
+    <t>Prices Paid</t>
+  </si>
+  <si>
+    <t>Employment</t>
+  </si>
+  <si>
+    <t>Inventories</t>
+  </si>
+  <si>
+    <t>CPI UMich (12m % YoY)</t>
+  </si>
+  <si>
+    <t>IG Spread (10Y)</t>
+  </si>
+  <si>
+    <t>IG Spread (5Y)</t>
+  </si>
+  <si>
+    <t>IG Yield (10Y)</t>
+  </si>
+  <si>
+    <t>IG Yield (5Y)</t>
+  </si>
+  <si>
+    <t>HY Spread (10Y)</t>
+  </si>
+  <si>
+    <t>HY Yield (10Y)</t>
+  </si>
+  <si>
+    <t>HY Spread (5Y)</t>
+  </si>
+  <si>
+    <t>HY Yield (5Y)</t>
+  </si>
+  <si>
+    <t>Implícita (10Y)</t>
+  </si>
+  <si>
+    <t>Implícita (1Y)</t>
+  </si>
+  <si>
+    <t>Implícita (20Y)</t>
+  </si>
+  <si>
+    <t>Implícita (2Y)</t>
+  </si>
+  <si>
+    <t>Implícita (3Y)</t>
+  </si>
+  <si>
+    <t>Implícita (5Y)</t>
+  </si>
+  <si>
+    <t>Implícita (6Y)</t>
+  </si>
+  <si>
+    <t>Implícita (7Y)</t>
+  </si>
+  <si>
+    <t>Veículos Pesados</t>
+  </si>
+  <si>
+    <t>Veículos Pesados (% YoY)</t>
+  </si>
+  <si>
+    <t>Veículos Leves</t>
+  </si>
+  <si>
+    <t>Veículos Leves (% YoY)</t>
+  </si>
+  <si>
+    <t>2-10Y</t>
+  </si>
+  <si>
+    <t>5-10Y</t>
+  </si>
+  <si>
+    <t>5-30Y</t>
+  </si>
+  <si>
+    <t>Pedidos Contínuos</t>
+  </si>
+  <si>
+    <t>Pedidos Iniciais</t>
+  </si>
+  <si>
+    <t>Pedidos Iniciais (4WMA)</t>
+  </si>
+  <si>
+    <t>Pedidos Iniciais (NSA)</t>
+  </si>
+  <si>
+    <t>Taxa de Contratação</t>
+  </si>
+  <si>
+    <t>Taxa de Saídas Voluntárias</t>
+  </si>
+  <si>
+    <t>Abertura de Vagas</t>
+  </si>
+  <si>
+    <t>Taxa de Abertura de Vagas</t>
+  </si>
+  <si>
+    <t>PCE (% YoY)</t>
+  </si>
+  <si>
+    <t>PPI (Índice)</t>
+  </si>
+  <si>
+    <t>PPI (% MoM)</t>
+  </si>
+  <si>
+    <t>PPI (% YoY)</t>
+  </si>
+  <si>
+    <t>Supercore (Índice)</t>
+  </si>
+  <si>
+    <t>Supercore (% MoM)</t>
+  </si>
+  <si>
+    <t>Supercore (% YoY)</t>
+  </si>
+  <si>
+    <t>Case-Shiller Home Price Index</t>
+  </si>
+  <si>
+    <t>Case-Shiller Home Price Index (% YoY)</t>
+  </si>
+  <si>
+    <t>Case-Shiller Home Price Index 20-City</t>
+  </si>
+  <si>
+    <t>Case-Shiller Home Price Index 20-City (% YoY)</t>
   </si>
 </sst>
 </file>
@@ -55872,8 +56164,8 @@
   <dimension ref="A1:E566"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A516" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B543" sqref="B543"/>
+      <pane ySplit="1" topLeftCell="A398" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B410" sqref="B410"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57052,6 +57344,9 @@
       <c r="D70" t="s">
         <v>4213</v>
       </c>
+      <c r="E70" t="s">
+        <v>4339</v>
+      </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
@@ -58481,6 +58776,9 @@
       <c r="D156" t="s">
         <v>4213</v>
       </c>
+      <c r="E156" t="s">
+        <v>4737</v>
+      </c>
     </row>
     <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
@@ -58495,6 +58793,9 @@
       <c r="D157" t="s">
         <v>4213</v>
       </c>
+      <c r="E157" t="s">
+        <v>4738</v>
+      </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
@@ -58509,6 +58810,9 @@
       <c r="D158" t="s">
         <v>4213</v>
       </c>
+      <c r="E158" t="s">
+        <v>4739</v>
+      </c>
     </row>
     <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
@@ -58523,6 +58827,9 @@
       <c r="D159" t="s">
         <v>4213</v>
       </c>
+      <c r="E159" t="s">
+        <v>4740</v>
+      </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
@@ -58678,6 +58985,9 @@
       <c r="D169" t="s">
         <v>4213</v>
       </c>
+      <c r="E169" t="s">
+        <v>4669</v>
+      </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
@@ -58692,6 +59002,9 @@
       <c r="D170" t="s">
         <v>4213</v>
       </c>
+      <c r="E170" t="s">
+        <v>4670</v>
+      </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
@@ -58706,6 +59019,9 @@
       <c r="D171" t="s">
         <v>4213</v>
       </c>
+      <c r="E171" t="s">
+        <v>4671</v>
+      </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
@@ -58720,6 +59036,9 @@
       <c r="D172" t="s">
         <v>4213</v>
       </c>
+      <c r="E172" t="s">
+        <v>4690</v>
+      </c>
     </row>
     <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
@@ -58734,6 +59053,9 @@
       <c r="D173" t="s">
         <v>4213</v>
       </c>
+      <c r="E173" t="s">
+        <v>4689</v>
+      </c>
     </row>
     <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
@@ -58748,6 +59070,9 @@
       <c r="D174" t="s">
         <v>4213</v>
       </c>
+      <c r="E174" t="s">
+        <v>4667</v>
+      </c>
     </row>
     <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
@@ -58762,6 +59087,9 @@
       <c r="D175" t="s">
         <v>4213</v>
       </c>
+      <c r="E175" t="s">
+        <v>4666</v>
+      </c>
     </row>
     <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
@@ -58776,6 +59104,9 @@
       <c r="D176" t="s">
         <v>4213</v>
       </c>
+      <c r="E176" t="s">
+        <v>4303</v>
+      </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
@@ -58790,6 +59121,9 @@
       <c r="D177" t="s">
         <v>4213</v>
       </c>
+      <c r="E177" t="s">
+        <v>4667</v>
+      </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
@@ -58804,6 +59138,9 @@
       <c r="D178" t="s">
         <v>4213</v>
       </c>
+      <c r="E178" t="s">
+        <v>4666</v>
+      </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
@@ -58818,6 +59155,9 @@
       <c r="D179" t="s">
         <v>4213</v>
       </c>
+      <c r="E179" t="s">
+        <v>4303</v>
+      </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
@@ -58832,6 +59172,9 @@
       <c r="D180" t="s">
         <v>4213</v>
       </c>
+      <c r="E180" t="s">
+        <v>4668</v>
+      </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
@@ -58846,6 +59189,9 @@
       <c r="D181" t="s">
         <v>4213</v>
       </c>
+      <c r="E181" t="s">
+        <v>4667</v>
+      </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
@@ -58860,6 +59206,9 @@
       <c r="D182" t="s">
         <v>4213</v>
       </c>
+      <c r="E182" t="s">
+        <v>4666</v>
+      </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
@@ -58874,6 +59223,9 @@
       <c r="D183" t="s">
         <v>4213</v>
       </c>
+      <c r="E183" t="s">
+        <v>4303</v>
+      </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
@@ -58916,6 +59268,9 @@
       <c r="D186" t="s">
         <v>4213</v>
       </c>
+      <c r="E186" t="s">
+        <v>4672</v>
+      </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
@@ -58930,6 +59285,9 @@
       <c r="D187" t="s">
         <v>4213</v>
       </c>
+      <c r="E187" t="s">
+        <v>4673</v>
+      </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
@@ -60148,6 +60506,9 @@
       <c r="D259" t="s">
         <v>4213</v>
       </c>
+      <c r="E259" t="s">
+        <v>4678</v>
+      </c>
     </row>
     <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
@@ -60162,6 +60523,9 @@
       <c r="D260" t="s">
         <v>4213</v>
       </c>
+      <c r="E260" t="s">
+        <v>4683</v>
+      </c>
     </row>
     <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
@@ -60176,6 +60540,9 @@
       <c r="D261" t="s">
         <v>4213</v>
       </c>
+      <c r="E261" t="s">
+        <v>4684</v>
+      </c>
     </row>
     <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
@@ -60190,6 +60557,9 @@
       <c r="D262" t="s">
         <v>4213</v>
       </c>
+      <c r="E262" t="s">
+        <v>4677</v>
+      </c>
     </row>
     <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
@@ -60204,6 +60574,9 @@
       <c r="D263" t="s">
         <v>4213</v>
       </c>
+      <c r="E263" t="s">
+        <v>4676</v>
+      </c>
     </row>
     <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
@@ -60218,6 +60591,9 @@
       <c r="D264" t="s">
         <v>4213</v>
       </c>
+      <c r="E264" t="s">
+        <v>4679</v>
+      </c>
     </row>
     <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
@@ -60232,6 +60608,9 @@
       <c r="D265" t="s">
         <v>4213</v>
       </c>
+      <c r="E265" t="s">
+        <v>4681</v>
+      </c>
     </row>
     <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
@@ -60246,6 +60625,9 @@
       <c r="D266" t="s">
         <v>4213</v>
       </c>
+      <c r="E266" t="s">
+        <v>4680</v>
+      </c>
     </row>
     <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
@@ -60294,6 +60676,9 @@
       <c r="D269" t="s">
         <v>4213</v>
       </c>
+      <c r="E269" t="s">
+        <v>4685</v>
+      </c>
     </row>
     <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
@@ -60308,6 +60693,9 @@
       <c r="D270" t="s">
         <v>4213</v>
       </c>
+      <c r="E270" t="s">
+        <v>4674</v>
+      </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
@@ -60322,6 +60710,9 @@
       <c r="D271" t="s">
         <v>4213</v>
       </c>
+      <c r="E271" t="s">
+        <v>4686</v>
+      </c>
     </row>
     <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
@@ -60336,6 +60727,9 @@
       <c r="D272" t="s">
         <v>4213</v>
       </c>
+      <c r="E272" t="s">
+        <v>4675</v>
+      </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
@@ -60350,6 +60744,9 @@
       <c r="D273" t="s">
         <v>4213</v>
       </c>
+      <c r="E273" t="s">
+        <v>4688</v>
+      </c>
     </row>
     <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
@@ -60364,6 +60761,9 @@
       <c r="D274" t="s">
         <v>4213</v>
       </c>
+      <c r="E274" t="s">
+        <v>4687</v>
+      </c>
     </row>
     <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
@@ -60378,6 +60778,9 @@
       <c r="D275" t="s">
         <v>4213</v>
       </c>
+      <c r="E275" t="s">
+        <v>4682</v>
+      </c>
     </row>
     <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
@@ -60443,6 +60846,9 @@
       <c r="D279" t="s">
         <v>4213</v>
       </c>
+      <c r="E279" t="s">
+        <v>4700</v>
+      </c>
     </row>
     <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
@@ -60457,6 +60863,9 @@
       <c r="D280" t="s">
         <v>4213</v>
       </c>
+      <c r="E280" t="s">
+        <v>4702</v>
+      </c>
     </row>
     <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
@@ -60471,6 +60880,9 @@
       <c r="D281" t="s">
         <v>4213</v>
       </c>
+      <c r="E281" t="s">
+        <v>4696</v>
+      </c>
     </row>
     <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
@@ -60485,6 +60897,9 @@
       <c r="D282" t="s">
         <v>4213</v>
       </c>
+      <c r="E282" t="s">
+        <v>4701</v>
+      </c>
     </row>
     <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
@@ -60499,6 +60914,9 @@
       <c r="D283" t="s">
         <v>4213</v>
       </c>
+      <c r="E283" t="s">
+        <v>4703</v>
+      </c>
     </row>
     <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
@@ -60513,6 +60931,9 @@
       <c r="D284" t="s">
         <v>4213</v>
       </c>
+      <c r="E284" t="s">
+        <v>4699</v>
+      </c>
     </row>
     <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
@@ -60527,6 +60948,9 @@
       <c r="D285" t="s">
         <v>4213</v>
       </c>
+      <c r="E285" t="s">
+        <v>4697</v>
+      </c>
     </row>
     <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
@@ -60541,6 +60965,9 @@
       <c r="D286" t="s">
         <v>4213</v>
       </c>
+      <c r="E286" t="s">
+        <v>4704</v>
+      </c>
     </row>
     <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
@@ -60555,6 +60982,9 @@
       <c r="D287" t="s">
         <v>4213</v>
       </c>
+      <c r="E287" t="s">
+        <v>4698</v>
+      </c>
     </row>
     <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
@@ -60569,6 +60999,9 @@
       <c r="D288" t="s">
         <v>4213</v>
       </c>
+      <c r="E288" t="s">
+        <v>4694</v>
+      </c>
     </row>
     <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
@@ -60583,6 +61016,9 @@
       <c r="D289" t="s">
         <v>4213</v>
       </c>
+      <c r="E289" t="s">
+        <v>4695</v>
+      </c>
     </row>
     <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
@@ -60597,6 +61033,9 @@
       <c r="D290" t="s">
         <v>4213</v>
       </c>
+      <c r="E290" t="s">
+        <v>4303</v>
+      </c>
     </row>
     <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
@@ -60611,6 +61050,9 @@
       <c r="D291" t="s">
         <v>4213</v>
       </c>
+      <c r="E291" t="s">
+        <v>4693</v>
+      </c>
     </row>
     <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
@@ -60873,6 +61315,9 @@
       <c r="D308" t="s">
         <v>4213</v>
       </c>
+      <c r="E308" t="s">
+        <v>4691</v>
+      </c>
     </row>
     <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
@@ -60887,6 +61332,9 @@
       <c r="D309" t="s">
         <v>4213</v>
       </c>
+      <c r="E309" t="s">
+        <v>4692</v>
+      </c>
     </row>
     <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
@@ -62192,6 +62640,9 @@
       <c r="D387" t="s">
         <v>4213</v>
       </c>
+      <c r="E387" t="s">
+        <v>4741</v>
+      </c>
     </row>
     <row r="388" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
@@ -62206,6 +62657,9 @@
       <c r="D388" t="s">
         <v>4213</v>
       </c>
+      <c r="E388" t="s">
+        <v>4742</v>
+      </c>
     </row>
     <row r="389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
@@ -62220,6 +62674,9 @@
       <c r="D389" t="s">
         <v>4213</v>
       </c>
+      <c r="E389" t="s">
+        <v>4743</v>
+      </c>
     </row>
     <row r="390" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
@@ -62346,6 +62803,9 @@
       <c r="D398" t="s">
         <v>4213</v>
       </c>
+      <c r="E398" t="s">
+        <v>4729</v>
+      </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
@@ -62360,6 +62820,9 @@
       <c r="D399" t="s">
         <v>4213</v>
       </c>
+      <c r="E399" t="s">
+        <v>4730</v>
+      </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
@@ -62374,8 +62837,11 @@
       <c r="D400" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="401" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E400" t="s">
+        <v>4731</v>
+      </c>
+    </row>
+    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>7</v>
       </c>
@@ -62388,8 +62854,11 @@
       <c r="D401" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="402" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E401" t="s">
+        <v>4732</v>
+      </c>
+    </row>
+    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>8</v>
       </c>
@@ -62402,8 +62871,11 @@
       <c r="D402" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="403" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E402" t="s">
+        <v>4733</v>
+      </c>
+    </row>
+    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>9</v>
       </c>
@@ -62416,8 +62888,11 @@
       <c r="D403" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="404" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E403" t="s">
+        <v>4734</v>
+      </c>
+    </row>
+    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>10</v>
       </c>
@@ -62430,8 +62905,11 @@
       <c r="D404" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="405" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E404" t="s">
+        <v>4735</v>
+      </c>
+    </row>
+    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>11</v>
       </c>
@@ -62444,8 +62922,11 @@
       <c r="D405" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="406" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E405" t="s">
+        <v>4736</v>
+      </c>
+    </row>
+    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>3962</v>
       </c>
@@ -62459,7 +62940,7 @@
         <v>4213</v>
       </c>
     </row>
-    <row r="407" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>3980</v>
       </c>
@@ -62473,7 +62954,7 @@
         <v>4213</v>
       </c>
     </row>
-    <row r="408" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>3964</v>
       </c>
@@ -62486,8 +62967,11 @@
       <c r="D408" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="409" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E408" t="s">
+        <v>4761</v>
+      </c>
+    </row>
+    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>3966</v>
       </c>
@@ -62500,8 +62984,11 @@
       <c r="D409" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="410" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E409" t="s">
+        <v>4762</v>
+      </c>
+    </row>
+    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>3963</v>
       </c>
@@ -62514,8 +63001,11 @@
       <c r="D410" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="411" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E410" t="s">
+        <v>4759</v>
+      </c>
+    </row>
+    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>3970</v>
       </c>
@@ -62528,8 +63018,11 @@
       <c r="D411" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="412" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E411" t="s">
+        <v>4760</v>
+      </c>
+    </row>
+    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>3930</v>
       </c>
@@ -62542,8 +63035,11 @@
       <c r="D412" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="413" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E412" t="s">
+        <v>4744</v>
+      </c>
+    </row>
+    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>3458</v>
       </c>
@@ -62556,8 +63052,11 @@
       <c r="D413" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="414" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E413" t="s">
+        <v>4711</v>
+      </c>
+    </row>
+    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>3451</v>
       </c>
@@ -62570,8 +63069,11 @@
       <c r="D414" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="415" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E414" t="s">
+        <v>4712</v>
+      </c>
+    </row>
+    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>3455</v>
       </c>
@@ -62584,8 +63086,11 @@
       <c r="D415" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="416" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E415" t="s">
+        <v>4713</v>
+      </c>
+    </row>
+    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>3449</v>
       </c>
@@ -62598,8 +63103,11 @@
       <c r="D416" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="417" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E416" t="s">
+        <v>4714</v>
+      </c>
+    </row>
+    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>415</v>
       </c>
@@ -62612,8 +63120,11 @@
       <c r="D417" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="418" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E417" t="s">
+        <v>4725</v>
+      </c>
+    </row>
+    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>118</v>
       </c>
@@ -62626,8 +63137,11 @@
       <c r="D418" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="419" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E418" t="s">
+        <v>4726</v>
+      </c>
+    </row>
+    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>416</v>
       </c>
@@ -62640,8 +63154,11 @@
       <c r="D419" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="420" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E419" t="s">
+        <v>4727</v>
+      </c>
+    </row>
+    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>117</v>
       </c>
@@ -62654,8 +63171,11 @@
       <c r="D420" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="421" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E420" t="s">
+        <v>4728</v>
+      </c>
+    </row>
+    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A421" s="2" t="s">
         <v>417</v>
       </c>
@@ -62668,8 +63188,11 @@
       <c r="D421" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="422" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E421" t="s">
+        <v>4721</v>
+      </c>
+    </row>
+    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>116</v>
       </c>
@@ -62682,8 +63205,11 @@
       <c r="D422" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="423" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E422" t="s">
+        <v>4723</v>
+      </c>
+    </row>
+    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>418</v>
       </c>
@@ -62696,8 +63222,11 @@
       <c r="D423" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="424" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E423" t="s">
+        <v>4722</v>
+      </c>
+    </row>
+    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>115</v>
       </c>
@@ -62710,8 +63239,11 @@
       <c r="D424" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="425" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E424" t="s">
+        <v>4724</v>
+      </c>
+    </row>
+    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>3539</v>
       </c>
@@ -62725,7 +63257,7 @@
         <v>4213</v>
       </c>
     </row>
-    <row r="426" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>3447</v>
       </c>
@@ -62738,8 +63270,11 @@
       <c r="D426" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="427" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E426" t="s">
+        <v>4708</v>
+      </c>
+    </row>
+    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>3446</v>
       </c>
@@ -62752,8 +63287,11 @@
       <c r="D427" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="428" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E427" t="s">
+        <v>4709</v>
+      </c>
+    </row>
+    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>3443</v>
       </c>
@@ -62766,8 +63304,11 @@
       <c r="D428" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="429" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E428" t="s">
+        <v>4710</v>
+      </c>
+    </row>
+    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>3986</v>
       </c>
@@ -62780,8 +63321,11 @@
       <c r="D429" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="430" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E429" t="s">
+        <v>4706</v>
+      </c>
+    </row>
+    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>3982</v>
       </c>
@@ -62794,8 +63338,11 @@
       <c r="D430" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="431" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E430" t="s">
+        <v>4707</v>
+      </c>
+    </row>
+    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>3983</v>
       </c>
@@ -62808,8 +63355,11 @@
       <c r="D431" t="s">
         <v>4213</v>
       </c>
-    </row>
-    <row r="432" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E431" t="s">
+        <v>4705</v>
+      </c>
+    </row>
+    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>3652</v>
       </c>
@@ -63084,6 +63634,9 @@
       <c r="D449" t="s">
         <v>4213</v>
       </c>
+      <c r="E449" t="s">
+        <v>4568</v>
+      </c>
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
@@ -63098,6 +63651,9 @@
       <c r="D450" t="s">
         <v>4213</v>
       </c>
+      <c r="E450" t="s">
+        <v>4567</v>
+      </c>
     </row>
     <row r="451" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
@@ -63112,6 +63668,9 @@
       <c r="D451" t="s">
         <v>4213</v>
       </c>
+      <c r="E451" t="s">
+        <v>4566</v>
+      </c>
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
@@ -63126,6 +63685,9 @@
       <c r="D452" t="s">
         <v>4213</v>
       </c>
+      <c r="E452" t="s">
+        <v>4745</v>
+      </c>
     </row>
     <row r="453" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
@@ -63140,6 +63702,9 @@
       <c r="D453" t="s">
         <v>4213</v>
       </c>
+      <c r="E453" t="s">
+        <v>4746</v>
+      </c>
     </row>
     <row r="454" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
@@ -63154,6 +63719,9 @@
       <c r="D454" t="s">
         <v>4213</v>
       </c>
+      <c r="E454" t="s">
+        <v>4747</v>
+      </c>
     </row>
     <row r="455" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
@@ -63185,6 +63753,9 @@
       <c r="D456" t="s">
         <v>4213</v>
       </c>
+      <c r="E456" t="s">
+        <v>4718</v>
+      </c>
     </row>
     <row r="457" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
@@ -63199,6 +63770,9 @@
       <c r="D457" t="s">
         <v>4213</v>
       </c>
+      <c r="E457" t="s">
+        <v>4719</v>
+      </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
@@ -63213,6 +63787,9 @@
       <c r="D458" t="s">
         <v>4213</v>
       </c>
+      <c r="E458" t="s">
+        <v>4716</v>
+      </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
@@ -63227,6 +63804,9 @@
       <c r="D459" t="s">
         <v>4213</v>
       </c>
+      <c r="E459" t="s">
+        <v>4717</v>
+      </c>
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
@@ -63241,6 +63821,9 @@
       <c r="D460" t="s">
         <v>4213</v>
       </c>
+      <c r="E460" t="s">
+        <v>4715</v>
+      </c>
     </row>
     <row r="461" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
@@ -63255,6 +63838,9 @@
       <c r="D461" t="s">
         <v>4213</v>
       </c>
+      <c r="E461" t="s">
+        <v>4718</v>
+      </c>
     </row>
     <row r="462" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
@@ -63269,6 +63855,9 @@
       <c r="D462" t="s">
         <v>4213</v>
       </c>
+      <c r="E462" t="s">
+        <v>4716</v>
+      </c>
     </row>
     <row r="463" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
@@ -63283,6 +63872,9 @@
       <c r="D463" t="s">
         <v>4213</v>
       </c>
+      <c r="E463" t="s">
+        <v>4717</v>
+      </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
@@ -63297,6 +63889,9 @@
       <c r="D464" t="s">
         <v>4213</v>
       </c>
+      <c r="E464" t="s">
+        <v>4751</v>
+      </c>
     </row>
     <row r="465" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
@@ -63311,6 +63906,9 @@
       <c r="D465" t="s">
         <v>4213</v>
       </c>
+      <c r="E465" t="s">
+        <v>4750</v>
+      </c>
     </row>
     <row r="466" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
@@ -63325,6 +63923,9 @@
       <c r="D466" t="s">
         <v>4213</v>
       </c>
+      <c r="E466" t="s">
+        <v>4749</v>
+      </c>
     </row>
     <row r="467" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
@@ -63367,6 +63968,9 @@
       <c r="D469" t="s">
         <v>4213</v>
       </c>
+      <c r="E469" t="s">
+        <v>4752</v>
+      </c>
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
@@ -63381,6 +63985,9 @@
       <c r="D470" t="s">
         <v>4213</v>
       </c>
+      <c r="E470" t="s">
+        <v>4753</v>
+      </c>
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
@@ -63395,6 +64002,9 @@
       <c r="D471" t="s">
         <v>4213</v>
       </c>
+      <c r="E471" t="s">
+        <v>4754</v>
+      </c>
     </row>
     <row r="472" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
@@ -63409,6 +64019,9 @@
       <c r="D472" t="s">
         <v>4213</v>
       </c>
+      <c r="E472" t="s">
+        <v>4755</v>
+      </c>
     </row>
     <row r="473" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
@@ -63423,6 +64036,9 @@
       <c r="D473" t="s">
         <v>4213</v>
       </c>
+      <c r="E473" t="s">
+        <v>4756</v>
+      </c>
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
@@ -63437,6 +64053,9 @@
       <c r="D474" t="s">
         <v>4213</v>
       </c>
+      <c r="E474" t="s">
+        <v>4757</v>
+      </c>
     </row>
     <row r="475" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
@@ -63451,6 +64070,9 @@
       <c r="D475" t="s">
         <v>4213</v>
       </c>
+      <c r="E475" t="s">
+        <v>4758</v>
+      </c>
     </row>
     <row r="476" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
@@ -63513,6 +64135,9 @@
       <c r="D479" t="s">
         <v>4213</v>
       </c>
+      <c r="E479" t="s">
+        <v>4666</v>
+      </c>
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
@@ -63527,6 +64152,9 @@
       <c r="D480" t="s">
         <v>4213</v>
       </c>
+      <c r="E480" t="s">
+        <v>4667</v>
+      </c>
     </row>
     <row r="481" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
@@ -63541,6 +64169,9 @@
       <c r="D481" t="s">
         <v>4213</v>
       </c>
+      <c r="E481" t="s">
+        <v>4720</v>
+      </c>
     </row>
     <row r="482" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
@@ -64257,6 +64888,9 @@
       <c r="D524" t="s">
         <v>4214</v>
       </c>
+      <c r="E524" t="s">
+        <v>4748</v>
+      </c>
     </row>
     <row r="525" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A525" s="14">
@@ -64408,7 +65042,7 @@
         <v>4216</v>
       </c>
       <c r="E533" t="s">
-        <v>4541</v>
+        <v>4542</v>
       </c>
     </row>
     <row r="534" spans="1:5" x14ac:dyDescent="0.25">
@@ -64498,7 +65132,7 @@
     </row>
     <row r="539" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A539" s="14">
-        <v>20540</v>
+        <v>20539</v>
       </c>
       <c r="B539" s="4" t="s">
         <v>4205</v>

</xml_diff>

<commit_message>
Inclusão de melhorias @202406171004
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6853BBD-BB9D-4D99-8063-79DDEAAE1C45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F21E6B-FCB3-42AB-BBDC-754687B980E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" tabRatio="754" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" tabRatio="754" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fixed_income_signals" sheetId="23" r:id="rId1"/>
@@ -28,28 +28,17 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fixed_income_signals!$A$1:$C$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">indicators!$A$1:$E$566</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15173" uniqueCount="5553">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15248" uniqueCount="5598">
   <si>
     <t>category</t>
   </si>
@@ -16708,6 +16697,141 @@
   </si>
   <si>
     <t>NEXA</t>
+  </si>
+  <si>
+    <t>SBOITOTL Index</t>
+  </si>
+  <si>
+    <t>us_nfib_small_business_optimism_index</t>
+  </si>
+  <si>
+    <t>SBOICAPX Index</t>
+  </si>
+  <si>
+    <t>us_nfib_small_business_actual_capex</t>
+  </si>
+  <si>
+    <t>SBOIEMPC Index</t>
+  </si>
+  <si>
+    <t>us_nfib_small_business_actual_employment_changes</t>
+  </si>
+  <si>
+    <t>SBOIARAT Index</t>
+  </si>
+  <si>
+    <t>us_nfib_small_business_actual_avg_rates_paid_st_loans</t>
+  </si>
+  <si>
+    <t>CUSR0000SAH1</t>
+  </si>
+  <si>
+    <t>us_cpi_shelter_index</t>
+  </si>
+  <si>
+    <t>CUSR0000SAS2RS</t>
+  </si>
+  <si>
+    <t>us_cpi_rent_of_shelter_index</t>
+  </si>
+  <si>
+    <t>CUSR0000SEFV</t>
+  </si>
+  <si>
+    <t>CUSR0000SAF11</t>
+  </si>
+  <si>
+    <t>us_cpi_food_at_home_index</t>
+  </si>
+  <si>
+    <t>us_cpi_food_away_from_home_index</t>
+  </si>
+  <si>
+    <t>Food Away From Home</t>
+  </si>
+  <si>
+    <t>Food At Home</t>
+  </si>
+  <si>
+    <t>STLFSI4</t>
+  </si>
+  <si>
+    <t>us_fed_financial_stress_index</t>
+  </si>
+  <si>
+    <t>St. Louis Fed Financial Stress Index</t>
+  </si>
+  <si>
+    <t>Chicago Fed National Financial Conditions Index</t>
+  </si>
+  <si>
+    <t>ANFCI</t>
+  </si>
+  <si>
+    <t>Chicago Fed Adjusted National Financial Conditions Index</t>
+  </si>
+  <si>
+    <t>NFCI</t>
+  </si>
+  <si>
+    <t>us_fed_national_fci</t>
+  </si>
+  <si>
+    <t>us_fed_adjusted_national_fci</t>
+  </si>
+  <si>
+    <t>Shelter</t>
+  </si>
+  <si>
+    <t>Rent of Shelter</t>
+  </si>
+  <si>
+    <t>Actual Capex</t>
+  </si>
+  <si>
+    <t>Actual Employment Changes</t>
+  </si>
+  <si>
+    <t>Actual Avg. Interest Rates Paid on ST Loans</t>
+  </si>
+  <si>
+    <t>Optimism Index</t>
+  </si>
+  <si>
+    <t>STLPPMDEF</t>
+  </si>
+  <si>
+    <t>STLPPM</t>
+  </si>
+  <si>
+    <t>Deflação</t>
+  </si>
+  <si>
+    <t>Acima de 2.5%</t>
+  </si>
+  <si>
+    <t>STLPPMMID</t>
+  </si>
+  <si>
+    <t>Entre 1.5 e 2.5%</t>
+  </si>
+  <si>
+    <t>us_pce_probability_deflation</t>
+  </si>
+  <si>
+    <t>us_pce_probability_above_25</t>
+  </si>
+  <si>
+    <t>us_pce_probability_between_15_25</t>
+  </si>
+  <si>
+    <t>STLPPMLOW</t>
+  </si>
+  <si>
+    <t>Entre 0 e 1.5%</t>
+  </si>
+  <si>
+    <t>us_pce_probability_between_0_15</t>
   </si>
 </sst>
 </file>
@@ -16793,7 +16917,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -16812,7 +16936,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -17146,7 +17269,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE9BFA3A-A372-440F-86E1-C70EDC1063D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -17446,7 +17569,7 @@
       <c r="A79" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C15" xr:uid="{FE9BFA3A-A372-440F-86E1-C70EDC1063D4}">
+  <autoFilter ref="A1:C15" xr:uid="{00000000-0009-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C16">
       <sortCondition ref="C1:C15"/>
     </sortState>
@@ -17457,7 +17580,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -18123,7 +18246,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Planilha7"/>
   <dimension ref="A1:C16"/>
   <sheetViews>
@@ -18264,7 +18387,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr codeName="Planilha8">
     <tabColor theme="9" tint="0.79998168889431442"/>
   </sheetPr>
@@ -18281,15 +18404,15 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr codeName="Planilha10"/>
   <dimension ref="A1:N1281"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B796" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A816" sqref="A816"/>
+      <selection pane="bottomRight" activeCell="D815" sqref="D815"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58536,7 +58659,7 @@
       <c r="I1278" s="6" t="s">
         <v>918</v>
       </c>
-      <c r="J1278" s="14" t="s">
+      <c r="J1278" s="6" t="s">
         <v>919</v>
       </c>
       <c r="K1278" s="8" t="s">
@@ -58649,7 +58772,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L1268" xr:uid="{00000000-0009-0000-0000-000003000000}">
+  <autoFilter ref="A1:L1268" xr:uid="{00000000-0009-0000-0000-000004000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:L1281">
       <sortCondition ref="A1:A1268"/>
     </sortState>
@@ -58663,7 +58786,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr codeName="Planilha11"/>
   <dimension ref="A1:B34"/>
   <sheetViews>
@@ -58955,7 +59078,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7D3F8C1-6196-49D7-A787-796087CD7CB3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:A780"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -62874,12 +62997,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2CB12C5-8725-4AAE-9F74-FA739078C419}">
-  <dimension ref="A1:E566"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:E581"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A398" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E426" sqref="E426"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A550" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F580" sqref="F580"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72320,8 +72443,263 @@
         <v>4627</v>
       </c>
     </row>
+    <row r="567" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A567" t="s">
+        <v>5553</v>
+      </c>
+      <c r="B567" t="s">
+        <v>5554</v>
+      </c>
+      <c r="C567" t="s">
+        <v>3544</v>
+      </c>
+      <c r="D567" t="s">
+        <v>4182</v>
+      </c>
+      <c r="E567" t="s">
+        <v>5585</v>
+      </c>
+    </row>
+    <row r="568" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A568" t="s">
+        <v>5555</v>
+      </c>
+      <c r="B568" t="s">
+        <v>5556</v>
+      </c>
+      <c r="C568" t="s">
+        <v>3544</v>
+      </c>
+      <c r="D568" t="s">
+        <v>4182</v>
+      </c>
+      <c r="E568" t="s">
+        <v>5582</v>
+      </c>
+    </row>
+    <row r="569" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A569" t="s">
+        <v>5557</v>
+      </c>
+      <c r="B569" t="s">
+        <v>5558</v>
+      </c>
+      <c r="C569" t="s">
+        <v>3544</v>
+      </c>
+      <c r="D569" t="s">
+        <v>4182</v>
+      </c>
+      <c r="E569" t="s">
+        <v>5583</v>
+      </c>
+    </row>
+    <row r="570" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A570" t="s">
+        <v>5559</v>
+      </c>
+      <c r="B570" t="s">
+        <v>5560</v>
+      </c>
+      <c r="C570" t="s">
+        <v>3544</v>
+      </c>
+      <c r="D570" t="s">
+        <v>4182</v>
+      </c>
+      <c r="E570" t="s">
+        <v>5584</v>
+      </c>
+    </row>
+    <row r="571" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A571" t="s">
+        <v>5561</v>
+      </c>
+      <c r="B571" t="s">
+        <v>5562</v>
+      </c>
+      <c r="C571" t="s">
+        <v>4075</v>
+      </c>
+      <c r="D571" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E571" t="s">
+        <v>5580</v>
+      </c>
+    </row>
+    <row r="572" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A572" t="s">
+        <v>5563</v>
+      </c>
+      <c r="B572" t="s">
+        <v>5564</v>
+      </c>
+      <c r="C572" t="s">
+        <v>4075</v>
+      </c>
+      <c r="D572" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E572" t="s">
+        <v>5581</v>
+      </c>
+    </row>
+    <row r="573" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A573" t="s">
+        <v>5565</v>
+      </c>
+      <c r="B573" t="s">
+        <v>5568</v>
+      </c>
+      <c r="C573" t="s">
+        <v>4075</v>
+      </c>
+      <c r="D573" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E573" t="s">
+        <v>5569</v>
+      </c>
+    </row>
+    <row r="574" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A574" t="s">
+        <v>5566</v>
+      </c>
+      <c r="B574" t="s">
+        <v>5567</v>
+      </c>
+      <c r="C574" t="s">
+        <v>4075</v>
+      </c>
+      <c r="D574" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E574" t="s">
+        <v>5570</v>
+      </c>
+    </row>
+    <row r="575" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A575" t="s">
+        <v>5571</v>
+      </c>
+      <c r="B575" t="s">
+        <v>5572</v>
+      </c>
+      <c r="C575" t="s">
+        <v>425</v>
+      </c>
+      <c r="D575" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E575" t="s">
+        <v>5573</v>
+      </c>
+    </row>
+    <row r="576" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A576" t="s">
+        <v>5577</v>
+      </c>
+      <c r="B576" t="s">
+        <v>5578</v>
+      </c>
+      <c r="C576" t="s">
+        <v>425</v>
+      </c>
+      <c r="D576" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E576" t="s">
+        <v>5574</v>
+      </c>
+    </row>
+    <row r="577" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A577" t="s">
+        <v>5575</v>
+      </c>
+      <c r="B577" t="s">
+        <v>5579</v>
+      </c>
+      <c r="C577" t="s">
+        <v>425</v>
+      </c>
+      <c r="D577" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E577" t="s">
+        <v>5576</v>
+      </c>
+    </row>
+    <row r="578" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A578" t="s">
+        <v>5586</v>
+      </c>
+      <c r="B578" t="s">
+        <v>5592</v>
+      </c>
+      <c r="C578" t="s">
+        <v>4075</v>
+      </c>
+      <c r="D578" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E578" t="s">
+        <v>5588</v>
+      </c>
+    </row>
+    <row r="579" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A579" t="s">
+        <v>5587</v>
+      </c>
+      <c r="B579" t="s">
+        <v>5593</v>
+      </c>
+      <c r="C579" t="s">
+        <v>4075</v>
+      </c>
+      <c r="D579" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E579" t="s">
+        <v>5589</v>
+      </c>
+    </row>
+    <row r="580" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A580" t="s">
+        <v>5590</v>
+      </c>
+      <c r="B580" t="s">
+        <v>5594</v>
+      </c>
+      <c r="C580" t="s">
+        <v>4075</v>
+      </c>
+      <c r="D580" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E580" t="s">
+        <v>5591</v>
+      </c>
+    </row>
+    <row r="581" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A581" t="s">
+        <v>5595</v>
+      </c>
+      <c r="B581" t="s">
+        <v>5597</v>
+      </c>
+      <c r="C581" t="s">
+        <v>4075</v>
+      </c>
+      <c r="D581" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E581" t="s">
+        <v>5596</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:E566" xr:uid="{F2CB12C5-8725-4AAE-9F74-FA739078C419}"/>
+  <autoFilter ref="A1:E566" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Inclusão de melhorias @202406181445
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C45E066A-1BE9-4D59-A0D1-19722AD881B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C52B91-2593-4EB9-9A62-2AC65E4E2404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14385" yWindow="285" windowWidth="19185" windowHeight="10065" tabRatio="754" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-19310" yWindow="3280" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fixed_income_signals" sheetId="23" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">equities!$A$1:$L$1268</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">equity_signals!$C$1:$C$79</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fixed_income_signals!$A$1:$C$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">indicators!$A$1:$E$566</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">indicators!$A$1:$E$569</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15271" uniqueCount="5593">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15294" uniqueCount="5603">
   <si>
     <t>category</t>
   </si>
@@ -16767,12 +16767,6 @@
     <t>Retail Sales</t>
   </si>
   <si>
-    <t>Retail Sales (% MoM)</t>
-  </si>
-  <si>
-    <t>Retail Sales (% YoY)</t>
-  </si>
-  <si>
     <t>DXY</t>
   </si>
   <si>
@@ -16828,6 +16822,42 @@
   </si>
   <si>
     <t>IPCA Administrados</t>
+  </si>
+  <si>
+    <t>Fed Funds Rate</t>
+  </si>
+  <si>
+    <t>Nonfarm Payrolls</t>
+  </si>
+  <si>
+    <t>New Home Sales</t>
+  </si>
+  <si>
+    <t>Housing Starts</t>
+  </si>
+  <si>
+    <t>Dívida Pública Total / PIB</t>
+  </si>
+  <si>
+    <t>Retail Sales Ex-Auto</t>
+  </si>
+  <si>
+    <t>us_advance_retail_sales_ex_auto_total</t>
+  </si>
+  <si>
+    <t>us_advance_retail_sales_ex_auto_yoy</t>
+  </si>
+  <si>
+    <t>us_advance_retail_sales_ex_auto_mom</t>
+  </si>
+  <si>
+    <t>RSTAXAUT Index</t>
+  </si>
+  <si>
+    <t>RSTAXMOM Index</t>
+  </si>
+  <si>
+    <t>RSTAXYOY Index</t>
   </si>
 </sst>
 </file>
@@ -62994,11 +63024,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E586"/>
+  <dimension ref="A1:E589"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A308" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B315" sqref="B315"/>
+      <pane ySplit="1" topLeftCell="A383" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D393" sqref="D393"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64212,7 +64242,7 @@
         <v>4182</v>
       </c>
       <c r="E72" t="s">
-        <v>5575</v>
+        <v>5573</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -64348,7 +64378,7 @@
         <v>4182</v>
       </c>
       <c r="E80" t="s">
-        <v>5574</v>
+        <v>5572</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -65819,7 +65849,7 @@
         <v>4182</v>
       </c>
       <c r="E169" t="s">
-        <v>5589</v>
+        <v>5587</v>
       </c>
     </row>
     <row r="170" spans="1:5" x14ac:dyDescent="0.25">
@@ -65836,7 +65866,7 @@
         <v>4182</v>
       </c>
       <c r="E170" t="s">
-        <v>5589</v>
+        <v>5587</v>
       </c>
     </row>
     <row r="171" spans="1:5" x14ac:dyDescent="0.25">
@@ -65853,7 +65883,7 @@
         <v>4182</v>
       </c>
       <c r="E171" t="s">
-        <v>5589</v>
+        <v>5587</v>
       </c>
     </row>
     <row r="172" spans="1:5" x14ac:dyDescent="0.25">
@@ -66102,7 +66132,7 @@
         <v>4182</v>
       </c>
       <c r="E186" t="s">
-        <v>5581</v>
+        <v>5579</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
@@ -66119,7 +66149,7 @@
         <v>4182</v>
       </c>
       <c r="E187" t="s">
-        <v>5582</v>
+        <v>5580</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
@@ -66252,7 +66282,7 @@
         <v>4182</v>
       </c>
       <c r="E195" t="s">
-        <v>5585</v>
+        <v>5583</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
@@ -66269,7 +66299,7 @@
         <v>4182</v>
       </c>
       <c r="E196" t="s">
-        <v>5585</v>
+        <v>5583</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
@@ -66286,7 +66316,7 @@
         <v>4182</v>
       </c>
       <c r="E197" t="s">
-        <v>5585</v>
+        <v>5583</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
@@ -66303,7 +66333,7 @@
         <v>4182</v>
       </c>
       <c r="E198" t="s">
-        <v>5585</v>
+        <v>5583</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
@@ -66320,7 +66350,7 @@
         <v>4182</v>
       </c>
       <c r="E199" t="s">
-        <v>5585</v>
+        <v>5583</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
@@ -66337,7 +66367,7 @@
         <v>4182</v>
       </c>
       <c r="E200" t="s">
-        <v>5586</v>
+        <v>5584</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
@@ -66354,7 +66384,7 @@
         <v>4182</v>
       </c>
       <c r="E201" t="s">
-        <v>5586</v>
+        <v>5584</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
@@ -66371,7 +66401,7 @@
         <v>4182</v>
       </c>
       <c r="E202" t="s">
-        <v>5586</v>
+        <v>5584</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
@@ -66388,7 +66418,7 @@
         <v>4182</v>
       </c>
       <c r="E203" t="s">
-        <v>5587</v>
+        <v>5585</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
@@ -66405,7 +66435,7 @@
         <v>4182</v>
       </c>
       <c r="E204" t="s">
-        <v>5587</v>
+        <v>5585</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
@@ -66422,7 +66452,7 @@
         <v>4182</v>
       </c>
       <c r="E205" t="s">
-        <v>5587</v>
+        <v>5585</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
@@ -66439,7 +66469,7 @@
         <v>4182</v>
       </c>
       <c r="E206" t="s">
-        <v>5588</v>
+        <v>5586</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
@@ -66456,7 +66486,7 @@
         <v>4182</v>
       </c>
       <c r="E207" t="s">
-        <v>5588</v>
+        <v>5586</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
@@ -66473,7 +66503,7 @@
         <v>4182</v>
       </c>
       <c r="E208" t="s">
-        <v>5588</v>
+        <v>5586</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
@@ -66524,7 +66554,7 @@
         <v>4182</v>
       </c>
       <c r="E211" t="s">
-        <v>5584</v>
+        <v>5582</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
@@ -66541,7 +66571,7 @@
         <v>4182</v>
       </c>
       <c r="E212" t="s">
-        <v>5584</v>
+        <v>5582</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
@@ -66558,7 +66588,7 @@
         <v>4182</v>
       </c>
       <c r="E213" t="s">
-        <v>5584</v>
+        <v>5582</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
@@ -66643,7 +66673,7 @@
         <v>4182</v>
       </c>
       <c r="E218" t="s">
-        <v>5583</v>
+        <v>5581</v>
       </c>
     </row>
     <row r="219" spans="1:5" x14ac:dyDescent="0.25">
@@ -66660,7 +66690,7 @@
         <v>4182</v>
       </c>
       <c r="E219" t="s">
-        <v>5583</v>
+        <v>5581</v>
       </c>
     </row>
     <row r="220" spans="1:5" x14ac:dyDescent="0.25">
@@ -66677,7 +66707,7 @@
         <v>4182</v>
       </c>
       <c r="E220" t="s">
-        <v>5583</v>
+        <v>5581</v>
       </c>
     </row>
     <row r="221" spans="1:5" x14ac:dyDescent="0.25">
@@ -67476,7 +67506,7 @@
         <v>4182</v>
       </c>
       <c r="E267" t="s">
-        <v>5590</v>
+        <v>5588</v>
       </c>
     </row>
     <row r="268" spans="1:5" x14ac:dyDescent="0.25">
@@ -67493,7 +67523,7 @@
         <v>4182</v>
       </c>
       <c r="E268" t="s">
-        <v>5590</v>
+        <v>5588</v>
       </c>
     </row>
     <row r="269" spans="1:5" x14ac:dyDescent="0.25">
@@ -67527,7 +67557,7 @@
         <v>4182</v>
       </c>
       <c r="E270" t="s">
-        <v>5591</v>
+        <v>5589</v>
       </c>
     </row>
     <row r="271" spans="1:5" x14ac:dyDescent="0.25">
@@ -67561,7 +67591,7 @@
         <v>4182</v>
       </c>
       <c r="E272" t="s">
-        <v>5592</v>
+        <v>5590</v>
       </c>
     </row>
     <row r="273" spans="1:5" x14ac:dyDescent="0.25">
@@ -67629,7 +67659,7 @@
         <v>4182</v>
       </c>
       <c r="E276" t="s">
-        <v>5590</v>
+        <v>5588</v>
       </c>
     </row>
     <row r="277" spans="1:5" x14ac:dyDescent="0.25">
@@ -69584,7 +69614,7 @@
         <v>4182</v>
       </c>
       <c r="E394" t="s">
-        <v>5572</v>
+        <v>5571</v>
       </c>
     </row>
     <row r="395" spans="1:5" x14ac:dyDescent="0.25">
@@ -69601,15 +69631,15 @@
         <v>4182</v>
       </c>
       <c r="E395" t="s">
-        <v>5573</v>
+        <v>5571</v>
       </c>
     </row>
     <row r="396" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
-        <v>4107</v>
+        <v>5600</v>
       </c>
       <c r="B396" t="s">
-        <v>4106</v>
+        <v>5597</v>
       </c>
       <c r="C396" t="s">
         <v>3544</v>
@@ -69617,13 +69647,16 @@
       <c r="D396" t="s">
         <v>4182</v>
       </c>
+      <c r="E396" t="s">
+        <v>5596</v>
+      </c>
     </row>
     <row r="397" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
-        <v>3918</v>
+        <v>5601</v>
       </c>
       <c r="B397" t="s">
-        <v>3919</v>
+        <v>5598</v>
       </c>
       <c r="C397" t="s">
         <v>3544</v>
@@ -69631,13 +69664,16 @@
       <c r="D397" t="s">
         <v>4182</v>
       </c>
+      <c r="E397" t="s">
+        <v>5596</v>
+      </c>
     </row>
     <row r="398" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
-        <v>11</v>
-      </c>
-      <c r="B398" s="3" t="s">
-        <v>156</v>
+        <v>5602</v>
+      </c>
+      <c r="B398" t="s">
+        <v>5599</v>
       </c>
       <c r="C398" t="s">
         <v>3544</v>
@@ -69646,15 +69682,15 @@
         <v>4182</v>
       </c>
       <c r="E398" t="s">
-        <v>4666</v>
+        <v>5596</v>
       </c>
     </row>
     <row r="399" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
-        <v>5</v>
-      </c>
-      <c r="B399" s="3" t="s">
-        <v>150</v>
+        <v>4107</v>
+      </c>
+      <c r="B399" t="s">
+        <v>4106</v>
       </c>
       <c r="C399" t="s">
         <v>3544</v>
@@ -69662,16 +69698,13 @@
       <c r="D399" t="s">
         <v>4182</v>
       </c>
-      <c r="E399" t="s">
-        <v>4667</v>
-      </c>
     </row>
     <row r="400" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
-        <v>12</v>
-      </c>
-      <c r="B400" s="3" t="s">
-        <v>157</v>
+        <v>3918</v>
+      </c>
+      <c r="B400" t="s">
+        <v>3919</v>
       </c>
       <c r="C400" t="s">
         <v>3544</v>
@@ -69679,16 +69712,13 @@
       <c r="D400" t="s">
         <v>4182</v>
       </c>
-      <c r="E400" t="s">
-        <v>4668</v>
-      </c>
     </row>
     <row r="401" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="B401" s="3" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="C401" t="s">
         <v>3544</v>
@@ -69697,15 +69727,15 @@
         <v>4182</v>
       </c>
       <c r="E401" t="s">
-        <v>4669</v>
+        <v>4666</v>
       </c>
     </row>
     <row r="402" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B402" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C402" t="s">
         <v>3544</v>
@@ -69714,15 +69744,15 @@
         <v>4182</v>
       </c>
       <c r="E402" t="s">
-        <v>4670</v>
+        <v>4667</v>
       </c>
     </row>
     <row r="403" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="B403" s="3" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
       <c r="C403" t="s">
         <v>3544</v>
@@ -69731,15 +69761,15 @@
         <v>4182</v>
       </c>
       <c r="E403" t="s">
-        <v>4671</v>
+        <v>4668</v>
       </c>
     </row>
     <row r="404" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B404" s="3" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C404" t="s">
         <v>3544</v>
@@ -69748,15 +69778,15 @@
         <v>4182</v>
       </c>
       <c r="E404" t="s">
-        <v>4672</v>
+        <v>4669</v>
       </c>
     </row>
     <row r="405" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B405" s="3" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C405" t="s">
         <v>3544</v>
@@ -69765,15 +69795,15 @@
         <v>4182</v>
       </c>
       <c r="E405" t="s">
-        <v>4673</v>
+        <v>4670</v>
       </c>
     </row>
     <row r="406" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
-        <v>3931</v>
-      </c>
-      <c r="B406" t="s">
-        <v>3943</v>
+        <v>8</v>
+      </c>
+      <c r="B406" s="3" t="s">
+        <v>153</v>
       </c>
       <c r="C406" t="s">
         <v>3544</v>
@@ -69781,13 +69811,16 @@
       <c r="D406" t="s">
         <v>4182</v>
       </c>
+      <c r="E406" t="s">
+        <v>4671</v>
+      </c>
     </row>
     <row r="407" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
-        <v>3949</v>
-      </c>
-      <c r="B407" t="s">
-        <v>3946</v>
+        <v>9</v>
+      </c>
+      <c r="B407" s="3" t="s">
+        <v>154</v>
       </c>
       <c r="C407" t="s">
         <v>3544</v>
@@ -69795,13 +69828,16 @@
       <c r="D407" t="s">
         <v>4182</v>
       </c>
+      <c r="E407" t="s">
+        <v>4672</v>
+      </c>
     </row>
     <row r="408" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
-        <v>3933</v>
-      </c>
-      <c r="B408" t="s">
-        <v>3936</v>
+        <v>10</v>
+      </c>
+      <c r="B408" s="3" t="s">
+        <v>155</v>
       </c>
       <c r="C408" t="s">
         <v>3544</v>
@@ -69810,15 +69846,15 @@
         <v>4182</v>
       </c>
       <c r="E408" t="s">
-        <v>4698</v>
+        <v>4673</v>
       </c>
     </row>
     <row r="409" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
-        <v>3935</v>
+        <v>3931</v>
       </c>
       <c r="B409" t="s">
-        <v>3937</v>
+        <v>3943</v>
       </c>
       <c r="C409" t="s">
         <v>3544</v>
@@ -69826,16 +69862,13 @@
       <c r="D409" t="s">
         <v>4182</v>
       </c>
-      <c r="E409" t="s">
-        <v>4699</v>
-      </c>
     </row>
     <row r="410" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
-        <v>3932</v>
+        <v>3949</v>
       </c>
       <c r="B410" t="s">
-        <v>3934</v>
+        <v>3946</v>
       </c>
       <c r="C410" t="s">
         <v>3544</v>
@@ -69843,16 +69876,13 @@
       <c r="D410" t="s">
         <v>4182</v>
       </c>
-      <c r="E410" t="s">
-        <v>4696</v>
-      </c>
     </row>
     <row r="411" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
-        <v>3939</v>
+        <v>3933</v>
       </c>
       <c r="B411" t="s">
-        <v>3938</v>
+        <v>3936</v>
       </c>
       <c r="C411" t="s">
         <v>3544</v>
@@ -69861,15 +69891,15 @@
         <v>4182</v>
       </c>
       <c r="E411" t="s">
-        <v>4697</v>
+        <v>4698</v>
       </c>
     </row>
     <row r="412" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
-        <v>3899</v>
+        <v>3935</v>
       </c>
       <c r="B412" t="s">
-        <v>3900</v>
+        <v>3937</v>
       </c>
       <c r="C412" t="s">
         <v>3544</v>
@@ -69878,15 +69908,15 @@
         <v>4182</v>
       </c>
       <c r="E412" t="s">
-        <v>4681</v>
+        <v>4699</v>
       </c>
     </row>
     <row r="413" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
-        <v>3435</v>
+        <v>3932</v>
       </c>
       <c r="B413" t="s">
-        <v>3434</v>
+        <v>3934</v>
       </c>
       <c r="C413" t="s">
         <v>3544</v>
@@ -69895,15 +69925,15 @@
         <v>4182</v>
       </c>
       <c r="E413" t="s">
-        <v>4648</v>
+        <v>4696</v>
       </c>
     </row>
     <row r="414" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
-        <v>3428</v>
+        <v>3939</v>
       </c>
       <c r="B414" t="s">
-        <v>3431</v>
+        <v>3938</v>
       </c>
       <c r="C414" t="s">
         <v>3544</v>
@@ -69912,15 +69942,15 @@
         <v>4182</v>
       </c>
       <c r="E414" t="s">
-        <v>4649</v>
+        <v>4697</v>
       </c>
     </row>
     <row r="415" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
-        <v>3432</v>
+        <v>3899</v>
       </c>
       <c r="B415" t="s">
-        <v>3433</v>
+        <v>3900</v>
       </c>
       <c r="C415" t="s">
         <v>3544</v>
@@ -69929,15 +69959,15 @@
         <v>4182</v>
       </c>
       <c r="E415" t="s">
-        <v>4650</v>
+        <v>4681</v>
       </c>
     </row>
     <row r="416" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
-        <v>3426</v>
+        <v>3435</v>
       </c>
       <c r="B416" t="s">
-        <v>4113</v>
+        <v>3434</v>
       </c>
       <c r="C416" t="s">
         <v>3544</v>
@@ -69946,15 +69976,15 @@
         <v>4182</v>
       </c>
       <c r="E416" t="s">
-        <v>4651</v>
+        <v>4648</v>
       </c>
     </row>
     <row r="417" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
-        <v>410</v>
+        <v>3428</v>
       </c>
       <c r="B417" t="s">
-        <v>222</v>
+        <v>3431</v>
       </c>
       <c r="C417" t="s">
         <v>3544</v>
@@ -69963,15 +69993,15 @@
         <v>4182</v>
       </c>
       <c r="E417" t="s">
-        <v>4662</v>
+        <v>4649</v>
       </c>
     </row>
     <row r="418" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
-        <v>113</v>
+        <v>3432</v>
       </c>
       <c r="B418" t="s">
-        <v>3414</v>
+        <v>3433</v>
       </c>
       <c r="C418" t="s">
         <v>3544</v>
@@ -69980,15 +70010,15 @@
         <v>4182</v>
       </c>
       <c r="E418" t="s">
-        <v>4663</v>
+        <v>4650</v>
       </c>
     </row>
     <row r="419" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
-        <v>411</v>
+        <v>3426</v>
       </c>
       <c r="B419" t="s">
-        <v>221</v>
+        <v>4113</v>
       </c>
       <c r="C419" t="s">
         <v>3544</v>
@@ -69997,15 +70027,15 @@
         <v>4182</v>
       </c>
       <c r="E419" t="s">
-        <v>4664</v>
+        <v>4651</v>
       </c>
     </row>
     <row r="420" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
-        <v>112</v>
+        <v>410</v>
       </c>
       <c r="B420" t="s">
-        <v>3413</v>
+        <v>222</v>
       </c>
       <c r="C420" t="s">
         <v>3544</v>
@@ -70014,15 +70044,15 @@
         <v>4182</v>
       </c>
       <c r="E420" t="s">
-        <v>4665</v>
+        <v>4662</v>
       </c>
     </row>
     <row r="421" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A421" s="2" t="s">
-        <v>412</v>
+      <c r="A421" t="s">
+        <v>113</v>
       </c>
       <c r="B421" t="s">
-        <v>220</v>
+        <v>3414</v>
       </c>
       <c r="C421" t="s">
         <v>3544</v>
@@ -70031,15 +70061,15 @@
         <v>4182</v>
       </c>
       <c r="E421" t="s">
-        <v>4658</v>
+        <v>4663</v>
       </c>
     </row>
     <row r="422" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
-        <v>111</v>
+        <v>411</v>
       </c>
       <c r="B422" t="s">
-        <v>3416</v>
+        <v>221</v>
       </c>
       <c r="C422" t="s">
         <v>3544</v>
@@ -70048,15 +70078,15 @@
         <v>4182</v>
       </c>
       <c r="E422" t="s">
-        <v>4660</v>
+        <v>4664</v>
       </c>
     </row>
     <row r="423" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
-        <v>413</v>
+        <v>112</v>
       </c>
       <c r="B423" t="s">
-        <v>219</v>
+        <v>3413</v>
       </c>
       <c r="C423" t="s">
         <v>3544</v>
@@ -70065,15 +70095,15 @@
         <v>4182</v>
       </c>
       <c r="E423" t="s">
-        <v>4659</v>
+        <v>4665</v>
       </c>
     </row>
     <row r="424" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A424" t="s">
-        <v>110</v>
+      <c r="A424" s="2" t="s">
+        <v>412</v>
       </c>
       <c r="B424" t="s">
-        <v>3415</v>
+        <v>220</v>
       </c>
       <c r="C424" t="s">
         <v>3544</v>
@@ -70082,15 +70112,15 @@
         <v>4182</v>
       </c>
       <c r="E424" t="s">
-        <v>4661</v>
+        <v>4658</v>
       </c>
     </row>
     <row r="425" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
-        <v>3516</v>
+        <v>111</v>
       </c>
       <c r="B425" t="s">
-        <v>3518</v>
+        <v>3416</v>
       </c>
       <c r="C425" t="s">
         <v>3544</v>
@@ -70098,13 +70128,16 @@
       <c r="D425" t="s">
         <v>4182</v>
       </c>
+      <c r="E425" t="s">
+        <v>4660</v>
+      </c>
     </row>
     <row r="426" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
-        <v>3424</v>
+        <v>413</v>
       </c>
       <c r="B426" t="s">
-        <v>3425</v>
+        <v>219</v>
       </c>
       <c r="C426" t="s">
         <v>3544</v>
@@ -70113,15 +70146,15 @@
         <v>4182</v>
       </c>
       <c r="E426" t="s">
-        <v>4645</v>
+        <v>4659</v>
       </c>
     </row>
     <row r="427" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
-        <v>3423</v>
+        <v>110</v>
       </c>
       <c r="B427" t="s">
-        <v>3422</v>
+        <v>3415</v>
       </c>
       <c r="C427" t="s">
         <v>3544</v>
@@ -70130,15 +70163,15 @@
         <v>4182</v>
       </c>
       <c r="E427" t="s">
-        <v>4646</v>
+        <v>4661</v>
       </c>
     </row>
     <row r="428" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
-        <v>3420</v>
+        <v>3516</v>
       </c>
       <c r="B428" t="s">
-        <v>3421</v>
+        <v>3518</v>
       </c>
       <c r="C428" t="s">
         <v>3544</v>
@@ -70146,16 +70179,13 @@
       <c r="D428" t="s">
         <v>4182</v>
       </c>
-      <c r="E428" t="s">
-        <v>4647</v>
-      </c>
     </row>
     <row r="429" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
-        <v>3955</v>
+        <v>3424</v>
       </c>
       <c r="B429" t="s">
-        <v>3954</v>
+        <v>3425</v>
       </c>
       <c r="C429" t="s">
         <v>3544</v>
@@ -70164,15 +70194,15 @@
         <v>4182</v>
       </c>
       <c r="E429" t="s">
-        <v>4643</v>
+        <v>4645</v>
       </c>
     </row>
     <row r="430" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
-        <v>3951</v>
+        <v>3423</v>
       </c>
       <c r="B430" t="s">
-        <v>3950</v>
+        <v>3422</v>
       </c>
       <c r="C430" t="s">
         <v>3544</v>
@@ -70181,15 +70211,15 @@
         <v>4182</v>
       </c>
       <c r="E430" t="s">
-        <v>4644</v>
+        <v>4646</v>
       </c>
     </row>
     <row r="431" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
-        <v>3952</v>
+        <v>3420</v>
       </c>
       <c r="B431" t="s">
-        <v>3953</v>
+        <v>3421</v>
       </c>
       <c r="C431" t="s">
         <v>3544</v>
@@ -70198,15 +70228,15 @@
         <v>4182</v>
       </c>
       <c r="E431" t="s">
-        <v>4642</v>
+        <v>4647</v>
       </c>
     </row>
     <row r="432" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
-        <v>3629</v>
-      </c>
-      <c r="B432" s="3" t="s">
-        <v>3630</v>
+        <v>3955</v>
+      </c>
+      <c r="B432" t="s">
+        <v>3954</v>
       </c>
       <c r="C432" t="s">
         <v>3544</v>
@@ -70214,13 +70244,16 @@
       <c r="D432" t="s">
         <v>4182</v>
       </c>
+      <c r="E432" t="s">
+        <v>4643</v>
+      </c>
     </row>
     <row r="433" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
-        <v>3922</v>
-      </c>
-      <c r="B433" s="3" t="s">
-        <v>3923</v>
+        <v>3951</v>
+      </c>
+      <c r="B433" t="s">
+        <v>3950</v>
       </c>
       <c r="C433" t="s">
         <v>3544</v>
@@ -70228,13 +70261,16 @@
       <c r="D433" t="s">
         <v>4182</v>
       </c>
+      <c r="E433" t="s">
+        <v>4644</v>
+      </c>
     </row>
     <row r="434" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
-        <v>21</v>
-      </c>
-      <c r="B434" s="3" t="s">
-        <v>407</v>
+        <v>3952</v>
+      </c>
+      <c r="B434" t="s">
+        <v>3953</v>
       </c>
       <c r="C434" t="s">
         <v>3544</v>
@@ -70242,13 +70278,16 @@
       <c r="D434" t="s">
         <v>4182</v>
       </c>
+      <c r="E434" t="s">
+        <v>4642</v>
+      </c>
     </row>
     <row r="435" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
-        <v>3784</v>
-      </c>
-      <c r="B435" t="s">
-        <v>3631</v>
+        <v>3629</v>
+      </c>
+      <c r="B435" s="3" t="s">
+        <v>3630</v>
       </c>
       <c r="C435" t="s">
         <v>3544</v>
@@ -70257,15 +70296,15 @@
         <v>4182</v>
       </c>
       <c r="E435" t="s">
-        <v>4319</v>
+        <v>5592</v>
       </c>
     </row>
     <row r="436" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
-        <v>3429</v>
-      </c>
-      <c r="B436" t="s">
-        <v>3444</v>
+        <v>3922</v>
+      </c>
+      <c r="B436" s="3" t="s">
+        <v>3923</v>
       </c>
       <c r="C436" t="s">
         <v>3544</v>
@@ -70274,15 +70313,15 @@
         <v>4182</v>
       </c>
       <c r="E436" t="s">
-        <v>4320</v>
+        <v>5592</v>
       </c>
     </row>
     <row r="437" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
-        <v>3446</v>
-      </c>
-      <c r="B437" t="s">
-        <v>3442</v>
+        <v>21</v>
+      </c>
+      <c r="B437" s="3" t="s">
+        <v>407</v>
       </c>
       <c r="C437" t="s">
         <v>3544</v>
@@ -70291,15 +70330,15 @@
         <v>4182</v>
       </c>
       <c r="E437" t="s">
-        <v>4321</v>
+        <v>5591</v>
       </c>
     </row>
     <row r="438" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
-        <v>16</v>
-      </c>
-      <c r="B438" s="3" t="s">
-        <v>354</v>
+        <v>3784</v>
+      </c>
+      <c r="B438" t="s">
+        <v>3631</v>
       </c>
       <c r="C438" t="s">
         <v>3544</v>
@@ -70308,15 +70347,15 @@
         <v>4182</v>
       </c>
       <c r="E438" t="s">
-        <v>4356</v>
+        <v>4319</v>
       </c>
     </row>
     <row r="439" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
-        <v>409</v>
-      </c>
-      <c r="B439" s="3" t="s">
-        <v>358</v>
+        <v>3429</v>
+      </c>
+      <c r="B439" t="s">
+        <v>3444</v>
       </c>
       <c r="C439" t="s">
         <v>3544</v>
@@ -70325,15 +70364,15 @@
         <v>4182</v>
       </c>
       <c r="E439" t="s">
-        <v>4357</v>
+        <v>4320</v>
       </c>
     </row>
     <row r="440" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
-        <v>14</v>
-      </c>
-      <c r="B440" s="3" t="s">
-        <v>355</v>
+        <v>3446</v>
+      </c>
+      <c r="B440" t="s">
+        <v>3442</v>
       </c>
       <c r="C440" t="s">
         <v>3544</v>
@@ -70342,15 +70381,15 @@
         <v>4182</v>
       </c>
       <c r="E440" t="s">
-        <v>4358</v>
+        <v>4321</v>
       </c>
     </row>
     <row r="441" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B441" s="3" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C441" t="s">
         <v>3544</v>
@@ -70359,15 +70398,15 @@
         <v>4182</v>
       </c>
       <c r="E441" t="s">
-        <v>4359</v>
+        <v>4356</v>
       </c>
     </row>
     <row r="442" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
-        <v>15</v>
+        <v>409</v>
       </c>
       <c r="B442" s="3" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="C442" t="s">
         <v>3544</v>
@@ -70376,15 +70415,15 @@
         <v>4182</v>
       </c>
       <c r="E442" t="s">
-        <v>4360</v>
+        <v>4357</v>
       </c>
     </row>
     <row r="443" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="B443" s="3" t="s">
-        <v>414</v>
+        <v>355</v>
       </c>
       <c r="C443" t="s">
         <v>3544</v>
@@ -70393,15 +70432,15 @@
         <v>4182</v>
       </c>
       <c r="E443" t="s">
-        <v>5567</v>
+        <v>4358</v>
       </c>
     </row>
     <row r="444" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="B444" s="3" t="s">
-        <v>415</v>
+        <v>356</v>
       </c>
       <c r="C444" t="s">
         <v>3544</v>
@@ -70410,15 +70449,15 @@
         <v>4182</v>
       </c>
       <c r="E444" t="s">
-        <v>5568</v>
+        <v>4359</v>
       </c>
     </row>
     <row r="445" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="B445" s="3" t="s">
-        <v>416</v>
+        <v>357</v>
       </c>
       <c r="C445" t="s">
         <v>3544</v>
@@ -70427,15 +70466,15 @@
         <v>4182</v>
       </c>
       <c r="E445" t="s">
-        <v>5569</v>
+        <v>4360</v>
       </c>
     </row>
     <row r="446" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B446" s="3" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="C446" t="s">
         <v>3544</v>
@@ -70444,15 +70483,15 @@
         <v>4182</v>
       </c>
       <c r="E446" t="s">
-        <v>5570</v>
+        <v>5567</v>
       </c>
     </row>
     <row r="447" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A447" t="s">
-        <v>3930</v>
-      </c>
-      <c r="B447" t="s">
-        <v>3942</v>
+        <v>3</v>
+      </c>
+      <c r="B447" s="3" t="s">
+        <v>415</v>
       </c>
       <c r="C447" t="s">
         <v>3544</v>
@@ -70460,13 +70499,16 @@
       <c r="D447" t="s">
         <v>4182</v>
       </c>
+      <c r="E447" t="s">
+        <v>5568</v>
+      </c>
     </row>
     <row r="448" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A448" t="s">
-        <v>3948</v>
-      </c>
-      <c r="B448" t="s">
-        <v>3945</v>
+        <v>4</v>
+      </c>
+      <c r="B448" s="3" t="s">
+        <v>416</v>
       </c>
       <c r="C448" t="s">
         <v>3544</v>
@@ -70474,13 +70516,16 @@
       <c r="D448" t="s">
         <v>4182</v>
       </c>
+      <c r="E448" t="s">
+        <v>5569</v>
+      </c>
     </row>
     <row r="449" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A449" t="s">
-        <v>3924</v>
-      </c>
-      <c r="B449" t="s">
-        <v>3940</v>
+        <v>1</v>
+      </c>
+      <c r="B449" s="3" t="s">
+        <v>417</v>
       </c>
       <c r="C449" t="s">
         <v>3544</v>
@@ -70489,15 +70534,15 @@
         <v>4182</v>
       </c>
       <c r="E449" t="s">
-        <v>4512</v>
+        <v>5570</v>
       </c>
     </row>
     <row r="450" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A450" t="s">
-        <v>3927</v>
+        <v>3930</v>
       </c>
       <c r="B450" t="s">
-        <v>3928</v>
+        <v>3942</v>
       </c>
       <c r="C450" t="s">
         <v>3544</v>
@@ -70506,15 +70551,15 @@
         <v>4182</v>
       </c>
       <c r="E450" t="s">
-        <v>4511</v>
+        <v>5594</v>
       </c>
     </row>
     <row r="451" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A451" t="s">
-        <v>3925</v>
+        <v>3948</v>
       </c>
       <c r="B451" t="s">
-        <v>3926</v>
+        <v>3945</v>
       </c>
       <c r="C451" t="s">
         <v>3544</v>
@@ -70523,15 +70568,15 @@
         <v>4182</v>
       </c>
       <c r="E451" t="s">
-        <v>4510</v>
+        <v>5594</v>
       </c>
     </row>
     <row r="452" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A452" t="s">
-        <v>3608</v>
+        <v>3924</v>
       </c>
       <c r="B452" t="s">
-        <v>3609</v>
+        <v>3940</v>
       </c>
       <c r="C452" t="s">
         <v>3544</v>
@@ -70540,15 +70585,15 @@
         <v>4182</v>
       </c>
       <c r="E452" t="s">
-        <v>4682</v>
+        <v>4512</v>
       </c>
     </row>
     <row r="453" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A453" t="s">
-        <v>3612</v>
+        <v>3927</v>
       </c>
       <c r="B453" t="s">
-        <v>3613</v>
+        <v>3928</v>
       </c>
       <c r="C453" t="s">
         <v>3544</v>
@@ -70557,15 +70602,15 @@
         <v>4182</v>
       </c>
       <c r="E453" t="s">
-        <v>4683</v>
+        <v>4511</v>
       </c>
     </row>
     <row r="454" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A454" t="s">
-        <v>3610</v>
+        <v>3925</v>
       </c>
       <c r="B454" t="s">
-        <v>3611</v>
+        <v>3926</v>
       </c>
       <c r="C454" t="s">
         <v>3544</v>
@@ -70574,15 +70619,15 @@
         <v>4182</v>
       </c>
       <c r="E454" t="s">
-        <v>4684</v>
+        <v>4510</v>
       </c>
     </row>
     <row r="455" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A455" t="s">
-        <v>3956</v>
+        <v>3608</v>
       </c>
       <c r="B455" t="s">
-        <v>3965</v>
+        <v>3609</v>
       </c>
       <c r="C455" t="s">
         <v>3544</v>
@@ -70591,15 +70636,15 @@
         <v>4182</v>
       </c>
       <c r="E455" t="s">
-        <v>4586</v>
+        <v>4682</v>
       </c>
     </row>
     <row r="456" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A456" t="s">
-        <v>3961</v>
+        <v>3612</v>
       </c>
       <c r="B456" t="s">
-        <v>3970</v>
+        <v>3613</v>
       </c>
       <c r="C456" t="s">
         <v>3544</v>
@@ -70608,15 +70653,15 @@
         <v>4182</v>
       </c>
       <c r="E456" t="s">
-        <v>4655</v>
+        <v>4683</v>
       </c>
     </row>
     <row r="457" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A457" t="s">
-        <v>3959</v>
+        <v>3610</v>
       </c>
       <c r="B457" t="s">
-        <v>3968</v>
+        <v>3611</v>
       </c>
       <c r="C457" t="s">
         <v>3544</v>
@@ -70625,15 +70670,15 @@
         <v>4182</v>
       </c>
       <c r="E457" t="s">
-        <v>4656</v>
+        <v>4684</v>
       </c>
     </row>
     <row r="458" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A458" t="s">
-        <v>3958</v>
+        <v>3956</v>
       </c>
       <c r="B458" t="s">
-        <v>3967</v>
+        <v>3965</v>
       </c>
       <c r="C458" t="s">
         <v>3544</v>
@@ -70642,15 +70687,15 @@
         <v>4182</v>
       </c>
       <c r="E458" t="s">
-        <v>4653</v>
+        <v>4586</v>
       </c>
     </row>
     <row r="459" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A459" t="s">
-        <v>3960</v>
+        <v>3961</v>
       </c>
       <c r="B459" t="s">
-        <v>3969</v>
+        <v>3970</v>
       </c>
       <c r="C459" t="s">
         <v>3544</v>
@@ -70659,15 +70704,15 @@
         <v>4182</v>
       </c>
       <c r="E459" t="s">
-        <v>4654</v>
+        <v>4655</v>
       </c>
     </row>
     <row r="460" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A460" t="s">
-        <v>3957</v>
+        <v>3959</v>
       </c>
       <c r="B460" t="s">
-        <v>3966</v>
+        <v>3968</v>
       </c>
       <c r="C460" t="s">
         <v>3544</v>
@@ -70676,15 +70721,15 @@
         <v>4182</v>
       </c>
       <c r="E460" t="s">
-        <v>4652</v>
+        <v>4656</v>
       </c>
     </row>
     <row r="461" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A461" t="s">
-        <v>3964</v>
+        <v>3958</v>
       </c>
       <c r="B461" t="s">
-        <v>3973</v>
+        <v>3967</v>
       </c>
       <c r="C461" t="s">
         <v>3544</v>
@@ -70693,15 +70738,15 @@
         <v>4182</v>
       </c>
       <c r="E461" t="s">
-        <v>4655</v>
+        <v>4653</v>
       </c>
     </row>
     <row r="462" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A462" t="s">
-        <v>3962</v>
+        <v>3960</v>
       </c>
       <c r="B462" t="s">
-        <v>3971</v>
+        <v>3969</v>
       </c>
       <c r="C462" t="s">
         <v>3544</v>
@@ -70710,15 +70755,15 @@
         <v>4182</v>
       </c>
       <c r="E462" t="s">
-        <v>4653</v>
+        <v>4654</v>
       </c>
     </row>
     <row r="463" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A463" t="s">
-        <v>3963</v>
+        <v>3957</v>
       </c>
       <c r="B463" t="s">
-        <v>3972</v>
+        <v>3966</v>
       </c>
       <c r="C463" t="s">
         <v>3544</v>
@@ -70727,15 +70772,15 @@
         <v>4182</v>
       </c>
       <c r="E463" t="s">
-        <v>4654</v>
+        <v>4652</v>
       </c>
     </row>
     <row r="464" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A464" t="s">
-        <v>4093</v>
+        <v>3964</v>
       </c>
       <c r="B464" t="s">
-        <v>4111</v>
+        <v>3973</v>
       </c>
       <c r="C464" t="s">
         <v>3544</v>
@@ -70744,15 +70789,15 @@
         <v>4182</v>
       </c>
       <c r="E464" t="s">
-        <v>4688</v>
+        <v>4655</v>
       </c>
     </row>
     <row r="465" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A465" t="s">
-        <v>4092</v>
+        <v>3962</v>
       </c>
       <c r="B465" t="s">
-        <v>4110</v>
+        <v>3971</v>
       </c>
       <c r="C465" t="s">
         <v>3544</v>
@@ -70761,15 +70806,15 @@
         <v>4182</v>
       </c>
       <c r="E465" t="s">
-        <v>4687</v>
+        <v>4653</v>
       </c>
     </row>
     <row r="466" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A466" t="s">
-        <v>3917</v>
+        <v>3963</v>
       </c>
       <c r="B466" t="s">
-        <v>4112</v>
+        <v>3972</v>
       </c>
       <c r="C466" t="s">
         <v>3544</v>
@@ -70778,15 +70823,15 @@
         <v>4182</v>
       </c>
       <c r="E466" t="s">
-        <v>4686</v>
+        <v>4654</v>
       </c>
     </row>
     <row r="467" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A467" t="s">
-        <v>3929</v>
+        <v>4093</v>
       </c>
       <c r="B467" t="s">
-        <v>3941</v>
+        <v>4111</v>
       </c>
       <c r="C467" t="s">
         <v>3544</v>
@@ -70794,13 +70839,16 @@
       <c r="D467" t="s">
         <v>4182</v>
       </c>
+      <c r="E467" t="s">
+        <v>4688</v>
+      </c>
     </row>
     <row r="468" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A468" t="s">
-        <v>3947</v>
+        <v>4092</v>
       </c>
       <c r="B468" t="s">
-        <v>3944</v>
+        <v>4110</v>
       </c>
       <c r="C468" t="s">
         <v>3544</v>
@@ -70808,13 +70856,16 @@
       <c r="D468" t="s">
         <v>4182</v>
       </c>
+      <c r="E468" t="s">
+        <v>4687</v>
+      </c>
     </row>
     <row r="469" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A469" t="s">
-        <v>4117</v>
+        <v>3917</v>
       </c>
       <c r="B469" t="s">
-        <v>3427</v>
+        <v>4112</v>
       </c>
       <c r="C469" t="s">
         <v>3544</v>
@@ -70823,15 +70874,15 @@
         <v>4182</v>
       </c>
       <c r="E469" t="s">
-        <v>4689</v>
+        <v>4686</v>
       </c>
     </row>
     <row r="470" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A470" t="s">
-        <v>4118</v>
+        <v>3929</v>
       </c>
       <c r="B470" t="s">
-        <v>4114</v>
+        <v>3941</v>
       </c>
       <c r="C470" t="s">
         <v>3544</v>
@@ -70840,15 +70891,15 @@
         <v>4182</v>
       </c>
       <c r="E470" t="s">
-        <v>4690</v>
+        <v>5593</v>
       </c>
     </row>
     <row r="471" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A471" t="s">
-        <v>4119</v>
+        <v>3947</v>
       </c>
       <c r="B471" t="s">
-        <v>4115</v>
+        <v>3944</v>
       </c>
       <c r="C471" t="s">
         <v>3544</v>
@@ -70857,15 +70908,15 @@
         <v>4182</v>
       </c>
       <c r="E471" t="s">
-        <v>4691</v>
+        <v>5593</v>
       </c>
     </row>
     <row r="472" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A472" t="s">
-        <v>4120</v>
+        <v>4117</v>
       </c>
       <c r="B472" t="s">
-        <v>4116</v>
+        <v>3427</v>
       </c>
       <c r="C472" t="s">
         <v>3544</v>
@@ -70874,15 +70925,15 @@
         <v>4182</v>
       </c>
       <c r="E472" t="s">
-        <v>4692</v>
+        <v>4689</v>
       </c>
     </row>
     <row r="473" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A473" t="s">
-        <v>3618</v>
-      </c>
-      <c r="B473" s="3" t="s">
-        <v>3619</v>
+        <v>4118</v>
+      </c>
+      <c r="B473" t="s">
+        <v>4114</v>
       </c>
       <c r="C473" t="s">
         <v>3544</v>
@@ -70891,15 +70942,15 @@
         <v>4182</v>
       </c>
       <c r="E473" t="s">
-        <v>4693</v>
+        <v>4690</v>
       </c>
     </row>
     <row r="474" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A474" t="s">
-        <v>3617</v>
-      </c>
-      <c r="B474" s="3" t="s">
-        <v>3615</v>
+        <v>4119</v>
+      </c>
+      <c r="B474" t="s">
+        <v>4115</v>
       </c>
       <c r="C474" t="s">
         <v>3544</v>
@@ -70908,15 +70959,15 @@
         <v>4182</v>
       </c>
       <c r="E474" t="s">
-        <v>4694</v>
+        <v>4691</v>
       </c>
     </row>
     <row r="475" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A475" t="s">
-        <v>3616</v>
-      </c>
-      <c r="B475" s="3" t="s">
-        <v>3614</v>
+        <v>4120</v>
+      </c>
+      <c r="B475" t="s">
+        <v>4116</v>
       </c>
       <c r="C475" t="s">
         <v>3544</v>
@@ -70925,15 +70976,15 @@
         <v>4182</v>
       </c>
       <c r="E475" t="s">
-        <v>4695</v>
+        <v>4692</v>
       </c>
     </row>
     <row r="476" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A476" t="s">
-        <v>3515</v>
-      </c>
-      <c r="B476" t="s">
-        <v>3517</v>
+        <v>3618</v>
+      </c>
+      <c r="B476" s="3" t="s">
+        <v>3619</v>
       </c>
       <c r="C476" t="s">
         <v>3544</v>
@@ -70941,13 +70992,16 @@
       <c r="D476" t="s">
         <v>4182</v>
       </c>
+      <c r="E476" t="s">
+        <v>4693</v>
+      </c>
     </row>
     <row r="477" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A477" t="s">
-        <v>3920</v>
-      </c>
-      <c r="B477" t="s">
-        <v>3921</v>
+        <v>3617</v>
+      </c>
+      <c r="B477" s="3" t="s">
+        <v>3615</v>
       </c>
       <c r="C477" t="s">
         <v>3544</v>
@@ -70956,15 +71010,15 @@
         <v>4182</v>
       </c>
       <c r="E477" t="s">
-        <v>4508</v>
+        <v>4694</v>
       </c>
     </row>
     <row r="478" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A478" t="s">
-        <v>4109</v>
-      </c>
-      <c r="B478" t="s">
-        <v>4108</v>
+        <v>3616</v>
+      </c>
+      <c r="B478" s="3" t="s">
+        <v>3614</v>
       </c>
       <c r="C478" t="s">
         <v>3544</v>
@@ -70973,15 +71027,15 @@
         <v>4182</v>
       </c>
       <c r="E478" t="s">
-        <v>4587</v>
+        <v>4695</v>
       </c>
     </row>
     <row r="479" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A479" t="s">
-        <v>3976</v>
+        <v>3515</v>
       </c>
       <c r="B479" t="s">
-        <v>3977</v>
+        <v>3517</v>
       </c>
       <c r="C479" t="s">
         <v>3544</v>
@@ -70989,16 +71043,13 @@
       <c r="D479" t="s">
         <v>4182</v>
       </c>
-      <c r="E479" t="s">
-        <v>4610</v>
-      </c>
     </row>
     <row r="480" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A480" t="s">
-        <v>3974</v>
+        <v>3920</v>
       </c>
       <c r="B480" t="s">
-        <v>3975</v>
+        <v>3921</v>
       </c>
       <c r="C480" t="s">
         <v>3544</v>
@@ -71007,15 +71058,15 @@
         <v>4182</v>
       </c>
       <c r="E480" t="s">
-        <v>4611</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="481" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A481" t="s">
-        <v>4121</v>
+        <v>4109</v>
       </c>
       <c r="B481" t="s">
-        <v>4122</v>
+        <v>4108</v>
       </c>
       <c r="C481" t="s">
         <v>3544</v>
@@ -71024,15 +71075,15 @@
         <v>4182</v>
       </c>
       <c r="E481" t="s">
-        <v>4657</v>
+        <v>4587</v>
       </c>
     </row>
     <row r="482" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A482" t="s">
-        <v>13</v>
-      </c>
-      <c r="B482" s="3" t="s">
-        <v>158</v>
+        <v>3976</v>
+      </c>
+      <c r="B482" t="s">
+        <v>3977</v>
       </c>
       <c r="C482" t="s">
         <v>3544</v>
@@ -71041,66 +71092,66 @@
         <v>4182</v>
       </c>
       <c r="E482" t="s">
-        <v>5566</v>
+        <v>4610</v>
       </c>
     </row>
     <row r="483" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A483" t="s">
-        <v>108</v>
+        <v>3974</v>
       </c>
       <c r="B483" t="s">
-        <v>189</v>
+        <v>3975</v>
       </c>
       <c r="C483" t="s">
-        <v>3545</v>
+        <v>3544</v>
       </c>
       <c r="D483" t="s">
         <v>4182</v>
       </c>
       <c r="E483" t="s">
-        <v>4327</v>
+        <v>4611</v>
       </c>
     </row>
     <row r="484" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A484" t="s">
-        <v>104</v>
+        <v>4121</v>
       </c>
       <c r="B484" t="s">
-        <v>193</v>
+        <v>4122</v>
       </c>
       <c r="C484" t="s">
-        <v>3545</v>
+        <v>3544</v>
       </c>
       <c r="D484" t="s">
         <v>4182</v>
       </c>
       <c r="E484" t="s">
-        <v>4477</v>
+        <v>4657</v>
       </c>
     </row>
     <row r="485" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A485" t="s">
-        <v>102</v>
-      </c>
-      <c r="B485" t="s">
-        <v>191</v>
+        <v>13</v>
+      </c>
+      <c r="B485" s="3" t="s">
+        <v>158</v>
       </c>
       <c r="C485" t="s">
-        <v>3545</v>
+        <v>3544</v>
       </c>
       <c r="D485" t="s">
         <v>4182</v>
       </c>
       <c r="E485" t="s">
-        <v>4478</v>
+        <v>5566</v>
       </c>
     </row>
     <row r="486" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A486" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B486" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C486" t="s">
         <v>3545</v>
@@ -71109,15 +71160,15 @@
         <v>4182</v>
       </c>
       <c r="E486" t="s">
-        <v>4479</v>
+        <v>4327</v>
       </c>
     </row>
     <row r="487" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A487" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B487" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C487" t="s">
         <v>3545</v>
@@ -71126,15 +71177,15 @@
         <v>4182</v>
       </c>
       <c r="E487" t="s">
-        <v>4480</v>
+        <v>4477</v>
       </c>
     </row>
     <row r="488" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A488" t="s">
-        <v>91</v>
+        <v>102</v>
       </c>
       <c r="B488" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="C488" t="s">
         <v>3545</v>
@@ -71143,15 +71194,15 @@
         <v>4182</v>
       </c>
       <c r="E488" t="s">
-        <v>4308</v>
+        <v>4478</v>
       </c>
     </row>
     <row r="489" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A489" t="s">
-        <v>99</v>
+        <v>103</v>
       </c>
       <c r="B489" t="s">
-        <v>181</v>
+        <v>192</v>
       </c>
       <c r="C489" t="s">
         <v>3545</v>
@@ -71160,15 +71211,15 @@
         <v>4182</v>
       </c>
       <c r="E489" t="s">
-        <v>4275</v>
+        <v>4479</v>
       </c>
     </row>
     <row r="490" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A490" t="s">
-        <v>92</v>
+        <v>105</v>
       </c>
       <c r="B490" t="s">
-        <v>175</v>
+        <v>194</v>
       </c>
       <c r="C490" t="s">
         <v>3545</v>
@@ -71177,15 +71228,15 @@
         <v>4182</v>
       </c>
       <c r="E490" t="s">
-        <v>4276</v>
+        <v>4480</v>
       </c>
     </row>
     <row r="491" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A491" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B491" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C491" t="s">
         <v>3545</v>
@@ -71194,15 +71245,15 @@
         <v>4182</v>
       </c>
       <c r="E491" t="s">
-        <v>4277</v>
+        <v>4308</v>
       </c>
     </row>
     <row r="492" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A492" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="B492" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="C492" t="s">
         <v>3545</v>
@@ -71211,15 +71262,15 @@
         <v>4182</v>
       </c>
       <c r="E492" t="s">
-        <v>4282</v>
+        <v>4275</v>
       </c>
     </row>
     <row r="493" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A493" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B493" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="C493" t="s">
         <v>3545</v>
@@ -71228,15 +71279,15 @@
         <v>4182</v>
       </c>
       <c r="E493" t="s">
-        <v>4283</v>
+        <v>4276</v>
       </c>
     </row>
     <row r="494" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A494" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B494" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C494" t="s">
         <v>3545</v>
@@ -71245,15 +71296,15 @@
         <v>4182</v>
       </c>
       <c r="E494" t="s">
-        <v>4287</v>
+        <v>4277</v>
       </c>
     </row>
     <row r="495" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A495" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="B495" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="C495" t="s">
         <v>3545</v>
@@ -71262,15 +71313,15 @@
         <v>4182</v>
       </c>
       <c r="E495" t="s">
-        <v>4289</v>
+        <v>4282</v>
       </c>
     </row>
     <row r="496" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A496" t="s">
-        <v>116</v>
+        <v>90</v>
       </c>
       <c r="B496" t="s">
-        <v>186</v>
+        <v>173</v>
       </c>
       <c r="C496" t="s">
         <v>3545</v>
@@ -71279,15 +71330,15 @@
         <v>4182</v>
       </c>
       <c r="E496" t="s">
-        <v>4330</v>
+        <v>4283</v>
       </c>
     </row>
     <row r="497" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A497" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="B497" t="s">
-        <v>187</v>
+        <v>177</v>
       </c>
       <c r="C497" t="s">
         <v>3545</v>
@@ -71296,15 +71347,15 @@
         <v>4182</v>
       </c>
       <c r="E497" t="s">
-        <v>4331</v>
+        <v>4287</v>
       </c>
     </row>
     <row r="498" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A498" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B498" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C498" t="s">
         <v>3545</v>
@@ -71313,15 +71364,15 @@
         <v>4182</v>
       </c>
       <c r="E498" t="s">
-        <v>4292</v>
+        <v>4289</v>
       </c>
     </row>
     <row r="499" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A499" t="s">
-        <v>98</v>
+        <v>116</v>
       </c>
       <c r="B499" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C499" t="s">
         <v>3545</v>
@@ -71330,15 +71381,15 @@
         <v>4182</v>
       </c>
       <c r="E499" t="s">
-        <v>4297</v>
+        <v>4330</v>
       </c>
     </row>
     <row r="500" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A500" t="s">
-        <v>117</v>
+        <v>107</v>
       </c>
       <c r="B500" t="s">
-        <v>3682</v>
+        <v>187</v>
       </c>
       <c r="C500" t="s">
         <v>3545</v>
@@ -71347,15 +71398,15 @@
         <v>4182</v>
       </c>
       <c r="E500" t="s">
-        <v>4332</v>
+        <v>4331</v>
       </c>
     </row>
     <row r="501" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A501" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="B501" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C501" t="s">
         <v>3545</v>
@@ -71364,15 +71415,15 @@
         <v>4182</v>
       </c>
       <c r="E501" t="s">
-        <v>4329</v>
+        <v>4292</v>
       </c>
     </row>
     <row r="502" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A502" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B502" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="C502" t="s">
         <v>3545</v>
@@ -71381,15 +71432,15 @@
         <v>4182</v>
       </c>
       <c r="E502" t="s">
-        <v>4305</v>
+        <v>4297</v>
       </c>
     </row>
     <row r="503" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A503" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="B503" t="s">
-        <v>185</v>
+        <v>3682</v>
       </c>
       <c r="C503" t="s">
         <v>3545</v>
@@ -71398,15 +71449,15 @@
         <v>4182</v>
       </c>
       <c r="E503" t="s">
-        <v>4259</v>
+        <v>4332</v>
       </c>
     </row>
     <row r="504" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A504" t="s">
-        <v>100</v>
+        <v>106</v>
       </c>
       <c r="B504" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="C504" t="s">
         <v>3545</v>
@@ -71415,15 +71466,15 @@
         <v>4182</v>
       </c>
       <c r="E504" t="s">
-        <v>4241</v>
+        <v>4329</v>
       </c>
     </row>
     <row r="505" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A505" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B505" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="C505" t="s">
         <v>3545</v>
@@ -71432,15 +71483,15 @@
         <v>4182</v>
       </c>
       <c r="E505" t="s">
-        <v>4249</v>
+        <v>4305</v>
       </c>
     </row>
     <row r="506" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A506" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B506" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="C506" t="s">
         <v>3545</v>
@@ -71449,66 +71500,66 @@
         <v>4182</v>
       </c>
       <c r="E506" t="s">
-        <v>4333</v>
+        <v>4259</v>
       </c>
     </row>
     <row r="507" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A507" t="s">
-        <v>4208</v>
+        <v>100</v>
       </c>
       <c r="B507" t="s">
-        <v>4198</v>
+        <v>183</v>
       </c>
       <c r="C507" t="s">
-        <v>3543</v>
+        <v>3545</v>
       </c>
       <c r="D507" t="s">
         <v>4182</v>
       </c>
-      <c r="E507" s="4" t="s">
-        <v>4482</v>
+      <c r="E507" t="s">
+        <v>4241</v>
       </c>
     </row>
     <row r="508" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A508" t="s">
-        <v>4209</v>
+        <v>101</v>
       </c>
       <c r="B508" t="s">
-        <v>4199</v>
+        <v>184</v>
       </c>
       <c r="C508" t="s">
-        <v>3543</v>
+        <v>3545</v>
       </c>
       <c r="D508" t="s">
         <v>4182</v>
       </c>
-      <c r="E508" s="4" t="s">
-        <v>4483</v>
+      <c r="E508" t="s">
+        <v>4249</v>
       </c>
     </row>
     <row r="509" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A509" t="s">
-        <v>4210</v>
+        <v>115</v>
       </c>
       <c r="B509" t="s">
-        <v>4200</v>
+        <v>190</v>
       </c>
       <c r="C509" t="s">
-        <v>3543</v>
+        <v>3545</v>
       </c>
       <c r="D509" t="s">
         <v>4182</v>
       </c>
-      <c r="E509" s="4" t="s">
-        <v>4484</v>
+      <c r="E509" t="s">
+        <v>4333</v>
       </c>
     </row>
     <row r="510" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A510" t="s">
-        <v>4211</v>
+        <v>4208</v>
       </c>
       <c r="B510" t="s">
-        <v>4201</v>
+        <v>4198</v>
       </c>
       <c r="C510" t="s">
         <v>3543</v>
@@ -71517,15 +71568,15 @@
         <v>4182</v>
       </c>
       <c r="E510" s="4" t="s">
-        <v>4485</v>
+        <v>4482</v>
       </c>
     </row>
     <row r="511" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A511" t="s">
-        <v>4212</v>
+        <v>4209</v>
       </c>
       <c r="B511" t="s">
-        <v>4202</v>
+        <v>4199</v>
       </c>
       <c r="C511" t="s">
         <v>3543</v>
@@ -71534,15 +71585,15 @@
         <v>4182</v>
       </c>
       <c r="E511" s="4" t="s">
-        <v>4486</v>
+        <v>4483</v>
       </c>
     </row>
     <row r="512" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A512" t="s">
-        <v>4213</v>
+        <v>4210</v>
       </c>
       <c r="B512" t="s">
-        <v>4203</v>
+        <v>4200</v>
       </c>
       <c r="C512" t="s">
         <v>3543</v>
@@ -71551,15 +71602,15 @@
         <v>4182</v>
       </c>
       <c r="E512" s="4" t="s">
-        <v>4487</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="513" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A513" t="s">
-        <v>4214</v>
+        <v>4211</v>
       </c>
       <c r="B513" t="s">
-        <v>4204</v>
+        <v>4201</v>
       </c>
       <c r="C513" t="s">
         <v>3543</v>
@@ -71568,15 +71619,15 @@
         <v>4182</v>
       </c>
       <c r="E513" s="4" t="s">
-        <v>4488</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="514" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A514" t="s">
-        <v>4215</v>
+        <v>4212</v>
       </c>
       <c r="B514" t="s">
-        <v>4205</v>
+        <v>4202</v>
       </c>
       <c r="C514" t="s">
         <v>3543</v>
@@ -71585,15 +71636,15 @@
         <v>4182</v>
       </c>
       <c r="E514" s="4" t="s">
-        <v>4489</v>
+        <v>4486</v>
       </c>
     </row>
     <row r="515" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A515" t="s">
-        <v>4216</v>
+        <v>4213</v>
       </c>
       <c r="B515" t="s">
-        <v>4206</v>
+        <v>4203</v>
       </c>
       <c r="C515" t="s">
         <v>3543</v>
@@ -71602,15 +71653,15 @@
         <v>4182</v>
       </c>
       <c r="E515" s="4" t="s">
-        <v>4490</v>
+        <v>4487</v>
       </c>
     </row>
     <row r="516" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A516" t="s">
-        <v>4217</v>
+        <v>4214</v>
       </c>
       <c r="B516" t="s">
-        <v>4207</v>
+        <v>4204</v>
       </c>
       <c r="C516" t="s">
         <v>3543</v>
@@ -71619,15 +71670,15 @@
         <v>4182</v>
       </c>
       <c r="E516" s="4" t="s">
-        <v>4491</v>
+        <v>4488</v>
       </c>
     </row>
     <row r="517" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A517" t="s">
-        <v>4223</v>
+        <v>4215</v>
       </c>
       <c r="B517" t="s">
-        <v>4224</v>
+        <v>4205</v>
       </c>
       <c r="C517" t="s">
         <v>3543</v>
@@ -71636,176 +71687,179 @@
         <v>4182</v>
       </c>
       <c r="E517" s="4" t="s">
-        <v>4481</v>
+        <v>4489</v>
       </c>
     </row>
     <row r="518" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A518" t="s">
-        <v>4225</v>
+        <v>4216</v>
       </c>
       <c r="B518" t="s">
-        <v>4226</v>
+        <v>4206</v>
       </c>
       <c r="C518" t="s">
-        <v>3544</v>
+        <v>3543</v>
       </c>
       <c r="D518" t="s">
         <v>4182</v>
       </c>
       <c r="E518" s="4" t="s">
-        <v>4588</v>
+        <v>4490</v>
       </c>
     </row>
     <row r="519" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A519" t="s">
-        <v>4227</v>
+        <v>4217</v>
       </c>
       <c r="B519" t="s">
-        <v>4230</v>
+        <v>4207</v>
       </c>
       <c r="C519" t="s">
-        <v>3544</v>
+        <v>3543</v>
       </c>
       <c r="D519" t="s">
         <v>4182</v>
       </c>
       <c r="E519" s="4" t="s">
-        <v>4492</v>
+        <v>4491</v>
       </c>
     </row>
     <row r="520" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A520" t="s">
-        <v>4228</v>
+        <v>4223</v>
       </c>
       <c r="B520" t="s">
-        <v>4229</v>
+        <v>4224</v>
       </c>
       <c r="C520" t="s">
-        <v>3544</v>
+        <v>3543</v>
       </c>
       <c r="D520" t="s">
         <v>4182</v>
       </c>
       <c r="E520" s="4" t="s">
-        <v>4493</v>
+        <v>4481</v>
       </c>
     </row>
     <row r="521" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A521" s="13" t="s">
-        <v>4179</v>
-      </c>
-      <c r="B521" s="4" t="s">
-        <v>4180</v>
+      <c r="A521" t="s">
+        <v>4225</v>
+      </c>
+      <c r="B521" t="s">
+        <v>4226</v>
       </c>
       <c r="C521" t="s">
-        <v>4065</v>
+        <v>3544</v>
       </c>
       <c r="D521" t="s">
-        <v>4183</v>
+        <v>4182</v>
+      </c>
+      <c r="E521" s="4" t="s">
+        <v>4588</v>
       </c>
     </row>
     <row r="522" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A522" s="13" t="s">
-        <v>4177</v>
-      </c>
-      <c r="B522" s="4" t="s">
-        <v>4178</v>
+      <c r="A522" t="s">
+        <v>4227</v>
+      </c>
+      <c r="B522" t="s">
+        <v>4230</v>
       </c>
       <c r="C522" t="s">
-        <v>4059</v>
+        <v>3544</v>
       </c>
       <c r="D522" t="s">
-        <v>4183</v>
+        <v>4182</v>
+      </c>
+      <c r="E522" s="4" t="s">
+        <v>4492</v>
       </c>
     </row>
     <row r="523" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>4231</v>
+        <v>4228</v>
       </c>
       <c r="B523" t="s">
-        <v>4232</v>
+        <v>4229</v>
       </c>
       <c r="C523" t="s">
-        <v>4059</v>
+        <v>3544</v>
       </c>
       <c r="D523" t="s">
-        <v>4183</v>
+        <v>4182</v>
+      </c>
+      <c r="E523" s="4" t="s">
+        <v>4493</v>
       </c>
     </row>
     <row r="524" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A524" t="s">
-        <v>4234</v>
-      </c>
-      <c r="B524" t="s">
-        <v>4233</v>
+      <c r="A524" s="13" t="s">
+        <v>4179</v>
+      </c>
+      <c r="B524" s="4" t="s">
+        <v>4180</v>
       </c>
       <c r="C524" t="s">
-        <v>4059</v>
+        <v>4065</v>
       </c>
       <c r="D524" t="s">
         <v>4183</v>
       </c>
-      <c r="E524" t="s">
+      <c r="E524" s="4" t="s">
+        <v>5595</v>
+      </c>
+    </row>
+    <row r="525" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A525" s="13" t="s">
+        <v>4177</v>
+      </c>
+      <c r="B525" s="4" t="s">
+        <v>4178</v>
+      </c>
+      <c r="C525" t="s">
+        <v>4059</v>
+      </c>
+      <c r="D525" t="s">
+        <v>4183</v>
+      </c>
+    </row>
+    <row r="526" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A526" t="s">
+        <v>4231</v>
+      </c>
+      <c r="B526" t="s">
+        <v>4232</v>
+      </c>
+      <c r="C526" t="s">
+        <v>4059</v>
+      </c>
+      <c r="D526" t="s">
+        <v>4183</v>
+      </c>
+    </row>
+    <row r="527" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A527" t="s">
+        <v>4234</v>
+      </c>
+      <c r="B527" t="s">
+        <v>4233</v>
+      </c>
+      <c r="C527" t="s">
+        <v>4059</v>
+      </c>
+      <c r="D527" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E527" t="s">
         <v>4685</v>
-      </c>
-    </row>
-    <row r="525" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A525" s="13">
-        <v>1376</v>
-      </c>
-      <c r="B525" s="4" t="s">
-        <v>4069</v>
-      </c>
-      <c r="C525" t="s">
-        <v>4073</v>
-      </c>
-      <c r="D525" t="s">
-        <v>4185</v>
-      </c>
-      <c r="E525" t="s">
-        <v>4494</v>
-      </c>
-    </row>
-    <row r="526" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A526" s="13">
-        <v>1374</v>
-      </c>
-      <c r="B526" s="4" t="s">
-        <v>4067</v>
-      </c>
-      <c r="C526" t="s">
-        <v>4073</v>
-      </c>
-      <c r="D526" t="s">
-        <v>4185</v>
-      </c>
-      <c r="E526" t="s">
-        <v>4589</v>
-      </c>
-    </row>
-    <row r="527" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A527" s="13">
-        <v>1375</v>
-      </c>
-      <c r="B527" s="4" t="s">
-        <v>4068</v>
-      </c>
-      <c r="C527" t="s">
-        <v>4073</v>
-      </c>
-      <c r="D527" t="s">
-        <v>4185</v>
-      </c>
-      <c r="E527" t="s">
-        <v>4495</v>
       </c>
     </row>
     <row r="528" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A528" s="13">
-        <v>1373</v>
+        <v>1376</v>
       </c>
       <c r="B528" s="4" t="s">
-        <v>4066</v>
+        <v>4069</v>
       </c>
       <c r="C528" t="s">
         <v>4073</v>
@@ -71814,15 +71868,15 @@
         <v>4185</v>
       </c>
       <c r="E528" t="s">
-        <v>4496</v>
+        <v>4494</v>
       </c>
     </row>
     <row r="529" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A529" s="13">
-        <v>1379</v>
+        <v>1374</v>
       </c>
       <c r="B529" s="4" t="s">
-        <v>4072</v>
+        <v>4067</v>
       </c>
       <c r="C529" t="s">
         <v>4073</v>
@@ -71831,15 +71885,15 @@
         <v>4185</v>
       </c>
       <c r="E529" t="s">
-        <v>4590</v>
+        <v>4589</v>
       </c>
     </row>
     <row r="530" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A530" s="13">
-        <v>1380</v>
+        <v>1375</v>
       </c>
       <c r="B530" s="4" t="s">
-        <v>4071</v>
+        <v>4068</v>
       </c>
       <c r="C530" t="s">
         <v>4073</v>
@@ -71848,15 +71902,15 @@
         <v>4185</v>
       </c>
       <c r="E530" t="s">
-        <v>4591</v>
+        <v>4495</v>
       </c>
     </row>
     <row r="531" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A531" s="13">
-        <v>1378</v>
+        <v>1373</v>
       </c>
       <c r="B531" s="4" t="s">
-        <v>4070</v>
+        <v>4066</v>
       </c>
       <c r="C531" t="s">
         <v>4073</v>
@@ -71870,47 +71924,47 @@
     </row>
     <row r="532" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A532" s="13">
-        <v>20716</v>
+        <v>1379</v>
       </c>
       <c r="B532" s="4" t="s">
-        <v>4166</v>
+        <v>4072</v>
       </c>
       <c r="C532" t="s">
-        <v>4062</v>
+        <v>4073</v>
       </c>
       <c r="D532" t="s">
         <v>4185</v>
       </c>
       <c r="E532" t="s">
-        <v>4505</v>
+        <v>4590</v>
       </c>
     </row>
     <row r="533" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A533" s="13">
-        <v>20715</v>
+        <v>1380</v>
       </c>
       <c r="B533" s="4" t="s">
-        <v>4167</v>
+        <v>4071</v>
       </c>
       <c r="C533" t="s">
-        <v>4062</v>
+        <v>4073</v>
       </c>
       <c r="D533" t="s">
         <v>4185</v>
       </c>
       <c r="E533" t="s">
-        <v>4506</v>
+        <v>4591</v>
       </c>
     </row>
     <row r="534" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A534" s="13">
-        <v>20714</v>
+        <v>1378</v>
       </c>
       <c r="B534" s="4" t="s">
-        <v>4061</v>
+        <v>4070</v>
       </c>
       <c r="C534" t="s">
-        <v>4062</v>
+        <v>4073</v>
       </c>
       <c r="D534" t="s">
         <v>4185</v>
@@ -71921,10 +71975,10 @@
     </row>
     <row r="535" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A535" s="13">
-        <v>27702</v>
+        <v>20716</v>
       </c>
       <c r="B535" s="4" t="s">
-        <v>4173</v>
+        <v>4166</v>
       </c>
       <c r="C535" t="s">
         <v>4062</v>
@@ -71933,15 +71987,15 @@
         <v>4185</v>
       </c>
       <c r="E535" t="s">
-        <v>4504</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="536" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A536" s="13">
-        <v>27701</v>
+        <v>20715</v>
       </c>
       <c r="B536" s="4" t="s">
-        <v>4172</v>
+        <v>4167</v>
       </c>
       <c r="C536" t="s">
         <v>4062</v>
@@ -71950,15 +72004,15 @@
         <v>4185</v>
       </c>
       <c r="E536" t="s">
-        <v>4503</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="537" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A537" s="13">
-        <v>20541</v>
+        <v>20714</v>
       </c>
       <c r="B537" s="4" t="s">
-        <v>4165</v>
+        <v>4061</v>
       </c>
       <c r="C537" t="s">
         <v>4062</v>
@@ -71967,15 +72021,15 @@
         <v>4185</v>
       </c>
       <c r="E537" t="s">
-        <v>4505</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="538" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A538" s="13">
-        <v>20540</v>
+        <v>27702</v>
       </c>
       <c r="B538" s="4" t="s">
-        <v>4164</v>
+        <v>4173</v>
       </c>
       <c r="C538" t="s">
         <v>4062</v>
@@ -71984,15 +72038,15 @@
         <v>4185</v>
       </c>
       <c r="E538" t="s">
-        <v>4506</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="539" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A539" s="13">
-        <v>20539</v>
+        <v>27701</v>
       </c>
       <c r="B539" s="4" t="s">
-        <v>4174</v>
+        <v>4172</v>
       </c>
       <c r="C539" t="s">
         <v>4062</v>
@@ -72001,15 +72055,15 @@
         <v>4185</v>
       </c>
       <c r="E539" t="s">
-        <v>4496</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="540" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A540" s="13">
-        <v>20606</v>
+        <v>20541</v>
       </c>
       <c r="B540" s="4" t="s">
-        <v>4171</v>
+        <v>4165</v>
       </c>
       <c r="C540" t="s">
         <v>4062</v>
@@ -72018,15 +72072,15 @@
         <v>4185</v>
       </c>
       <c r="E540" t="s">
-        <v>4608</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="541" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A541" s="13">
-        <v>20594</v>
+        <v>20540</v>
       </c>
       <c r="B541" s="4" t="s">
-        <v>4169</v>
+        <v>4164</v>
       </c>
       <c r="C541" t="s">
         <v>4062</v>
@@ -72035,15 +72089,15 @@
         <v>4185</v>
       </c>
       <c r="E541" t="s">
-        <v>4609</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="542" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A542" s="13">
-        <v>25359</v>
+        <v>20539</v>
       </c>
       <c r="B542" s="4" t="s">
-        <v>4604</v>
+        <v>4174</v>
       </c>
       <c r="C542" t="s">
         <v>4062</v>
@@ -72052,15 +72106,15 @@
         <v>4185</v>
       </c>
       <c r="E542" t="s">
-        <v>4505</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="543" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A543" s="13">
-        <v>25358</v>
+        <v>20606</v>
       </c>
       <c r="B543" s="4" t="s">
-        <v>4603</v>
+        <v>4171</v>
       </c>
       <c r="C543" t="s">
         <v>4062</v>
@@ -72069,15 +72123,15 @@
         <v>4185</v>
       </c>
       <c r="E543" t="s">
-        <v>4506</v>
+        <v>4608</v>
       </c>
     </row>
     <row r="544" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A544" s="13">
-        <v>25357</v>
+        <v>20594</v>
       </c>
       <c r="B544" s="4" t="s">
-        <v>4605</v>
+        <v>4169</v>
       </c>
       <c r="C544" t="s">
         <v>4062</v>
@@ -72086,15 +72140,15 @@
         <v>4185</v>
       </c>
       <c r="E544" t="s">
-        <v>4496</v>
+        <v>4609</v>
       </c>
     </row>
     <row r="545" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A545" s="13">
-        <v>20570</v>
+        <v>25359</v>
       </c>
       <c r="B545" s="4" t="s">
-        <v>4170</v>
+        <v>4604</v>
       </c>
       <c r="C545" t="s">
         <v>4062</v>
@@ -72103,15 +72157,15 @@
         <v>4185</v>
       </c>
       <c r="E545" t="s">
-        <v>4606</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="546" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A546" s="13">
-        <v>20543</v>
+        <v>25358</v>
       </c>
       <c r="B546" s="4" t="s">
-        <v>4168</v>
+        <v>4603</v>
       </c>
       <c r="C546" t="s">
         <v>4062</v>
@@ -72120,15 +72174,15 @@
         <v>4185</v>
       </c>
       <c r="E546" t="s">
-        <v>4607</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="547" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A547" s="13">
-        <v>21084</v>
+        <v>25357</v>
       </c>
       <c r="B547" s="4" t="s">
-        <v>4175</v>
+        <v>4605</v>
       </c>
       <c r="C547" t="s">
         <v>4062</v>
@@ -72137,15 +72191,15 @@
         <v>4185</v>
       </c>
       <c r="E547" t="s">
-        <v>4505</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="548" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A548" s="13">
-        <v>21083</v>
+        <v>20570</v>
       </c>
       <c r="B548" s="4" t="s">
-        <v>4176</v>
+        <v>4170</v>
       </c>
       <c r="C548" t="s">
         <v>4062</v>
@@ -72154,66 +72208,66 @@
         <v>4185</v>
       </c>
       <c r="E548" t="s">
-        <v>4506</v>
+        <v>4606</v>
       </c>
     </row>
     <row r="549" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A549" s="13">
-        <v>13762</v>
+        <v>20543</v>
       </c>
       <c r="B549" s="4" t="s">
-        <v>4063</v>
+        <v>4168</v>
       </c>
       <c r="C549" t="s">
-        <v>4065</v>
+        <v>4062</v>
       </c>
       <c r="D549" t="s">
         <v>4185</v>
       </c>
       <c r="E549" t="s">
-        <v>4498</v>
+        <v>4607</v>
       </c>
     </row>
     <row r="550" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A550" s="13">
-        <v>4536</v>
+        <v>21084</v>
       </c>
       <c r="B550" s="4" t="s">
-        <v>4064</v>
+        <v>4175</v>
       </c>
       <c r="C550" t="s">
-        <v>4065</v>
+        <v>4062</v>
       </c>
       <c r="D550" t="s">
         <v>4185</v>
       </c>
       <c r="E550" t="s">
-        <v>4499</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="551" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A551" s="13">
-        <v>4513</v>
+        <v>21083</v>
       </c>
       <c r="B551" s="4" t="s">
-        <v>4131</v>
+        <v>4176</v>
       </c>
       <c r="C551" t="s">
-        <v>4065</v>
+        <v>4062</v>
       </c>
       <c r="D551" t="s">
         <v>4185</v>
       </c>
       <c r="E551" t="s">
-        <v>4500</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="552" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A552" s="13">
-        <v>5727</v>
+        <v>13762</v>
       </c>
       <c r="B552" s="4" t="s">
-        <v>4132</v>
+        <v>4063</v>
       </c>
       <c r="C552" t="s">
         <v>4065</v>
@@ -72222,15 +72276,15 @@
         <v>4185</v>
       </c>
       <c r="E552" t="s">
-        <v>4502</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="553" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A553" s="13">
-        <v>5793</v>
+        <v>4536</v>
       </c>
       <c r="B553" s="4" t="s">
-        <v>4133</v>
+        <v>4064</v>
       </c>
       <c r="C553" t="s">
         <v>4065</v>
@@ -72239,100 +72293,100 @@
         <v>4185</v>
       </c>
       <c r="E553" t="s">
-        <v>4501</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="554" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A554" s="13">
-        <v>13521</v>
+        <v>4513</v>
       </c>
       <c r="B554" s="4" t="s">
-        <v>4074</v>
+        <v>4131</v>
       </c>
       <c r="C554" t="s">
-        <v>4075</v>
+        <v>4065</v>
       </c>
       <c r="D554" t="s">
         <v>4185</v>
       </c>
       <c r="E554" t="s">
-        <v>4497</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="555" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A555" s="13">
-        <v>28784</v>
+        <v>5727</v>
       </c>
       <c r="B555" s="4" t="s">
-        <v>4060</v>
+        <v>4132</v>
       </c>
       <c r="C555" t="s">
-        <v>4059</v>
+        <v>4065</v>
       </c>
       <c r="D555" t="s">
         <v>4185</v>
       </c>
       <c r="E555" t="s">
+        <v>4502</v>
+      </c>
+    </row>
+    <row r="556" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A556" s="13">
+        <v>5793</v>
+      </c>
+      <c r="B556" s="4" t="s">
+        <v>4133</v>
+      </c>
+      <c r="C556" t="s">
+        <v>4065</v>
+      </c>
+      <c r="D556" t="s">
+        <v>4185</v>
+      </c>
+      <c r="E556" t="s">
+        <v>4501</v>
+      </c>
+    </row>
+    <row r="557" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A557" s="13">
+        <v>13521</v>
+      </c>
+      <c r="B557" s="4" t="s">
+        <v>4074</v>
+      </c>
+      <c r="C557" t="s">
+        <v>4075</v>
+      </c>
+      <c r="D557" t="s">
+        <v>4185</v>
+      </c>
+      <c r="E557" t="s">
+        <v>4497</v>
+      </c>
+    </row>
+    <row r="558" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A558" s="13">
+        <v>28784</v>
+      </c>
+      <c r="B558" s="4" t="s">
+        <v>4060</v>
+      </c>
+      <c r="C558" t="s">
+        <v>4059</v>
+      </c>
+      <c r="D558" t="s">
+        <v>4185</v>
+      </c>
+      <c r="E558" t="s">
         <v>4496</v>
-      </c>
-    </row>
-    <row r="556" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A556" t="s">
-        <v>4336</v>
-      </c>
-      <c r="B556" t="s">
-        <v>4343</v>
-      </c>
-      <c r="C556" t="s">
-        <v>3544</v>
-      </c>
-      <c r="D556" t="s">
-        <v>4182</v>
-      </c>
-      <c r="E556" t="s">
-        <v>4592</v>
-      </c>
-    </row>
-    <row r="557" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A557" t="s">
-        <v>4337</v>
-      </c>
-      <c r="B557" t="s">
-        <v>4344</v>
-      </c>
-      <c r="C557" t="s">
-        <v>3544</v>
-      </c>
-      <c r="D557" t="s">
-        <v>4182</v>
-      </c>
-      <c r="E557" t="s">
-        <v>4593</v>
-      </c>
-    </row>
-    <row r="558" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A558" t="s">
-        <v>4335</v>
-      </c>
-      <c r="B558" t="s">
-        <v>4345</v>
-      </c>
-      <c r="C558" t="s">
-        <v>3544</v>
-      </c>
-      <c r="D558" t="s">
-        <v>4182</v>
-      </c>
-      <c r="E558" t="s">
-        <v>4594</v>
       </c>
     </row>
     <row r="559" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A559" t="s">
-        <v>4334</v>
+        <v>4336</v>
       </c>
       <c r="B559" t="s">
-        <v>4346</v>
+        <v>4343</v>
       </c>
       <c r="C559" t="s">
         <v>3544</v>
@@ -72341,15 +72395,15 @@
         <v>4182</v>
       </c>
       <c r="E559" t="s">
-        <v>4595</v>
+        <v>4592</v>
       </c>
     </row>
     <row r="560" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A560" t="s">
-        <v>4338</v>
+        <v>4337</v>
       </c>
       <c r="B560" t="s">
-        <v>4347</v>
+        <v>4344</v>
       </c>
       <c r="C560" t="s">
         <v>3544</v>
@@ -72358,15 +72412,15 @@
         <v>4182</v>
       </c>
       <c r="E560" t="s">
-        <v>4596</v>
+        <v>4593</v>
       </c>
     </row>
     <row r="561" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A561" t="s">
-        <v>4339</v>
+        <v>4335</v>
       </c>
       <c r="B561" t="s">
-        <v>4348</v>
+        <v>4345</v>
       </c>
       <c r="C561" t="s">
         <v>3544</v>
@@ -72375,15 +72429,15 @@
         <v>4182</v>
       </c>
       <c r="E561" t="s">
-        <v>4597</v>
+        <v>4594</v>
       </c>
     </row>
     <row r="562" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A562" t="s">
-        <v>4340</v>
+        <v>4334</v>
       </c>
       <c r="B562" t="s">
-        <v>4349</v>
+        <v>4346</v>
       </c>
       <c r="C562" t="s">
         <v>3544</v>
@@ -72392,15 +72446,15 @@
         <v>4182</v>
       </c>
       <c r="E562" t="s">
-        <v>4598</v>
+        <v>4595</v>
       </c>
     </row>
     <row r="563" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A563" t="s">
-        <v>4341</v>
+        <v>4338</v>
       </c>
       <c r="B563" t="s">
-        <v>4350</v>
+        <v>4347</v>
       </c>
       <c r="C563" t="s">
         <v>3544</v>
@@ -72409,15 +72463,15 @@
         <v>4182</v>
       </c>
       <c r="E563" t="s">
-        <v>4599</v>
+        <v>4596</v>
       </c>
     </row>
     <row r="564" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A564" t="s">
-        <v>4342</v>
+        <v>4339</v>
       </c>
       <c r="B564" t="s">
-        <v>4351</v>
+        <v>4348</v>
       </c>
       <c r="C564" t="s">
         <v>3544</v>
@@ -72426,15 +72480,15 @@
         <v>4182</v>
       </c>
       <c r="E564" t="s">
-        <v>4600</v>
+        <v>4597</v>
       </c>
     </row>
     <row r="565" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A565" t="s">
-        <v>4352</v>
+        <v>4340</v>
       </c>
       <c r="B565" t="s">
-        <v>4353</v>
+        <v>4349</v>
       </c>
       <c r="C565" t="s">
         <v>3544</v>
@@ -72443,15 +72497,15 @@
         <v>4182</v>
       </c>
       <c r="E565" t="s">
-        <v>4601</v>
+        <v>4598</v>
       </c>
     </row>
     <row r="566" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A566" t="s">
-        <v>4354</v>
+        <v>4341</v>
       </c>
       <c r="B566" t="s">
-        <v>4355</v>
+        <v>4350</v>
       </c>
       <c r="C566" t="s">
         <v>3544</v>
@@ -72460,15 +72514,15 @@
         <v>4182</v>
       </c>
       <c r="E566" t="s">
-        <v>4602</v>
+        <v>4599</v>
       </c>
     </row>
     <row r="567" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A567" t="s">
-        <v>5521</v>
+        <v>4342</v>
       </c>
       <c r="B567" t="s">
-        <v>5522</v>
+        <v>4351</v>
       </c>
       <c r="C567" t="s">
         <v>3544</v>
@@ -72477,15 +72531,15 @@
         <v>4182</v>
       </c>
       <c r="E567" t="s">
-        <v>5553</v>
+        <v>4600</v>
       </c>
     </row>
     <row r="568" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A568" t="s">
-        <v>5523</v>
+        <v>4352</v>
       </c>
       <c r="B568" t="s">
-        <v>5524</v>
+        <v>4353</v>
       </c>
       <c r="C568" t="s">
         <v>3544</v>
@@ -72494,15 +72548,15 @@
         <v>4182</v>
       </c>
       <c r="E568" t="s">
-        <v>5550</v>
+        <v>4601</v>
       </c>
     </row>
     <row r="569" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A569" t="s">
-        <v>5525</v>
+        <v>4354</v>
       </c>
       <c r="B569" t="s">
-        <v>5526</v>
+        <v>4355</v>
       </c>
       <c r="C569" t="s">
         <v>3544</v>
@@ -72511,15 +72565,15 @@
         <v>4182</v>
       </c>
       <c r="E569" t="s">
-        <v>5551</v>
+        <v>4602</v>
       </c>
     </row>
     <row r="570" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A570" t="s">
-        <v>5527</v>
+        <v>5521</v>
       </c>
       <c r="B570" t="s">
-        <v>5528</v>
+        <v>5522</v>
       </c>
       <c r="C570" t="s">
         <v>3544</v>
@@ -72528,66 +72582,66 @@
         <v>4182</v>
       </c>
       <c r="E570" t="s">
-        <v>5552</v>
+        <v>5553</v>
       </c>
     </row>
     <row r="571" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A571" t="s">
-        <v>5529</v>
+        <v>5523</v>
       </c>
       <c r="B571" t="s">
-        <v>5530</v>
+        <v>5524</v>
       </c>
       <c r="C571" t="s">
-        <v>4075</v>
+        <v>3544</v>
       </c>
       <c r="D571" t="s">
-        <v>4183</v>
+        <v>4182</v>
       </c>
       <c r="E571" t="s">
-        <v>5548</v>
+        <v>5550</v>
       </c>
     </row>
     <row r="572" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A572" t="s">
-        <v>5531</v>
+        <v>5525</v>
       </c>
       <c r="B572" t="s">
-        <v>5532</v>
+        <v>5526</v>
       </c>
       <c r="C572" t="s">
-        <v>4075</v>
+        <v>3544</v>
       </c>
       <c r="D572" t="s">
-        <v>4183</v>
+        <v>4182</v>
       </c>
       <c r="E572" t="s">
-        <v>5549</v>
+        <v>5551</v>
       </c>
     </row>
     <row r="573" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A573" t="s">
-        <v>5533</v>
+        <v>5527</v>
       </c>
       <c r="B573" t="s">
-        <v>5536</v>
+        <v>5528</v>
       </c>
       <c r="C573" t="s">
-        <v>4075</v>
+        <v>3544</v>
       </c>
       <c r="D573" t="s">
-        <v>4183</v>
+        <v>4182</v>
       </c>
       <c r="E573" t="s">
-        <v>5537</v>
+        <v>5552</v>
       </c>
     </row>
     <row r="574" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A574" t="s">
-        <v>5534</v>
+        <v>5529</v>
       </c>
       <c r="B574" t="s">
-        <v>5535</v>
+        <v>5530</v>
       </c>
       <c r="C574" t="s">
         <v>4075</v>
@@ -72596,117 +72650,117 @@
         <v>4183</v>
       </c>
       <c r="E574" t="s">
-        <v>5538</v>
+        <v>5548</v>
       </c>
     </row>
     <row r="575" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A575" t="s">
-        <v>5539</v>
+        <v>5531</v>
       </c>
       <c r="B575" t="s">
-        <v>5540</v>
+        <v>5532</v>
       </c>
       <c r="C575" t="s">
-        <v>425</v>
+        <v>4075</v>
       </c>
       <c r="D575" t="s">
         <v>4183</v>
       </c>
       <c r="E575" t="s">
-        <v>5541</v>
+        <v>5549</v>
       </c>
     </row>
     <row r="576" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A576" t="s">
-        <v>5545</v>
+        <v>5533</v>
       </c>
       <c r="B576" t="s">
-        <v>5546</v>
+        <v>5536</v>
       </c>
       <c r="C576" t="s">
-        <v>425</v>
+        <v>4075</v>
       </c>
       <c r="D576" t="s">
         <v>4183</v>
       </c>
       <c r="E576" t="s">
-        <v>5542</v>
+        <v>5537</v>
       </c>
     </row>
     <row r="577" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A577" t="s">
-        <v>5543</v>
+        <v>5534</v>
       </c>
       <c r="B577" t="s">
-        <v>5547</v>
+        <v>5535</v>
       </c>
       <c r="C577" t="s">
-        <v>425</v>
+        <v>4075</v>
       </c>
       <c r="D577" t="s">
         <v>4183</v>
       </c>
       <c r="E577" t="s">
-        <v>5544</v>
+        <v>5538</v>
       </c>
     </row>
     <row r="578" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A578" t="s">
-        <v>5554</v>
+        <v>5539</v>
       </c>
       <c r="B578" t="s">
-        <v>5560</v>
+        <v>5540</v>
       </c>
       <c r="C578" t="s">
-        <v>4075</v>
+        <v>425</v>
       </c>
       <c r="D578" t="s">
         <v>4183</v>
       </c>
       <c r="E578" t="s">
-        <v>5556</v>
+        <v>5541</v>
       </c>
     </row>
     <row r="579" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A579" t="s">
-        <v>5555</v>
+        <v>5545</v>
       </c>
       <c r="B579" t="s">
-        <v>5561</v>
+        <v>5546</v>
       </c>
       <c r="C579" t="s">
-        <v>4075</v>
+        <v>425</v>
       </c>
       <c r="D579" t="s">
         <v>4183</v>
       </c>
       <c r="E579" t="s">
-        <v>5557</v>
+        <v>5542</v>
       </c>
     </row>
     <row r="580" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A580" t="s">
-        <v>5558</v>
+        <v>5543</v>
       </c>
       <c r="B580" t="s">
-        <v>5562</v>
+        <v>5547</v>
       </c>
       <c r="C580" t="s">
-        <v>4075</v>
+        <v>425</v>
       </c>
       <c r="D580" t="s">
         <v>4183</v>
       </c>
       <c r="E580" t="s">
-        <v>5559</v>
+        <v>5544</v>
       </c>
     </row>
     <row r="581" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A581" t="s">
-        <v>5563</v>
+        <v>5554</v>
       </c>
       <c r="B581" t="s">
-        <v>5565</v>
+        <v>5560</v>
       </c>
       <c r="C581" t="s">
         <v>4075</v>
@@ -72715,66 +72769,117 @@
         <v>4183</v>
       </c>
       <c r="E581" t="s">
+        <v>5556</v>
+      </c>
+    </row>
+    <row r="582" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A582" t="s">
+        <v>5555</v>
+      </c>
+      <c r="B582" t="s">
+        <v>5561</v>
+      </c>
+      <c r="C582" t="s">
+        <v>4075</v>
+      </c>
+      <c r="D582" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E582" t="s">
+        <v>5557</v>
+      </c>
+    </row>
+    <row r="583" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A583" t="s">
+        <v>5558</v>
+      </c>
+      <c r="B583" t="s">
+        <v>5562</v>
+      </c>
+      <c r="C583" t="s">
+        <v>4075</v>
+      </c>
+      <c r="D583" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E583" t="s">
+        <v>5559</v>
+      </c>
+    </row>
+    <row r="584" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A584" t="s">
+        <v>5563</v>
+      </c>
+      <c r="B584" t="s">
+        <v>5565</v>
+      </c>
+      <c r="C584" t="s">
+        <v>4075</v>
+      </c>
+      <c r="D584" t="s">
+        <v>4183</v>
+      </c>
+      <c r="E584" t="s">
         <v>5564</v>
-      </c>
-    </row>
-    <row r="582" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B582" t="s">
-        <v>5576</v>
-      </c>
-      <c r="C582" t="s">
-        <v>3544</v>
-      </c>
-      <c r="E582" t="s">
-        <v>4667</v>
-      </c>
-    </row>
-    <row r="583" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B583" t="s">
-        <v>5577</v>
-      </c>
-      <c r="C583" t="s">
-        <v>3544</v>
-      </c>
-      <c r="E583" t="s">
-        <v>4669</v>
-      </c>
-    </row>
-    <row r="584" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B584" t="s">
-        <v>5578</v>
-      </c>
-      <c r="C584" t="s">
-        <v>3544</v>
-      </c>
-      <c r="E584" t="s">
-        <v>4670</v>
       </c>
     </row>
     <row r="585" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B585" t="s">
-        <v>5579</v>
+        <v>5574</v>
       </c>
       <c r="C585" t="s">
         <v>3544</v>
       </c>
       <c r="E585" t="s">
-        <v>4671</v>
+        <v>4667</v>
       </c>
     </row>
     <row r="586" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B586" t="s">
-        <v>5580</v>
+        <v>5575</v>
       </c>
       <c r="C586" t="s">
         <v>3544</v>
       </c>
       <c r="E586" t="s">
+        <v>4669</v>
+      </c>
+    </row>
+    <row r="587" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B587" t="s">
+        <v>5576</v>
+      </c>
+      <c r="C587" t="s">
+        <v>3544</v>
+      </c>
+      <c r="E587" t="s">
+        <v>4670</v>
+      </c>
+    </row>
+    <row r="588" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B588" t="s">
+        <v>5577</v>
+      </c>
+      <c r="C588" t="s">
+        <v>3544</v>
+      </c>
+      <c r="E588" t="s">
+        <v>4671</v>
+      </c>
+    </row>
+    <row r="589" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B589" t="s">
+        <v>5578</v>
+      </c>
+      <c r="C589" t="s">
+        <v>3544</v>
+      </c>
+      <c r="E589" t="s">
         <v>4666</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E566" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
+  <autoFilter ref="A1:E569" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Inclusão de melhorias @202406190956
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7C52B91-2593-4EB9-9A62-2AC65E4E2404}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36FDADED-30EC-4B14-AB41-3B749A29C9A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="3280" windowWidth="19420" windowHeight="10300" tabRatio="754" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" tabRatio="754" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fixed_income_signals" sheetId="23" r:id="rId1"/>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15294" uniqueCount="5603">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15338" uniqueCount="5625">
   <si>
     <t>category</t>
   </si>
@@ -16858,6 +16858,72 @@
   </si>
   <si>
     <t>RSTAXYOY Index</t>
+  </si>
+  <si>
+    <t>futures</t>
+  </si>
+  <si>
+    <t>ODA Comdty</t>
+  </si>
+  <si>
+    <t>UCA Curncy</t>
+  </si>
+  <si>
+    <t>XBA Index</t>
+  </si>
+  <si>
+    <t>WDOA Curncy</t>
+  </si>
+  <si>
+    <t>LSA Comdty</t>
+  </si>
+  <si>
+    <t>QBTA Curncy</t>
+  </si>
+  <si>
+    <t>AXA Comdty</t>
+  </si>
+  <si>
+    <t>CRDA Comdty</t>
+  </si>
+  <si>
+    <t>boi gordo</t>
+  </si>
+  <si>
+    <t>THEA Comdty</t>
+  </si>
+  <si>
+    <t>BMA Curncy</t>
+  </si>
+  <si>
+    <t>br_di_futures</t>
+  </si>
+  <si>
+    <t>br_usd_futures</t>
+  </si>
+  <si>
+    <t>br_ibovespa_mini_futures</t>
+  </si>
+  <si>
+    <t>br_ibovespa_futures</t>
+  </si>
+  <si>
+    <t>br_usd_mini_futures</t>
+  </si>
+  <si>
+    <t>br_bitcoin_futures</t>
+  </si>
+  <si>
+    <t>br_corn_futures</t>
+  </si>
+  <si>
+    <t>br_coffee_futures</t>
+  </si>
+  <si>
+    <t>br_ethanol_futures</t>
+  </si>
+  <si>
+    <t>br_eur_futures</t>
   </si>
 </sst>
 </file>
@@ -17611,7 +17677,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B68" sqref="B68"/>
+      <selection pane="bottomLeft" activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18434,11 +18500,11 @@
   <sheetPr codeName="Planilha10"/>
   <dimension ref="A1:N1281"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B796" activePane="bottomRight" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B758" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D815" sqref="D815"/>
+      <selection pane="bottomRight" activeCell="G798" sqref="G798"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63024,11 +63090,11 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E589"/>
+  <dimension ref="A1:E600"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A383" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D393" sqref="D393"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A562" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B601" sqref="B601"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -72878,6 +72944,160 @@
         <v>4666</v>
       </c>
     </row>
+    <row r="590" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A590" t="s">
+        <v>5604</v>
+      </c>
+      <c r="B590" t="s">
+        <v>5615</v>
+      </c>
+      <c r="C590" t="s">
+        <v>5603</v>
+      </c>
+      <c r="D590" t="s">
+        <v>4182</v>
+      </c>
+    </row>
+    <row r="591" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A591" t="s">
+        <v>5605</v>
+      </c>
+      <c r="B591" t="s">
+        <v>5616</v>
+      </c>
+      <c r="C591" t="s">
+        <v>5603</v>
+      </c>
+      <c r="D591" t="s">
+        <v>4182</v>
+      </c>
+    </row>
+    <row r="592" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A592" t="s">
+        <v>5606</v>
+      </c>
+      <c r="B592" t="s">
+        <v>5617</v>
+      </c>
+      <c r="C592" t="s">
+        <v>5603</v>
+      </c>
+      <c r="D592" t="s">
+        <v>4182</v>
+      </c>
+    </row>
+    <row r="593" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A593" t="s">
+        <v>3339</v>
+      </c>
+      <c r="B593" t="s">
+        <v>5618</v>
+      </c>
+      <c r="C593" t="s">
+        <v>5603</v>
+      </c>
+      <c r="D593" t="s">
+        <v>4182</v>
+      </c>
+    </row>
+    <row r="594" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A594" t="s">
+        <v>5607</v>
+      </c>
+      <c r="B594" t="s">
+        <v>5619</v>
+      </c>
+      <c r="C594" t="s">
+        <v>5603</v>
+      </c>
+      <c r="D594" t="s">
+        <v>4182</v>
+      </c>
+    </row>
+    <row r="595" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A595" t="s">
+        <v>5608</v>
+      </c>
+      <c r="B595" t="s">
+        <v>5612</v>
+      </c>
+      <c r="C595" t="s">
+        <v>5603</v>
+      </c>
+      <c r="D595" t="s">
+        <v>4182</v>
+      </c>
+    </row>
+    <row r="596" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A596" t="s">
+        <v>5609</v>
+      </c>
+      <c r="B596" t="s">
+        <v>5620</v>
+      </c>
+      <c r="C596" t="s">
+        <v>5603</v>
+      </c>
+      <c r="D596" t="s">
+        <v>4182</v>
+      </c>
+    </row>
+    <row r="597" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A597" t="s">
+        <v>5610</v>
+      </c>
+      <c r="B597" t="s">
+        <v>5622</v>
+      </c>
+      <c r="C597" t="s">
+        <v>5603</v>
+      </c>
+      <c r="D597" t="s">
+        <v>4182</v>
+      </c>
+    </row>
+    <row r="598" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A598" t="s">
+        <v>5611</v>
+      </c>
+      <c r="B598" t="s">
+        <v>5621</v>
+      </c>
+      <c r="C598" t="s">
+        <v>5603</v>
+      </c>
+      <c r="D598" t="s">
+        <v>4182</v>
+      </c>
+    </row>
+    <row r="599" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A599" t="s">
+        <v>5613</v>
+      </c>
+      <c r="B599" t="s">
+        <v>5623</v>
+      </c>
+      <c r="C599" t="s">
+        <v>5603</v>
+      </c>
+      <c r="D599" t="s">
+        <v>4182</v>
+      </c>
+    </row>
+    <row r="600" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A600" t="s">
+        <v>5614</v>
+      </c>
+      <c r="B600" t="s">
+        <v>5624</v>
+      </c>
+      <c r="C600" t="s">
+        <v>5603</v>
+      </c>
+      <c r="D600" t="s">
+        <v>4182</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E569" xr:uid="{00000000-0009-0000-0000-000007000000}"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Inclusão de melhorias @202406211030
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C5F4A24-2594-4865-B972-9EC65A9D577D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4C2BD5-4808-4BBF-996B-2C28775AD450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" tabRatio="754" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" tabRatio="754" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="fixed_income_signals" sheetId="23" r:id="rId1"/>
-    <sheet name="equity_signals" sheetId="19" r:id="rId2"/>
-    <sheet name="index_signals" sheetId="14" r:id="rId3"/>
+    <sheet name="index_signals" sheetId="14" r:id="rId2"/>
+    <sheet name="equity_signals" sheetId="19" r:id="rId3"/>
     <sheet name="&gt;" sheetId="9" r:id="rId4"/>
     <sheet name="equities" sheetId="3" r:id="rId5"/>
     <sheet name="anbima" sheetId="13" r:id="rId6"/>
@@ -25,7 +25,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">equities!$A$1:$L$1268</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">equity_signals!$A$1:$D$61</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">equity_signals!$A$1:$D$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fixed_income_signals!$A$1:$C$15</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">indicators!$A$1:$E$600</definedName>
   </definedNames>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15492" uniqueCount="5664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15492" uniqueCount="5665">
   <si>
     <t>category</t>
   </si>
@@ -17042,6 +17042,9 @@
   </si>
   <si>
     <t>cost_of_capital</t>
+  </si>
+  <si>
+    <t>ICB</t>
   </si>
 </sst>
 </file>
@@ -17790,908 +17793,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:D79"/>
-  <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B57" sqref="B57"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>3351</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>3408</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>5660</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3387</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3742</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3904</v>
-      </c>
-      <c r="D2" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3382</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3383</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3904</v>
-      </c>
-      <c r="D3" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3767</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3768</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3904</v>
-      </c>
-      <c r="D4" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3378</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3380</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3904</v>
-      </c>
-      <c r="D5" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3372</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3376</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3904</v>
-      </c>
-      <c r="D6" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3371</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3375</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3904</v>
-      </c>
-      <c r="D7" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3392</v>
-      </c>
-      <c r="B8" t="s">
-        <v>3393</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3904</v>
-      </c>
-      <c r="D8" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
-        <v>3390</v>
-      </c>
-      <c r="B9" t="s">
-        <v>3391</v>
-      </c>
-      <c r="C9" t="s">
-        <v>3904</v>
-      </c>
-      <c r="D9" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>3388</v>
-      </c>
-      <c r="B10" t="s">
-        <v>3389</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3904</v>
-      </c>
-      <c r="D10" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>3379</v>
-      </c>
-      <c r="B11" t="s">
-        <v>3381</v>
-      </c>
-      <c r="C11" t="s">
-        <v>3904</v>
-      </c>
-      <c r="D11" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>3370</v>
-      </c>
-      <c r="B12" t="s">
-        <v>3374</v>
-      </c>
-      <c r="C12" t="s">
-        <v>3904</v>
-      </c>
-      <c r="D12" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>3384</v>
-      </c>
-      <c r="B13" t="s">
-        <v>3385</v>
-      </c>
-      <c r="C13" t="s">
-        <v>3904</v>
-      </c>
-      <c r="D13" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>3373</v>
-      </c>
-      <c r="B14" t="s">
-        <v>3377</v>
-      </c>
-      <c r="C14" t="s">
-        <v>3904</v>
-      </c>
-      <c r="D14" t="s">
-        <v>3904</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>4053</v>
-      </c>
-      <c r="B15" t="s">
-        <v>4054</v>
-      </c>
-      <c r="C15" t="s">
-        <v>4056</v>
-      </c>
-      <c r="D15" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>4052</v>
-      </c>
-      <c r="B16" t="s">
-        <v>4055</v>
-      </c>
-      <c r="C16" t="s">
-        <v>4056</v>
-      </c>
-      <c r="D16" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>5653</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>5656</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5656</v>
-      </c>
-      <c r="D17" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>5651</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>5654</v>
-      </c>
-      <c r="C18" t="s">
-        <v>5656</v>
-      </c>
-      <c r="D18" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>5652</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>5655</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5656</v>
-      </c>
-      <c r="D19" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>3747</v>
-      </c>
-      <c r="B20" t="s">
-        <v>3806</v>
-      </c>
-      <c r="C20" t="s">
-        <v>3905</v>
-      </c>
-      <c r="D20" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>3748</v>
-      </c>
-      <c r="B21" t="s">
-        <v>3805</v>
-      </c>
-      <c r="C21" t="s">
-        <v>3905</v>
-      </c>
-      <c r="D21" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>3790</v>
-      </c>
-      <c r="B22" t="s">
-        <v>3791</v>
-      </c>
-      <c r="C22" t="s">
-        <v>3903</v>
-      </c>
-      <c r="D22" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>3397</v>
-      </c>
-      <c r="B23" t="s">
-        <v>3396</v>
-      </c>
-      <c r="C23" t="s">
-        <v>3903</v>
-      </c>
-      <c r="D23" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>3364</v>
-      </c>
-      <c r="B24" t="s">
-        <v>3368</v>
-      </c>
-      <c r="C24" t="s">
-        <v>3903</v>
-      </c>
-      <c r="D24" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>3363</v>
-      </c>
-      <c r="B25" t="s">
-        <v>3367</v>
-      </c>
-      <c r="C25" t="s">
-        <v>3903</v>
-      </c>
-      <c r="D25" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>3361</v>
-      </c>
-      <c r="B26" t="s">
-        <v>3365</v>
-      </c>
-      <c r="C26" t="s">
-        <v>3903</v>
-      </c>
-      <c r="D26" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>3762</v>
-      </c>
-      <c r="B27" t="s">
-        <v>3765</v>
-      </c>
-      <c r="C27" t="s">
-        <v>3903</v>
-      </c>
-      <c r="D27" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>3763</v>
-      </c>
-      <c r="B28" t="s">
-        <v>3766</v>
-      </c>
-      <c r="C28" t="s">
-        <v>3903</v>
-      </c>
-      <c r="D28" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>3761</v>
-      </c>
-      <c r="B29" t="s">
-        <v>3764</v>
-      </c>
-      <c r="C29" t="s">
-        <v>3903</v>
-      </c>
-      <c r="D29" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>3362</v>
-      </c>
-      <c r="B30" t="s">
-        <v>3366</v>
-      </c>
-      <c r="C30" t="s">
-        <v>3903</v>
-      </c>
-      <c r="D30" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>3358</v>
-      </c>
-      <c r="B31" t="s">
-        <v>3395</v>
-      </c>
-      <c r="C31" t="s">
-        <v>3912</v>
-      </c>
-      <c r="D31" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>3401</v>
-      </c>
-      <c r="B32" t="s">
-        <v>3404</v>
-      </c>
-      <c r="C32" t="s">
-        <v>3907</v>
-      </c>
-      <c r="D32" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>3402</v>
-      </c>
-      <c r="B33" t="s">
-        <v>3405</v>
-      </c>
-      <c r="C33" t="s">
-        <v>3907</v>
-      </c>
-      <c r="D33" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>3403</v>
-      </c>
-      <c r="B34" t="s">
-        <v>3406</v>
-      </c>
-      <c r="C34" t="s">
-        <v>3907</v>
-      </c>
-      <c r="D34" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>3749</v>
-      </c>
-      <c r="B35" t="s">
-        <v>3750</v>
-      </c>
-      <c r="C35" t="s">
-        <v>3902</v>
-      </c>
-      <c r="D35" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>3751</v>
-      </c>
-      <c r="B36" t="s">
-        <v>3752</v>
-      </c>
-      <c r="C36" t="s">
-        <v>3902</v>
-      </c>
-      <c r="D36" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>3901</v>
-      </c>
-      <c r="B37" s="4" t="s">
-        <v>3902</v>
-      </c>
-      <c r="C37" t="s">
-        <v>3902</v>
-      </c>
-      <c r="D37" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>3754</v>
-      </c>
-      <c r="B38" t="s">
-        <v>3760</v>
-      </c>
-      <c r="C38" t="s">
-        <v>3906</v>
-      </c>
-      <c r="D38" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>3755</v>
-      </c>
-      <c r="B39" t="s">
-        <v>3758</v>
-      </c>
-      <c r="C39" t="s">
-        <v>3906</v>
-      </c>
-      <c r="D39" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>3756</v>
-      </c>
-      <c r="B40" t="s">
-        <v>3759</v>
-      </c>
-      <c r="C40" t="s">
-        <v>3906</v>
-      </c>
-      <c r="D40" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>3753</v>
-      </c>
-      <c r="B41" t="s">
-        <v>3757</v>
-      </c>
-      <c r="C41" t="s">
-        <v>3906</v>
-      </c>
-      <c r="D41" t="s">
-        <v>5657</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>4057</v>
-      </c>
-      <c r="B42" t="s">
-        <v>4058</v>
-      </c>
-      <c r="C42" t="s">
-        <v>4058</v>
-      </c>
-      <c r="D42" t="s">
-        <v>5659</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>3400</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>3412</v>
-      </c>
-      <c r="C43" t="s">
-        <v>3909</v>
-      </c>
-      <c r="D43" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>3915</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>3916</v>
-      </c>
-      <c r="C44" t="s">
-        <v>3909</v>
-      </c>
-      <c r="D44" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>3357</v>
-      </c>
-      <c r="B45" t="s">
-        <v>3394</v>
-      </c>
-      <c r="C45" t="s">
-        <v>3909</v>
-      </c>
-      <c r="D45" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>3913</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>3914</v>
-      </c>
-      <c r="C46" t="s">
-        <v>3909</v>
-      </c>
-      <c r="D46" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>3356</v>
-      </c>
-      <c r="B47" t="s">
-        <v>3399</v>
-      </c>
-      <c r="C47" t="s">
-        <v>3909</v>
-      </c>
-      <c r="D47" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>3411</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>3409</v>
-      </c>
-      <c r="C48" t="s">
-        <v>3909</v>
-      </c>
-      <c r="D48" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>3359</v>
-      </c>
-      <c r="B49" t="s">
-        <v>3398</v>
-      </c>
-      <c r="C49" t="s">
-        <v>3909</v>
-      </c>
-      <c r="D49" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>3352</v>
-      </c>
-      <c r="B50" t="s">
-        <v>3354</v>
-      </c>
-      <c r="C50" t="s">
-        <v>3909</v>
-      </c>
-      <c r="D50" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>3353</v>
-      </c>
-      <c r="B51" t="s">
-        <v>3355</v>
-      </c>
-      <c r="C51" t="s">
-        <v>3909</v>
-      </c>
-      <c r="D51" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>4036</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>4035</v>
-      </c>
-      <c r="C52" t="s">
-        <v>3911</v>
-      </c>
-      <c r="D52" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>3796</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>3803</v>
-      </c>
-      <c r="C53" t="s">
-        <v>3911</v>
-      </c>
-      <c r="D53" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>3410</v>
-      </c>
-      <c r="B54" t="s">
-        <v>3804</v>
-      </c>
-      <c r="C54" t="s">
-        <v>3910</v>
-      </c>
-      <c r="D54" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>3797</v>
-      </c>
-      <c r="B55" t="s">
-        <v>3801</v>
-      </c>
-      <c r="C55" t="s">
-        <v>3910</v>
-      </c>
-      <c r="D55" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>3793</v>
-      </c>
-      <c r="B56" t="s">
-        <v>3800</v>
-      </c>
-      <c r="C56" t="s">
-        <v>3910</v>
-      </c>
-      <c r="D56" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
-        <v>3795</v>
-      </c>
-      <c r="B57" t="s">
-        <v>3799</v>
-      </c>
-      <c r="C57" t="s">
-        <v>3910</v>
-      </c>
-      <c r="D57" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>3794</v>
-      </c>
-      <c r="B58" t="s">
-        <v>3802</v>
-      </c>
-      <c r="C58" t="s">
-        <v>3910</v>
-      </c>
-      <c r="D58" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>3792</v>
-      </c>
-      <c r="B59" t="s">
-        <v>3798</v>
-      </c>
-      <c r="C59" t="s">
-        <v>3910</v>
-      </c>
-      <c r="D59" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>3743</v>
-      </c>
-      <c r="B60" t="s">
-        <v>3745</v>
-      </c>
-      <c r="C60" t="s">
-        <v>3908</v>
-      </c>
-      <c r="D60" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>3744</v>
-      </c>
-      <c r="B61" t="s">
-        <v>3746</v>
-      </c>
-      <c r="C61" t="s">
-        <v>3908</v>
-      </c>
-      <c r="D61" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>5661</v>
-      </c>
-      <c r="B62" t="s">
-        <v>5662</v>
-      </c>
-      <c r="C62" t="s">
-        <v>5663</v>
-      </c>
-      <c r="D62" t="s">
-        <v>5658</v>
-      </c>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A77" s="3"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A79" s="3"/>
-    </row>
-  </sheetData>
-  <autoFilter ref="A1:D61" xr:uid="{00000000-0001-0000-0100-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D61">
-      <sortCondition ref="D1:D61"/>
-    </sortState>
-  </autoFilter>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Planilha7"/>
   <dimension ref="A1:C16"/>
@@ -18827,6 +17928,908 @@
       <c r="B16" s="3"/>
     </row>
   </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:D79"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F60" sqref="F60"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="33.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3351</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3408</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>5660</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3387</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3742</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3904</v>
+      </c>
+      <c r="D2" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3382</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3383</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3904</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3767</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3768</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3904</v>
+      </c>
+      <c r="D4" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3378</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3380</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3904</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3372</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3376</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3904</v>
+      </c>
+      <c r="D6" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3371</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3375</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3904</v>
+      </c>
+      <c r="D7" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3392</v>
+      </c>
+      <c r="B8" t="s">
+        <v>3393</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3904</v>
+      </c>
+      <c r="D8" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="4" t="s">
+        <v>3390</v>
+      </c>
+      <c r="B9" t="s">
+        <v>3391</v>
+      </c>
+      <c r="C9" t="s">
+        <v>3904</v>
+      </c>
+      <c r="D9" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3388</v>
+      </c>
+      <c r="B10" t="s">
+        <v>3389</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3904</v>
+      </c>
+      <c r="D10" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3379</v>
+      </c>
+      <c r="B11" t="s">
+        <v>3381</v>
+      </c>
+      <c r="C11" t="s">
+        <v>3904</v>
+      </c>
+      <c r="D11" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3370</v>
+      </c>
+      <c r="B12" t="s">
+        <v>3374</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3904</v>
+      </c>
+      <c r="D12" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3384</v>
+      </c>
+      <c r="B13" t="s">
+        <v>3385</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3904</v>
+      </c>
+      <c r="D13" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3373</v>
+      </c>
+      <c r="B14" t="s">
+        <v>3377</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3904</v>
+      </c>
+      <c r="D14" t="s">
+        <v>3904</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>4053</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4054</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4056</v>
+      </c>
+      <c r="D15" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>4052</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4056</v>
+      </c>
+      <c r="D16" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>5653</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>5656</v>
+      </c>
+      <c r="C17" t="s">
+        <v>5656</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5651</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>5654</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5656</v>
+      </c>
+      <c r="D18" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>5652</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>5655</v>
+      </c>
+      <c r="C19" t="s">
+        <v>5656</v>
+      </c>
+      <c r="D19" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3747</v>
+      </c>
+      <c r="B20" t="s">
+        <v>3806</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3905</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3748</v>
+      </c>
+      <c r="B21" t="s">
+        <v>3805</v>
+      </c>
+      <c r="C21" t="s">
+        <v>3905</v>
+      </c>
+      <c r="D21" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3790</v>
+      </c>
+      <c r="B22" t="s">
+        <v>3791</v>
+      </c>
+      <c r="C22" t="s">
+        <v>3903</v>
+      </c>
+      <c r="D22" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3397</v>
+      </c>
+      <c r="B23" t="s">
+        <v>3396</v>
+      </c>
+      <c r="C23" t="s">
+        <v>3903</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3364</v>
+      </c>
+      <c r="B24" t="s">
+        <v>3368</v>
+      </c>
+      <c r="C24" t="s">
+        <v>3903</v>
+      </c>
+      <c r="D24" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3363</v>
+      </c>
+      <c r="B25" t="s">
+        <v>3367</v>
+      </c>
+      <c r="C25" t="s">
+        <v>3903</v>
+      </c>
+      <c r="D25" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3361</v>
+      </c>
+      <c r="B26" t="s">
+        <v>3365</v>
+      </c>
+      <c r="C26" t="s">
+        <v>3903</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>3762</v>
+      </c>
+      <c r="B27" t="s">
+        <v>3765</v>
+      </c>
+      <c r="C27" t="s">
+        <v>3903</v>
+      </c>
+      <c r="D27" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>3763</v>
+      </c>
+      <c r="B28" t="s">
+        <v>3766</v>
+      </c>
+      <c r="C28" t="s">
+        <v>3903</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3761</v>
+      </c>
+      <c r="B29" t="s">
+        <v>3764</v>
+      </c>
+      <c r="C29" t="s">
+        <v>3903</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>3362</v>
+      </c>
+      <c r="B30" t="s">
+        <v>3366</v>
+      </c>
+      <c r="C30" t="s">
+        <v>3903</v>
+      </c>
+      <c r="D30" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>3358</v>
+      </c>
+      <c r="B31" t="s">
+        <v>3395</v>
+      </c>
+      <c r="C31" t="s">
+        <v>3912</v>
+      </c>
+      <c r="D31" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3401</v>
+      </c>
+      <c r="B32" t="s">
+        <v>3404</v>
+      </c>
+      <c r="C32" t="s">
+        <v>3907</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>3402</v>
+      </c>
+      <c r="B33" t="s">
+        <v>3405</v>
+      </c>
+      <c r="C33" t="s">
+        <v>3907</v>
+      </c>
+      <c r="D33" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>3403</v>
+      </c>
+      <c r="B34" t="s">
+        <v>3406</v>
+      </c>
+      <c r="C34" t="s">
+        <v>3907</v>
+      </c>
+      <c r="D34" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>3749</v>
+      </c>
+      <c r="B35" t="s">
+        <v>3750</v>
+      </c>
+      <c r="C35" t="s">
+        <v>3902</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>3751</v>
+      </c>
+      <c r="B36" t="s">
+        <v>3752</v>
+      </c>
+      <c r="C36" t="s">
+        <v>3902</v>
+      </c>
+      <c r="D36" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="4" t="s">
+        <v>3901</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>3902</v>
+      </c>
+      <c r="C37" t="s">
+        <v>3902</v>
+      </c>
+      <c r="D37" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>3754</v>
+      </c>
+      <c r="B38" t="s">
+        <v>3760</v>
+      </c>
+      <c r="C38" t="s">
+        <v>3906</v>
+      </c>
+      <c r="D38" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>3755</v>
+      </c>
+      <c r="B39" t="s">
+        <v>3758</v>
+      </c>
+      <c r="C39" t="s">
+        <v>3906</v>
+      </c>
+      <c r="D39" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>3756</v>
+      </c>
+      <c r="B40" t="s">
+        <v>3759</v>
+      </c>
+      <c r="C40" t="s">
+        <v>3906</v>
+      </c>
+      <c r="D40" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>3753</v>
+      </c>
+      <c r="B41" t="s">
+        <v>3757</v>
+      </c>
+      <c r="C41" t="s">
+        <v>3906</v>
+      </c>
+      <c r="D41" t="s">
+        <v>5657</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>4057</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4058</v>
+      </c>
+      <c r="C42" t="s">
+        <v>4058</v>
+      </c>
+      <c r="D42" t="s">
+        <v>5659</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>3400</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>3412</v>
+      </c>
+      <c r="C43" t="s">
+        <v>3909</v>
+      </c>
+      <c r="D43" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>3915</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>3916</v>
+      </c>
+      <c r="C44" t="s">
+        <v>3909</v>
+      </c>
+      <c r="D44" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>3357</v>
+      </c>
+      <c r="B45" t="s">
+        <v>3394</v>
+      </c>
+      <c r="C45" t="s">
+        <v>3909</v>
+      </c>
+      <c r="D45" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>3913</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>3914</v>
+      </c>
+      <c r="C46" t="s">
+        <v>3909</v>
+      </c>
+      <c r="D46" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>3356</v>
+      </c>
+      <c r="B47" t="s">
+        <v>3399</v>
+      </c>
+      <c r="C47" t="s">
+        <v>3909</v>
+      </c>
+      <c r="D47" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>3411</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>3409</v>
+      </c>
+      <c r="C48" t="s">
+        <v>3909</v>
+      </c>
+      <c r="D48" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>3359</v>
+      </c>
+      <c r="B49" t="s">
+        <v>3398</v>
+      </c>
+      <c r="C49" t="s">
+        <v>3909</v>
+      </c>
+      <c r="D49" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>3352</v>
+      </c>
+      <c r="B50" t="s">
+        <v>3354</v>
+      </c>
+      <c r="C50" t="s">
+        <v>3909</v>
+      </c>
+      <c r="D50" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>3353</v>
+      </c>
+      <c r="B51" t="s">
+        <v>3355</v>
+      </c>
+      <c r="C51" t="s">
+        <v>3909</v>
+      </c>
+      <c r="D51" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>4036</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>4035</v>
+      </c>
+      <c r="C52" t="s">
+        <v>3911</v>
+      </c>
+      <c r="D52" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>3796</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>3803</v>
+      </c>
+      <c r="C53" t="s">
+        <v>3911</v>
+      </c>
+      <c r="D53" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>3410</v>
+      </c>
+      <c r="B54" t="s">
+        <v>3804</v>
+      </c>
+      <c r="C54" t="s">
+        <v>3910</v>
+      </c>
+      <c r="D54" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>3797</v>
+      </c>
+      <c r="B55" t="s">
+        <v>3801</v>
+      </c>
+      <c r="C55" t="s">
+        <v>3910</v>
+      </c>
+      <c r="D55" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>3793</v>
+      </c>
+      <c r="B56" t="s">
+        <v>3800</v>
+      </c>
+      <c r="C56" t="s">
+        <v>3910</v>
+      </c>
+      <c r="D56" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="4" t="s">
+        <v>3795</v>
+      </c>
+      <c r="B57" t="s">
+        <v>3799</v>
+      </c>
+      <c r="C57" t="s">
+        <v>3910</v>
+      </c>
+      <c r="D57" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>3794</v>
+      </c>
+      <c r="B58" t="s">
+        <v>3802</v>
+      </c>
+      <c r="C58" t="s">
+        <v>3910</v>
+      </c>
+      <c r="D58" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>3792</v>
+      </c>
+      <c r="B59" t="s">
+        <v>3798</v>
+      </c>
+      <c r="C59" t="s">
+        <v>3910</v>
+      </c>
+      <c r="D59" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>3743</v>
+      </c>
+      <c r="B60" t="s">
+        <v>3745</v>
+      </c>
+      <c r="C60" t="s">
+        <v>3908</v>
+      </c>
+      <c r="D60" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>3744</v>
+      </c>
+      <c r="B61" t="s">
+        <v>3746</v>
+      </c>
+      <c r="C61" t="s">
+        <v>3908</v>
+      </c>
+      <c r="D61" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>5661</v>
+      </c>
+      <c r="B62" t="s">
+        <v>5662</v>
+      </c>
+      <c r="C62" t="s">
+        <v>5663</v>
+      </c>
+      <c r="D62" t="s">
+        <v>5658</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="3"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:D61" xr:uid="{00000000-0001-0000-0100-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D61">
+      <sortCondition ref="D1:D61"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
@@ -63446,9 +63449,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:E608"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C35" sqref="C35"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63847,7 +63850,7 @@
         <v>4182</v>
       </c>
       <c r="E23" t="s">
-        <v>4270</v>
+        <v>5664</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Inclusão de melhorias @202406240928
</commit_message>
<xml_diff>
--- a/data/cadastro-base.xlsx
+++ b/data/cadastro-base.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\_Cross Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB4C2BD5-4808-4BBF-996B-2C28775AD450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C436A2F3-96B1-42E0-98C9-26DD051B7F23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" tabRatio="754" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,14 +20,15 @@
     <sheet name="equities" sheetId="3" r:id="rId5"/>
     <sheet name="anbima" sheetId="13" r:id="rId6"/>
     <sheet name="fixed_income" sheetId="25" r:id="rId7"/>
-    <sheet name="indicators" sheetId="22" r:id="rId8"/>
-    <sheet name="Planilha1" sheetId="26" r:id="rId9"/>
+    <sheet name="jgp" sheetId="27" r:id="rId8"/>
+    <sheet name="indicators" sheetId="22" r:id="rId9"/>
+    <sheet name="Planilha1" sheetId="26" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">equities!$A$1:$L$1268</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">equity_signals!$A$1:$D$61</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">fixed_income_signals!$A$1:$C$15</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">indicators!$A$1:$E$600</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">indicators!$A$1:$E$600</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -50,7 +51,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15492" uniqueCount="5665">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15502" uniqueCount="5673">
   <si>
     <t>category</t>
   </si>
@@ -17045,6 +17046,30 @@
   </si>
   <si>
     <t>ICB</t>
+  </si>
+  <si>
+    <t>IDEXCDI Index</t>
+  </si>
+  <si>
+    <t>br_jgp_idex_cdi</t>
+  </si>
+  <si>
+    <t>jgp_idex_cdi_core</t>
+  </si>
+  <si>
+    <t>jgp_idex_cdi_geral</t>
+  </si>
+  <si>
+    <t>jgp_idex_cdi_low_rated</t>
+  </si>
+  <si>
+    <t>https://jgp-credito-s3.s3.sa-east-1.amazonaws.com/idex/idex_cdi_geral_datafile.xlsx</t>
+  </si>
+  <si>
+    <t>https://jgp-credito-s3.s3.sa-east-1.amazonaws.com/idex/idex_cdi_core_datafile.xlsx</t>
+  </si>
+  <si>
+    <t>https://jgp-credito-s3.s3.sa-east-1.amazonaws.com/idex/idex_cdi_low_rated_datafile.xlsx</t>
   </si>
 </sst>
 </file>
@@ -17792,6 +17817,157 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A168553-459F-4B39-B5B2-1331C03883DB}">
+  <dimension ref="A1:E8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>3435</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3434</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3544</v>
+      </c>
+      <c r="D1" t="s">
+        <v>4182</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4644</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3428</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3431</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3544</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4182</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4645</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3432</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3433</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3544</v>
+      </c>
+      <c r="D3" t="s">
+        <v>4182</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4646</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3424</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3425</v>
+      </c>
+      <c r="C4" t="s">
+        <v>3544</v>
+      </c>
+      <c r="D4" t="s">
+        <v>4182</v>
+      </c>
+      <c r="E4" t="s">
+        <v>4641</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3423</v>
+      </c>
+      <c r="B5" t="s">
+        <v>3422</v>
+      </c>
+      <c r="C5" t="s">
+        <v>3544</v>
+      </c>
+      <c r="D5" t="s">
+        <v>4182</v>
+      </c>
+      <c r="E5" t="s">
+        <v>4642</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3420</v>
+      </c>
+      <c r="B6" t="s">
+        <v>3421</v>
+      </c>
+      <c r="C6" t="s">
+        <v>3544</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4182</v>
+      </c>
+      <c r="E6" t="s">
+        <v>4643</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4117</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3427</v>
+      </c>
+      <c r="C7" t="s">
+        <v>3544</v>
+      </c>
+      <c r="D7" t="s">
+        <v>4182</v>
+      </c>
+      <c r="E7" t="s">
+        <v>4685</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3426</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4113</v>
+      </c>
+      <c r="C8" t="s">
+        <v>3544</v>
+      </c>
+      <c r="D8" t="s">
+        <v>4182</v>
+      </c>
+      <c r="E8" t="s">
+        <v>4647</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr codeName="Planilha7"/>
@@ -59241,7 +59417,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
+      <selection pane="bottomLeft" activeCell="G40" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59532,7 +59708,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63446,12 +63622,63 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:E608"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98FB1145-2B5C-4773-9AEB-92B09B76617C}">
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E22" sqref="E22"/>
+      <selection pane="bottomLeft" activeCell="O22" sqref="O22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3547</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3546</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5668</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5670</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5667</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5671</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5669</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5672</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
+  <dimension ref="A1:E609"/>
+  <sheetViews>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A591" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B609" sqref="B609"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -73591,6 +73818,14 @@
         <v>4667</v>
       </c>
     </row>
+    <row r="609" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A609" t="s">
+        <v>5665</v>
+      </c>
+      <c r="B609" t="s">
+        <v>5666</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:E600" xr:uid="{00000000-0009-0000-0000-000007000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E608">
@@ -73600,155 +73835,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A168553-459F-4B39-B5B2-1331C03883DB}">
-  <dimension ref="A1:E8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3435</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3434</v>
-      </c>
-      <c r="C1" t="s">
-        <v>3544</v>
-      </c>
-      <c r="D1" t="s">
-        <v>4182</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4644</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>3428</v>
-      </c>
-      <c r="B2" t="s">
-        <v>3431</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3544</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4182</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4645</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>3432</v>
-      </c>
-      <c r="B3" t="s">
-        <v>3433</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3544</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4182</v>
-      </c>
-      <c r="E3" t="s">
-        <v>4646</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3424</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3425</v>
-      </c>
-      <c r="C4" t="s">
-        <v>3544</v>
-      </c>
-      <c r="D4" t="s">
-        <v>4182</v>
-      </c>
-      <c r="E4" t="s">
-        <v>4641</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>3423</v>
-      </c>
-      <c r="B5" t="s">
-        <v>3422</v>
-      </c>
-      <c r="C5" t="s">
-        <v>3544</v>
-      </c>
-      <c r="D5" t="s">
-        <v>4182</v>
-      </c>
-      <c r="E5" t="s">
-        <v>4642</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>3420</v>
-      </c>
-      <c r="B6" t="s">
-        <v>3421</v>
-      </c>
-      <c r="C6" t="s">
-        <v>3544</v>
-      </c>
-      <c r="D6" t="s">
-        <v>4182</v>
-      </c>
-      <c r="E6" t="s">
-        <v>4643</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4117</v>
-      </c>
-      <c r="B7" t="s">
-        <v>3427</v>
-      </c>
-      <c r="C7" t="s">
-        <v>3544</v>
-      </c>
-      <c r="D7" t="s">
-        <v>4182</v>
-      </c>
-      <c r="E7" t="s">
-        <v>4685</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3426</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4113</v>
-      </c>
-      <c r="C8" t="s">
-        <v>3544</v>
-      </c>
-      <c r="D8" t="s">
-        <v>4182</v>
-      </c>
-      <c r="E8" t="s">
-        <v>4647</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>